<commit_message>
Ajuste semana 1. Acomodar actividades lunes-miercoles
</commit_message>
<xml_diff>
--- a/Programar_dias.xlsx
+++ b/Programar_dias.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Estudio\OneDrive - Universidad de Antioquia\Estudio\Materias\Informatica II\Calendario_semanal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B26B377-FCEC-4039-B32A-E29088CAD095}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5404D0EF-79F6-4B02-B1B8-BDA8314D6A56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{CC961CB2-F623-4B13-8239-4B70F16E4462}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{CC961CB2-F623-4B13-8239-4B70F16E4462}"/>
   </bookViews>
   <sheets>
     <sheet name="Semana 1" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="60">
   <si>
     <t>LUNES</t>
   </si>
@@ -257,9 +257,6 @@
     <t>Yoga</t>
   </si>
   <si>
-    <t>Repasar Circuitos</t>
-  </si>
-  <si>
     <t>Programar</t>
   </si>
   <si>
@@ -279,13 +276,16 @@
   </si>
   <si>
     <t>Feb 27- Marzo 5</t>
+  </si>
+  <si>
+    <t>Estudiar Fisica</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -343,8 +343,14 @@
       <name val="Yu Gothic UI"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Yu Gothic UI"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="20">
+  <fills count="21">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -459,6 +465,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF33CCFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="5">
     <border>
@@ -524,7 +536,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -551,11 +563,35 @@
     <xf numFmtId="0" fontId="2" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="19" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -563,31 +599,58 @@
     <xf numFmtId="0" fontId="2" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="14" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -602,28 +665,19 @@
     <xf numFmtId="0" fontId="1" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -632,53 +686,32 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="20" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="20" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="17" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="17" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="17" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="16" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="19" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="1" fillId="20" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="20" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="20" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -686,6 +719,12 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF33CCFF"/>
+      <color rgb="FF0099FF"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -996,8 +1035,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC99D917-8B13-4626-B576-50715BED7B7E}">
   <dimension ref="A1:J19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12:G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1042,9 +1081,7 @@
       <c r="A2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="10" t="s">
-        <v>28</v>
-      </c>
+      <c r="B2" s="3"/>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
@@ -1056,7 +1093,7 @@
       <c r="A3" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="11"/>
+      <c r="B3" s="3"/>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
@@ -1068,20 +1105,18 @@
       <c r="A4" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="51" t="s">
+      <c r="B4" s="3"/>
+      <c r="C4" s="13" t="s">
         <v>11</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="E4" s="51" t="s">
-        <v>11</v>
-      </c>
-      <c r="F4" s="46" t="s">
-        <v>55</v>
+      <c r="E4" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" s="11" t="s">
+        <v>54</v>
       </c>
       <c r="G4" s="3"/>
       <c r="H4" s="3"/>
@@ -1090,17 +1125,19 @@
       <c r="A5" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="3"/>
-      <c r="C5" s="20" t="s">
+      <c r="B5" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="57" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="46" t="s">
-        <v>55</v>
-      </c>
-      <c r="E5" s="20" t="s">
+      <c r="D5" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="E5" s="57" t="s">
         <v>13</v>
       </c>
-      <c r="F5" s="51" t="s">
+      <c r="F5" s="13" t="s">
         <v>11</v>
       </c>
       <c r="G5" s="4" t="s">
@@ -1114,43 +1151,43 @@
       <c r="A6" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="51" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" s="22"/>
-      <c r="D6" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="E6" s="22"/>
-      <c r="F6" s="27" t="s">
+      <c r="B6" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="59"/>
+      <c r="D6" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" s="59"/>
+      <c r="F6" s="57" t="s">
         <v>15</v>
       </c>
-      <c r="G6" s="46" t="s">
-        <v>55</v>
-      </c>
-      <c r="H6" s="46" t="s">
-        <v>55</v>
+      <c r="G6" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="H6" s="11" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="30" t="s">
+      <c r="B7" s="55" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="40" t="s">
-        <v>52</v>
-      </c>
-      <c r="D7" s="11"/>
-      <c r="E7" s="42" t="s">
+      <c r="C7" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7" s="3"/>
+      <c r="E7" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="F7" s="28"/>
-      <c r="G7" s="16" t="s">
+      <c r="F7" s="58"/>
+      <c r="G7" s="33" t="s">
         <v>49</v>
       </c>
-      <c r="H7" s="42" t="s">
+      <c r="H7" s="27" t="s">
         <v>19</v>
       </c>
     </row>
@@ -1158,39 +1195,39 @@
       <c r="A8" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="31"/>
-      <c r="C8" s="41"/>
-      <c r="D8" s="51" t="s">
-        <v>11</v>
-      </c>
-      <c r="E8" s="43"/>
-      <c r="F8" s="29"/>
-      <c r="G8" s="17"/>
-      <c r="H8" s="43"/>
+      <c r="B8" s="56"/>
+      <c r="C8" s="17"/>
+      <c r="D8" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="E8" s="28"/>
+      <c r="F8" s="59"/>
+      <c r="G8" s="34"/>
+      <c r="H8" s="28"/>
     </row>
     <row r="9" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B9" s="35" t="s">
-        <v>45</v>
-      </c>
-      <c r="C9" s="37" t="s">
+      <c r="B9" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" s="55" t="s">
         <v>22</v>
       </c>
-      <c r="D9" s="30" t="s">
+      <c r="D9" s="55" t="s">
         <v>17</v>
       </c>
-      <c r="E9" s="37" t="s">
+      <c r="E9" s="55" t="s">
         <v>22</v>
       </c>
-      <c r="F9" s="16" t="s">
+      <c r="F9" s="33" t="s">
         <v>49</v>
       </c>
-      <c r="G9" s="18" t="s">
+      <c r="G9" s="22" t="s">
         <v>50</v>
       </c>
-      <c r="H9" s="18" t="s">
+      <c r="H9" s="22" t="s">
         <v>50</v>
       </c>
     </row>
@@ -1198,31 +1235,31 @@
       <c r="A10" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B10" s="36"/>
-      <c r="C10" s="38"/>
-      <c r="D10" s="31"/>
-      <c r="E10" s="38"/>
-      <c r="F10" s="17"/>
-      <c r="G10" s="19"/>
-      <c r="H10" s="19"/>
+      <c r="B10" s="15"/>
+      <c r="C10" s="56"/>
+      <c r="D10" s="56"/>
+      <c r="E10" s="56"/>
+      <c r="F10" s="34"/>
+      <c r="G10" s="23"/>
+      <c r="H10" s="23"/>
     </row>
     <row r="11" spans="1:10" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B11" s="20" t="s">
+      <c r="B11" s="57" t="s">
         <v>25</v>
       </c>
-      <c r="C11" s="23" t="s">
+      <c r="C11" s="55" t="s">
         <v>26</v>
       </c>
-      <c r="D11" s="25" t="s">
+      <c r="D11" s="55" t="s">
         <v>27</v>
       </c>
-      <c r="E11" s="23" t="s">
+      <c r="E11" s="55" t="s">
         <v>26</v>
       </c>
-      <c r="F11" s="25" t="s">
+      <c r="F11" s="55" t="s">
         <v>44</v>
       </c>
       <c r="G11" s="3"/>
@@ -1232,15 +1269,15 @@
       <c r="A12" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="B12" s="21"/>
-      <c r="C12" s="24"/>
-      <c r="D12" s="26"/>
-      <c r="E12" s="24"/>
-      <c r="F12" s="26"/>
+      <c r="B12" s="58"/>
+      <c r="C12" s="56"/>
+      <c r="D12" s="56"/>
+      <c r="E12" s="56"/>
+      <c r="F12" s="56"/>
       <c r="G12" s="44" t="s">
-        <v>54</v>
-      </c>
-      <c r="H12" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="H12" s="16" t="s">
         <v>28</v>
       </c>
     </row>
@@ -1248,8 +1285,8 @@
       <c r="A13" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B13" s="22"/>
-      <c r="C13" s="51" t="s">
+      <c r="B13" s="59"/>
+      <c r="C13" s="13" t="s">
         <v>11</v>
       </c>
       <c r="D13" s="7" t="s">
@@ -1260,29 +1297,27 @@
         <v>42</v>
       </c>
       <c r="G13" s="45"/>
-      <c r="H13" s="11"/>
+      <c r="H13" s="17"/>
     </row>
     <row r="14" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B14" s="51" t="s">
-        <v>11</v>
-      </c>
-      <c r="C14" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="D14" s="51" t="s">
+      <c r="B14" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="C14" s="3"/>
+      <c r="D14" s="13" t="s">
         <v>11</v>
       </c>
       <c r="E14" s="3"/>
-      <c r="F14" s="51" t="s">
-        <v>11</v>
-      </c>
-      <c r="G14" s="14" t="s">
+      <c r="F14" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="G14" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="H14" s="12" t="s">
+      <c r="H14" s="20" t="s">
         <v>18</v>
       </c>
       <c r="J14" s="8"/>
@@ -1291,37 +1326,37 @@
       <c r="A15" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="B15" s="16" t="s">
-        <v>49</v>
-      </c>
-      <c r="C15" s="11"/>
-      <c r="D15" s="12" t="s">
+      <c r="B15" s="3"/>
+      <c r="C15" s="53" t="s">
+        <v>45</v>
+      </c>
+      <c r="D15" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="E15" s="51" t="s">
-        <v>11</v>
-      </c>
-      <c r="F15" s="32" t="s">
+      <c r="E15" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="F15" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="G15" s="15"/>
-      <c r="H15" s="13"/>
+      <c r="G15" s="19"/>
+      <c r="H15" s="21"/>
     </row>
     <row r="16" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="B16" s="17"/>
-      <c r="C16" s="3"/>
-      <c r="D16" s="13"/>
-      <c r="E16" s="10" t="s">
+      <c r="B16" s="3"/>
+      <c r="C16" s="54"/>
+      <c r="D16" s="21"/>
+      <c r="E16" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="F16" s="33"/>
-      <c r="G16" s="10" t="s">
+      <c r="F16" s="25"/>
+      <c r="G16" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="H16" s="10" t="s">
+      <c r="H16" s="16" t="s">
         <v>28</v>
       </c>
     </row>
@@ -1329,30 +1364,29 @@
       <c r="A17" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="B17" s="46" t="s">
-        <v>55</v>
-      </c>
-      <c r="C17" s="3"/>
-      <c r="D17" s="14" t="s">
+      <c r="B17" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="D17" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="E17" s="11"/>
-      <c r="F17" s="34"/>
-      <c r="G17" s="11"/>
-      <c r="H17" s="11"/>
+      <c r="E17" s="17"/>
+      <c r="F17" s="26"/>
+      <c r="G17" s="17"/>
+      <c r="H17" s="17"/>
     </row>
     <row r="18" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="B18" s="12" t="s">
+      <c r="B18" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="C18" s="18" t="s">
-        <v>50</v>
-      </c>
-      <c r="D18" s="15"/>
-      <c r="E18" s="18" t="s">
+      <c r="C18" s="53" t="s">
+        <v>45</v>
+      </c>
+      <c r="D18" s="19"/>
+      <c r="E18" s="22" t="s">
         <v>50</v>
       </c>
       <c r="F18" s="3"/>
@@ -1363,28 +1397,30 @@
       <c r="A19" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="B19" s="13"/>
-      <c r="C19" s="19"/>
+      <c r="B19" s="21"/>
+      <c r="C19" s="54"/>
       <c r="D19" s="3"/>
-      <c r="E19" s="19"/>
+      <c r="E19" s="23"/>
       <c r="F19" s="3"/>
       <c r="G19" s="3"/>
       <c r="H19" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="37">
-    <mergeCell ref="E16:E17"/>
+  <mergeCells count="33">
     <mergeCell ref="B18:B19"/>
     <mergeCell ref="G9:G10"/>
     <mergeCell ref="G12:G13"/>
-    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="B11:B13"/>
+    <mergeCell ref="E11:E12"/>
+    <mergeCell ref="F11:F12"/>
+    <mergeCell ref="C15:C16"/>
     <mergeCell ref="H7:H8"/>
     <mergeCell ref="C9:C10"/>
     <mergeCell ref="D9:D10"/>
     <mergeCell ref="E9:E10"/>
     <mergeCell ref="H12:H13"/>
     <mergeCell ref="C7:C8"/>
-    <mergeCell ref="D6:D7"/>
     <mergeCell ref="F9:F10"/>
     <mergeCell ref="E7:E8"/>
     <mergeCell ref="H9:H10"/>
@@ -1392,24 +1428,18 @@
     <mergeCell ref="C5:C6"/>
     <mergeCell ref="E5:E6"/>
     <mergeCell ref="F6:F8"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="B11:B13"/>
     <mergeCell ref="C11:C12"/>
     <mergeCell ref="D11:D12"/>
-    <mergeCell ref="E11:E12"/>
-    <mergeCell ref="F11:F12"/>
     <mergeCell ref="H16:H17"/>
     <mergeCell ref="D17:D18"/>
-    <mergeCell ref="C14:C15"/>
     <mergeCell ref="H14:H15"/>
-    <mergeCell ref="B15:B16"/>
     <mergeCell ref="D15:D16"/>
     <mergeCell ref="C18:C19"/>
     <mergeCell ref="E18:E19"/>
     <mergeCell ref="G14:G15"/>
     <mergeCell ref="G16:G17"/>
     <mergeCell ref="F15:F17"/>
+    <mergeCell ref="E16:E17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1420,8 +1450,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF8929EB-A174-48F2-BDBD-469036EC404B}">
   <dimension ref="A1:H19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6:D7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" activeCellId="1" sqref="B3 B4:B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1484,12 +1514,12 @@
       <c r="G3" s="3"/>
       <c r="H3" s="3"/>
     </row>
-    <row r="4" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="50" t="s">
-        <v>58</v>
+      <c r="B4" s="51" t="s">
+        <v>57</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>11</v>
@@ -1500,8 +1530,8 @@
       <c r="E4" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="F4" s="46" t="s">
-        <v>55</v>
+      <c r="F4" s="11" t="s">
+        <v>54</v>
       </c>
       <c r="G4" s="3"/>
       <c r="H4" s="4" t="s">
@@ -1512,14 +1542,14 @@
       <c r="A5" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="19"/>
-      <c r="C5" s="20" t="s">
+      <c r="B5" s="52"/>
+      <c r="C5" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="46" t="s">
-        <v>55</v>
-      </c>
-      <c r="E5" s="20" t="s">
+      <c r="D5" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="E5" s="35" t="s">
         <v>13</v>
       </c>
       <c r="F5" s="5" t="s">
@@ -1537,40 +1567,40 @@
       <c r="B6" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="22"/>
+      <c r="C6" s="36"/>
       <c r="D6" s="44" t="s">
+        <v>53</v>
+      </c>
+      <c r="E6" s="36"/>
+      <c r="F6" s="37" t="s">
+        <v>15</v>
+      </c>
+      <c r="G6" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="E6" s="22"/>
-      <c r="F6" s="27" t="s">
-        <v>15</v>
-      </c>
-      <c r="G6" s="46" t="s">
-        <v>55</v>
-      </c>
-      <c r="H6" s="46" t="s">
-        <v>55</v>
+      <c r="H6" s="11" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="30" t="s">
+      <c r="B7" s="31" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="18" t="s">
+      <c r="C7" s="22" t="s">
         <v>50</v>
       </c>
       <c r="D7" s="45"/>
       <c r="E7" s="44" t="s">
-        <v>54</v>
-      </c>
-      <c r="F7" s="28"/>
-      <c r="G7" s="32" t="s">
+        <v>53</v>
+      </c>
+      <c r="F7" s="38"/>
+      <c r="G7" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="H7" s="14" t="s">
+      <c r="H7" s="18" t="s">
         <v>19</v>
       </c>
     </row>
@@ -1578,35 +1608,35 @@
       <c r="A8" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="31"/>
-      <c r="C8" s="19"/>
+      <c r="B8" s="32"/>
+      <c r="C8" s="23"/>
       <c r="D8" s="5" t="s">
         <v>11</v>
       </c>
       <c r="E8" s="45"/>
-      <c r="F8" s="29"/>
-      <c r="G8" s="33"/>
-      <c r="H8" s="15"/>
+      <c r="F8" s="39"/>
+      <c r="G8" s="25"/>
+      <c r="H8" s="19"/>
     </row>
     <row r="9" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B9" s="10" t="s">
+      <c r="B9" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="C9" s="48" t="s">
-        <v>57</v>
-      </c>
-      <c r="D9" s="30" t="s">
+      <c r="C9" s="47" t="s">
+        <v>56</v>
+      </c>
+      <c r="D9" s="31" t="s">
         <v>43</v>
       </c>
-      <c r="E9" s="48" t="s">
-        <v>57</v>
+      <c r="E9" s="47" t="s">
+        <v>56</v>
       </c>
       <c r="F9" s="3"/>
-      <c r="G9" s="34"/>
-      <c r="H9" s="35" t="s">
+      <c r="G9" s="26"/>
+      <c r="H9" s="49" t="s">
         <v>45</v>
       </c>
     </row>
@@ -1614,34 +1644,34 @@
       <c r="A10" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B10" s="11"/>
-      <c r="C10" s="49"/>
-      <c r="D10" s="31"/>
-      <c r="E10" s="49"/>
+      <c r="B10" s="17"/>
+      <c r="C10" s="48"/>
+      <c r="D10" s="32"/>
+      <c r="E10" s="48"/>
       <c r="F10" s="3"/>
       <c r="G10" s="3"/>
-      <c r="H10" s="36"/>
+      <c r="H10" s="50"/>
     </row>
     <row r="11" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B11" s="20" t="s">
+      <c r="B11" s="35" t="s">
         <v>25</v>
       </c>
-      <c r="C11" s="23" t="s">
+      <c r="C11" s="40" t="s">
         <v>47</v>
       </c>
-      <c r="D11" s="25" t="s">
+      <c r="D11" s="42" t="s">
         <v>46</v>
       </c>
-      <c r="E11" s="27" t="s">
-        <v>56</v>
-      </c>
-      <c r="F11" s="25" t="s">
+      <c r="E11" s="37" t="s">
+        <v>55</v>
+      </c>
+      <c r="F11" s="42" t="s">
         <v>27</v>
       </c>
-      <c r="G11" s="10" t="s">
+      <c r="G11" s="16" t="s">
         <v>28</v>
       </c>
       <c r="H11" s="3"/>
@@ -1650,19 +1680,19 @@
       <c r="A12" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="B12" s="21"/>
-      <c r="C12" s="24"/>
-      <c r="D12" s="26"/>
-      <c r="E12" s="29"/>
-      <c r="F12" s="26"/>
-      <c r="G12" s="11"/>
+      <c r="B12" s="46"/>
+      <c r="C12" s="41"/>
+      <c r="D12" s="43"/>
+      <c r="E12" s="39"/>
+      <c r="F12" s="43"/>
+      <c r="G12" s="17"/>
       <c r="H12" s="3"/>
     </row>
     <row r="13" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B13" s="22"/>
+      <c r="B13" s="36"/>
       <c r="C13" s="5" t="s">
         <v>11</v>
       </c>
@@ -1685,22 +1715,22 @@
       <c r="B14" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="10" t="s">
+      <c r="C14" s="16" t="s">
         <v>28</v>
       </c>
       <c r="D14" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E14" s="16" t="s">
+      <c r="E14" s="33" t="s">
         <v>33</v>
       </c>
       <c r="F14" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="G14" s="14" t="s">
+      <c r="G14" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="H14" s="16" t="s">
+      <c r="H14" s="33" t="s">
         <v>33</v>
       </c>
     </row>
@@ -1708,37 +1738,37 @@
       <c r="A15" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="B15" s="14" t="s">
+      <c r="B15" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="C15" s="11"/>
-      <c r="D15" s="32" t="s">
+      <c r="C15" s="17"/>
+      <c r="D15" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="E15" s="17"/>
-      <c r="F15" s="16" t="s">
+      <c r="E15" s="34"/>
+      <c r="F15" s="33" t="s">
         <v>33</v>
       </c>
-      <c r="G15" s="15"/>
-      <c r="H15" s="17"/>
+      <c r="G15" s="19"/>
+      <c r="H15" s="34"/>
     </row>
     <row r="16" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="B16" s="15"/>
-      <c r="C16" s="16" t="s">
+      <c r="B16" s="19"/>
+      <c r="C16" s="33" t="s">
         <v>33</v>
       </c>
-      <c r="D16" s="33"/>
-      <c r="E16" s="46" t="s">
-        <v>55</v>
-      </c>
-      <c r="F16" s="17"/>
-      <c r="G16" s="16" t="s">
+      <c r="D16" s="25"/>
+      <c r="E16" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="F16" s="34"/>
+      <c r="G16" s="33" t="s">
         <v>33</v>
       </c>
-      <c r="H16" s="10" t="s">
+      <c r="H16" s="16" t="s">
         <v>28</v>
       </c>
     </row>
@@ -1746,28 +1776,28 @@
       <c r="A17" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="B17" s="12" t="s">
+      <c r="B17" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="C17" s="17"/>
-      <c r="D17" s="34"/>
-      <c r="E17" s="35" t="s">
+      <c r="C17" s="34"/>
+      <c r="D17" s="26"/>
+      <c r="E17" s="49" t="s">
         <v>45</v>
       </c>
       <c r="F17" s="3"/>
-      <c r="G17" s="17"/>
-      <c r="H17" s="11"/>
+      <c r="G17" s="34"/>
+      <c r="H17" s="17"/>
     </row>
     <row r="18" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="B18" s="13"/>
-      <c r="C18" s="46" t="s">
-        <v>55</v>
+      <c r="B18" s="21"/>
+      <c r="C18" s="11" t="s">
+        <v>54</v>
       </c>
       <c r="D18" s="3"/>
-      <c r="E18" s="36"/>
+      <c r="E18" s="50"/>
       <c r="F18" s="3"/>
       <c r="G18" s="3"/>
       <c r="H18" s="3"/>
@@ -1786,8 +1816,6 @@
     </row>
   </sheetData>
   <mergeCells count="33">
-    <mergeCell ref="D15:D17"/>
-    <mergeCell ref="E17:E18"/>
     <mergeCell ref="H16:H17"/>
     <mergeCell ref="B17:B18"/>
     <mergeCell ref="E14:E15"/>
@@ -1797,13 +1825,14 @@
     <mergeCell ref="C16:C17"/>
     <mergeCell ref="H14:H15"/>
     <mergeCell ref="G16:G17"/>
-    <mergeCell ref="E7:E8"/>
     <mergeCell ref="F15:F16"/>
     <mergeCell ref="B11:B13"/>
     <mergeCell ref="C11:C12"/>
     <mergeCell ref="D11:D12"/>
     <mergeCell ref="E11:E12"/>
     <mergeCell ref="F11:F12"/>
+    <mergeCell ref="D15:D17"/>
+    <mergeCell ref="E17:E18"/>
     <mergeCell ref="C5:C6"/>
     <mergeCell ref="E5:E6"/>
     <mergeCell ref="F6:F8"/>
@@ -1813,6 +1842,7 @@
     <mergeCell ref="C7:C8"/>
     <mergeCell ref="D6:D7"/>
     <mergeCell ref="B4:B5"/>
+    <mergeCell ref="E7:E8"/>
     <mergeCell ref="H7:H8"/>
     <mergeCell ref="C9:C10"/>
     <mergeCell ref="D9:D10"/>
@@ -1847,7 +1877,7 @@
   <sheetData>
     <row r="1" spans="1:8" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -1911,8 +1941,8 @@
       <c r="E4" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="F4" s="52" t="s">
-        <v>55</v>
+      <c r="F4" s="14" t="s">
+        <v>54</v>
       </c>
       <c r="G4" s="3"/>
       <c r="H4" s="3"/>
@@ -1921,16 +1951,16 @@
       <c r="A5" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="52" t="s">
-        <v>55</v>
-      </c>
-      <c r="C5" s="20" t="s">
+      <c r="B5" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="C5" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="52" t="s">
-        <v>55</v>
-      </c>
-      <c r="E5" s="20" t="s">
+      <c r="D5" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="E5" s="35" t="s">
         <v>13</v>
       </c>
       <c r="F5" s="5" t="s">
@@ -1950,40 +1980,40 @@
       <c r="B6" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="22"/>
+      <c r="C6" s="36"/>
       <c r="D6" s="44" t="s">
+        <v>53</v>
+      </c>
+      <c r="E6" s="36"/>
+      <c r="F6" s="37" t="s">
+        <v>15</v>
+      </c>
+      <c r="G6" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="E6" s="22"/>
-      <c r="F6" s="27" t="s">
-        <v>15</v>
-      </c>
-      <c r="G6" s="52" t="s">
-        <v>55</v>
-      </c>
-      <c r="H6" s="52" t="s">
-        <v>55</v>
+      <c r="H6" s="14" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="30" t="s">
+      <c r="B7" s="31" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="35" t="s">
+      <c r="C7" s="49" t="s">
         <v>45</v>
       </c>
       <c r="D7" s="45"/>
       <c r="E7" s="44" t="s">
-        <v>54</v>
-      </c>
-      <c r="F7" s="28"/>
-      <c r="G7" s="32" t="s">
+        <v>53</v>
+      </c>
+      <c r="F7" s="38"/>
+      <c r="G7" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="H7" s="14" t="s">
+      <c r="H7" s="18" t="s">
         <v>19</v>
       </c>
     </row>
@@ -1991,37 +2021,37 @@
       <c r="A8" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="31"/>
-      <c r="C8" s="36"/>
+      <c r="B8" s="32"/>
+      <c r="C8" s="50"/>
       <c r="D8" s="5" t="s">
         <v>11</v>
       </c>
       <c r="E8" s="45"/>
-      <c r="F8" s="29"/>
-      <c r="G8" s="33"/>
-      <c r="H8" s="15"/>
+      <c r="F8" s="39"/>
+      <c r="G8" s="25"/>
+      <c r="H8" s="19"/>
     </row>
     <row r="9" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B9" s="10" t="s">
+      <c r="B9" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="C9" s="37" t="s">
+      <c r="C9" s="29" t="s">
         <v>48</v>
       </c>
-      <c r="D9" s="30" t="s">
+      <c r="D9" s="31" t="s">
         <v>17</v>
       </c>
-      <c r="E9" s="37" t="s">
+      <c r="E9" s="29" t="s">
         <v>22</v>
       </c>
-      <c r="F9" s="50" t="s">
-        <v>58</v>
-      </c>
-      <c r="G9" s="34"/>
-      <c r="H9" s="35" t="s">
+      <c r="F9" s="51" t="s">
+        <v>57</v>
+      </c>
+      <c r="G9" s="26"/>
+      <c r="H9" s="49" t="s">
         <v>45</v>
       </c>
     </row>
@@ -2029,34 +2059,34 @@
       <c r="A10" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B10" s="11"/>
-      <c r="C10" s="38"/>
-      <c r="D10" s="31"/>
-      <c r="E10" s="38"/>
-      <c r="F10" s="19"/>
+      <c r="B10" s="17"/>
+      <c r="C10" s="30"/>
+      <c r="D10" s="32"/>
+      <c r="E10" s="30"/>
+      <c r="F10" s="23"/>
       <c r="G10" s="3"/>
-      <c r="H10" s="36"/>
+      <c r="H10" s="50"/>
     </row>
     <row r="11" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B11" s="20" t="s">
+      <c r="B11" s="35" t="s">
         <v>25</v>
       </c>
-      <c r="C11" s="23" t="s">
+      <c r="C11" s="40" t="s">
         <v>26</v>
       </c>
-      <c r="D11" s="25" t="s">
+      <c r="D11" s="42" t="s">
         <v>27</v>
       </c>
-      <c r="E11" s="23" t="s">
+      <c r="E11" s="40" t="s">
         <v>26</v>
       </c>
-      <c r="F11" s="25" t="s">
+      <c r="F11" s="42" t="s">
         <v>27</v>
       </c>
-      <c r="G11" s="10" t="s">
+      <c r="G11" s="16" t="s">
         <v>28</v>
       </c>
       <c r="H11" s="3"/>
@@ -2065,26 +2095,26 @@
       <c r="A12" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="B12" s="21"/>
-      <c r="C12" s="24"/>
-      <c r="D12" s="26"/>
-      <c r="E12" s="24"/>
-      <c r="F12" s="26"/>
-      <c r="G12" s="11"/>
+      <c r="B12" s="46"/>
+      <c r="C12" s="41"/>
+      <c r="D12" s="43"/>
+      <c r="E12" s="41"/>
+      <c r="F12" s="43"/>
+      <c r="G12" s="17"/>
       <c r="H12" s="3"/>
     </row>
     <row r="13" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B13" s="22"/>
-      <c r="C13" s="50" t="s">
-        <v>58</v>
+      <c r="B13" s="36"/>
+      <c r="C13" s="51" t="s">
+        <v>57</v>
       </c>
       <c r="D13" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="E13" s="10" t="s">
+      <c r="E13" s="16" t="s">
         <v>28</v>
       </c>
       <c r="F13" s="9" t="s">
@@ -2100,15 +2130,15 @@
       <c r="B14" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="19"/>
+      <c r="C14" s="23"/>
       <c r="D14" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E14" s="11"/>
+      <c r="E14" s="17"/>
       <c r="F14" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="G14" s="14" t="s">
+      <c r="G14" s="18" t="s">
         <v>19</v>
       </c>
       <c r="H14" s="3"/>
@@ -2117,41 +2147,41 @@
       <c r="A15" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="B15" s="16" t="s">
+      <c r="B15" s="33" t="s">
         <v>33</v>
       </c>
-      <c r="C15" s="39" t="s">
+      <c r="C15" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="D15" s="12" t="s">
+      <c r="D15" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="E15" s="39" t="s">
+      <c r="E15" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="F15" s="12" t="s">
+      <c r="F15" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="G15" s="15"/>
+      <c r="G15" s="19"/>
       <c r="H15" s="3"/>
     </row>
     <row r="16" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="B16" s="17"/>
+      <c r="B16" s="34"/>
       <c r="C16" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D16" s="13"/>
+      <c r="D16" s="21"/>
       <c r="E16" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="F16" s="13"/>
-      <c r="G16" s="35" t="s">
+      <c r="F16" s="21"/>
+      <c r="G16" s="49" t="s">
         <v>45</v>
       </c>
-      <c r="H16" s="10" t="s">
+      <c r="H16" s="16" t="s">
         <v>28</v>
       </c>
     </row>
@@ -2159,29 +2189,29 @@
       <c r="A17" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="B17" s="12" t="s">
+      <c r="B17" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="C17" s="52" t="s">
-        <v>55</v>
-      </c>
-      <c r="D17" s="14" t="s">
+      <c r="C17" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="D17" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="E17" s="52" t="s">
-        <v>55</v>
+      <c r="E17" s="14" t="s">
+        <v>54</v>
       </c>
       <c r="F17" s="3"/>
-      <c r="G17" s="36"/>
-      <c r="H17" s="11"/>
+      <c r="G17" s="50"/>
+      <c r="H17" s="17"/>
     </row>
     <row r="18" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="B18" s="13"/>
+      <c r="B18" s="21"/>
       <c r="C18" s="3"/>
-      <c r="D18" s="15"/>
+      <c r="D18" s="19"/>
       <c r="E18" s="3"/>
       <c r="F18" s="3"/>
       <c r="G18" s="3"/>
@@ -2321,8 +2351,8 @@
       <c r="E4" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="F4" s="52" t="s">
-        <v>55</v>
+      <c r="F4" s="14" t="s">
+        <v>54</v>
       </c>
       <c r="G4" s="3"/>
       <c r="H4" s="3"/>
@@ -2331,16 +2361,16 @@
       <c r="A5" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="52" t="s">
-        <v>55</v>
-      </c>
-      <c r="C5" s="20" t="s">
+      <c r="B5" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="C5" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="52" t="s">
-        <v>55</v>
-      </c>
-      <c r="E5" s="20" t="s">
+      <c r="D5" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="E5" s="35" t="s">
         <v>13</v>
       </c>
       <c r="F5" s="5" t="s">
@@ -2360,38 +2390,38 @@
       <c r="B6" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="22"/>
+      <c r="C6" s="36"/>
       <c r="D6" s="3"/>
-      <c r="E6" s="22"/>
-      <c r="F6" s="27" t="s">
+      <c r="E6" s="36"/>
+      <c r="F6" s="37" t="s">
         <v>15</v>
       </c>
-      <c r="G6" s="52" t="s">
-        <v>55</v>
-      </c>
-      <c r="H6" s="52" t="s">
-        <v>55</v>
+      <c r="G6" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="H6" s="14" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="30" t="s">
+      <c r="B7" s="31" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="35" t="s">
+      <c r="C7" s="49" t="s">
         <v>45</v>
       </c>
-      <c r="D7" s="47" t="s">
-        <v>53</v>
+      <c r="D7" s="12" t="s">
+        <v>52</v>
       </c>
       <c r="E7" s="3"/>
-      <c r="F7" s="28"/>
-      <c r="G7" s="32" t="s">
+      <c r="F7" s="38"/>
+      <c r="G7" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="H7" s="14" t="s">
+      <c r="H7" s="18" t="s">
         <v>19</v>
       </c>
     </row>
@@ -2399,35 +2429,35 @@
       <c r="A8" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="31"/>
-      <c r="C8" s="36"/>
+      <c r="B8" s="32"/>
+      <c r="C8" s="50"/>
       <c r="D8" s="5" t="s">
         <v>11</v>
       </c>
       <c r="E8" s="3"/>
-      <c r="F8" s="29"/>
-      <c r="G8" s="33"/>
-      <c r="H8" s="15"/>
+      <c r="F8" s="39"/>
+      <c r="G8" s="25"/>
+      <c r="H8" s="19"/>
     </row>
     <row r="9" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B9" s="10" t="s">
+      <c r="B9" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="C9" s="37" t="s">
+      <c r="C9" s="29" t="s">
         <v>22</v>
       </c>
-      <c r="D9" s="30" t="s">
+      <c r="D9" s="31" t="s">
         <v>17</v>
       </c>
-      <c r="E9" s="37" t="s">
+      <c r="E9" s="29" t="s">
         <v>22</v>
       </c>
       <c r="F9" s="3"/>
-      <c r="G9" s="34"/>
-      <c r="H9" s="10" t="s">
+      <c r="G9" s="26"/>
+      <c r="H9" s="16" t="s">
         <v>28</v>
       </c>
     </row>
@@ -2435,34 +2465,34 @@
       <c r="A10" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B10" s="11"/>
-      <c r="C10" s="38"/>
-      <c r="D10" s="31"/>
-      <c r="E10" s="38"/>
+      <c r="B10" s="17"/>
+      <c r="C10" s="30"/>
+      <c r="D10" s="32"/>
+      <c r="E10" s="30"/>
       <c r="F10" s="3"/>
       <c r="G10" s="3"/>
-      <c r="H10" s="11"/>
+      <c r="H10" s="17"/>
     </row>
     <row r="11" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B11" s="20" t="s">
+      <c r="B11" s="35" t="s">
         <v>25</v>
       </c>
-      <c r="C11" s="23" t="s">
+      <c r="C11" s="40" t="s">
         <v>26</v>
       </c>
-      <c r="D11" s="25" t="s">
+      <c r="D11" s="42" t="s">
         <v>27</v>
       </c>
-      <c r="E11" s="23" t="s">
+      <c r="E11" s="40" t="s">
         <v>26</v>
       </c>
-      <c r="F11" s="25" t="s">
+      <c r="F11" s="42" t="s">
         <v>27</v>
       </c>
-      <c r="G11" s="10" t="s">
+      <c r="G11" s="16" t="s">
         <v>28</v>
       </c>
       <c r="H11" s="3"/>
@@ -2471,27 +2501,27 @@
       <c r="A12" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="B12" s="21"/>
-      <c r="C12" s="24"/>
-      <c r="D12" s="26"/>
-      <c r="E12" s="24"/>
-      <c r="F12" s="26"/>
-      <c r="G12" s="11"/>
+      <c r="B12" s="46"/>
+      <c r="C12" s="41"/>
+      <c r="D12" s="43"/>
+      <c r="E12" s="41"/>
+      <c r="F12" s="43"/>
+      <c r="G12" s="17"/>
       <c r="H12" s="3"/>
     </row>
     <row r="13" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B13" s="22"/>
+      <c r="B13" s="36"/>
       <c r="C13" s="44" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D13" s="7" t="s">
         <v>31</v>
       </c>
       <c r="E13" s="44" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F13" s="9" t="s">
         <v>42</v>
@@ -2514,7 +2544,7 @@
       <c r="F14" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="G14" s="12" t="s">
+      <c r="G14" s="20" t="s">
         <v>18</v>
       </c>
       <c r="H14" s="3"/>
@@ -2523,37 +2553,37 @@
       <c r="A15" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="B15" s="14" t="s">
+      <c r="B15" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="C15" s="39" t="s">
+      <c r="C15" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="D15" s="12" t="s">
+      <c r="D15" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="E15" s="39" t="s">
+      <c r="E15" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="F15" s="14" t="s">
+      <c r="F15" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="G15" s="13"/>
+      <c r="G15" s="21"/>
       <c r="H15" s="3"/>
     </row>
     <row r="16" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="B16" s="15"/>
+      <c r="B16" s="19"/>
       <c r="C16" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D16" s="13"/>
+      <c r="D16" s="21"/>
       <c r="E16" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="F16" s="15"/>
+      <c r="F16" s="19"/>
       <c r="G16" s="3"/>
       <c r="H16" s="3"/>
     </row>
@@ -2561,21 +2591,21 @@
       <c r="A17" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="B17" s="12" t="s">
+      <c r="B17" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="C17" s="52" t="s">
-        <v>55</v>
-      </c>
-      <c r="D17" s="14" t="s">
+      <c r="C17" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="D17" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="E17" s="52" t="s">
-        <v>55</v>
+      <c r="E17" s="14" t="s">
+        <v>54</v>
       </c>
       <c r="F17" s="3"/>
       <c r="G17" s="3"/>
-      <c r="H17" s="12" t="s">
+      <c r="H17" s="20" t="s">
         <v>18</v>
       </c>
     </row>
@@ -2583,13 +2613,13 @@
       <c r="A18" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="B18" s="13"/>
+      <c r="B18" s="21"/>
       <c r="C18" s="3"/>
-      <c r="D18" s="15"/>
+      <c r="D18" s="19"/>
       <c r="E18" s="3"/>
       <c r="F18" s="3"/>
       <c r="G18" s="3"/>
-      <c r="H18" s="13"/>
+      <c r="H18" s="21"/>
     </row>
     <row r="19" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
@@ -2605,7 +2635,12 @@
     </row>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="H9:H10"/>
+    <mergeCell ref="H17:H18"/>
+    <mergeCell ref="B11:B13"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="E11:E12"/>
+    <mergeCell ref="F11:F12"/>
     <mergeCell ref="B17:B18"/>
     <mergeCell ref="D17:D18"/>
     <mergeCell ref="G14:G15"/>
@@ -2614,12 +2649,6 @@
     <mergeCell ref="F15:F16"/>
     <mergeCell ref="C13:C14"/>
     <mergeCell ref="E13:E14"/>
-    <mergeCell ref="H17:H18"/>
-    <mergeCell ref="B11:B13"/>
-    <mergeCell ref="C11:C12"/>
-    <mergeCell ref="D11:D12"/>
-    <mergeCell ref="E11:E12"/>
-    <mergeCell ref="F11:F12"/>
     <mergeCell ref="C5:C6"/>
     <mergeCell ref="E5:E6"/>
     <mergeCell ref="F6:F8"/>
@@ -2632,6 +2661,7 @@
     <mergeCell ref="D9:D10"/>
     <mergeCell ref="E9:E10"/>
     <mergeCell ref="G11:G12"/>
+    <mergeCell ref="H9:H10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>

</xml_diff>

<commit_message>
Re ajuste semana 1
</commit_message>
<xml_diff>
--- a/Programar_dias.xlsx
+++ b/Programar_dias.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Estudio\OneDrive - Universidad de Antioquia\Estudio\Materias\Informatica II\Calendario_semanal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5404D0EF-79F6-4B02-B1B8-BDA8314D6A56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7705FF1-A41E-475B-AC1F-CF984CD49336}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{CC961CB2-F623-4B13-8239-4B70F16E4462}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="62">
   <si>
     <t>LUNES</t>
   </si>
@@ -204,21 +204,6 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">FÍSICA CAMP. </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Yu Gothic UI"/>
-        <family val="2"/>
-      </rPr>
-      <t>PARCIAL</t>
-    </r>
-  </si>
-  <si>
-    <r>
       <t xml:space="preserve">CIRCUITOS II. </t>
     </r>
     <r>
@@ -280,12 +265,34 @@
   <si>
     <t>Estudiar Fisica</t>
   </si>
+  <si>
+    <t>Estudiar Info II</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FÍSICA CAMP. </t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">FÍSICA CAMP. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Yu Gothic UI"/>
+        <family val="2"/>
+      </rPr>
+      <t>PARCIAL</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -349,8 +356,24 @@
       <name val="Yu Gothic UI"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Yu Gothic UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Yu Gothic UI"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="21">
+  <fills count="16">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -377,19 +400,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFD60093"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF9933"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -402,18 +413,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF00FF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -462,12 +461,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF33CCFF"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -536,7 +529,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -556,162 +549,150 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="17" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="19" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="17" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="17" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="16" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="16" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="20" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="20" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="20" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="20" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="20" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -721,6 +702,7 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFFFFF66"/>
       <color rgb="FF33CCFF"/>
       <color rgb="FF0099FF"/>
     </mruColors>
@@ -1035,8 +1017,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC99D917-8B13-4626-B576-50715BED7B7E}">
   <dimension ref="A1:J19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12:G13"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1115,8 +1097,8 @@
       <c r="E4" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="F4" s="11" t="s">
-        <v>54</v>
+      <c r="F4" s="14" t="s">
+        <v>53</v>
       </c>
       <c r="G4" s="3"/>
       <c r="H4" s="3"/>
@@ -1128,13 +1110,13 @@
       <c r="B5" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="57" t="s">
+      <c r="C5" s="44" t="s">
         <v>13</v>
       </c>
       <c r="D5" s="11" t="s">
-        <v>54</v>
-      </c>
-      <c r="E5" s="57" t="s">
+        <v>53</v>
+      </c>
+      <c r="E5" s="44" t="s">
         <v>13</v>
       </c>
       <c r="F5" s="13" t="s">
@@ -1154,40 +1136,40 @@
       <c r="B6" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="59"/>
+      <c r="C6" s="46"/>
       <c r="D6" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="E6" s="59"/>
-      <c r="F6" s="57" t="s">
+      <c r="E6" s="46"/>
+      <c r="F6" s="44" t="s">
         <v>15</v>
       </c>
-      <c r="G6" s="11" t="s">
-        <v>54</v>
-      </c>
-      <c r="H6" s="11" t="s">
-        <v>54</v>
+      <c r="G6" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="H6" s="14" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="55" t="s">
+      <c r="B7" s="47" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="16" t="s">
+      <c r="C7" s="26" t="s">
         <v>28</v>
       </c>
       <c r="D7" s="3"/>
-      <c r="E7" s="27" t="s">
-        <v>19</v>
-      </c>
-      <c r="F7" s="58"/>
-      <c r="G7" s="33" t="s">
+      <c r="E7" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="H7" s="27" t="s">
+      <c r="F7" s="45"/>
+      <c r="G7" s="28" t="s">
+        <v>48</v>
+      </c>
+      <c r="H7" s="24" t="s">
         <v>19</v>
       </c>
     </row>
@@ -1195,15 +1177,15 @@
       <c r="A8" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="56"/>
-      <c r="C8" s="17"/>
+      <c r="B8" s="48"/>
+      <c r="C8" s="27"/>
       <c r="D8" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="E8" s="28"/>
-      <c r="F8" s="59"/>
-      <c r="G8" s="34"/>
-      <c r="H8" s="28"/>
+        <v>58</v>
+      </c>
+      <c r="E8" s="19"/>
+      <c r="F8" s="46"/>
+      <c r="G8" s="29"/>
+      <c r="H8" s="25"/>
     </row>
     <row r="9" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
@@ -1212,23 +1194,23 @@
       <c r="B9" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="C9" s="55" t="s">
+      <c r="C9" s="47" t="s">
         <v>22</v>
       </c>
-      <c r="D9" s="55" t="s">
+      <c r="D9" s="47" t="s">
         <v>17</v>
       </c>
-      <c r="E9" s="55" t="s">
+      <c r="E9" s="47" t="s">
         <v>22</v>
       </c>
-      <c r="F9" s="33" t="s">
+      <c r="F9" s="28" t="s">
+        <v>48</v>
+      </c>
+      <c r="G9" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="G9" s="22" t="s">
-        <v>50</v>
-      </c>
-      <c r="H9" s="22" t="s">
-        <v>50</v>
+      <c r="H9" s="26" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="16.5" x14ac:dyDescent="0.3">
@@ -1236,31 +1218,31 @@
         <v>23</v>
       </c>
       <c r="B10" s="15"/>
-      <c r="C10" s="56"/>
-      <c r="D10" s="56"/>
-      <c r="E10" s="56"/>
-      <c r="F10" s="34"/>
-      <c r="G10" s="23"/>
-      <c r="H10" s="23"/>
+      <c r="C10" s="48"/>
+      <c r="D10" s="48"/>
+      <c r="E10" s="48"/>
+      <c r="F10" s="29"/>
+      <c r="G10" s="19"/>
+      <c r="H10" s="27"/>
     </row>
     <row r="11" spans="1:10" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B11" s="57" t="s">
+      <c r="B11" s="44" t="s">
         <v>25</v>
       </c>
-      <c r="C11" s="55" t="s">
+      <c r="C11" s="47" t="s">
         <v>26</v>
       </c>
-      <c r="D11" s="55" t="s">
+      <c r="D11" s="47" t="s">
         <v>27</v>
       </c>
-      <c r="E11" s="55" t="s">
+      <c r="E11" s="47" t="s">
         <v>26</v>
       </c>
-      <c r="F11" s="55" t="s">
-        <v>44</v>
+      <c r="F11" s="47" t="s">
+        <v>60</v>
       </c>
       <c r="G11" s="3"/>
       <c r="H11" s="3"/>
@@ -1269,15 +1251,15 @@
       <c r="A12" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="B12" s="58"/>
-      <c r="C12" s="56"/>
-      <c r="D12" s="56"/>
-      <c r="E12" s="56"/>
-      <c r="F12" s="56"/>
-      <c r="G12" s="44" t="s">
-        <v>53</v>
-      </c>
-      <c r="H12" s="16" t="s">
+      <c r="B12" s="45"/>
+      <c r="C12" s="48"/>
+      <c r="D12" s="48"/>
+      <c r="E12" s="48"/>
+      <c r="F12" s="48"/>
+      <c r="G12" s="20" t="s">
+        <v>52</v>
+      </c>
+      <c r="H12" s="26" t="s">
         <v>28</v>
       </c>
     </row>
@@ -1285,19 +1267,21 @@
       <c r="A13" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B13" s="59"/>
+      <c r="B13" s="46"/>
       <c r="C13" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="D13" s="7" t="s">
+      <c r="D13" s="39" t="s">
         <v>31</v>
       </c>
-      <c r="E13" s="3"/>
+      <c r="E13" s="13" t="s">
+        <v>11</v>
+      </c>
       <c r="F13" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="G13" s="45"/>
-      <c r="H13" s="17"/>
+      <c r="G13" s="21"/>
+      <c r="H13" s="27"/>
     </row>
     <row r="14" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
@@ -1307,17 +1291,12 @@
         <v>11</v>
       </c>
       <c r="C14" s="3"/>
-      <c r="D14" s="13" t="s">
-        <v>11</v>
-      </c>
+      <c r="D14" s="40"/>
       <c r="E14" s="3"/>
-      <c r="F14" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="G14" s="18" t="s">
+      <c r="G14" s="30" t="s">
         <v>19</v>
       </c>
-      <c r="H14" s="20" t="s">
+      <c r="H14" s="32" t="s">
         <v>18</v>
       </c>
       <c r="J14" s="8"/>
@@ -1327,69 +1306,66 @@
         <v>34</v>
       </c>
       <c r="B15" s="3"/>
-      <c r="C15" s="53" t="s">
+      <c r="C15" s="22" t="s">
         <v>45</v>
       </c>
-      <c r="D15" s="20" t="s">
-        <v>18</v>
-      </c>
-      <c r="E15" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="F15" s="24" t="s">
-        <v>18</v>
-      </c>
-      <c r="G15" s="19"/>
-      <c r="H15" s="21"/>
+      <c r="D15" s="41" t="s">
+        <v>59</v>
+      </c>
+      <c r="F15" s="3"/>
+      <c r="G15" s="31"/>
+      <c r="H15" s="33"/>
     </row>
     <row r="16" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
         <v>35</v>
       </c>
       <c r="B16" s="3"/>
-      <c r="C16" s="54"/>
-      <c r="D16" s="21"/>
-      <c r="E16" s="16" t="s">
+      <c r="C16" s="23"/>
+      <c r="D16" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="E16" s="26" t="s">
         <v>28</v>
       </c>
-      <c r="F16" s="25"/>
-      <c r="G16" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="H16" s="16" t="s">
-        <v>28</v>
-      </c>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
+      <c r="H16" s="34"/>
     </row>
     <row r="17" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
         <v>36</v>
       </c>
       <c r="B17" s="11" t="s">
-        <v>54</v>
-      </c>
-      <c r="D17" s="18" t="s">
+        <v>53</v>
+      </c>
+      <c r="D17" s="30" t="s">
         <v>19</v>
       </c>
-      <c r="E17" s="17"/>
-      <c r="F17" s="26"/>
-      <c r="G17" s="17"/>
-      <c r="H17" s="17"/>
+      <c r="E17" s="27"/>
+      <c r="F17" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="G17" s="3"/>
+      <c r="H17" s="3"/>
     </row>
     <row r="18" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="B18" s="20" t="s">
+      <c r="B18" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="C18" s="53" t="s">
+      <c r="C18" s="22" t="s">
         <v>45</v>
       </c>
-      <c r="D18" s="19"/>
-      <c r="E18" s="22" t="s">
-        <v>50</v>
-      </c>
-      <c r="F18" s="3"/>
+      <c r="D18" s="31"/>
+      <c r="E18" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="F18" s="16" t="s">
+        <v>18</v>
+      </c>
       <c r="G18" s="3"/>
       <c r="H18" s="3"/>
     </row>
@@ -1397,16 +1373,39 @@
       <c r="A19" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="B19" s="21"/>
-      <c r="C19" s="54"/>
+      <c r="B19" s="17"/>
+      <c r="C19" s="23"/>
       <c r="D19" s="3"/>
-      <c r="E19" s="23"/>
-      <c r="F19" s="3"/>
+      <c r="E19" s="17"/>
+      <c r="F19" s="17"/>
       <c r="G19" s="3"/>
       <c r="H19" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="33">
+  <mergeCells count="31">
+    <mergeCell ref="H9:H10"/>
+    <mergeCell ref="D17:D18"/>
+    <mergeCell ref="C18:C19"/>
+    <mergeCell ref="E7:E8"/>
+    <mergeCell ref="G14:G15"/>
+    <mergeCell ref="E16:E17"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="E18:E19"/>
+    <mergeCell ref="F18:F19"/>
+    <mergeCell ref="H14:H16"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="F6:F8"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="H7:H8"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="E9:E10"/>
+    <mergeCell ref="H12:H13"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="F9:F10"/>
+    <mergeCell ref="G7:G8"/>
     <mergeCell ref="B18:B19"/>
     <mergeCell ref="G9:G10"/>
     <mergeCell ref="G12:G13"/>
@@ -1415,31 +1414,6 @@
     <mergeCell ref="E11:E12"/>
     <mergeCell ref="F11:F12"/>
     <mergeCell ref="C15:C16"/>
-    <mergeCell ref="H7:H8"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="D9:D10"/>
-    <mergeCell ref="E9:E10"/>
-    <mergeCell ref="H12:H13"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="F9:F10"/>
-    <mergeCell ref="E7:E8"/>
-    <mergeCell ref="H9:H10"/>
-    <mergeCell ref="G7:G8"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="E5:E6"/>
-    <mergeCell ref="F6:F8"/>
-    <mergeCell ref="C11:C12"/>
-    <mergeCell ref="D11:D12"/>
-    <mergeCell ref="H16:H17"/>
-    <mergeCell ref="D17:D18"/>
-    <mergeCell ref="H14:H15"/>
-    <mergeCell ref="D15:D16"/>
-    <mergeCell ref="C18:C19"/>
-    <mergeCell ref="E18:E19"/>
-    <mergeCell ref="G14:G15"/>
-    <mergeCell ref="G16:G17"/>
-    <mergeCell ref="F15:F17"/>
-    <mergeCell ref="E16:E17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1451,7 +1425,7 @@
   <dimension ref="A1:H19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" activeCellId="1" sqref="B3 B4:B5"/>
+      <selection activeCell="E16" activeCellId="1" sqref="C18 E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1518,8 +1492,8 @@
       <c r="A4" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="51" t="s">
-        <v>57</v>
+      <c r="B4" s="37" t="s">
+        <v>56</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>11</v>
@@ -1530,8 +1504,8 @@
       <c r="E4" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="F4" s="11" t="s">
-        <v>54</v>
+      <c r="F4" s="14" t="s">
+        <v>53</v>
       </c>
       <c r="G4" s="3"/>
       <c r="H4" s="4" t="s">
@@ -1542,14 +1516,14 @@
       <c r="A5" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="52"/>
-      <c r="C5" s="35" t="s">
+      <c r="B5" s="38"/>
+      <c r="C5" s="44" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="11" t="s">
-        <v>54</v>
-      </c>
-      <c r="E5" s="35" t="s">
+      <c r="D5" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="E5" s="44" t="s">
         <v>13</v>
       </c>
       <c r="F5" s="5" t="s">
@@ -1567,40 +1541,40 @@
       <c r="B6" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="36"/>
-      <c r="D6" s="44" t="s">
+      <c r="C6" s="46"/>
+      <c r="D6" s="49" t="s">
+        <v>52</v>
+      </c>
+      <c r="E6" s="46"/>
+      <c r="F6" s="44" t="s">
+        <v>15</v>
+      </c>
+      <c r="G6" s="14" t="s">
         <v>53</v>
       </c>
-      <c r="E6" s="36"/>
-      <c r="F6" s="37" t="s">
-        <v>15</v>
-      </c>
-      <c r="G6" s="11" t="s">
-        <v>54</v>
-      </c>
-      <c r="H6" s="11" t="s">
-        <v>54</v>
+      <c r="H6" s="14" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="31" t="s">
+      <c r="B7" s="47" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="22" t="s">
-        <v>50</v>
-      </c>
-      <c r="D7" s="45"/>
-      <c r="E7" s="44" t="s">
-        <v>53</v>
-      </c>
-      <c r="F7" s="38"/>
-      <c r="G7" s="24" t="s">
+      <c r="C7" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="D7" s="50"/>
+      <c r="E7" s="20" t="s">
+        <v>52</v>
+      </c>
+      <c r="F7" s="45"/>
+      <c r="G7" s="32" t="s">
         <v>18</v>
       </c>
-      <c r="H7" s="18" t="s">
+      <c r="H7" s="30" t="s">
         <v>19</v>
       </c>
     </row>
@@ -1608,35 +1582,35 @@
       <c r="A8" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="32"/>
-      <c r="C8" s="23"/>
+      <c r="B8" s="48"/>
+      <c r="C8" s="19"/>
       <c r="D8" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E8" s="45"/>
-      <c r="F8" s="39"/>
-      <c r="G8" s="25"/>
-      <c r="H8" s="19"/>
+      <c r="E8" s="21"/>
+      <c r="F8" s="46"/>
+      <c r="G8" s="33"/>
+      <c r="H8" s="31"/>
     </row>
     <row r="9" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B9" s="16" t="s">
+      <c r="B9" s="26" t="s">
         <v>28</v>
       </c>
-      <c r="C9" s="47" t="s">
-        <v>56</v>
-      </c>
-      <c r="D9" s="31" t="s">
+      <c r="C9" s="44" t="s">
+        <v>55</v>
+      </c>
+      <c r="D9" s="42" t="s">
         <v>43</v>
       </c>
-      <c r="E9" s="47" t="s">
-        <v>56</v>
+      <c r="E9" s="44" t="s">
+        <v>55</v>
       </c>
       <c r="F9" s="3"/>
-      <c r="G9" s="26"/>
-      <c r="H9" s="49" t="s">
+      <c r="G9" s="34"/>
+      <c r="H9" s="35" t="s">
         <v>45</v>
       </c>
     </row>
@@ -1644,34 +1618,34 @@
       <c r="A10" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B10" s="17"/>
-      <c r="C10" s="48"/>
-      <c r="D10" s="32"/>
-      <c r="E10" s="48"/>
+      <c r="B10" s="27"/>
+      <c r="C10" s="46"/>
+      <c r="D10" s="43"/>
+      <c r="E10" s="46"/>
       <c r="F10" s="3"/>
       <c r="G10" s="3"/>
-      <c r="H10" s="50"/>
+      <c r="H10" s="36"/>
     </row>
     <row r="11" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B11" s="35" t="s">
+      <c r="B11" s="44" t="s">
         <v>25</v>
       </c>
-      <c r="C11" s="40" t="s">
-        <v>47</v>
-      </c>
-      <c r="D11" s="42" t="s">
+      <c r="C11" s="42" t="s">
         <v>46</v>
       </c>
-      <c r="E11" s="37" t="s">
-        <v>55</v>
-      </c>
-      <c r="F11" s="42" t="s">
-        <v>27</v>
-      </c>
-      <c r="G11" s="16" t="s">
+      <c r="D11" s="44" t="s">
+        <v>60</v>
+      </c>
+      <c r="E11" s="44" t="s">
+        <v>54</v>
+      </c>
+      <c r="F11" s="47" t="s">
+        <v>44</v>
+      </c>
+      <c r="G11" s="26" t="s">
         <v>28</v>
       </c>
       <c r="H11" s="3"/>
@@ -1680,19 +1654,19 @@
       <c r="A12" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="B12" s="46"/>
-      <c r="C12" s="41"/>
-      <c r="D12" s="43"/>
-      <c r="E12" s="39"/>
-      <c r="F12" s="43"/>
-      <c r="G12" s="17"/>
+      <c r="B12" s="45"/>
+      <c r="C12" s="43"/>
+      <c r="D12" s="46"/>
+      <c r="E12" s="46"/>
+      <c r="F12" s="48"/>
+      <c r="G12" s="27"/>
       <c r="H12" s="3"/>
     </row>
     <row r="13" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B13" s="36"/>
+      <c r="B13" s="46"/>
       <c r="C13" s="5" t="s">
         <v>11</v>
       </c>
@@ -1715,22 +1689,22 @@
       <c r="B14" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="16" t="s">
+      <c r="C14" s="26" t="s">
         <v>28</v>
       </c>
       <c r="D14" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E14" s="33" t="s">
+      <c r="E14" s="28" t="s">
         <v>33</v>
       </c>
       <c r="F14" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="G14" s="18" t="s">
+      <c r="G14" s="30" t="s">
         <v>19</v>
       </c>
-      <c r="H14" s="33" t="s">
+      <c r="H14" s="28" t="s">
         <v>33</v>
       </c>
     </row>
@@ -1738,37 +1712,37 @@
       <c r="A15" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="B15" s="18" t="s">
+      <c r="B15" s="30" t="s">
         <v>19</v>
       </c>
-      <c r="C15" s="17"/>
-      <c r="D15" s="24" t="s">
+      <c r="C15" s="27"/>
+      <c r="D15" s="32" t="s">
         <v>18</v>
       </c>
-      <c r="E15" s="34"/>
-      <c r="F15" s="33" t="s">
+      <c r="E15" s="29"/>
+      <c r="F15" s="28" t="s">
         <v>33</v>
       </c>
-      <c r="G15" s="19"/>
-      <c r="H15" s="34"/>
+      <c r="G15" s="31"/>
+      <c r="H15" s="29"/>
     </row>
     <row r="16" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="B16" s="19"/>
-      <c r="C16" s="33" t="s">
+      <c r="B16" s="31"/>
+      <c r="C16" s="28" t="s">
         <v>33</v>
       </c>
-      <c r="D16" s="25"/>
-      <c r="E16" s="11" t="s">
-        <v>54</v>
-      </c>
-      <c r="F16" s="34"/>
-      <c r="G16" s="33" t="s">
+      <c r="D16" s="33"/>
+      <c r="E16" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="F16" s="29"/>
+      <c r="G16" s="28" t="s">
         <v>33</v>
       </c>
-      <c r="H16" s="16" t="s">
+      <c r="H16" s="26" t="s">
         <v>28</v>
       </c>
     </row>
@@ -1776,28 +1750,28 @@
       <c r="A17" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="B17" s="20" t="s">
+      <c r="B17" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="C17" s="34"/>
-      <c r="D17" s="26"/>
-      <c r="E17" s="49" t="s">
+      <c r="C17" s="29"/>
+      <c r="D17" s="34"/>
+      <c r="E17" s="35" t="s">
         <v>45</v>
       </c>
       <c r="F17" s="3"/>
-      <c r="G17" s="34"/>
-      <c r="H17" s="17"/>
+      <c r="G17" s="29"/>
+      <c r="H17" s="27"/>
     </row>
     <row r="18" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="B18" s="21"/>
-      <c r="C18" s="11" t="s">
-        <v>54</v>
+      <c r="B18" s="17"/>
+      <c r="C18" s="14" t="s">
+        <v>53</v>
       </c>
       <c r="D18" s="3"/>
-      <c r="E18" s="50"/>
+      <c r="E18" s="36"/>
       <c r="F18" s="3"/>
       <c r="G18" s="3"/>
       <c r="H18" s="3"/>
@@ -1816,6 +1790,27 @@
     </row>
   </sheetData>
   <mergeCells count="33">
+    <mergeCell ref="H7:H8"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="E9:E10"/>
+    <mergeCell ref="G11:G12"/>
+    <mergeCell ref="H9:H10"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="F6:F8"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="G7:G9"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="E7:E8"/>
+    <mergeCell ref="B11:B13"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="E11:E12"/>
+    <mergeCell ref="F11:F12"/>
     <mergeCell ref="H16:H17"/>
     <mergeCell ref="B17:B18"/>
     <mergeCell ref="E14:E15"/>
@@ -1826,29 +1821,8 @@
     <mergeCell ref="H14:H15"/>
     <mergeCell ref="G16:G17"/>
     <mergeCell ref="F15:F16"/>
-    <mergeCell ref="B11:B13"/>
-    <mergeCell ref="C11:C12"/>
-    <mergeCell ref="D11:D12"/>
-    <mergeCell ref="E11:E12"/>
-    <mergeCell ref="F11:F12"/>
     <mergeCell ref="D15:D17"/>
     <mergeCell ref="E17:E18"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="E5:E6"/>
-    <mergeCell ref="F6:F8"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="G7:G9"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="D6:D7"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="E7:E8"/>
-    <mergeCell ref="H7:H8"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="D9:D10"/>
-    <mergeCell ref="E9:E10"/>
-    <mergeCell ref="G11:G12"/>
-    <mergeCell ref="H9:H10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1860,7 +1834,7 @@
   <dimension ref="A1:H19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1877,7 +1851,7 @@
   <sheetData>
     <row r="1" spans="1:8" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -1942,7 +1916,7 @@
         <v>11</v>
       </c>
       <c r="F4" s="14" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G4" s="3"/>
       <c r="H4" s="3"/>
@@ -1952,15 +1926,15 @@
         <v>12</v>
       </c>
       <c r="B5" s="14" t="s">
-        <v>54</v>
-      </c>
-      <c r="C5" s="35" t="s">
+        <v>53</v>
+      </c>
+      <c r="C5" s="44" t="s">
         <v>13</v>
       </c>
       <c r="D5" s="14" t="s">
-        <v>54</v>
-      </c>
-      <c r="E5" s="35" t="s">
+        <v>53</v>
+      </c>
+      <c r="E5" s="44" t="s">
         <v>13</v>
       </c>
       <c r="F5" s="5" t="s">
@@ -1980,40 +1954,40 @@
       <c r="B6" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="36"/>
-      <c r="D6" s="44" t="s">
+      <c r="C6" s="46"/>
+      <c r="D6" s="49" t="s">
+        <v>52</v>
+      </c>
+      <c r="E6" s="46"/>
+      <c r="F6" s="44" t="s">
+        <v>15</v>
+      </c>
+      <c r="G6" s="14" t="s">
         <v>53</v>
       </c>
-      <c r="E6" s="36"/>
-      <c r="F6" s="37" t="s">
-        <v>15</v>
-      </c>
-      <c r="G6" s="14" t="s">
-        <v>54</v>
-      </c>
       <c r="H6" s="14" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="31" t="s">
+      <c r="B7" s="47" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="49" t="s">
+      <c r="C7" s="35" t="s">
         <v>45</v>
       </c>
-      <c r="D7" s="45"/>
-      <c r="E7" s="44" t="s">
-        <v>53</v>
-      </c>
-      <c r="F7" s="38"/>
-      <c r="G7" s="24" t="s">
+      <c r="D7" s="50"/>
+      <c r="E7" s="20" t="s">
+        <v>52</v>
+      </c>
+      <c r="F7" s="45"/>
+      <c r="G7" s="51" t="s">
         <v>18</v>
       </c>
-      <c r="H7" s="18" t="s">
+      <c r="H7" s="30" t="s">
         <v>19</v>
       </c>
     </row>
@@ -2021,37 +1995,37 @@
       <c r="A8" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="32"/>
-      <c r="C8" s="50"/>
-      <c r="D8" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="E8" s="45"/>
-      <c r="F8" s="39"/>
-      <c r="G8" s="25"/>
-      <c r="H8" s="19"/>
+      <c r="B8" s="48"/>
+      <c r="C8" s="36"/>
+      <c r="D8" s="55" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8" s="21"/>
+      <c r="F8" s="46"/>
+      <c r="G8" s="52"/>
+      <c r="H8" s="31"/>
     </row>
     <row r="9" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B9" s="16" t="s">
+      <c r="B9" s="26" t="s">
         <v>28</v>
       </c>
-      <c r="C9" s="29" t="s">
-        <v>48</v>
-      </c>
-      <c r="D9" s="31" t="s">
+      <c r="C9" s="42" t="s">
+        <v>47</v>
+      </c>
+      <c r="D9" s="47" t="s">
         <v>17</v>
       </c>
-      <c r="E9" s="29" t="s">
+      <c r="E9" s="47" t="s">
         <v>22</v>
       </c>
-      <c r="F9" s="51" t="s">
-        <v>57</v>
-      </c>
-      <c r="G9" s="26"/>
-      <c r="H9" s="49" t="s">
+      <c r="F9" s="37" t="s">
+        <v>56</v>
+      </c>
+      <c r="G9" s="53"/>
+      <c r="H9" s="35" t="s">
         <v>45</v>
       </c>
     </row>
@@ -2059,34 +2033,34 @@
       <c r="A10" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B10" s="17"/>
-      <c r="C10" s="30"/>
-      <c r="D10" s="32"/>
-      <c r="E10" s="30"/>
-      <c r="F10" s="23"/>
+      <c r="B10" s="27"/>
+      <c r="C10" s="43"/>
+      <c r="D10" s="48"/>
+      <c r="E10" s="48"/>
+      <c r="F10" s="19"/>
       <c r="G10" s="3"/>
-      <c r="H10" s="50"/>
+      <c r="H10" s="36"/>
     </row>
     <row r="11" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B11" s="35" t="s">
+      <c r="B11" s="44" t="s">
         <v>25</v>
       </c>
-      <c r="C11" s="40" t="s">
+      <c r="C11" s="47" t="s">
         <v>26</v>
       </c>
       <c r="D11" s="42" t="s">
+        <v>61</v>
+      </c>
+      <c r="E11" s="47" t="s">
+        <v>26</v>
+      </c>
+      <c r="F11" s="47" t="s">
         <v>27</v>
       </c>
-      <c r="E11" s="40" t="s">
-        <v>26</v>
-      </c>
-      <c r="F11" s="42" t="s">
-        <v>27</v>
-      </c>
-      <c r="G11" s="16" t="s">
+      <c r="G11" s="26" t="s">
         <v>28</v>
       </c>
       <c r="H11" s="3"/>
@@ -2095,26 +2069,26 @@
       <c r="A12" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="B12" s="46"/>
-      <c r="C12" s="41"/>
+      <c r="B12" s="45"/>
+      <c r="C12" s="48"/>
       <c r="D12" s="43"/>
-      <c r="E12" s="41"/>
-      <c r="F12" s="43"/>
-      <c r="G12" s="17"/>
+      <c r="E12" s="48"/>
+      <c r="F12" s="48"/>
+      <c r="G12" s="27"/>
       <c r="H12" s="3"/>
     </row>
     <row r="13" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B13" s="36"/>
-      <c r="C13" s="51" t="s">
-        <v>57</v>
+      <c r="B13" s="46"/>
+      <c r="C13" s="49" t="s">
+        <v>56</v>
       </c>
       <c r="D13" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="E13" s="16" t="s">
+      <c r="E13" s="26" t="s">
         <v>28</v>
       </c>
       <c r="F13" s="9" t="s">
@@ -2130,15 +2104,15 @@
       <c r="B14" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="23"/>
+      <c r="C14" s="54"/>
       <c r="D14" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E14" s="17"/>
+      <c r="E14" s="27"/>
       <c r="F14" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="G14" s="18" t="s">
+      <c r="G14" s="30" t="s">
         <v>19</v>
       </c>
       <c r="H14" s="3"/>
@@ -2147,41 +2121,41 @@
       <c r="A15" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="B15" s="33" t="s">
+      <c r="B15" s="28" t="s">
         <v>33</v>
       </c>
       <c r="C15" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="D15" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="D15" s="16" t="s">
         <v>18</v>
       </c>
       <c r="E15" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="F15" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="F15" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="G15" s="19"/>
+      <c r="G15" s="31"/>
       <c r="H15" s="3"/>
     </row>
     <row r="16" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="B16" s="34"/>
+      <c r="B16" s="29"/>
       <c r="C16" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D16" s="21"/>
+      <c r="D16" s="17"/>
       <c r="E16" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="F16" s="21"/>
-      <c r="G16" s="49" t="s">
+      <c r="F16" s="17"/>
+      <c r="G16" s="35" t="s">
         <v>45</v>
       </c>
-      <c r="H16" s="16" t="s">
+      <c r="H16" s="26" t="s">
         <v>28</v>
       </c>
     </row>
@@ -2189,29 +2163,29 @@
       <c r="A17" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="B17" s="20" t="s">
+      <c r="B17" s="16" t="s">
         <v>18</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>54</v>
-      </c>
-      <c r="D17" s="18" t="s">
+        <v>53</v>
+      </c>
+      <c r="D17" s="30" t="s">
         <v>19</v>
       </c>
       <c r="E17" s="14" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F17" s="3"/>
-      <c r="G17" s="50"/>
-      <c r="H17" s="17"/>
+      <c r="G17" s="36"/>
+      <c r="H17" s="27"/>
     </row>
     <row r="18" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="B18" s="21"/>
+      <c r="B18" s="17"/>
       <c r="C18" s="3"/>
-      <c r="D18" s="19"/>
+      <c r="D18" s="31"/>
       <c r="E18" s="3"/>
       <c r="F18" s="3"/>
       <c r="G18" s="3"/>
@@ -2231,21 +2205,12 @@
     </row>
   </sheetData>
   <mergeCells count="31">
-    <mergeCell ref="H16:H17"/>
-    <mergeCell ref="B17:B18"/>
-    <mergeCell ref="D17:D18"/>
-    <mergeCell ref="F15:F16"/>
-    <mergeCell ref="B15:B16"/>
-    <mergeCell ref="D15:D16"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="E13:E14"/>
-    <mergeCell ref="G16:G17"/>
-    <mergeCell ref="G14:G15"/>
-    <mergeCell ref="B11:B13"/>
-    <mergeCell ref="C11:C12"/>
-    <mergeCell ref="D11:D12"/>
-    <mergeCell ref="E11:E12"/>
-    <mergeCell ref="F11:F12"/>
+    <mergeCell ref="H7:H8"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="E9:E10"/>
+    <mergeCell ref="G11:G12"/>
+    <mergeCell ref="H9:H10"/>
     <mergeCell ref="C5:C6"/>
     <mergeCell ref="E5:E6"/>
     <mergeCell ref="F6:F8"/>
@@ -2256,14 +2221,24 @@
     <mergeCell ref="D6:D7"/>
     <mergeCell ref="E7:E8"/>
     <mergeCell ref="F9:F10"/>
-    <mergeCell ref="H7:H8"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="D9:D10"/>
-    <mergeCell ref="E9:E10"/>
-    <mergeCell ref="G11:G12"/>
-    <mergeCell ref="H9:H10"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="E13:E14"/>
+    <mergeCell ref="G16:G17"/>
+    <mergeCell ref="G14:G15"/>
+    <mergeCell ref="B11:B13"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="E11:E12"/>
+    <mergeCell ref="F11:F12"/>
+    <mergeCell ref="H16:H17"/>
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="D17:D18"/>
+    <mergeCell ref="F15:F16"/>
+    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="D15:D16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2272,7 +2247,7 @@
   <dimension ref="A1:H19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H17" sqref="H17:H18"/>
+      <selection activeCell="G7" sqref="G7:G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2352,7 +2327,7 @@
         <v>11</v>
       </c>
       <c r="F4" s="14" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G4" s="3"/>
       <c r="H4" s="3"/>
@@ -2362,15 +2337,15 @@
         <v>12</v>
       </c>
       <c r="B5" s="14" t="s">
-        <v>54</v>
-      </c>
-      <c r="C5" s="35" t="s">
+        <v>53</v>
+      </c>
+      <c r="C5" s="44" t="s">
         <v>13</v>
       </c>
       <c r="D5" s="14" t="s">
-        <v>54</v>
-      </c>
-      <c r="E5" s="35" t="s">
+        <v>53</v>
+      </c>
+      <c r="E5" s="44" t="s">
         <v>13</v>
       </c>
       <c r="F5" s="5" t="s">
@@ -2390,38 +2365,38 @@
       <c r="B6" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="36"/>
+      <c r="C6" s="46"/>
       <c r="D6" s="3"/>
-      <c r="E6" s="36"/>
-      <c r="F6" s="37" t="s">
+      <c r="E6" s="46"/>
+      <c r="F6" s="44" t="s">
         <v>15</v>
       </c>
       <c r="G6" s="14" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H6" s="14" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="31" t="s">
+      <c r="B7" s="47" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="49" t="s">
+      <c r="C7" s="35" t="s">
         <v>45</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E7" s="3"/>
-      <c r="F7" s="38"/>
-      <c r="G7" s="24" t="s">
+      <c r="F7" s="45"/>
+      <c r="G7" s="32" t="s">
         <v>18</v>
       </c>
-      <c r="H7" s="18" t="s">
+      <c r="H7" s="30" t="s">
         <v>19</v>
       </c>
     </row>
@@ -2429,35 +2404,35 @@
       <c r="A8" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="32"/>
-      <c r="C8" s="50"/>
+      <c r="B8" s="48"/>
+      <c r="C8" s="36"/>
       <c r="D8" s="5" t="s">
         <v>11</v>
       </c>
       <c r="E8" s="3"/>
-      <c r="F8" s="39"/>
-      <c r="G8" s="25"/>
-      <c r="H8" s="19"/>
+      <c r="F8" s="46"/>
+      <c r="G8" s="33"/>
+      <c r="H8" s="31"/>
     </row>
     <row r="9" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B9" s="16" t="s">
+      <c r="B9" s="26" t="s">
         <v>28</v>
       </c>
-      <c r="C9" s="29" t="s">
+      <c r="C9" s="47" t="s">
         <v>22</v>
       </c>
-      <c r="D9" s="31" t="s">
+      <c r="D9" s="47" t="s">
         <v>17</v>
       </c>
-      <c r="E9" s="29" t="s">
+      <c r="E9" s="47" t="s">
         <v>22</v>
       </c>
       <c r="F9" s="3"/>
-      <c r="G9" s="26"/>
-      <c r="H9" s="16" t="s">
+      <c r="G9" s="34"/>
+      <c r="H9" s="26" t="s">
         <v>28</v>
       </c>
     </row>
@@ -2465,34 +2440,34 @@
       <c r="A10" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B10" s="17"/>
-      <c r="C10" s="30"/>
-      <c r="D10" s="32"/>
-      <c r="E10" s="30"/>
+      <c r="B10" s="27"/>
+      <c r="C10" s="48"/>
+      <c r="D10" s="48"/>
+      <c r="E10" s="48"/>
       <c r="F10" s="3"/>
       <c r="G10" s="3"/>
-      <c r="H10" s="17"/>
+      <c r="H10" s="27"/>
     </row>
     <row r="11" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B11" s="35" t="s">
+      <c r="B11" s="44" t="s">
         <v>25</v>
       </c>
-      <c r="C11" s="40" t="s">
+      <c r="C11" s="47" t="s">
         <v>26</v>
       </c>
-      <c r="D11" s="42" t="s">
+      <c r="D11" s="47" t="s">
         <v>27</v>
       </c>
-      <c r="E11" s="40" t="s">
+      <c r="E11" s="47" t="s">
         <v>26</v>
       </c>
-      <c r="F11" s="42" t="s">
+      <c r="F11" s="47" t="s">
         <v>27</v>
       </c>
-      <c r="G11" s="16" t="s">
+      <c r="G11" s="26" t="s">
         <v>28</v>
       </c>
       <c r="H11" s="3"/>
@@ -2501,27 +2476,27 @@
       <c r="A12" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="B12" s="46"/>
-      <c r="C12" s="41"/>
-      <c r="D12" s="43"/>
-      <c r="E12" s="41"/>
-      <c r="F12" s="43"/>
-      <c r="G12" s="17"/>
+      <c r="B12" s="45"/>
+      <c r="C12" s="48"/>
+      <c r="D12" s="48"/>
+      <c r="E12" s="48"/>
+      <c r="F12" s="48"/>
+      <c r="G12" s="27"/>
       <c r="H12" s="3"/>
     </row>
     <row r="13" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B13" s="36"/>
-      <c r="C13" s="44" t="s">
-        <v>53</v>
+      <c r="B13" s="46"/>
+      <c r="C13" s="20" t="s">
+        <v>52</v>
       </c>
       <c r="D13" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="E13" s="44" t="s">
-        <v>53</v>
+      <c r="E13" s="20" t="s">
+        <v>52</v>
       </c>
       <c r="F13" s="9" t="s">
         <v>42</v>
@@ -2536,15 +2511,15 @@
       <c r="B14" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="45"/>
+      <c r="C14" s="21"/>
       <c r="D14" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E14" s="45"/>
+      <c r="E14" s="21"/>
       <c r="F14" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="G14" s="20" t="s">
+      <c r="G14" s="16" t="s">
         <v>18</v>
       </c>
       <c r="H14" s="3"/>
@@ -2553,37 +2528,37 @@
       <c r="A15" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="B15" s="18" t="s">
+      <c r="B15" s="30" t="s">
         <v>19</v>
       </c>
       <c r="C15" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="D15" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="D15" s="16" t="s">
         <v>18</v>
       </c>
       <c r="E15" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="F15" s="18" t="s">
+        <v>50</v>
+      </c>
+      <c r="F15" s="30" t="s">
         <v>19</v>
       </c>
-      <c r="G15" s="21"/>
+      <c r="G15" s="17"/>
       <c r="H15" s="3"/>
     </row>
     <row r="16" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="B16" s="19"/>
+      <c r="B16" s="31"/>
       <c r="C16" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D16" s="21"/>
+      <c r="D16" s="17"/>
       <c r="E16" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="F16" s="19"/>
+      <c r="F16" s="31"/>
       <c r="G16" s="3"/>
       <c r="H16" s="3"/>
     </row>
@@ -2591,21 +2566,21 @@
       <c r="A17" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="B17" s="20" t="s">
+      <c r="B17" s="16" t="s">
         <v>18</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>54</v>
-      </c>
-      <c r="D17" s="18" t="s">
+        <v>53</v>
+      </c>
+      <c r="D17" s="30" t="s">
         <v>19</v>
       </c>
       <c r="E17" s="14" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F17" s="3"/>
       <c r="G17" s="3"/>
-      <c r="H17" s="20" t="s">
+      <c r="H17" s="16" t="s">
         <v>18</v>
       </c>
     </row>
@@ -2613,13 +2588,13 @@
       <c r="A18" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="B18" s="21"/>
+      <c r="B18" s="17"/>
       <c r="C18" s="3"/>
-      <c r="D18" s="19"/>
+      <c r="D18" s="31"/>
       <c r="E18" s="3"/>
       <c r="F18" s="3"/>
       <c r="G18" s="3"/>
-      <c r="H18" s="21"/>
+      <c r="H18" s="17"/>
     </row>
     <row r="19" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
@@ -2635,6 +2610,19 @@
     </row>
   </sheetData>
   <mergeCells count="27">
+    <mergeCell ref="H7:H8"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="E9:E10"/>
+    <mergeCell ref="G11:G12"/>
+    <mergeCell ref="H9:H10"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="F6:F8"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="G7:G9"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="C7:C8"/>
     <mergeCell ref="H17:H18"/>
     <mergeCell ref="B11:B13"/>
     <mergeCell ref="C11:C12"/>
@@ -2649,19 +2637,6 @@
     <mergeCell ref="F15:F16"/>
     <mergeCell ref="C13:C14"/>
     <mergeCell ref="E13:E14"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="E5:E6"/>
-    <mergeCell ref="F6:F8"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="G7:G9"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="H7:H8"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="D9:D10"/>
-    <mergeCell ref="E9:E10"/>
-    <mergeCell ref="G11:G12"/>
-    <mergeCell ref="H9:H10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>

</xml_diff>

<commit_message>
Nueva actividad, ajustar horas estudio
</commit_message>
<xml_diff>
--- a/Programar_dias.xlsx
+++ b/Programar_dias.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Estudio\OneDrive - Universidad de Antioquia\Estudio\Materias\Informatica II\Calendario_semanal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A281488-3D14-475A-8466-FC1CB648171E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56CA7780-4508-47D0-B9BD-D0C1FEF4B21B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{CC961CB2-F623-4B13-8239-4B70F16E4462}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{CC961CB2-F623-4B13-8239-4B70F16E4462}"/>
   </bookViews>
   <sheets>
     <sheet name="Semana 1" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="61">
   <si>
     <t>LUNES</t>
   </si>
@@ -248,9 +248,6 @@
     <t>Estudiar Inglés</t>
   </si>
   <si>
-    <t xml:space="preserve">CIRCUITOS II. </t>
-  </si>
-  <si>
     <t xml:space="preserve">MATH. ESPECIALES </t>
   </si>
   <si>
@@ -283,6 +280,9 @@
       </rPr>
       <t>PARCIAL</t>
     </r>
+  </si>
+  <si>
+    <t>CIRCUITOS II</t>
   </si>
 </sst>
 </file>
@@ -370,7 +370,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="16">
+  <fills count="17">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -461,6 +461,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="5">
     <border>
@@ -526,7 +532,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -577,118 +583,130 @@
     <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="13" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="15" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="15" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1014,8 +1032,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC99D917-8B13-4626-B576-50715BED7B7E}">
   <dimension ref="A1:J19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8:G9"/>
+    <sheetView topLeftCell="A4" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="H16" sqref="H16:H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1103,22 +1121,20 @@
       <c r="B5" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="26" t="s">
+      <c r="C5" s="24" t="s">
         <v>13</v>
       </c>
       <c r="D5" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="E5" s="26" t="s">
+      <c r="E5" s="24" t="s">
         <v>13</v>
       </c>
       <c r="F5" s="13" t="s">
         <v>11</v>
       </c>
       <c r="G5" s="3"/>
-      <c r="H5" s="4" t="s">
-        <v>10</v>
-      </c>
+      <c r="H5" s="3"/>
     </row>
     <row r="6" spans="1:10" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
@@ -1127,54 +1143,52 @@
       <c r="B6" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="28"/>
+      <c r="C6" s="26"/>
       <c r="D6" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="E6" s="28"/>
-      <c r="F6" s="26" t="s">
+      <c r="E6" s="26"/>
+      <c r="F6" s="24" t="s">
         <v>15</v>
       </c>
       <c r="G6" s="3"/>
-      <c r="H6" s="14" t="s">
-        <v>52</v>
-      </c>
+      <c r="H6" s="3"/>
     </row>
     <row r="7" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="24" t="s">
+      <c r="B7" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="33" t="s">
+      <c r="C7" s="18" t="s">
         <v>28</v>
       </c>
       <c r="D7" s="3"/>
-      <c r="E7" s="20" t="s">
+      <c r="E7" s="31" t="s">
         <v>48</v>
       </c>
-      <c r="F7" s="27"/>
+      <c r="F7" s="25"/>
       <c r="G7" s="3"/>
-      <c r="H7" s="42" t="s">
-        <v>19</v>
+      <c r="H7" s="4" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="25"/>
-      <c r="C8" s="34"/>
+      <c r="B8" s="23"/>
+      <c r="C8" s="19"/>
       <c r="D8" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="E8" s="21"/>
-      <c r="F8" s="28"/>
-      <c r="G8" s="20" t="s">
-        <v>48</v>
-      </c>
-      <c r="H8" s="43"/>
+        <v>56</v>
+      </c>
+      <c r="E8" s="32"/>
+      <c r="F8" s="26"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="20" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="9" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
@@ -1183,78 +1197,77 @@
       <c r="B9" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="C9" s="24" t="s">
+      <c r="C9" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="D9" s="24" t="s">
+      <c r="D9" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="E9" s="24" t="s">
+      <c r="E9" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="F9" s="33" t="s">
+      <c r="F9" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="G9" s="21"/>
-      <c r="H9" s="33" t="s">
-        <v>28</v>
-      </c>
+      <c r="G9" s="3"/>
+      <c r="H9" s="21"/>
     </row>
     <row r="10" spans="1:10" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>23</v>
       </c>
       <c r="B10" s="15"/>
-      <c r="C10" s="25"/>
-      <c r="D10" s="25"/>
-      <c r="E10" s="25"/>
-      <c r="F10" s="34"/>
-      <c r="H10" s="34"/>
+      <c r="C10" s="23"/>
+      <c r="D10" s="23"/>
+      <c r="E10" s="23"/>
+      <c r="F10" s="19"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
     </row>
     <row r="11" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B11" s="26" t="s">
+      <c r="B11" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="C11" s="24" t="s">
+      <c r="C11" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="D11" s="24" t="s">
+      <c r="D11" s="22" t="s">
         <v>27</v>
       </c>
       <c r="E11" s="3"/>
-      <c r="F11" s="24" t="s">
-        <v>59</v>
-      </c>
-      <c r="G11" s="3"/>
-      <c r="H11" s="3"/>
-    </row>
-    <row r="12" spans="1:10" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="F11" s="22" t="s">
+        <v>58</v>
+      </c>
+      <c r="G11" s="31" t="s">
+        <v>48</v>
+      </c>
+      <c r="H11" s="20" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="B12" s="27"/>
-      <c r="C12" s="25"/>
-      <c r="D12" s="25"/>
-      <c r="F12" s="25"/>
-      <c r="G12" s="22" t="s">
-        <v>51</v>
-      </c>
-      <c r="H12" s="33" t="s">
-        <v>28</v>
-      </c>
+      <c r="B12" s="25"/>
+      <c r="C12" s="23"/>
+      <c r="D12" s="23"/>
+      <c r="F12" s="23"/>
+      <c r="G12" s="32"/>
+      <c r="H12" s="21"/>
     </row>
     <row r="13" spans="1:10" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B13" s="28"/>
+      <c r="B13" s="26"/>
       <c r="C13" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="D13" s="37" t="s">
+      <c r="D13" s="33" t="s">
         <v>31</v>
       </c>
       <c r="E13" s="13" t="s">
@@ -1263,8 +1276,9 @@
       <c r="F13" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="G13" s="23"/>
-      <c r="H13" s="34"/>
+      <c r="H13" s="13" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="14" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
@@ -1274,12 +1288,14 @@
         <v>11</v>
       </c>
       <c r="C14" s="3"/>
-      <c r="D14" s="38"/>
-      <c r="G14" s="31" t="s">
-        <v>19</v>
-      </c>
-      <c r="H14" s="39" t="s">
-        <v>18</v>
+      <c r="D14" s="34"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="27" t="s">
+        <v>45</v>
+      </c>
+      <c r="H14" s="3" t="s">
+        <v>42</v>
       </c>
       <c r="J14" s="8"/>
     </row>
@@ -1288,34 +1304,38 @@
         <v>34</v>
       </c>
       <c r="B15" s="3"/>
-      <c r="C15" s="29" t="s">
+      <c r="C15" s="27" t="s">
         <v>45</v>
       </c>
       <c r="D15" s="16" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E15" s="3"/>
       <c r="F15" s="3"/>
-      <c r="G15" s="32"/>
-      <c r="H15" s="40"/>
+      <c r="G15" s="28"/>
+      <c r="H15" s="13" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="16" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
         <v>35</v>
       </c>
       <c r="B16" s="3"/>
-      <c r="C16" s="30"/>
+      <c r="C16" s="28"/>
       <c r="D16" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="E16" s="33" t="s">
+      <c r="E16" s="18" t="s">
         <v>28</v>
       </c>
       <c r="F16" s="3"/>
-      <c r="G16" s="39" t="s">
+      <c r="G16" s="35" t="s">
         <v>18</v>
       </c>
-      <c r="H16" s="41"/>
+      <c r="H16" s="18" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="17" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
@@ -1326,59 +1346,50 @@
       </c>
       <c r="C17" s="3"/>
       <c r="D17" s="3"/>
-      <c r="E17" s="34"/>
+      <c r="E17" s="19"/>
       <c r="F17" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="G17" s="40"/>
-      <c r="H17" s="3"/>
+      <c r="G17" s="36"/>
+      <c r="H17" s="19"/>
     </row>
     <row r="18" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="B18" s="18" t="s">
+      <c r="B18" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="C18" s="29" t="s">
+      <c r="C18" s="27" t="s">
         <v>45</v>
       </c>
-      <c r="D18" s="31" t="s">
+      <c r="D18" s="29" t="s">
         <v>19</v>
       </c>
-      <c r="E18" s="18" t="s">
+      <c r="E18" s="20" t="s">
         <v>18</v>
       </c>
       <c r="F18" s="3"/>
-      <c r="G18" s="41"/>
-      <c r="H18" s="3"/>
+      <c r="G18" s="37"/>
+      <c r="H18" s="20" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="19" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="B19" s="19"/>
-      <c r="C19" s="30"/>
-      <c r="D19" s="32"/>
-      <c r="E19" s="19"/>
+      <c r="B19" s="21"/>
+      <c r="C19" s="28"/>
+      <c r="D19" s="30"/>
+      <c r="E19" s="21"/>
       <c r="F19" s="3"/>
       <c r="G19" s="3"/>
-      <c r="H19" s="3"/>
+      <c r="H19" s="21"/>
     </row>
   </sheetData>
-  <mergeCells count="29">
-    <mergeCell ref="H9:H10"/>
-    <mergeCell ref="C18:C19"/>
-    <mergeCell ref="E7:E8"/>
-    <mergeCell ref="G14:G15"/>
-    <mergeCell ref="E16:E17"/>
-    <mergeCell ref="D13:D14"/>
-    <mergeCell ref="E18:E19"/>
-    <mergeCell ref="H14:H16"/>
-    <mergeCell ref="H7:H8"/>
-    <mergeCell ref="H12:H13"/>
-    <mergeCell ref="G16:G18"/>
-    <mergeCell ref="G8:G9"/>
+  <mergeCells count="28">
+    <mergeCell ref="H18:H19"/>
     <mergeCell ref="C5:C6"/>
     <mergeCell ref="E5:E6"/>
     <mergeCell ref="F6:F8"/>
@@ -1389,13 +1400,23 @@
     <mergeCell ref="E9:E10"/>
     <mergeCell ref="C7:C8"/>
     <mergeCell ref="F9:F10"/>
+    <mergeCell ref="E7:E8"/>
+    <mergeCell ref="H16:H17"/>
     <mergeCell ref="B18:B19"/>
-    <mergeCell ref="G12:G13"/>
     <mergeCell ref="B7:B8"/>
     <mergeCell ref="B11:B13"/>
     <mergeCell ref="F11:F12"/>
     <mergeCell ref="C15:C16"/>
     <mergeCell ref="D18:D19"/>
+    <mergeCell ref="C18:C19"/>
+    <mergeCell ref="G14:G15"/>
+    <mergeCell ref="E16:E17"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="E18:E19"/>
+    <mergeCell ref="G16:G18"/>
+    <mergeCell ref="G11:G12"/>
+    <mergeCell ref="H8:H9"/>
+    <mergeCell ref="H11:H12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1406,8 +1427,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF8929EB-A174-48F2-BDBD-469036EC404B}">
   <dimension ref="A1:H19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E16" activeCellId="1" sqref="C18 E16"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7:E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1446,7 +1467,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>7</v>
       </c>
@@ -1463,7 +1484,9 @@
         <v>8</v>
       </c>
       <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
+      <c r="C3" s="14" t="s">
+        <v>52</v>
+      </c>
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
@@ -1474,8 +1497,8 @@
       <c r="A4" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="50" t="s">
-        <v>55</v>
+      <c r="B4" s="5" t="s">
+        <v>11</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>11</v>
@@ -1494,18 +1517,20 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="51"/>
-      <c r="C5" s="26" t="s">
+      <c r="B5" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="24" t="s">
         <v>13</v>
       </c>
       <c r="D5" s="14" t="s">
         <v>52</v>
       </c>
-      <c r="E5" s="26" t="s">
+      <c r="E5" s="24" t="s">
         <v>13</v>
       </c>
       <c r="F5" s="5" t="s">
@@ -1520,15 +1545,13 @@
       <c r="A6" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" s="28"/>
+      <c r="B6" s="21"/>
+      <c r="C6" s="26"/>
       <c r="D6" s="48" t="s">
         <v>51</v>
       </c>
-      <c r="E6" s="28"/>
-      <c r="F6" s="26" t="s">
+      <c r="E6" s="26"/>
+      <c r="F6" s="24" t="s">
         <v>15</v>
       </c>
       <c r="G6" s="14" t="s">
@@ -1542,21 +1565,21 @@
       <c r="A7" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="24" t="s">
+      <c r="B7" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="20" t="s">
+      <c r="C7" s="31" t="s">
         <v>48</v>
       </c>
       <c r="D7" s="49"/>
-      <c r="E7" s="22" t="s">
+      <c r="E7" s="50" t="s">
         <v>51</v>
       </c>
-      <c r="F7" s="27"/>
-      <c r="G7" s="39" t="s">
+      <c r="F7" s="25"/>
+      <c r="G7" s="35" t="s">
         <v>18</v>
       </c>
-      <c r="H7" s="31" t="s">
+      <c r="H7" s="29" t="s">
         <v>19</v>
       </c>
     </row>
@@ -1564,91 +1587,93 @@
       <c r="A8" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="25"/>
-      <c r="C8" s="21"/>
+      <c r="B8" s="23"/>
+      <c r="C8" s="32"/>
       <c r="D8" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E8" s="23"/>
-      <c r="F8" s="28"/>
-      <c r="G8" s="40"/>
-      <c r="H8" s="32"/>
+      <c r="E8" s="51"/>
+      <c r="F8" s="26"/>
+      <c r="G8" s="36"/>
+      <c r="H8" s="30"/>
     </row>
     <row r="9" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B9" s="33" t="s">
+      <c r="B9" s="58" t="s">
         <v>28</v>
       </c>
-      <c r="C9" s="26" t="s">
-        <v>54</v>
-      </c>
-      <c r="D9" s="46" t="s">
+      <c r="C9" s="24" t="s">
+        <v>53</v>
+      </c>
+      <c r="D9" s="44" t="s">
         <v>43</v>
       </c>
-      <c r="E9" s="26" t="s">
-        <v>54</v>
+      <c r="E9" s="24" t="s">
+        <v>53</v>
       </c>
       <c r="F9" s="3"/>
-      <c r="G9" s="41"/>
-      <c r="H9" s="44" t="s">
+      <c r="G9" s="37"/>
+      <c r="H9" s="40" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A10" s="3" t="s">
+    <row r="10" spans="1:8" ht="33" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B10" s="34"/>
-      <c r="C10" s="28"/>
-      <c r="D10" s="47"/>
-      <c r="E10" s="28"/>
+      <c r="B10" s="59" t="s">
+        <v>33</v>
+      </c>
+      <c r="C10" s="26"/>
+      <c r="D10" s="45"/>
+      <c r="E10" s="26"/>
       <c r="F10" s="3"/>
       <c r="G10" s="3"/>
-      <c r="H10" s="45"/>
+      <c r="H10" s="41"/>
     </row>
     <row r="11" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B11" s="26" t="s">
+      <c r="B11" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="C11" s="46" t="s">
+      <c r="C11" s="24" t="s">
+        <v>60</v>
+      </c>
+      <c r="D11" s="24" t="s">
+        <v>58</v>
+      </c>
+      <c r="E11" s="44" t="s">
         <v>46</v>
       </c>
-      <c r="D11" s="26" t="s">
-        <v>59</v>
-      </c>
-      <c r="E11" s="26" t="s">
-        <v>53</v>
-      </c>
-      <c r="F11" s="24" t="s">
+      <c r="F11" s="46" t="s">
         <v>44</v>
       </c>
-      <c r="G11" s="33" t="s">
+      <c r="G11" s="18" t="s">
         <v>28</v>
       </c>
       <c r="H11" s="3"/>
     </row>
-    <row r="12" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="B12" s="27"/>
-      <c r="C12" s="47"/>
-      <c r="D12" s="28"/>
-      <c r="E12" s="28"/>
-      <c r="F12" s="25"/>
-      <c r="G12" s="34"/>
+      <c r="B12" s="25"/>
+      <c r="C12" s="26"/>
+      <c r="D12" s="26"/>
+      <c r="E12" s="45"/>
+      <c r="F12" s="47"/>
+      <c r="G12" s="19"/>
       <c r="H12" s="3"/>
     </row>
     <row r="13" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B13" s="28"/>
+      <c r="B13" s="26"/>
       <c r="C13" s="5" t="s">
         <v>11</v>
       </c>
@@ -1668,25 +1693,25 @@
       <c r="A14" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B14" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C14" s="33" t="s">
-        <v>28</v>
+      <c r="B14" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="C14" s="29" t="s">
+        <v>19</v>
       </c>
       <c r="D14" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E14" s="35" t="s">
+      <c r="E14" s="38" t="s">
         <v>33</v>
       </c>
       <c r="F14" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="G14" s="31" t="s">
+      <c r="G14" s="29" t="s">
         <v>19</v>
       </c>
-      <c r="H14" s="35" t="s">
+      <c r="H14" s="38" t="s">
         <v>33</v>
       </c>
     </row>
@@ -1694,37 +1719,39 @@
       <c r="A15" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="B15" s="31" t="s">
-        <v>19</v>
-      </c>
-      <c r="C15" s="34"/>
-      <c r="D15" s="39" t="s">
+      <c r="B15" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C15" s="30"/>
+      <c r="D15" s="35" t="s">
         <v>18</v>
       </c>
-      <c r="E15" s="36"/>
-      <c r="F15" s="35" t="s">
+      <c r="E15" s="39"/>
+      <c r="F15" s="38" t="s">
         <v>33</v>
       </c>
-      <c r="G15" s="32"/>
-      <c r="H15" s="36"/>
-    </row>
-    <row r="16" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="G15" s="30"/>
+      <c r="H15" s="39"/>
+    </row>
+    <row r="16" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="B16" s="32"/>
-      <c r="C16" s="35" t="s">
+      <c r="B16" s="42" t="s">
+        <v>45</v>
+      </c>
+      <c r="C16" s="38" t="s">
         <v>33</v>
       </c>
-      <c r="D16" s="40"/>
+      <c r="D16" s="36"/>
       <c r="E16" s="14" t="s">
         <v>52</v>
       </c>
-      <c r="F16" s="36"/>
-      <c r="G16" s="35" t="s">
+      <c r="F16" s="39"/>
+      <c r="G16" s="38" t="s">
         <v>33</v>
       </c>
-      <c r="H16" s="33" t="s">
+      <c r="H16" s="18" t="s">
         <v>28</v>
       </c>
     </row>
@@ -1732,28 +1759,28 @@
       <c r="A17" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="B17" s="18" t="s">
-        <v>18</v>
-      </c>
-      <c r="C17" s="36"/>
-      <c r="D17" s="41"/>
-      <c r="E17" s="44" t="s">
+      <c r="B17" s="43"/>
+      <c r="C17" s="39"/>
+      <c r="D17" s="37"/>
+      <c r="E17" s="40" t="s">
         <v>45</v>
       </c>
       <c r="F17" s="3"/>
-      <c r="G17" s="36"/>
-      <c r="H17" s="34"/>
-    </row>
-    <row r="18" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="G17" s="39"/>
+      <c r="H17" s="19"/>
+    </row>
+    <row r="18" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="B18" s="19"/>
-      <c r="C18" s="14" t="s">
-        <v>52</v>
+      <c r="B18" s="57" t="s">
+        <v>19</v>
+      </c>
+      <c r="C18" s="20" t="s">
+        <v>18</v>
       </c>
       <c r="D18" s="3"/>
-      <c r="E18" s="45"/>
+      <c r="E18" s="41"/>
       <c r="F18" s="3"/>
       <c r="G18" s="3"/>
       <c r="H18" s="3"/>
@@ -1763,7 +1790,7 @@
         <v>38</v>
       </c>
       <c r="B19" s="3"/>
-      <c r="C19" s="3"/>
+      <c r="C19" s="21"/>
       <c r="D19" s="3"/>
       <c r="E19" s="3"/>
       <c r="F19" s="3"/>
@@ -1771,7 +1798,7 @@
       <c r="H19" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="33">
+  <mergeCells count="32">
     <mergeCell ref="H7:H8"/>
     <mergeCell ref="C9:C10"/>
     <mergeCell ref="D9:D10"/>
@@ -1783,21 +1810,19 @@
     <mergeCell ref="F6:F8"/>
     <mergeCell ref="B7:B8"/>
     <mergeCell ref="G7:G9"/>
-    <mergeCell ref="B9:B10"/>
     <mergeCell ref="C7:C8"/>
     <mergeCell ref="D6:D7"/>
-    <mergeCell ref="B4:B5"/>
     <mergeCell ref="E7:E8"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="B16:B17"/>
     <mergeCell ref="B11:B13"/>
+    <mergeCell ref="E11:E12"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="F11:F12"/>
     <mergeCell ref="C11:C12"/>
-    <mergeCell ref="D11:D12"/>
-    <mergeCell ref="E11:E12"/>
-    <mergeCell ref="F11:F12"/>
     <mergeCell ref="H16:H17"/>
-    <mergeCell ref="B17:B18"/>
     <mergeCell ref="E14:E15"/>
     <mergeCell ref="G14:G15"/>
-    <mergeCell ref="B15:B16"/>
     <mergeCell ref="C14:C15"/>
     <mergeCell ref="C16:C17"/>
     <mergeCell ref="H14:H15"/>
@@ -1805,6 +1830,7 @@
     <mergeCell ref="F15:F16"/>
     <mergeCell ref="D15:D17"/>
     <mergeCell ref="E17:E18"/>
+    <mergeCell ref="C18:C19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1816,7 +1842,7 @@
   <dimension ref="A1:H19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="B14" sqref="B14:B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1833,7 +1859,7 @@
   <sheetData>
     <row r="1" spans="1:8" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -1910,13 +1936,13 @@
       <c r="B5" s="14" t="s">
         <v>52</v>
       </c>
-      <c r="C5" s="26" t="s">
+      <c r="C5" s="24" t="s">
         <v>13</v>
       </c>
       <c r="D5" s="14" t="s">
         <v>52</v>
       </c>
-      <c r="E5" s="26" t="s">
+      <c r="E5" s="24" t="s">
         <v>13</v>
       </c>
       <c r="F5" s="5" t="s">
@@ -1936,12 +1962,12 @@
       <c r="B6" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="28"/>
+      <c r="C6" s="26"/>
       <c r="D6" s="48" t="s">
         <v>51</v>
       </c>
-      <c r="E6" s="28"/>
-      <c r="F6" s="26" t="s">
+      <c r="E6" s="26"/>
+      <c r="F6" s="24" t="s">
         <v>15</v>
       </c>
       <c r="G6" s="14" t="s">
@@ -1955,21 +1981,21 @@
       <c r="A7" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="24" t="s">
+      <c r="B7" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="44" t="s">
+      <c r="C7" s="40" t="s">
         <v>45</v>
       </c>
       <c r="D7" s="49"/>
-      <c r="E7" s="22" t="s">
+      <c r="E7" s="50" t="s">
         <v>51</v>
       </c>
-      <c r="F7" s="27"/>
+      <c r="F7" s="25"/>
       <c r="G7" s="53" t="s">
         <v>18</v>
       </c>
-      <c r="H7" s="31" t="s">
+      <c r="H7" s="29" t="s">
         <v>19</v>
       </c>
     </row>
@@ -1977,37 +2003,37 @@
       <c r="A8" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="25"/>
-      <c r="C8" s="45"/>
+      <c r="B8" s="23"/>
+      <c r="C8" s="41"/>
       <c r="D8" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="E8" s="23"/>
-      <c r="F8" s="28"/>
+      <c r="E8" s="51"/>
+      <c r="F8" s="26"/>
       <c r="G8" s="54"/>
-      <c r="H8" s="32"/>
+      <c r="H8" s="30"/>
     </row>
     <row r="9" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B9" s="33" t="s">
+      <c r="B9" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="C9" s="46" t="s">
+      <c r="C9" s="44" t="s">
         <v>47</v>
       </c>
-      <c r="D9" s="24" t="s">
+      <c r="D9" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="E9" s="24" t="s">
+      <c r="E9" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="F9" s="50" t="s">
-        <v>55</v>
+      <c r="F9" s="56" t="s">
+        <v>54</v>
       </c>
       <c r="G9" s="55"/>
-      <c r="H9" s="44" t="s">
+      <c r="H9" s="40" t="s">
         <v>45</v>
       </c>
     </row>
@@ -2015,34 +2041,34 @@
       <c r="A10" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B10" s="34"/>
-      <c r="C10" s="47"/>
-      <c r="D10" s="25"/>
-      <c r="E10" s="25"/>
-      <c r="F10" s="21"/>
+      <c r="B10" s="19"/>
+      <c r="C10" s="45"/>
+      <c r="D10" s="23"/>
+      <c r="E10" s="23"/>
+      <c r="F10" s="32"/>
       <c r="G10" s="3"/>
-      <c r="H10" s="45"/>
+      <c r="H10" s="41"/>
     </row>
     <row r="11" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B11" s="26" t="s">
+      <c r="B11" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="C11" s="24" t="s">
+      <c r="C11" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="D11" s="46" t="s">
-        <v>60</v>
-      </c>
-      <c r="E11" s="24" t="s">
+      <c r="D11" s="44" t="s">
+        <v>59</v>
+      </c>
+      <c r="E11" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="F11" s="24" t="s">
+      <c r="F11" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="G11" s="33" t="s">
+      <c r="G11" s="18" t="s">
         <v>28</v>
       </c>
       <c r="H11" s="3"/>
@@ -2051,26 +2077,26 @@
       <c r="A12" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="B12" s="27"/>
-      <c r="C12" s="25"/>
-      <c r="D12" s="47"/>
-      <c r="E12" s="25"/>
-      <c r="F12" s="25"/>
-      <c r="G12" s="34"/>
+      <c r="B12" s="25"/>
+      <c r="C12" s="23"/>
+      <c r="D12" s="45"/>
+      <c r="E12" s="23"/>
+      <c r="F12" s="23"/>
+      <c r="G12" s="19"/>
       <c r="H12" s="3"/>
     </row>
     <row r="13" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B13" s="28"/>
+      <c r="B13" s="26"/>
       <c r="C13" s="48" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D13" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="E13" s="33" t="s">
+      <c r="E13" s="18" t="s">
         <v>28</v>
       </c>
       <c r="F13" s="9" t="s">
@@ -2083,18 +2109,18 @@
       <c r="A14" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B14" s="5" t="s">
-        <v>11</v>
+      <c r="B14" s="9" t="s">
+        <v>42</v>
       </c>
       <c r="C14" s="52"/>
       <c r="D14" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E14" s="34"/>
+      <c r="E14" s="19"/>
       <c r="F14" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="G14" s="31" t="s">
+      <c r="G14" s="29" t="s">
         <v>19</v>
       </c>
       <c r="H14" s="3"/>
@@ -2103,41 +2129,41 @@
       <c r="A15" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="B15" s="35" t="s">
-        <v>33</v>
+      <c r="B15" s="5" t="s">
+        <v>11</v>
       </c>
       <c r="C15" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="D15" s="18" t="s">
+      <c r="D15" s="20" t="s">
         <v>18</v>
       </c>
       <c r="E15" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="F15" s="18" t="s">
+      <c r="F15" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="G15" s="32"/>
+      <c r="G15" s="30"/>
       <c r="H15" s="3"/>
     </row>
     <row r="16" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="B16" s="36"/>
+      <c r="B16" s="3"/>
       <c r="C16" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D16" s="19"/>
+      <c r="D16" s="21"/>
       <c r="E16" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="F16" s="19"/>
-      <c r="G16" s="44" t="s">
+      <c r="F16" s="21"/>
+      <c r="G16" s="40" t="s">
         <v>45</v>
       </c>
-      <c r="H16" s="33" t="s">
+      <c r="H16" s="18" t="s">
         <v>28</v>
       </c>
     </row>
@@ -2145,29 +2171,27 @@
       <c r="A17" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="B17" s="18" t="s">
-        <v>18</v>
-      </c>
+      <c r="B17" s="3"/>
       <c r="C17" s="14" t="s">
         <v>52</v>
       </c>
-      <c r="D17" s="31" t="s">
+      <c r="D17" s="29" t="s">
         <v>19</v>
       </c>
       <c r="E17" s="14" t="s">
         <v>52</v>
       </c>
       <c r="F17" s="3"/>
-      <c r="G17" s="45"/>
-      <c r="H17" s="34"/>
+      <c r="G17" s="41"/>
+      <c r="H17" s="19"/>
     </row>
     <row r="18" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="B18" s="19"/>
+      <c r="B18" s="3"/>
       <c r="C18" s="3"/>
-      <c r="D18" s="32"/>
+      <c r="D18" s="30"/>
       <c r="E18" s="3"/>
       <c r="F18" s="3"/>
       <c r="G18" s="3"/>
@@ -2186,7 +2210,7 @@
       <c r="H19" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="31">
+  <mergeCells count="29">
     <mergeCell ref="H7:H8"/>
     <mergeCell ref="C9:C10"/>
     <mergeCell ref="D9:D10"/>
@@ -2203,21 +2227,19 @@
     <mergeCell ref="D6:D7"/>
     <mergeCell ref="E7:E8"/>
     <mergeCell ref="F9:F10"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="E13:E14"/>
-    <mergeCell ref="G16:G17"/>
-    <mergeCell ref="G14:G15"/>
     <mergeCell ref="B11:B13"/>
     <mergeCell ref="C11:C12"/>
     <mergeCell ref="D11:D12"/>
     <mergeCell ref="E11:E12"/>
     <mergeCell ref="F11:F12"/>
     <mergeCell ref="H16:H17"/>
-    <mergeCell ref="B17:B18"/>
     <mergeCell ref="D17:D18"/>
     <mergeCell ref="F15:F16"/>
-    <mergeCell ref="B15:B16"/>
     <mergeCell ref="D15:D16"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="E13:E14"/>
+    <mergeCell ref="G16:G17"/>
+    <mergeCell ref="G14:G15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2229,7 +2251,7 @@
   <dimension ref="A1:H19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G7" sqref="G7:G9"/>
+      <selection activeCell="B14" sqref="B14:B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2321,13 +2343,13 @@
       <c r="B5" s="14" t="s">
         <v>52</v>
       </c>
-      <c r="C5" s="26" t="s">
+      <c r="C5" s="24" t="s">
         <v>13</v>
       </c>
       <c r="D5" s="14" t="s">
         <v>52</v>
       </c>
-      <c r="E5" s="26" t="s">
+      <c r="E5" s="24" t="s">
         <v>13</v>
       </c>
       <c r="F5" s="5" t="s">
@@ -2347,10 +2369,10 @@
       <c r="B6" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="28"/>
+      <c r="C6" s="26"/>
       <c r="D6" s="3"/>
-      <c r="E6" s="28"/>
-      <c r="F6" s="26" t="s">
+      <c r="E6" s="26"/>
+      <c r="F6" s="24" t="s">
         <v>15</v>
       </c>
       <c r="G6" s="14" t="s">
@@ -2364,21 +2386,21 @@
       <c r="A7" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="24" t="s">
+      <c r="B7" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="44" t="s">
+      <c r="C7" s="40" t="s">
         <v>45</v>
       </c>
       <c r="D7" s="12" t="s">
         <v>50</v>
       </c>
       <c r="E7" s="3"/>
-      <c r="F7" s="27"/>
-      <c r="G7" s="39" t="s">
+      <c r="F7" s="25"/>
+      <c r="G7" s="35" t="s">
         <v>18</v>
       </c>
-      <c r="H7" s="31" t="s">
+      <c r="H7" s="29" t="s">
         <v>19</v>
       </c>
     </row>
@@ -2386,35 +2408,35 @@
       <c r="A8" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="25"/>
-      <c r="C8" s="45"/>
+      <c r="B8" s="23"/>
+      <c r="C8" s="41"/>
       <c r="D8" s="5" t="s">
         <v>11</v>
       </c>
       <c r="E8" s="3"/>
-      <c r="F8" s="28"/>
-      <c r="G8" s="40"/>
-      <c r="H8" s="32"/>
+      <c r="F8" s="26"/>
+      <c r="G8" s="36"/>
+      <c r="H8" s="30"/>
     </row>
     <row r="9" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B9" s="33" t="s">
+      <c r="B9" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="C9" s="24" t="s">
+      <c r="C9" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="D9" s="24" t="s">
+      <c r="D9" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="E9" s="24" t="s">
+      <c r="E9" s="22" t="s">
         <v>22</v>
       </c>
       <c r="F9" s="3"/>
-      <c r="G9" s="41"/>
-      <c r="H9" s="33" t="s">
+      <c r="G9" s="37"/>
+      <c r="H9" s="18" t="s">
         <v>28</v>
       </c>
     </row>
@@ -2422,34 +2444,34 @@
       <c r="A10" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B10" s="34"/>
-      <c r="C10" s="25"/>
-      <c r="D10" s="25"/>
-      <c r="E10" s="25"/>
+      <c r="B10" s="19"/>
+      <c r="C10" s="23"/>
+      <c r="D10" s="23"/>
+      <c r="E10" s="23"/>
       <c r="F10" s="3"/>
       <c r="G10" s="3"/>
-      <c r="H10" s="34"/>
+      <c r="H10" s="19"/>
     </row>
     <row r="11" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B11" s="26" t="s">
+      <c r="B11" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="C11" s="24" t="s">
+      <c r="C11" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="D11" s="24" t="s">
+      <c r="D11" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="E11" s="24" t="s">
+      <c r="E11" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="F11" s="24" t="s">
+      <c r="F11" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="G11" s="33" t="s">
+      <c r="G11" s="18" t="s">
         <v>28</v>
       </c>
       <c r="H11" s="3"/>
@@ -2458,26 +2480,26 @@
       <c r="A12" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="B12" s="27"/>
-      <c r="C12" s="25"/>
-      <c r="D12" s="25"/>
-      <c r="E12" s="25"/>
-      <c r="F12" s="25"/>
-      <c r="G12" s="34"/>
+      <c r="B12" s="25"/>
+      <c r="C12" s="23"/>
+      <c r="D12" s="23"/>
+      <c r="E12" s="23"/>
+      <c r="F12" s="23"/>
+      <c r="G12" s="19"/>
       <c r="H12" s="3"/>
     </row>
     <row r="13" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B13" s="28"/>
-      <c r="C13" s="22" t="s">
+      <c r="B13" s="26"/>
+      <c r="C13" s="50" t="s">
         <v>51</v>
       </c>
       <c r="D13" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="E13" s="22" t="s">
+      <c r="E13" s="50" t="s">
         <v>51</v>
       </c>
       <c r="F13" s="9" t="s">
@@ -2490,71 +2512,69 @@
       <c r="A14" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B14" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C14" s="23"/>
+      <c r="B14" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="C14" s="51"/>
       <c r="D14" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E14" s="23"/>
+      <c r="E14" s="51"/>
       <c r="F14" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="G14" s="18" t="s">
+      <c r="G14" s="20" t="s">
         <v>18</v>
       </c>
       <c r="H14" s="3"/>
     </row>
-    <row r="15" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="B15" s="31" t="s">
-        <v>19</v>
+      <c r="B15" s="5" t="s">
+        <v>11</v>
       </c>
       <c r="C15" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="D15" s="18" t="s">
+      <c r="D15" s="20" t="s">
         <v>18</v>
       </c>
       <c r="E15" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="F15" s="31" t="s">
+      <c r="F15" s="29" t="s">
         <v>19</v>
       </c>
-      <c r="G15" s="19"/>
+      <c r="G15" s="21"/>
       <c r="H15" s="3"/>
     </row>
     <row r="16" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="B16" s="32"/>
+      <c r="B16" s="3"/>
       <c r="C16" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D16" s="19"/>
+      <c r="D16" s="21"/>
       <c r="E16" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="F16" s="32"/>
+      <c r="F16" s="30"/>
       <c r="G16" s="3"/>
       <c r="H16" s="3"/>
     </row>
-    <row r="17" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="B17" s="18" t="s">
-        <v>18</v>
-      </c>
+      <c r="B17" s="3"/>
       <c r="C17" s="14" t="s">
         <v>52</v>
       </c>
-      <c r="D17" s="31" t="s">
+      <c r="D17" s="29" t="s">
         <v>19</v>
       </c>
       <c r="E17" s="14" t="s">
@@ -2562,7 +2582,7 @@
       </c>
       <c r="F17" s="3"/>
       <c r="G17" s="3"/>
-      <c r="H17" s="18" t="s">
+      <c r="H17" s="20" t="s">
         <v>18</v>
       </c>
     </row>
@@ -2570,13 +2590,13 @@
       <c r="A18" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="B18" s="19"/>
+      <c r="B18" s="3"/>
       <c r="C18" s="3"/>
-      <c r="D18" s="32"/>
+      <c r="D18" s="30"/>
       <c r="E18" s="3"/>
       <c r="F18" s="3"/>
       <c r="G18" s="3"/>
-      <c r="H18" s="19"/>
+      <c r="H18" s="21"/>
     </row>
     <row r="19" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
@@ -2591,7 +2611,7 @@
       <c r="H19" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="27">
+  <mergeCells count="25">
     <mergeCell ref="H7:H8"/>
     <mergeCell ref="C9:C10"/>
     <mergeCell ref="D9:D10"/>
@@ -2611,10 +2631,8 @@
     <mergeCell ref="D11:D12"/>
     <mergeCell ref="E11:E12"/>
     <mergeCell ref="F11:F12"/>
-    <mergeCell ref="B17:B18"/>
     <mergeCell ref="D17:D18"/>
     <mergeCell ref="G14:G15"/>
-    <mergeCell ref="B15:B16"/>
     <mergeCell ref="D15:D16"/>
     <mergeCell ref="F15:F16"/>
     <mergeCell ref="C13:C14"/>

</xml_diff>

<commit_message>
Inicio Ajuste próximas semanas
</commit_message>
<xml_diff>
--- a/Programar_dias.xlsx
+++ b/Programar_dias.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Estudio\OneDrive - Universidad de Antioquia\Estudio\Materias\Informatica II\Calendario_semanal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56CA7780-4508-47D0-B9BD-D0C1FEF4B21B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08A6CEFD-8284-4ED9-9E46-C77E2277E192}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{CC961CB2-F623-4B13-8239-4B70F16E4462}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="74">
   <si>
     <t>LUNES</t>
   </si>
@@ -167,21 +167,6 @@
   </si>
   <si>
     <t>Tenis</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">MÉTODOS N. </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Yu Gothic UI"/>
-        <family val="2"/>
-      </rPr>
-      <t>PARCIAL</t>
-    </r>
   </si>
   <si>
     <r>
@@ -284,12 +269,54 @@
   <si>
     <t>CIRCUITOS II</t>
   </si>
+  <si>
+    <t>Estd. Circuitos</t>
+  </si>
+  <si>
+    <t>Mercado</t>
+  </si>
+  <si>
+    <t>Estudiar Especiales (1:30)</t>
+  </si>
+  <si>
+    <t>Kaggle</t>
+  </si>
+  <si>
+    <t>MÉTODOS N. PARCIAL</t>
+  </si>
+  <si>
+    <t>Estud. Inglés</t>
+  </si>
+  <si>
+    <t>Descansar</t>
+  </si>
+  <si>
+    <t>Ver videos de interés</t>
+  </si>
+  <si>
+    <t>Ver series.</t>
+  </si>
+  <si>
+    <t>Arte</t>
+  </si>
+  <si>
+    <t>Escribir</t>
+  </si>
+  <si>
+    <t>Leer</t>
+  </si>
+  <si>
+    <t>Estud Info II</t>
+  </si>
+  <si>
+    <t>Asesoría Esp.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -361,14 +388,6 @@
       <name val="Yu Gothic UI"/>
       <family val="2"/>
     </font>
-    <font>
-      <b/>
-      <i/>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Yu Gothic UI"/>
-      <family val="2"/>
-    </font>
   </fonts>
   <fills count="17">
     <fill>
@@ -386,12 +405,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF66FFFF"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF99FF99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -463,7 +476,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.39997558519241921"/>
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -532,7 +551,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -546,47 +565,87 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -595,44 +654,56 @@
     <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -643,71 +714,35 @@
     <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="15" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="15" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1033,7 +1068,7 @@
   <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView topLeftCell="A4" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16:H17"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1103,7 +1138,7 @@
         <v>9</v>
       </c>
       <c r="B4" s="3"/>
-      <c r="C4" s="13" t="s">
+      <c r="C4" s="12" t="s">
         <v>11</v>
       </c>
       <c r="D4" s="4" t="s">
@@ -1118,19 +1153,19 @@
       <c r="A5" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="15" t="s">
+      <c r="B5" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="24" t="s">
+      <c r="C5" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="11" t="s">
-        <v>52</v>
-      </c>
-      <c r="E5" s="24" t="s">
+      <c r="D5" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="E5" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="F5" s="13" t="s">
+      <c r="F5" s="12" t="s">
         <v>11</v>
       </c>
       <c r="G5" s="3"/>
@@ -1140,15 +1175,15 @@
       <c r="A6" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" s="26"/>
-      <c r="D6" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="E6" s="26"/>
-      <c r="F6" s="24" t="s">
+      <c r="B6" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="31"/>
+      <c r="D6" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" s="31"/>
+      <c r="F6" s="29" t="s">
         <v>15</v>
       </c>
       <c r="G6" s="3"/>
@@ -1158,17 +1193,17 @@
       <c r="A7" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="22" t="s">
+      <c r="B7" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="18" t="s">
+      <c r="C7" s="36" t="s">
         <v>28</v>
       </c>
       <c r="D7" s="3"/>
-      <c r="E7" s="31" t="s">
-        <v>48</v>
-      </c>
-      <c r="F7" s="25"/>
+      <c r="E7" s="40" t="s">
+        <v>47</v>
+      </c>
+      <c r="F7" s="30"/>
       <c r="G7" s="3"/>
       <c r="H7" s="4" t="s">
         <v>10</v>
@@ -1178,15 +1213,15 @@
       <c r="A8" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="23"/>
-      <c r="C8" s="19"/>
+      <c r="B8" s="28"/>
+      <c r="C8" s="37"/>
       <c r="D8" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="E8" s="32"/>
-      <c r="F8" s="26"/>
+        <v>55</v>
+      </c>
+      <c r="E8" s="41"/>
+      <c r="F8" s="31"/>
       <c r="G8" s="3"/>
-      <c r="H8" s="20" t="s">
+      <c r="H8" s="25" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1194,33 +1229,33 @@
       <c r="A9" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B9" s="15" t="s">
+      <c r="B9" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="C9" s="22" t="s">
+      <c r="C9" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="D9" s="22" t="s">
+      <c r="D9" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="E9" s="22" t="s">
+      <c r="E9" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="F9" s="18" t="s">
+      <c r="F9" s="36" t="s">
         <v>28</v>
       </c>
       <c r="G9" s="3"/>
-      <c r="H9" s="21"/>
+      <c r="H9" s="26"/>
     </row>
     <row r="10" spans="1:10" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B10" s="15"/>
-      <c r="C10" s="23"/>
-      <c r="D10" s="23"/>
-      <c r="E10" s="23"/>
-      <c r="F10" s="19"/>
+      <c r="B10" s="14"/>
+      <c r="C10" s="28"/>
+      <c r="D10" s="28"/>
+      <c r="E10" s="28"/>
+      <c r="F10" s="37"/>
       <c r="G10" s="3"/>
       <c r="H10" s="3"/>
     </row>
@@ -1228,55 +1263,55 @@
       <c r="A11" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B11" s="24" t="s">
+      <c r="B11" s="29" t="s">
         <v>25</v>
       </c>
-      <c r="C11" s="22" t="s">
+      <c r="C11" s="27" t="s">
         <v>26</v>
       </c>
-      <c r="D11" s="22" t="s">
+      <c r="D11" s="27" t="s">
         <v>27</v>
       </c>
       <c r="E11" s="3"/>
-      <c r="F11" s="22" t="s">
-        <v>58</v>
-      </c>
-      <c r="G11" s="31" t="s">
-        <v>48</v>
-      </c>
-      <c r="H11" s="20" t="s">
+      <c r="F11" s="27" t="s">
+        <v>57</v>
+      </c>
+      <c r="G11" s="40" t="s">
+        <v>47</v>
+      </c>
+      <c r="H11" s="25" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="6" t="s">
+      <c r="A12" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="B12" s="25"/>
-      <c r="C12" s="23"/>
-      <c r="D12" s="23"/>
-      <c r="F12" s="23"/>
-      <c r="G12" s="32"/>
-      <c r="H12" s="21"/>
+      <c r="B12" s="30"/>
+      <c r="C12" s="28"/>
+      <c r="D12" s="28"/>
+      <c r="F12" s="28"/>
+      <c r="G12" s="41"/>
+      <c r="H12" s="26"/>
     </row>
     <row r="13" spans="1:10" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B13" s="26"/>
-      <c r="C13" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="D13" s="33" t="s">
+      <c r="B13" s="31"/>
+      <c r="C13" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="D13" s="38" t="s">
         <v>31</v>
       </c>
-      <c r="E13" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="F13" s="9" t="s">
+      <c r="E13" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="F13" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="H13" s="13" t="s">
+      <c r="H13" s="12" t="s">
         <v>11</v>
       </c>
     </row>
@@ -1284,36 +1319,36 @@
       <c r="A14" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B14" s="13" t="s">
+      <c r="B14" s="12" t="s">
         <v>11</v>
       </c>
       <c r="C14" s="3"/>
-      <c r="D14" s="34"/>
+      <c r="D14" s="39"/>
       <c r="E14" s="3"/>
       <c r="F14" s="3"/>
-      <c r="G14" s="27" t="s">
-        <v>45</v>
+      <c r="G14" s="32" t="s">
+        <v>44</v>
       </c>
       <c r="H14" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="J14" s="8"/>
+      <c r="J14" s="7"/>
     </row>
     <row r="15" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
         <v>34</v>
       </c>
       <c r="B15" s="3"/>
-      <c r="C15" s="27" t="s">
-        <v>45</v>
-      </c>
-      <c r="D15" s="16" t="s">
-        <v>57</v>
+      <c r="C15" s="32" t="s">
+        <v>44</v>
+      </c>
+      <c r="D15" s="15" t="s">
+        <v>56</v>
       </c>
       <c r="E15" s="3"/>
       <c r="F15" s="3"/>
-      <c r="G15" s="28"/>
-      <c r="H15" s="13" t="s">
+      <c r="G15" s="33"/>
+      <c r="H15" s="12" t="s">
         <v>11</v>
       </c>
     </row>
@@ -1322,18 +1357,18 @@
         <v>35</v>
       </c>
       <c r="B16" s="3"/>
-      <c r="C16" s="28"/>
-      <c r="D16" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="E16" s="18" t="s">
+      <c r="C16" s="33"/>
+      <c r="D16" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="E16" s="36" t="s">
         <v>28</v>
       </c>
       <c r="F16" s="3"/>
-      <c r="G16" s="35" t="s">
+      <c r="G16" s="42" t="s">
         <v>18</v>
       </c>
-      <c r="H16" s="18" t="s">
+      <c r="H16" s="36" t="s">
         <v>28</v>
       </c>
     </row>
@@ -1341,37 +1376,37 @@
       <c r="A17" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="B17" s="11" t="s">
-        <v>52</v>
+      <c r="B17" s="10" t="s">
+        <v>51</v>
       </c>
       <c r="C17" s="3"/>
       <c r="D17" s="3"/>
-      <c r="E17" s="19"/>
-      <c r="F17" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="G17" s="36"/>
-      <c r="H17" s="19"/>
+      <c r="E17" s="37"/>
+      <c r="F17" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="G17" s="43"/>
+      <c r="H17" s="37"/>
     </row>
     <row r="18" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="B18" s="20" t="s">
+      <c r="B18" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="C18" s="27" t="s">
-        <v>45</v>
-      </c>
-      <c r="D18" s="29" t="s">
+      <c r="C18" s="32" t="s">
+        <v>44</v>
+      </c>
+      <c r="D18" s="34" t="s">
         <v>19</v>
       </c>
-      <c r="E18" s="20" t="s">
+      <c r="E18" s="25" t="s">
         <v>18</v>
       </c>
       <c r="F18" s="3"/>
-      <c r="G18" s="37"/>
-      <c r="H18" s="20" t="s">
+      <c r="G18" s="44"/>
+      <c r="H18" s="25" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1379,17 +1414,17 @@
       <c r="A19" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="B19" s="21"/>
-      <c r="C19" s="28"/>
-      <c r="D19" s="30"/>
-      <c r="E19" s="21"/>
+      <c r="B19" s="26"/>
+      <c r="C19" s="33"/>
+      <c r="D19" s="35"/>
+      <c r="E19" s="26"/>
       <c r="F19" s="3"/>
       <c r="G19" s="3"/>
-      <c r="H19" s="21"/>
+      <c r="H19" s="26"/>
     </row>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="H18:H19"/>
+    <mergeCell ref="G11:G12"/>
     <mergeCell ref="C5:C6"/>
     <mergeCell ref="E5:E6"/>
     <mergeCell ref="F6:F8"/>
@@ -1401,7 +1436,8 @@
     <mergeCell ref="C7:C8"/>
     <mergeCell ref="F9:F10"/>
     <mergeCell ref="E7:E8"/>
-    <mergeCell ref="H16:H17"/>
+    <mergeCell ref="H8:H9"/>
+    <mergeCell ref="H11:H12"/>
     <mergeCell ref="B18:B19"/>
     <mergeCell ref="B7:B8"/>
     <mergeCell ref="B11:B13"/>
@@ -1409,14 +1445,13 @@
     <mergeCell ref="C15:C16"/>
     <mergeCell ref="D18:D19"/>
     <mergeCell ref="C18:C19"/>
-    <mergeCell ref="G14:G15"/>
     <mergeCell ref="E16:E17"/>
     <mergeCell ref="D13:D14"/>
     <mergeCell ref="E18:E19"/>
+    <mergeCell ref="H18:H19"/>
+    <mergeCell ref="H16:H17"/>
+    <mergeCell ref="G14:G15"/>
     <mergeCell ref="G16:G18"/>
-    <mergeCell ref="G11:G12"/>
-    <mergeCell ref="H8:H9"/>
-    <mergeCell ref="H11:H12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1425,10 +1460,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF8929EB-A174-48F2-BDBD-469036EC404B}">
-  <dimension ref="A1:H19"/>
+  <dimension ref="A1:J19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7:E8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1437,11 +1472,14 @@
     <col min="2" max="2" width="16.85546875" customWidth="1"/>
     <col min="3" max="3" width="15.85546875" customWidth="1"/>
     <col min="4" max="4" width="15.28515625" customWidth="1"/>
-    <col min="5" max="7" width="16" customWidth="1"/>
+    <col min="5" max="5" width="19.5703125" customWidth="1"/>
+    <col min="6" max="6" width="18.140625" customWidth="1"/>
+    <col min="7" max="7" width="16" customWidth="1"/>
     <col min="8" max="8" width="15.5703125" customWidth="1"/>
+    <col min="10" max="10" width="20.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>40</v>
       </c>
@@ -1467,7 +1505,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>7</v>
       </c>
@@ -1478,280 +1516,296 @@
       <c r="F2" s="3"/>
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
-    </row>
-    <row r="3" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="J2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B3" s="3"/>
-      <c r="C3" s="14" t="s">
-        <v>52</v>
-      </c>
+      <c r="C3" s="3"/>
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
-    </row>
-    <row r="4" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G3" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="H3" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="J3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="F4" s="14" t="s">
-        <v>52</v>
+      <c r="B4" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="45" t="s">
+        <v>44</v>
+      </c>
+      <c r="E4" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" s="13" t="s">
+        <v>51</v>
       </c>
       <c r="G4" s="3"/>
-      <c r="H4" s="4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="H4" s="26"/>
+      <c r="J4" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="20" t="s">
+      <c r="B5" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="24" t="s">
+      <c r="C5" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="14" t="s">
-        <v>52</v>
-      </c>
-      <c r="E5" s="24" t="s">
+      <c r="D5" s="46"/>
+      <c r="E5" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="F5" s="5" t="s">
+      <c r="F5" s="12" t="s">
         <v>11</v>
       </c>
       <c r="G5" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="H5" s="3"/>
-    </row>
-    <row r="6" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="H5" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="J5" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="21"/>
-      <c r="C6" s="26"/>
-      <c r="D6" s="48" t="s">
+      <c r="B6" s="26"/>
+      <c r="C6" s="31"/>
+      <c r="D6" s="47" t="s">
+        <v>33</v>
+      </c>
+      <c r="E6" s="31"/>
+      <c r="F6" s="29" t="s">
+        <v>15</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="H6" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="E6" s="26"/>
-      <c r="F6" s="24" t="s">
-        <v>15</v>
-      </c>
-      <c r="G6" s="14" t="s">
-        <v>52</v>
-      </c>
-      <c r="H6" s="14" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="J6" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="22" t="s">
+      <c r="B7" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="31" t="s">
-        <v>48</v>
-      </c>
-      <c r="D7" s="49"/>
-      <c r="E7" s="50" t="s">
-        <v>51</v>
-      </c>
-      <c r="F7" s="25"/>
-      <c r="G7" s="35" t="s">
+      <c r="C7" s="47" t="s">
+        <v>33</v>
+      </c>
+      <c r="D7" s="48"/>
+      <c r="E7" s="64" t="s">
+        <v>33</v>
+      </c>
+      <c r="F7" s="30"/>
+      <c r="G7" s="42" t="s">
         <v>18</v>
       </c>
-      <c r="H7" s="29" t="s">
+      <c r="H7" s="34" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="J7" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="23"/>
-      <c r="C8" s="32"/>
-      <c r="D8" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="E8" s="51"/>
-      <c r="F8" s="26"/>
-      <c r="G8" s="36"/>
-      <c r="H8" s="30"/>
-    </row>
-    <row r="9" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="28"/>
+      <c r="C8" s="48"/>
+      <c r="D8" s="36" t="s">
+        <v>28</v>
+      </c>
+      <c r="E8" s="65" t="s">
+        <v>55</v>
+      </c>
+      <c r="F8" s="31"/>
+      <c r="G8" s="43"/>
+      <c r="H8" s="35"/>
+    </row>
+    <row r="9" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B9" s="58" t="s">
-        <v>28</v>
-      </c>
-      <c r="C9" s="24" t="s">
-        <v>53</v>
-      </c>
-      <c r="D9" s="44" t="s">
-        <v>43</v>
-      </c>
-      <c r="E9" s="24" t="s">
-        <v>53</v>
-      </c>
-      <c r="F9" s="3"/>
-      <c r="G9" s="37"/>
-      <c r="H9" s="40" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" ht="33" x14ac:dyDescent="0.3">
+      <c r="B9" s="40" t="s">
+        <v>47</v>
+      </c>
+      <c r="C9" s="29" t="s">
+        <v>52</v>
+      </c>
+      <c r="D9" s="37"/>
+      <c r="E9" s="29" t="s">
+        <v>52</v>
+      </c>
+      <c r="F9" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="G9" s="44"/>
+      <c r="H9" s="51" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B10" s="59" t="s">
-        <v>33</v>
-      </c>
-      <c r="C10" s="26"/>
-      <c r="D10" s="45"/>
-      <c r="E10" s="26"/>
+      <c r="B10" s="41"/>
+      <c r="C10" s="31"/>
+      <c r="D10" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="E10" s="31"/>
       <c r="F10" s="3"/>
       <c r="G10" s="3"/>
-      <c r="H10" s="41"/>
-    </row>
-    <row r="11" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="H10" s="52"/>
+    </row>
+    <row r="11" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B11" s="24" t="s">
+      <c r="B11" s="29" t="s">
         <v>25</v>
       </c>
-      <c r="C11" s="24" t="s">
-        <v>60</v>
-      </c>
-      <c r="D11" s="24" t="s">
-        <v>58</v>
-      </c>
-      <c r="E11" s="44" t="s">
-        <v>46</v>
-      </c>
-      <c r="F11" s="46" t="s">
-        <v>44</v>
-      </c>
-      <c r="G11" s="18" t="s">
+      <c r="C11" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="D11" s="29" t="s">
+        <v>57</v>
+      </c>
+      <c r="E11" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="F11" s="49" t="s">
+        <v>43</v>
+      </c>
+      <c r="G11" s="36" t="s">
         <v>28</v>
       </c>
       <c r="H11" s="3"/>
     </row>
-    <row r="12" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="6" t="s">
+    <row r="12" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="B12" s="25"/>
-      <c r="C12" s="26"/>
-      <c r="D12" s="26"/>
-      <c r="E12" s="45"/>
-      <c r="F12" s="47"/>
-      <c r="G12" s="19"/>
+      <c r="B12" s="30"/>
+      <c r="C12" s="31"/>
+      <c r="D12" s="31"/>
+      <c r="E12" s="31"/>
+      <c r="F12" s="50"/>
+      <c r="G12" s="37"/>
       <c r="H12" s="3"/>
     </row>
-    <row r="13" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B13" s="26"/>
-      <c r="C13" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D13" s="7" t="s">
+      <c r="B13" s="31"/>
+      <c r="C13" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="D13" s="38" t="s">
         <v>31</v>
       </c>
-      <c r="E13" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="F13" s="9" t="s">
+      <c r="E13" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="F13" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="G13" s="3"/>
-      <c r="H13" s="3"/>
-    </row>
-    <row r="14" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G13" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="H13" s="42" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B14" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="C14" s="29" t="s">
-        <v>19</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="E14" s="38" t="s">
-        <v>33</v>
-      </c>
-      <c r="F14" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="G14" s="29" t="s">
-        <v>19</v>
-      </c>
-      <c r="H14" s="38" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="3"/>
+      <c r="C14" s="36" t="s">
+        <v>28</v>
+      </c>
+      <c r="D14" s="39"/>
+      <c r="E14" s="36" t="s">
+        <v>28</v>
+      </c>
+      <c r="F14" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="G14" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="H14" s="43"/>
+    </row>
+    <row r="15" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="B15" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C15" s="30"/>
-      <c r="D15" s="35" t="s">
-        <v>18</v>
-      </c>
-      <c r="E15" s="39"/>
-      <c r="F15" s="38" t="s">
+      <c r="B15" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="C15" s="37"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="37"/>
+      <c r="F15" s="47" t="s">
+        <v>62</v>
+      </c>
+      <c r="G15" s="47" t="s">
         <v>33</v>
       </c>
-      <c r="G15" s="30"/>
-      <c r="H15" s="39"/>
-    </row>
-    <row r="16" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="H15" s="44"/>
+    </row>
+    <row r="16" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="B16" s="42" t="s">
-        <v>45</v>
-      </c>
-      <c r="C16" s="38" t="s">
-        <v>33</v>
-      </c>
-      <c r="D16" s="36"/>
-      <c r="E16" s="14" t="s">
-        <v>52</v>
-      </c>
-      <c r="F16" s="39"/>
-      <c r="G16" s="38" t="s">
-        <v>33</v>
-      </c>
-      <c r="H16" s="18" t="s">
+      <c r="B16" s="45" t="s">
+        <v>44</v>
+      </c>
+      <c r="C16" s="45" t="s">
+        <v>44</v>
+      </c>
+      <c r="D16" s="3"/>
+      <c r="E16" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="F16" s="48"/>
+      <c r="G16" s="48"/>
+      <c r="H16" s="36" t="s">
         <v>28</v>
       </c>
     </row>
@@ -1759,30 +1813,42 @@
       <c r="A17" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="B17" s="43"/>
-      <c r="C17" s="39"/>
-      <c r="D17" s="37"/>
-      <c r="E17" s="40" t="s">
-        <v>45</v>
-      </c>
-      <c r="F17" s="3"/>
-      <c r="G17" s="39"/>
-      <c r="H17" s="19"/>
+      <c r="B17" s="46"/>
+      <c r="C17" s="46"/>
+      <c r="D17" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="E17" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="F17" s="19" t="s">
+        <v>63</v>
+      </c>
+      <c r="G17" s="3"/>
+      <c r="H17" s="37"/>
     </row>
     <row r="18" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="B18" s="57" t="s">
+      <c r="B18" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="C18" s="20" t="s">
+      <c r="C18" s="47" t="s">
+        <v>33</v>
+      </c>
+      <c r="D18" s="47" t="s">
+        <v>33</v>
+      </c>
+      <c r="E18" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="F18" s="42" t="s">
         <v>18</v>
       </c>
-      <c r="D18" s="3"/>
-      <c r="E18" s="41"/>
-      <c r="F18" s="3"/>
-      <c r="G18" s="3"/>
+      <c r="G18" s="19" t="s">
+        <v>63</v>
+      </c>
       <c r="H18" s="3"/>
     </row>
     <row r="19" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
@@ -1790,47 +1856,51 @@
         <v>38</v>
       </c>
       <c r="B19" s="3"/>
-      <c r="C19" s="21"/>
-      <c r="D19" s="3"/>
-      <c r="E19" s="3"/>
-      <c r="F19" s="3"/>
+      <c r="C19" s="48"/>
+      <c r="D19" s="48"/>
+      <c r="E19" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="F19" s="44"/>
       <c r="G19" s="3"/>
       <c r="H19" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="32">
-    <mergeCell ref="H7:H8"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="D9:D10"/>
-    <mergeCell ref="E9:E10"/>
+  <mergeCells count="34">
     <mergeCell ref="G11:G12"/>
     <mergeCell ref="H9:H10"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="E5:E6"/>
-    <mergeCell ref="F6:F8"/>
     <mergeCell ref="B7:B8"/>
     <mergeCell ref="G7:G9"/>
     <mergeCell ref="C7:C8"/>
     <mergeCell ref="D6:D7"/>
-    <mergeCell ref="E7:E8"/>
     <mergeCell ref="B5:B6"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="E9:E10"/>
     <mergeCell ref="B16:B17"/>
     <mergeCell ref="B11:B13"/>
     <mergeCell ref="E11:E12"/>
     <mergeCell ref="D11:D12"/>
     <mergeCell ref="F11:F12"/>
     <mergeCell ref="C11:C12"/>
+    <mergeCell ref="H3:H4"/>
+    <mergeCell ref="F18:F19"/>
     <mergeCell ref="H16:H17"/>
     <mergeCell ref="E14:E15"/>
-    <mergeCell ref="G14:G15"/>
     <mergeCell ref="C14:C15"/>
     <mergeCell ref="C16:C17"/>
-    <mergeCell ref="H14:H15"/>
-    <mergeCell ref="G16:G17"/>
+    <mergeCell ref="G15:G16"/>
     <mergeCell ref="F15:F16"/>
-    <mergeCell ref="D15:D17"/>
-    <mergeCell ref="E17:E18"/>
     <mergeCell ref="C18:C19"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="D18:D19"/>
+    <mergeCell ref="H13:H15"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="F6:F8"/>
+    <mergeCell ref="H7:H8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1842,7 +1912,7 @@
   <dimension ref="A1:H19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14:B15"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1859,7 +1929,7 @@
   <sheetData>
     <row r="1" spans="1:8" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -1914,17 +1984,17 @@
       <c r="B4" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="12" t="s">
         <v>11</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="E4" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="F4" s="14" t="s">
-        <v>52</v>
+      <c r="E4" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" s="13" t="s">
+        <v>51</v>
       </c>
       <c r="G4" s="3"/>
       <c r="H4" s="3"/>
@@ -1933,19 +2003,19 @@
       <c r="A5" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="14" t="s">
-        <v>52</v>
-      </c>
-      <c r="C5" s="24" t="s">
+      <c r="B5" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="C5" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="14" t="s">
-        <v>52</v>
-      </c>
-      <c r="E5" s="24" t="s">
+      <c r="D5" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="E5" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="F5" s="5" t="s">
+      <c r="F5" s="12" t="s">
         <v>11</v>
       </c>
       <c r="G5" s="4" t="s">
@@ -1959,43 +2029,43 @@
       <c r="A6" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" s="26"/>
-      <c r="D6" s="48" t="s">
+      <c r="B6" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="31"/>
+      <c r="D6" s="22" t="s">
+        <v>63</v>
+      </c>
+      <c r="E6" s="31"/>
+      <c r="F6" s="29" t="s">
+        <v>15</v>
+      </c>
+      <c r="G6" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="E6" s="26"/>
-      <c r="F6" s="24" t="s">
-        <v>15</v>
-      </c>
-      <c r="G6" s="14" t="s">
-        <v>52</v>
-      </c>
-      <c r="H6" s="14" t="s">
-        <v>52</v>
+      <c r="H6" s="13" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="22" t="s">
-        <v>17</v>
-      </c>
-      <c r="C7" s="40" t="s">
-        <v>45</v>
-      </c>
-      <c r="D7" s="49"/>
-      <c r="E7" s="50" t="s">
-        <v>51</v>
-      </c>
-      <c r="F7" s="25"/>
-      <c r="G7" s="53" t="s">
+      <c r="B7" s="49" t="s">
+        <v>64</v>
+      </c>
+      <c r="C7" s="51" t="s">
+        <v>44</v>
+      </c>
+      <c r="D7" s="24"/>
+      <c r="E7" s="61" t="s">
+        <v>50</v>
+      </c>
+      <c r="F7" s="30"/>
+      <c r="G7" s="58" t="s">
         <v>18</v>
       </c>
-      <c r="H7" s="29" t="s">
+      <c r="H7" s="34" t="s">
         <v>19</v>
       </c>
     </row>
@@ -2003,103 +2073,105 @@
       <c r="A8" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="23"/>
-      <c r="C8" s="41"/>
-      <c r="D8" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="E8" s="51"/>
-      <c r="F8" s="26"/>
-      <c r="G8" s="54"/>
-      <c r="H8" s="30"/>
+      <c r="B8" s="50"/>
+      <c r="C8" s="52"/>
+      <c r="D8" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8" s="62"/>
+      <c r="F8" s="31"/>
+      <c r="G8" s="59"/>
+      <c r="H8" s="35"/>
     </row>
     <row r="9" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B9" s="18" t="s">
+      <c r="B9" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="C9" s="44" t="s">
-        <v>47</v>
-      </c>
-      <c r="D9" s="22" t="s">
+      <c r="C9" s="56" t="s">
+        <v>46</v>
+      </c>
+      <c r="D9" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="E9" s="22" t="s">
+      <c r="E9" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="F9" s="56" t="s">
-        <v>54</v>
-      </c>
-      <c r="G9" s="55"/>
-      <c r="H9" s="40" t="s">
-        <v>45</v>
+      <c r="F9" s="63" t="s">
+        <v>53</v>
+      </c>
+      <c r="G9" s="60"/>
+      <c r="H9" s="51" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B10" s="19"/>
-      <c r="C10" s="45"/>
-      <c r="D10" s="23"/>
-      <c r="E10" s="23"/>
-      <c r="F10" s="32"/>
+      <c r="B10" s="21" t="s">
+        <v>73</v>
+      </c>
+      <c r="C10" s="57"/>
+      <c r="D10" s="28"/>
+      <c r="E10" s="28"/>
+      <c r="F10" s="41"/>
       <c r="G10" s="3"/>
-      <c r="H10" s="41"/>
-    </row>
-    <row r="11" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="H10" s="52"/>
+    </row>
+    <row r="11" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B11" s="24" t="s">
+      <c r="B11" s="29" t="s">
         <v>25</v>
       </c>
-      <c r="C11" s="22" t="s">
-        <v>26</v>
-      </c>
-      <c r="D11" s="44" t="s">
+      <c r="C11" s="29" t="s">
         <v>59</v>
       </c>
-      <c r="E11" s="22" t="s">
-        <v>26</v>
-      </c>
-      <c r="F11" s="22" t="s">
+      <c r="D11" s="56" t="s">
+        <v>58</v>
+      </c>
+      <c r="E11" s="56" t="s">
+        <v>45</v>
+      </c>
+      <c r="F11" s="27" t="s">
         <v>27</v>
       </c>
-      <c r="G11" s="18" t="s">
+      <c r="G11" s="36" t="s">
         <v>28</v>
       </c>
       <c r="H11" s="3"/>
     </row>
     <row r="12" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A12" s="6" t="s">
+      <c r="A12" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="B12" s="25"/>
-      <c r="C12" s="23"/>
-      <c r="D12" s="45"/>
-      <c r="E12" s="23"/>
-      <c r="F12" s="23"/>
-      <c r="G12" s="19"/>
+      <c r="B12" s="30"/>
+      <c r="C12" s="31"/>
+      <c r="D12" s="57"/>
+      <c r="E12" s="57"/>
+      <c r="F12" s="28"/>
+      <c r="G12" s="37"/>
       <c r="H12" s="3"/>
     </row>
-    <row r="13" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B13" s="26"/>
-      <c r="C13" s="48" t="s">
-        <v>54</v>
-      </c>
-      <c r="D13" s="7" t="s">
+      <c r="B13" s="31"/>
+      <c r="C13" s="36" t="s">
+        <v>28</v>
+      </c>
+      <c r="D13" s="38" t="s">
         <v>31</v>
       </c>
-      <c r="E13" s="18" t="s">
+      <c r="E13" s="36" t="s">
         <v>28</v>
       </c>
-      <c r="F13" s="9" t="s">
+      <c r="F13" s="8" t="s">
         <v>42</v>
       </c>
       <c r="G13" s="3"/>
@@ -2109,18 +2181,16 @@
       <c r="A14" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B14" s="9" t="s">
+      <c r="B14" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="C14" s="52"/>
-      <c r="D14" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="E14" s="19"/>
-      <c r="F14" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="G14" s="29" t="s">
+      <c r="C14" s="37"/>
+      <c r="D14" s="39"/>
+      <c r="E14" s="37"/>
+      <c r="F14" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="G14" s="34" t="s">
         <v>19</v>
       </c>
       <c r="H14" s="3"/>
@@ -2129,22 +2199,22 @@
       <c r="A15" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="B15" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C15" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="D15" s="20" t="s">
+      <c r="B15" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="C15" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="D15" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="E15" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="F15" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="E15" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="F15" s="20" t="s">
-        <v>18</v>
-      </c>
-      <c r="G15" s="30"/>
+      <c r="G15" s="35"/>
       <c r="H15" s="3"/>
     </row>
     <row r="16" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
@@ -2152,18 +2222,17 @@
         <v>35</v>
       </c>
       <c r="B16" s="3"/>
-      <c r="C16" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D16" s="21"/>
-      <c r="E16" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="F16" s="21"/>
-      <c r="G16" s="40" t="s">
-        <v>45</v>
-      </c>
-      <c r="H16" s="18" t="s">
+      <c r="C16" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="E16" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="F16" s="26"/>
+      <c r="G16" s="51" t="s">
+        <v>44</v>
+      </c>
+      <c r="H16" s="36" t="s">
         <v>28</v>
       </c>
     </row>
@@ -2171,27 +2240,31 @@
       <c r="A17" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="B17" s="3"/>
-      <c r="C17" s="14" t="s">
-        <v>52</v>
-      </c>
-      <c r="D17" s="29" t="s">
+      <c r="B17" s="20" t="s">
+        <v>72</v>
+      </c>
+      <c r="C17" s="53" t="s">
         <v>19</v>
       </c>
-      <c r="E17" s="14" t="s">
-        <v>52</v>
+      <c r="D17" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="E17" s="13" t="s">
+        <v>51</v>
       </c>
       <c r="F17" s="3"/>
-      <c r="G17" s="41"/>
-      <c r="H17" s="19"/>
+      <c r="G17" s="52"/>
+      <c r="H17" s="37"/>
     </row>
     <row r="18" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="B18" s="3"/>
-      <c r="C18" s="3"/>
-      <c r="D18" s="30"/>
+      <c r="B18" s="22" t="s">
+        <v>63</v>
+      </c>
+      <c r="C18" s="54"/>
+      <c r="D18" s="26"/>
       <c r="E18" s="3"/>
       <c r="F18" s="3"/>
       <c r="G18" s="3"/>
@@ -2202,7 +2275,7 @@
         <v>38</v>
       </c>
       <c r="B19" s="3"/>
-      <c r="C19" s="3"/>
+      <c r="C19" s="55"/>
       <c r="D19" s="3"/>
       <c r="E19" s="3"/>
       <c r="F19" s="3"/>
@@ -2210,36 +2283,35 @@
       <c r="H19" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="29">
+  <mergeCells count="28">
+    <mergeCell ref="G7:G9"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="E7:E8"/>
+    <mergeCell ref="F9:F10"/>
     <mergeCell ref="H7:H8"/>
     <mergeCell ref="C9:C10"/>
     <mergeCell ref="D9:D10"/>
     <mergeCell ref="E9:E10"/>
-    <mergeCell ref="G11:G12"/>
     <mergeCell ref="H9:H10"/>
+    <mergeCell ref="B11:B13"/>
+    <mergeCell ref="E11:E12"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="F11:F12"/>
     <mergeCell ref="C5:C6"/>
     <mergeCell ref="E5:E6"/>
     <mergeCell ref="F6:F8"/>
     <mergeCell ref="B7:B8"/>
-    <mergeCell ref="G7:G9"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="D6:D7"/>
-    <mergeCell ref="E7:E8"/>
-    <mergeCell ref="F9:F10"/>
-    <mergeCell ref="B11:B13"/>
     <mergeCell ref="C11:C12"/>
-    <mergeCell ref="D11:D12"/>
-    <mergeCell ref="E11:E12"/>
-    <mergeCell ref="F11:F12"/>
+    <mergeCell ref="C17:C19"/>
+    <mergeCell ref="D13:D14"/>
     <mergeCell ref="H16:H17"/>
+    <mergeCell ref="F15:F16"/>
     <mergeCell ref="D17:D18"/>
-    <mergeCell ref="F15:F16"/>
-    <mergeCell ref="D15:D16"/>
     <mergeCell ref="C13:C14"/>
     <mergeCell ref="E13:E14"/>
     <mergeCell ref="G16:G17"/>
     <mergeCell ref="G14:G15"/>
+    <mergeCell ref="G11:G12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2251,7 +2323,7 @@
   <dimension ref="A1:H19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14:B15"/>
+      <selection activeCell="D14" activeCellId="9" sqref="C16 B15 B6 C4 D8 E4 F5 F14 E16 D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2321,17 +2393,17 @@
         <v>9</v>
       </c>
       <c r="B4" s="3"/>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="12" t="s">
         <v>11</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="E4" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="F4" s="14" t="s">
-        <v>52</v>
+      <c r="E4" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" s="13" t="s">
+        <v>51</v>
       </c>
       <c r="G4" s="3"/>
       <c r="H4" s="3"/>
@@ -2340,19 +2412,19 @@
       <c r="A5" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="14" t="s">
-        <v>52</v>
-      </c>
-      <c r="C5" s="24" t="s">
+      <c r="B5" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="C5" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="14" t="s">
-        <v>52</v>
-      </c>
-      <c r="E5" s="24" t="s">
+      <c r="D5" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="E5" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="F5" s="5" t="s">
+      <c r="F5" s="12" t="s">
         <v>11</v>
       </c>
       <c r="G5" s="4" t="s">
@@ -2366,41 +2438,41 @@
       <c r="A6" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" s="26"/>
+      <c r="B6" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="31"/>
       <c r="D6" s="3"/>
-      <c r="E6" s="26"/>
-      <c r="F6" s="24" t="s">
+      <c r="E6" s="31"/>
+      <c r="F6" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="G6" s="14" t="s">
-        <v>52</v>
-      </c>
-      <c r="H6" s="14" t="s">
-        <v>52</v>
+      <c r="G6" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="H6" s="13" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="22" t="s">
+      <c r="B7" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="40" t="s">
-        <v>45</v>
-      </c>
-      <c r="D7" s="12" t="s">
-        <v>50</v>
+      <c r="C7" s="51" t="s">
+        <v>44</v>
+      </c>
+      <c r="D7" s="11" t="s">
+        <v>49</v>
       </c>
       <c r="E7" s="3"/>
-      <c r="F7" s="25"/>
-      <c r="G7" s="35" t="s">
+      <c r="F7" s="30"/>
+      <c r="G7" s="42" t="s">
         <v>18</v>
       </c>
-      <c r="H7" s="29" t="s">
+      <c r="H7" s="34" t="s">
         <v>19</v>
       </c>
     </row>
@@ -2408,35 +2480,35 @@
       <c r="A8" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="23"/>
-      <c r="C8" s="41"/>
-      <c r="D8" s="5" t="s">
+      <c r="B8" s="28"/>
+      <c r="C8" s="52"/>
+      <c r="D8" s="12" t="s">
         <v>11</v>
       </c>
       <c r="E8" s="3"/>
-      <c r="F8" s="26"/>
-      <c r="G8" s="36"/>
-      <c r="H8" s="30"/>
+      <c r="F8" s="31"/>
+      <c r="G8" s="43"/>
+      <c r="H8" s="35"/>
     </row>
     <row r="9" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B9" s="18" t="s">
+      <c r="B9" s="36" t="s">
         <v>28</v>
       </c>
-      <c r="C9" s="22" t="s">
+      <c r="C9" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="D9" s="22" t="s">
+      <c r="D9" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="E9" s="22" t="s">
+      <c r="E9" s="27" t="s">
         <v>22</v>
       </c>
       <c r="F9" s="3"/>
-      <c r="G9" s="37"/>
-      <c r="H9" s="18" t="s">
+      <c r="G9" s="44"/>
+      <c r="H9" s="36" t="s">
         <v>28</v>
       </c>
     </row>
@@ -2444,65 +2516,65 @@
       <c r="A10" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B10" s="19"/>
-      <c r="C10" s="23"/>
-      <c r="D10" s="23"/>
-      <c r="E10" s="23"/>
+      <c r="B10" s="37"/>
+      <c r="C10" s="28"/>
+      <c r="D10" s="28"/>
+      <c r="E10" s="28"/>
       <c r="F10" s="3"/>
       <c r="G10" s="3"/>
-      <c r="H10" s="19"/>
+      <c r="H10" s="37"/>
     </row>
     <row r="11" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B11" s="24" t="s">
+      <c r="B11" s="29" t="s">
         <v>25</v>
       </c>
-      <c r="C11" s="22" t="s">
+      <c r="C11" s="27" t="s">
         <v>26</v>
       </c>
-      <c r="D11" s="22" t="s">
+      <c r="D11" s="27" t="s">
         <v>27</v>
       </c>
-      <c r="E11" s="22" t="s">
+      <c r="E11" s="27" t="s">
         <v>26</v>
       </c>
-      <c r="F11" s="22" t="s">
+      <c r="F11" s="27" t="s">
         <v>27</v>
       </c>
-      <c r="G11" s="18" t="s">
+      <c r="G11" s="36" t="s">
         <v>28</v>
       </c>
       <c r="H11" s="3"/>
     </row>
     <row r="12" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A12" s="6" t="s">
+      <c r="A12" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="B12" s="25"/>
-      <c r="C12" s="23"/>
-      <c r="D12" s="23"/>
-      <c r="E12" s="23"/>
-      <c r="F12" s="23"/>
-      <c r="G12" s="19"/>
+      <c r="B12" s="30"/>
+      <c r="C12" s="28"/>
+      <c r="D12" s="28"/>
+      <c r="E12" s="28"/>
+      <c r="F12" s="28"/>
+      <c r="G12" s="37"/>
       <c r="H12" s="3"/>
     </row>
     <row r="13" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B13" s="26"/>
-      <c r="C13" s="50" t="s">
-        <v>51</v>
-      </c>
-      <c r="D13" s="7" t="s">
+      <c r="B13" s="31"/>
+      <c r="C13" s="61" t="s">
+        <v>50</v>
+      </c>
+      <c r="D13" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="E13" s="50" t="s">
-        <v>51</v>
-      </c>
-      <c r="F13" s="9" t="s">
+      <c r="E13" s="61" t="s">
+        <v>50</v>
+      </c>
+      <c r="F13" s="8" t="s">
         <v>42</v>
       </c>
       <c r="G13" s="3"/>
@@ -2512,18 +2584,18 @@
       <c r="A14" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B14" s="9" t="s">
+      <c r="B14" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="C14" s="51"/>
-      <c r="D14" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="E14" s="51"/>
-      <c r="F14" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="G14" s="20" t="s">
+      <c r="C14" s="62"/>
+      <c r="D14" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="E14" s="62"/>
+      <c r="F14" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="G14" s="25" t="s">
         <v>18</v>
       </c>
       <c r="H14" s="3"/>
@@ -2532,22 +2604,22 @@
       <c r="A15" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="B15" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C15" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="D15" s="20" t="s">
+      <c r="B15" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="C15" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="D15" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="E15" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="F15" s="29" t="s">
+      <c r="E15" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="F15" s="34" t="s">
         <v>19</v>
       </c>
-      <c r="G15" s="21"/>
+      <c r="G15" s="26"/>
       <c r="H15" s="3"/>
     </row>
     <row r="16" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
@@ -2555,14 +2627,14 @@
         <v>35</v>
       </c>
       <c r="B16" s="3"/>
-      <c r="C16" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D16" s="21"/>
-      <c r="E16" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="F16" s="30"/>
+      <c r="C16" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="D16" s="26"/>
+      <c r="E16" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="F16" s="35"/>
       <c r="G16" s="3"/>
       <c r="H16" s="3"/>
     </row>
@@ -2571,18 +2643,18 @@
         <v>36</v>
       </c>
       <c r="B17" s="3"/>
-      <c r="C17" s="14" t="s">
-        <v>52</v>
-      </c>
-      <c r="D17" s="29" t="s">
+      <c r="C17" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="D17" s="34" t="s">
         <v>19</v>
       </c>
-      <c r="E17" s="14" t="s">
-        <v>52</v>
+      <c r="E17" s="13" t="s">
+        <v>51</v>
       </c>
       <c r="F17" s="3"/>
       <c r="G17" s="3"/>
-      <c r="H17" s="20" t="s">
+      <c r="H17" s="25" t="s">
         <v>18</v>
       </c>
     </row>
@@ -2592,11 +2664,11 @@
       </c>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
-      <c r="D18" s="30"/>
+      <c r="D18" s="35"/>
       <c r="E18" s="3"/>
       <c r="F18" s="3"/>
       <c r="G18" s="3"/>
-      <c r="H18" s="21"/>
+      <c r="H18" s="26"/>
     </row>
     <row r="19" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">

</xml_diff>

<commit_message>
Nuevo horario para siguientes semanas.
</commit_message>
<xml_diff>
--- a/Programar_dias.xlsx
+++ b/Programar_dias.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Estudio\OneDrive - Universidad de Antioquia\Estudio\Materias\Informatica II\Calendario_semanal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08A6CEFD-8284-4ED9-9E46-C77E2277E192}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1438537A-D84A-4FA5-8008-6D52DC7AA0E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{CC961CB2-F623-4B13-8239-4B70F16E4462}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="341" uniqueCount="79">
   <si>
     <t>LUNES</t>
   </si>
@@ -224,9 +224,6 @@
     <t>Yoga</t>
   </si>
   <si>
-    <t>Programar</t>
-  </si>
-  <si>
     <t>Programar Kaggle</t>
   </si>
   <si>
@@ -270,9 +267,6 @@
     <t>CIRCUITOS II</t>
   </si>
   <si>
-    <t>Estd. Circuitos</t>
-  </si>
-  <si>
     <t>Mercado</t>
   </si>
   <si>
@@ -306,10 +300,31 @@
     <t>Leer</t>
   </si>
   <si>
-    <t>Estud Info II</t>
-  </si>
-  <si>
     <t>Asesoría Esp.</t>
+  </si>
+  <si>
+    <t>Informe Lab.</t>
+  </si>
+  <si>
+    <t>Repaso Info II</t>
+  </si>
+  <si>
+    <t>Repaso M. Esp</t>
+  </si>
+  <si>
+    <t>Repaso Circuitos</t>
+  </si>
+  <si>
+    <t>LAB INFORMÁTICA</t>
+  </si>
+  <si>
+    <t>Est. Especiales</t>
+  </si>
+  <si>
+    <t>Repaso Metodos</t>
+  </si>
+  <si>
+    <t>Est. Física.</t>
   </si>
 </sst>
 </file>
@@ -389,7 +404,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="17">
+  <fills count="21">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -486,6 +501,30 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCC66FF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="5">
     <border>
@@ -551,7 +590,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="73">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -581,9 +620,6 @@
     <xf numFmtId="0" fontId="2" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -600,15 +636,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -618,8 +648,38 @@
     <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -627,21 +687,6 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -654,24 +699,12 @@
     <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -682,15 +715,21 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -699,19 +738,22 @@
     <xf numFmtId="0" fontId="4" fillId="14" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -720,29 +762,47 @@
     <xf numFmtId="0" fontId="1" fillId="14" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="17" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -752,6 +812,7 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFCC66FF"/>
       <color rgb="FFFFFF66"/>
       <color rgb="FF33CCFF"/>
       <color rgb="FF0099FF"/>
@@ -1138,7 +1199,7 @@
         <v>9</v>
       </c>
       <c r="B4" s="3"/>
-      <c r="C4" s="12" t="s">
+      <c r="C4" s="11" t="s">
         <v>11</v>
       </c>
       <c r="D4" s="4" t="s">
@@ -1153,19 +1214,19 @@
       <c r="A5" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="14" t="s">
+      <c r="B5" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="29" t="s">
+      <c r="C5" s="25" t="s">
         <v>13</v>
       </c>
       <c r="D5" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="E5" s="29" t="s">
+        <v>50</v>
+      </c>
+      <c r="E5" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="F5" s="12" t="s">
+      <c r="F5" s="11" t="s">
         <v>11</v>
       </c>
       <c r="G5" s="3"/>
@@ -1175,15 +1236,15 @@
       <c r="A6" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" s="31"/>
-      <c r="D6" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="E6" s="31"/>
-      <c r="F6" s="29" t="s">
+      <c r="B6" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="26"/>
+      <c r="D6" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" s="26"/>
+      <c r="F6" s="25" t="s">
         <v>15</v>
       </c>
       <c r="G6" s="3"/>
@@ -1193,17 +1254,17 @@
       <c r="A7" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="27" t="s">
+      <c r="B7" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="36" t="s">
+      <c r="C7" s="30" t="s">
         <v>28</v>
       </c>
       <c r="D7" s="3"/>
-      <c r="E7" s="40" t="s">
+      <c r="E7" s="23" t="s">
         <v>47</v>
       </c>
-      <c r="F7" s="30"/>
+      <c r="F7" s="27"/>
       <c r="G7" s="3"/>
       <c r="H7" s="4" t="s">
         <v>10</v>
@@ -1213,15 +1274,15 @@
       <c r="A8" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="28"/>
-      <c r="C8" s="37"/>
+      <c r="B8" s="29"/>
+      <c r="C8" s="31"/>
       <c r="D8" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="E8" s="41"/>
-      <c r="F8" s="31"/>
+        <v>54</v>
+      </c>
+      <c r="E8" s="24"/>
+      <c r="F8" s="26"/>
       <c r="G8" s="3"/>
-      <c r="H8" s="25" t="s">
+      <c r="H8" s="32" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1229,33 +1290,33 @@
       <c r="A9" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B9" s="14" t="s">
+      <c r="B9" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="C9" s="27" t="s">
+      <c r="C9" s="28" t="s">
         <v>22</v>
       </c>
-      <c r="D9" s="27" t="s">
+      <c r="D9" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="E9" s="27" t="s">
+      <c r="E9" s="28" t="s">
         <v>22</v>
       </c>
-      <c r="F9" s="36" t="s">
+      <c r="F9" s="30" t="s">
         <v>28</v>
       </c>
       <c r="G9" s="3"/>
-      <c r="H9" s="26"/>
+      <c r="H9" s="33"/>
     </row>
     <row r="10" spans="1:10" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B10" s="14"/>
-      <c r="C10" s="28"/>
-      <c r="D10" s="28"/>
-      <c r="E10" s="28"/>
-      <c r="F10" s="37"/>
+      <c r="B10" s="13"/>
+      <c r="C10" s="29"/>
+      <c r="D10" s="29"/>
+      <c r="E10" s="29"/>
+      <c r="F10" s="31"/>
       <c r="G10" s="3"/>
       <c r="H10" s="3"/>
     </row>
@@ -1263,23 +1324,23 @@
       <c r="A11" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B11" s="29" t="s">
+      <c r="B11" s="25" t="s">
         <v>25</v>
       </c>
-      <c r="C11" s="27" t="s">
+      <c r="C11" s="28" t="s">
         <v>26</v>
       </c>
-      <c r="D11" s="27" t="s">
+      <c r="D11" s="28" t="s">
         <v>27</v>
       </c>
       <c r="E11" s="3"/>
-      <c r="F11" s="27" t="s">
-        <v>57</v>
-      </c>
-      <c r="G11" s="40" t="s">
+      <c r="F11" s="28" t="s">
+        <v>56</v>
+      </c>
+      <c r="G11" s="23" t="s">
         <v>47</v>
       </c>
-      <c r="H11" s="25" t="s">
+      <c r="H11" s="32" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1287,31 +1348,31 @@
       <c r="A12" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="B12" s="30"/>
-      <c r="C12" s="28"/>
-      <c r="D12" s="28"/>
-      <c r="F12" s="28"/>
-      <c r="G12" s="41"/>
-      <c r="H12" s="26"/>
+      <c r="B12" s="27"/>
+      <c r="C12" s="29"/>
+      <c r="D12" s="29"/>
+      <c r="F12" s="29"/>
+      <c r="G12" s="24"/>
+      <c r="H12" s="33"/>
     </row>
     <row r="13" spans="1:10" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B13" s="31"/>
-      <c r="C13" s="12" t="s">
+      <c r="B13" s="26"/>
+      <c r="C13" s="11" t="s">
         <v>11</v>
       </c>
       <c r="D13" s="38" t="s">
         <v>31</v>
       </c>
-      <c r="E13" s="12" t="s">
+      <c r="E13" s="11" t="s">
         <v>11</v>
       </c>
       <c r="F13" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="H13" s="12" t="s">
+      <c r="H13" s="11" t="s">
         <v>11</v>
       </c>
     </row>
@@ -1319,14 +1380,14 @@
       <c r="A14" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B14" s="12" t="s">
+      <c r="B14" s="11" t="s">
         <v>11</v>
       </c>
       <c r="C14" s="3"/>
       <c r="D14" s="39"/>
       <c r="E14" s="3"/>
       <c r="F14" s="3"/>
-      <c r="G14" s="32" t="s">
+      <c r="G14" s="34" t="s">
         <v>44</v>
       </c>
       <c r="H14" s="3" t="s">
@@ -1339,16 +1400,16 @@
         <v>34</v>
       </c>
       <c r="B15" s="3"/>
-      <c r="C15" s="32" t="s">
+      <c r="C15" s="34" t="s">
         <v>44</v>
       </c>
-      <c r="D15" s="15" t="s">
-        <v>56</v>
+      <c r="D15" s="14" t="s">
+        <v>55</v>
       </c>
       <c r="E15" s="3"/>
       <c r="F15" s="3"/>
-      <c r="G15" s="33"/>
-      <c r="H15" s="12" t="s">
+      <c r="G15" s="35"/>
+      <c r="H15" s="11" t="s">
         <v>11</v>
       </c>
     </row>
@@ -1357,18 +1418,18 @@
         <v>35</v>
       </c>
       <c r="B16" s="3"/>
-      <c r="C16" s="33"/>
-      <c r="D16" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="E16" s="36" t="s">
+      <c r="C16" s="35"/>
+      <c r="D16" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="E16" s="30" t="s">
         <v>28</v>
       </c>
       <c r="F16" s="3"/>
-      <c r="G16" s="42" t="s">
+      <c r="G16" s="40" t="s">
         <v>18</v>
       </c>
-      <c r="H16" s="36" t="s">
+      <c r="H16" s="30" t="s">
         <v>28</v>
       </c>
     </row>
@@ -1377,36 +1438,36 @@
         <v>36</v>
       </c>
       <c r="B17" s="10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C17" s="3"/>
       <c r="D17" s="3"/>
-      <c r="E17" s="37"/>
-      <c r="F17" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="G17" s="43"/>
-      <c r="H17" s="37"/>
+      <c r="E17" s="31"/>
+      <c r="F17" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="G17" s="41"/>
+      <c r="H17" s="31"/>
     </row>
     <row r="18" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="B18" s="25" t="s">
+      <c r="B18" s="32" t="s">
         <v>18</v>
       </c>
-      <c r="C18" s="32" t="s">
+      <c r="C18" s="34" t="s">
         <v>44</v>
       </c>
-      <c r="D18" s="34" t="s">
+      <c r="D18" s="36" t="s">
         <v>19</v>
       </c>
-      <c r="E18" s="25" t="s">
+      <c r="E18" s="32" t="s">
         <v>18</v>
       </c>
       <c r="F18" s="3"/>
-      <c r="G18" s="44"/>
-      <c r="H18" s="25" t="s">
+      <c r="G18" s="42"/>
+      <c r="H18" s="32" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1414,28 +1475,16 @@
       <c r="A19" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="B19" s="26"/>
-      <c r="C19" s="33"/>
-      <c r="D19" s="35"/>
-      <c r="E19" s="26"/>
+      <c r="B19" s="33"/>
+      <c r="C19" s="35"/>
+      <c r="D19" s="37"/>
+      <c r="E19" s="33"/>
       <c r="F19" s="3"/>
       <c r="G19" s="3"/>
-      <c r="H19" s="26"/>
+      <c r="H19" s="33"/>
     </row>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="G11:G12"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="E5:E6"/>
-    <mergeCell ref="F6:F8"/>
-    <mergeCell ref="C11:C12"/>
-    <mergeCell ref="D11:D12"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="D9:D10"/>
-    <mergeCell ref="E9:E10"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="F9:F10"/>
-    <mergeCell ref="E7:E8"/>
     <mergeCell ref="H8:H9"/>
     <mergeCell ref="H11:H12"/>
     <mergeCell ref="B18:B19"/>
@@ -1452,6 +1501,18 @@
     <mergeCell ref="H16:H17"/>
     <mergeCell ref="G14:G15"/>
     <mergeCell ref="G16:G18"/>
+    <mergeCell ref="G11:G12"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="F6:F8"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="E9:E10"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="F9:F10"/>
+    <mergeCell ref="E7:E8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1462,24 +1523,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF8929EB-A174-48F2-BDBD-469036EC404B}">
   <dimension ref="A1:J19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7:G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.85546875" customWidth="1"/>
-    <col min="2" max="2" width="16.85546875" customWidth="1"/>
-    <col min="3" max="3" width="15.85546875" customWidth="1"/>
-    <col min="4" max="4" width="15.28515625" customWidth="1"/>
-    <col min="5" max="5" width="19.5703125" customWidth="1"/>
-    <col min="6" max="6" width="18.140625" customWidth="1"/>
-    <col min="7" max="7" width="16" customWidth="1"/>
-    <col min="8" max="8" width="15.5703125" customWidth="1"/>
+    <col min="1" max="8" width="18.7109375" customWidth="1"/>
     <col min="10" max="10" width="20.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>40</v>
       </c>
@@ -1505,7 +1559,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>7</v>
       </c>
@@ -1517,10 +1571,10 @@
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
       <c r="J2" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" ht="16.5" x14ac:dyDescent="0.3">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>8</v>
       </c>
@@ -1529,56 +1583,56 @@
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
-      <c r="G3" s="15" t="s">
-        <v>56</v>
-      </c>
-      <c r="H3" s="25" t="s">
+      <c r="G3" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="H3" s="32" t="s">
         <v>18</v>
       </c>
       <c r="J3" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" s="45" t="s">
+      <c r="B4" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="47" t="s">
         <v>44</v>
       </c>
-      <c r="E4" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="F4" s="13" t="s">
-        <v>51</v>
+      <c r="E4" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" s="12" t="s">
+        <v>50</v>
       </c>
       <c r="G4" s="3"/>
-      <c r="H4" s="26"/>
+      <c r="H4" s="33"/>
       <c r="J4" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="25" t="s">
+      <c r="B5" s="32" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="29" t="s">
+      <c r="C5" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="46"/>
-      <c r="E5" s="29" t="s">
+      <c r="D5" s="48"/>
+      <c r="E5" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="F5" s="12" t="s">
+      <c r="F5" s="11" t="s">
         <v>11</v>
       </c>
       <c r="G5" s="4" t="s">
@@ -1588,285 +1642,303 @@
         <v>10</v>
       </c>
       <c r="J5" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="26"/>
-      <c r="C6" s="31"/>
-      <c r="D6" s="47" t="s">
+      <c r="B6" s="33"/>
+      <c r="C6" s="26"/>
+      <c r="D6" s="45" t="s">
         <v>33</v>
       </c>
-      <c r="E6" s="31"/>
-      <c r="F6" s="29" t="s">
+      <c r="E6" s="26"/>
+      <c r="F6" s="25" t="s">
         <v>15</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="H6" s="13" t="s">
-        <v>51</v>
+        <v>59</v>
+      </c>
+      <c r="H6" s="12" t="s">
+        <v>50</v>
       </c>
       <c r="J6" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="27" t="s">
+      <c r="B7" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="47" t="s">
+      <c r="C7" s="45" t="s">
         <v>33</v>
       </c>
-      <c r="D7" s="48"/>
-      <c r="E7" s="64" t="s">
+      <c r="D7" s="46"/>
+      <c r="E7" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="F7" s="30"/>
-      <c r="G7" s="42" t="s">
+      <c r="F7" s="27"/>
+      <c r="G7" s="40" t="s">
         <v>18</v>
       </c>
-      <c r="H7" s="34" t="s">
+      <c r="H7" s="36" t="s">
         <v>19</v>
       </c>
       <c r="J7" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" ht="16.5" x14ac:dyDescent="0.3">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="28"/>
-      <c r="C8" s="48"/>
-      <c r="D8" s="36" t="s">
+      <c r="B8" s="29"/>
+      <c r="C8" s="46"/>
+      <c r="D8" s="30" t="s">
         <v>28</v>
       </c>
-      <c r="E8" s="65" t="s">
-        <v>55</v>
-      </c>
-      <c r="F8" s="31"/>
-      <c r="G8" s="43"/>
-      <c r="H8" s="35"/>
-    </row>
-    <row r="9" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E8" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="F8" s="26"/>
+      <c r="G8" s="41"/>
+      <c r="H8" s="37"/>
+    </row>
+    <row r="9" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B9" s="40" t="s">
+      <c r="B9" s="23" t="s">
         <v>47</v>
       </c>
-      <c r="C9" s="29" t="s">
-        <v>52</v>
-      </c>
-      <c r="D9" s="37"/>
-      <c r="E9" s="29" t="s">
-        <v>52</v>
-      </c>
-      <c r="F9" s="17" t="s">
+      <c r="C9" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="D9" s="31"/>
+      <c r="E9" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="F9" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="G9" s="44"/>
-      <c r="H9" s="51" t="s">
+      <c r="G9" s="42"/>
+      <c r="H9" s="43" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B10" s="41"/>
-      <c r="C10" s="31"/>
-      <c r="D10" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="E10" s="31"/>
+      <c r="B10" s="24"/>
+      <c r="C10" s="26"/>
+      <c r="D10" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="E10" s="26"/>
       <c r="F10" s="3"/>
       <c r="G10" s="3"/>
-      <c r="H10" s="52"/>
-    </row>
-    <row r="11" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="H10" s="44"/>
+    </row>
+    <row r="11" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B11" s="29" t="s">
+      <c r="B11" s="25" t="s">
         <v>25</v>
       </c>
-      <c r="C11" s="29" t="s">
-        <v>59</v>
-      </c>
-      <c r="D11" s="29" t="s">
-        <v>57</v>
-      </c>
-      <c r="E11" s="29" t="s">
-        <v>59</v>
+      <c r="C11" s="25" t="s">
+        <v>58</v>
+      </c>
+      <c r="D11" s="25" t="s">
+        <v>56</v>
+      </c>
+      <c r="E11" s="25" t="s">
+        <v>58</v>
       </c>
       <c r="F11" s="49" t="s">
         <v>43</v>
       </c>
-      <c r="G11" s="36" t="s">
+      <c r="G11" s="30" t="s">
         <v>28</v>
       </c>
       <c r="H11" s="3"/>
     </row>
-    <row r="12" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="B12" s="30"/>
-      <c r="C12" s="31"/>
-      <c r="D12" s="31"/>
-      <c r="E12" s="31"/>
+      <c r="B12" s="27"/>
+      <c r="C12" s="26"/>
+      <c r="D12" s="26"/>
+      <c r="E12" s="26"/>
       <c r="F12" s="50"/>
-      <c r="G12" s="37"/>
+      <c r="G12" s="31"/>
       <c r="H12" s="3"/>
     </row>
-    <row r="13" spans="1:10" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B13" s="31"/>
-      <c r="C13" s="12" t="s">
+      <c r="B13" s="26"/>
+      <c r="C13" s="11" t="s">
         <v>11</v>
       </c>
       <c r="D13" s="38" t="s">
         <v>31</v>
       </c>
-      <c r="E13" s="12" t="s">
+      <c r="E13" s="11" t="s">
         <v>11</v>
       </c>
       <c r="F13" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="G13" s="13" t="s">
-        <v>51</v>
-      </c>
-      <c r="H13" s="42" t="s">
+      <c r="G13" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="H13" s="40" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
         <v>32</v>
       </c>
       <c r="B14" s="3"/>
-      <c r="C14" s="36" t="s">
+      <c r="C14" s="30" t="s">
         <v>28</v>
       </c>
       <c r="D14" s="39"/>
-      <c r="E14" s="36" t="s">
-        <v>28</v>
-      </c>
-      <c r="F14" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="G14" s="17" t="s">
-        <v>60</v>
-      </c>
-      <c r="H14" s="43"/>
-    </row>
-    <row r="15" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F14" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="G14" s="63" t="s">
+        <v>71</v>
+      </c>
+      <c r="H14" s="41"/>
+    </row>
+    <row r="15" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="B15" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="C15" s="37"/>
+      <c r="B15" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="C15" s="31"/>
       <c r="D15" s="3"/>
-      <c r="E15" s="37"/>
-      <c r="F15" s="47" t="s">
-        <v>62</v>
-      </c>
-      <c r="G15" s="47" t="s">
+      <c r="E15" s="30" t="s">
+        <v>28</v>
+      </c>
+      <c r="F15" s="45" t="s">
+        <v>60</v>
+      </c>
+      <c r="G15" s="45" t="s">
         <v>33</v>
       </c>
-      <c r="H15" s="44"/>
-    </row>
-    <row r="16" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="H15" s="42"/>
+    </row>
+    <row r="16" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="B16" s="45" t="s">
+      <c r="B16" s="47" t="s">
         <v>44</v>
       </c>
-      <c r="C16" s="45" t="s">
+      <c r="C16" s="47" t="s">
         <v>44</v>
       </c>
       <c r="D16" s="3"/>
-      <c r="E16" s="13" t="s">
-        <v>51</v>
-      </c>
-      <c r="F16" s="48"/>
-      <c r="G16" s="48"/>
-      <c r="H16" s="36" t="s">
+      <c r="E16" s="31"/>
+      <c r="F16" s="46"/>
+      <c r="G16" s="46"/>
+      <c r="H16" s="67" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="B17" s="46"/>
-      <c r="C17" s="46"/>
-      <c r="D17" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="E17" s="17" t="s">
-        <v>19</v>
-      </c>
-      <c r="F17" s="19" t="s">
-        <v>63</v>
+      <c r="B17" s="48"/>
+      <c r="C17" s="48"/>
+      <c r="D17" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="E17" s="30" t="s">
+        <v>28</v>
+      </c>
+      <c r="F17" s="17" t="s">
+        <v>61</v>
       </c>
       <c r="G17" s="3"/>
-      <c r="H17" s="37"/>
-    </row>
-    <row r="18" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="H17" s="68"/>
+    </row>
+    <row r="18" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="B18" s="16" t="s">
+      <c r="B18" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="C18" s="47" t="s">
+      <c r="C18" s="45" t="s">
         <v>33</v>
       </c>
-      <c r="D18" s="47" t="s">
+      <c r="D18" s="45" t="s">
         <v>33</v>
       </c>
-      <c r="E18" s="15" t="s">
-        <v>56</v>
-      </c>
-      <c r="F18" s="42" t="s">
+      <c r="E18" s="31"/>
+      <c r="F18" s="40" t="s">
         <v>18</v>
       </c>
-      <c r="G18" s="19" t="s">
-        <v>63</v>
-      </c>
-      <c r="H18" s="3"/>
-    </row>
-    <row r="19" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="G18" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="H18" s="69"/>
+    </row>
+    <row r="19" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
         <v>38</v>
       </c>
       <c r="B19" s="3"/>
-      <c r="C19" s="48"/>
-      <c r="D19" s="48"/>
-      <c r="E19" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="F19" s="44"/>
-      <c r="G19" s="3"/>
-      <c r="H19" s="3"/>
+      <c r="C19" s="46"/>
+      <c r="D19" s="46"/>
+      <c r="E19" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="F19" s="42"/>
+      <c r="G19" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="H19" s="66" t="s">
+        <v>76</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="34">
+  <mergeCells count="35">
+    <mergeCell ref="H7:H8"/>
+    <mergeCell ref="E15:E16"/>
+    <mergeCell ref="E17:E18"/>
+    <mergeCell ref="H16:H18"/>
+    <mergeCell ref="F18:F19"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="C16:C17"/>
+    <mergeCell ref="G15:G16"/>
+    <mergeCell ref="F15:F16"/>
+    <mergeCell ref="C18:C19"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="D18:D19"/>
+    <mergeCell ref="H13:H15"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="B11:B13"/>
+    <mergeCell ref="E11:E12"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="F11:F12"/>
+    <mergeCell ref="C11:C12"/>
     <mergeCell ref="G11:G12"/>
     <mergeCell ref="H9:H10"/>
     <mergeCell ref="B7:B8"/>
@@ -1879,28 +1951,10 @@
     <mergeCell ref="D8:D9"/>
     <mergeCell ref="C9:C10"/>
     <mergeCell ref="E9:E10"/>
-    <mergeCell ref="B16:B17"/>
-    <mergeCell ref="B11:B13"/>
-    <mergeCell ref="E11:E12"/>
-    <mergeCell ref="D11:D12"/>
-    <mergeCell ref="F11:F12"/>
-    <mergeCell ref="C11:C12"/>
     <mergeCell ref="H3:H4"/>
-    <mergeCell ref="F18:F19"/>
-    <mergeCell ref="H16:H17"/>
-    <mergeCell ref="E14:E15"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="C16:C17"/>
-    <mergeCell ref="G15:G16"/>
-    <mergeCell ref="F15:F16"/>
-    <mergeCell ref="C18:C19"/>
-    <mergeCell ref="D13:D14"/>
-    <mergeCell ref="D18:D19"/>
-    <mergeCell ref="H13:H15"/>
     <mergeCell ref="C5:C6"/>
     <mergeCell ref="E5:E6"/>
     <mergeCell ref="F6:F8"/>
-    <mergeCell ref="H7:H8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1911,25 +1965,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B17F021-0D0A-4F72-92FE-4A0D3181A797}">
   <dimension ref="A1:H19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11:G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.5703125" customWidth="1"/>
-    <col min="2" max="2" width="15.5703125" customWidth="1"/>
-    <col min="3" max="3" width="15.85546875" customWidth="1"/>
-    <col min="4" max="4" width="15.28515625" customWidth="1"/>
-    <col min="5" max="5" width="16.42578125" customWidth="1"/>
-    <col min="6" max="6" width="16" customWidth="1"/>
-    <col min="7" max="7" width="15.5703125" customWidth="1"/>
-    <col min="8" max="8" width="14.85546875" customWidth="1"/>
+    <col min="1" max="8" width="18.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -1953,7 +2000,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>7</v>
       </c>
@@ -1965,7 +2012,7 @@
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
     </row>
-    <row r="3" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>8</v>
       </c>
@@ -1977,45 +2024,45 @@
       <c r="G3" s="3"/>
       <c r="H3" s="3"/>
     </row>
-    <row r="4" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>9</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="12" t="s">
+      <c r="C4" s="11" t="s">
         <v>11</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="E4" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="F4" s="13" t="s">
-        <v>51</v>
+      <c r="E4" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" s="12" t="s">
+        <v>50</v>
       </c>
       <c r="G4" s="3"/>
       <c r="H4" s="3"/>
     </row>
-    <row r="5" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="13" t="s">
-        <v>65</v>
-      </c>
-      <c r="C5" s="29" t="s">
+      <c r="B5" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="C5" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="13" t="s">
-        <v>51</v>
-      </c>
-      <c r="E5" s="29" t="s">
+      <c r="D5" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="E5" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="F5" s="12" t="s">
+      <c r="F5" s="11" t="s">
         <v>11</v>
       </c>
       <c r="G5" s="4" t="s">
@@ -2025,257 +2072,261 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" s="31"/>
-      <c r="D6" s="22" t="s">
-        <v>63</v>
-      </c>
-      <c r="E6" s="31"/>
-      <c r="F6" s="29" t="s">
+      <c r="B6" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="26"/>
+      <c r="D6" s="19" t="s">
+        <v>61</v>
+      </c>
+      <c r="E6" s="26"/>
+      <c r="F6" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="G6" s="13" t="s">
-        <v>51</v>
-      </c>
-      <c r="H6" s="13" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="H6" s="12" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>16</v>
       </c>
       <c r="B7" s="49" t="s">
-        <v>64</v>
-      </c>
-      <c r="C7" s="51" t="s">
+        <v>62</v>
+      </c>
+      <c r="C7" s="43" t="s">
         <v>44</v>
       </c>
-      <c r="D7" s="24"/>
-      <c r="E7" s="61" t="s">
-        <v>50</v>
-      </c>
-      <c r="F7" s="30"/>
-      <c r="G7" s="58" t="s">
+      <c r="D7" s="63" t="s">
+        <v>71</v>
+      </c>
+      <c r="E7" s="54" t="s">
+        <v>49</v>
+      </c>
+      <c r="F7" s="27"/>
+      <c r="G7" s="51" t="s">
         <v>18</v>
       </c>
-      <c r="H7" s="34" t="s">
+      <c r="H7" s="59" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>20</v>
       </c>
       <c r="B8" s="50"/>
-      <c r="C8" s="52"/>
-      <c r="D8" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="E8" s="62"/>
-      <c r="F8" s="31"/>
-      <c r="G8" s="59"/>
-      <c r="H8" s="35"/>
-    </row>
-    <row r="9" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="C8" s="44"/>
+      <c r="D8" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8" s="55"/>
+      <c r="F8" s="26"/>
+      <c r="G8" s="52"/>
+      <c r="H8" s="61"/>
+    </row>
+    <row r="9" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B9" s="23" t="s">
+      <c r="B9" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="C9" s="56" t="s">
+      <c r="C9" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="D9" s="28" t="s">
+        <v>17</v>
+      </c>
+      <c r="E9" s="57" t="s">
         <v>46</v>
       </c>
-      <c r="D9" s="27" t="s">
-        <v>17</v>
-      </c>
-      <c r="E9" s="27" t="s">
-        <v>22</v>
-      </c>
-      <c r="F9" s="63" t="s">
-        <v>53</v>
-      </c>
-      <c r="G9" s="60"/>
-      <c r="H9" s="51" t="s">
+      <c r="F9" s="56" t="s">
+        <v>52</v>
+      </c>
+      <c r="G9" s="53"/>
+      <c r="H9" s="43" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B10" s="21" t="s">
-        <v>73</v>
-      </c>
-      <c r="C10" s="57"/>
-      <c r="D10" s="28"/>
-      <c r="E10" s="28"/>
-      <c r="F10" s="41"/>
+      <c r="B10" s="18" t="s">
+        <v>70</v>
+      </c>
+      <c r="C10" s="26"/>
+      <c r="D10" s="29"/>
+      <c r="E10" s="58"/>
+      <c r="F10" s="24"/>
       <c r="G10" s="3"/>
-      <c r="H10" s="52"/>
-    </row>
-    <row r="11" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="H10" s="44"/>
+    </row>
+    <row r="11" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B11" s="29" t="s">
+      <c r="B11" s="25" t="s">
         <v>25</v>
       </c>
-      <c r="C11" s="29" t="s">
-        <v>59</v>
-      </c>
-      <c r="D11" s="56" t="s">
+      <c r="C11" s="25" t="s">
         <v>58</v>
       </c>
-      <c r="E11" s="56" t="s">
+      <c r="D11" s="57" t="s">
+        <v>57</v>
+      </c>
+      <c r="E11" s="57" t="s">
         <v>45</v>
       </c>
-      <c r="F11" s="27" t="s">
+      <c r="F11" s="28" t="s">
         <v>27</v>
       </c>
-      <c r="G11" s="36" t="s">
+      <c r="G11" s="30" t="s">
         <v>28</v>
       </c>
       <c r="H11" s="3"/>
     </row>
-    <row r="12" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="B12" s="30"/>
-      <c r="C12" s="31"/>
-      <c r="D12" s="57"/>
-      <c r="E12" s="57"/>
-      <c r="F12" s="28"/>
-      <c r="G12" s="37"/>
-      <c r="H12" s="3"/>
-    </row>
-    <row r="13" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="27"/>
+      <c r="C12" s="26"/>
+      <c r="D12" s="58"/>
+      <c r="E12" s="58"/>
+      <c r="F12" s="29"/>
+      <c r="G12" s="31"/>
+      <c r="H12" s="45" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B13" s="31"/>
-      <c r="C13" s="36" t="s">
+      <c r="B13" s="26"/>
+      <c r="C13" s="30" t="s">
         <v>28</v>
       </c>
       <c r="D13" s="38" t="s">
         <v>31</v>
       </c>
-      <c r="E13" s="36" t="s">
+      <c r="E13" s="30" t="s">
         <v>28</v>
       </c>
       <c r="F13" s="8" t="s">
         <v>42</v>
       </c>
       <c r="G13" s="3"/>
-      <c r="H13" s="3"/>
-    </row>
-    <row r="14" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="H13" s="46"/>
+    </row>
+    <row r="14" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
         <v>32</v>
       </c>
       <c r="B14" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="C14" s="37"/>
+      <c r="C14" s="31"/>
       <c r="D14" s="39"/>
-      <c r="E14" s="37"/>
-      <c r="F14" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="G14" s="34" t="s">
+      <c r="E14" s="31"/>
+      <c r="F14" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="G14" s="59" t="s">
         <v>19</v>
       </c>
       <c r="H14" s="3"/>
     </row>
-    <row r="15" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="B15" s="12" t="s">
+      <c r="B15" s="11" t="s">
         <v>11</v>
       </c>
       <c r="C15" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="D15" s="12" t="s">
+      <c r="D15" s="11" t="s">
         <v>11</v>
       </c>
       <c r="E15" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="F15" s="25" t="s">
-        <v>18</v>
-      </c>
-      <c r="G15" s="35"/>
+      <c r="G15" s="61"/>
       <c r="H15" s="3"/>
     </row>
-    <row r="16" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="B16" s="3"/>
-      <c r="C16" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="E16" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="F16" s="26"/>
-      <c r="G16" s="51" t="s">
+      <c r="B16" s="45" t="s">
+        <v>33</v>
+      </c>
+      <c r="C16" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="D16" s="63" t="s">
+        <v>71</v>
+      </c>
+      <c r="E16" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="F16" s="32" t="s">
+        <v>18</v>
+      </c>
+      <c r="G16" s="43" t="s">
         <v>44</v>
       </c>
-      <c r="H16" s="36" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="H16" s="3"/>
+    </row>
+    <row r="17" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="B17" s="20" t="s">
-        <v>72</v>
-      </c>
-      <c r="C17" s="53" t="s">
+      <c r="B17" s="46"/>
+      <c r="C17" s="59" t="s">
         <v>19</v>
       </c>
-      <c r="D17" s="25" t="s">
+      <c r="D17" s="32" t="s">
         <v>18</v>
       </c>
-      <c r="E17" s="13" t="s">
-        <v>51</v>
-      </c>
-      <c r="F17" s="3"/>
-      <c r="G17" s="52"/>
-      <c r="H17" s="37"/>
-    </row>
-    <row r="18" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="E17" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="F17" s="33"/>
+      <c r="G17" s="44"/>
+      <c r="H17" s="30" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="B18" s="22" t="s">
-        <v>63</v>
-      </c>
-      <c r="C18" s="54"/>
-      <c r="D18" s="26"/>
+      <c r="B18" s="19" t="s">
+        <v>61</v>
+      </c>
+      <c r="C18" s="60"/>
+      <c r="D18" s="33"/>
       <c r="E18" s="3"/>
-      <c r="F18" s="3"/>
-      <c r="G18" s="3"/>
-      <c r="H18" s="3"/>
-    </row>
-    <row r="19" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="G18" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="H18" s="31"/>
+    </row>
+    <row r="19" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
         <v>38</v>
       </c>
       <c r="B19" s="3"/>
-      <c r="C19" s="55"/>
+      <c r="C19" s="61"/>
       <c r="D19" s="3"/>
       <c r="E19" s="3"/>
       <c r="F19" s="3"/>
@@ -2283,16 +2334,20 @@
       <c r="H19" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="28">
-    <mergeCell ref="G7:G9"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="E7:E8"/>
-    <mergeCell ref="F9:F10"/>
-    <mergeCell ref="H7:H8"/>
+  <mergeCells count="30">
+    <mergeCell ref="G11:G12"/>
     <mergeCell ref="C9:C10"/>
-    <mergeCell ref="D9:D10"/>
-    <mergeCell ref="E9:E10"/>
-    <mergeCell ref="H9:H10"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="H12:H13"/>
+    <mergeCell ref="H17:H18"/>
+    <mergeCell ref="F16:F17"/>
+    <mergeCell ref="C17:C19"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="D17:D18"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="E13:E14"/>
+    <mergeCell ref="G16:G17"/>
+    <mergeCell ref="G14:G15"/>
     <mergeCell ref="B11:B13"/>
     <mergeCell ref="E11:E12"/>
     <mergeCell ref="D11:D12"/>
@@ -2302,16 +2357,14 @@
     <mergeCell ref="F6:F8"/>
     <mergeCell ref="B7:B8"/>
     <mergeCell ref="C11:C12"/>
-    <mergeCell ref="C17:C19"/>
-    <mergeCell ref="D13:D14"/>
-    <mergeCell ref="H16:H17"/>
-    <mergeCell ref="F15:F16"/>
-    <mergeCell ref="D17:D18"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="E13:E14"/>
-    <mergeCell ref="G16:G17"/>
-    <mergeCell ref="G14:G15"/>
-    <mergeCell ref="G11:G12"/>
+    <mergeCell ref="G7:G9"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="E7:E8"/>
+    <mergeCell ref="F9:F10"/>
+    <mergeCell ref="H7:H8"/>
+    <mergeCell ref="E9:E10"/>
+    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="H9:H10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2320,25 +2373,19 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68112DEB-F6E4-415D-A916-ADDDEC95DDF2}">
-  <dimension ref="A1:H19"/>
+  <dimension ref="A1:H20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D14" activeCellId="9" sqref="C16 B15 B6 C4 D8 E4 F5 F14 E16 D14"/>
+    <sheetView topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.5703125" customWidth="1"/>
-    <col min="2" max="2" width="15.5703125" customWidth="1"/>
-    <col min="3" max="3" width="15.85546875" customWidth="1"/>
-    <col min="4" max="4" width="15.28515625" customWidth="1"/>
-    <col min="5" max="5" width="16.42578125" customWidth="1"/>
-    <col min="6" max="6" width="16" customWidth="1"/>
-    <col min="7" max="7" width="16.7109375" customWidth="1"/>
-    <col min="8" max="8" width="15.42578125" customWidth="1"/>
+    <col min="1" max="1" width="17.42578125" customWidth="1"/>
+    <col min="2" max="8" width="18.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>41</v>
       </c>
@@ -2364,7 +2411,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>7</v>
       </c>
@@ -2376,7 +2423,7 @@
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
     </row>
-    <row r="3" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>8</v>
       </c>
@@ -2388,327 +2435,345 @@
       <c r="G3" s="3"/>
       <c r="H3" s="3"/>
     </row>
-    <row r="4" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>9</v>
       </c>
       <c r="B4" s="3"/>
-      <c r="C4" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E4" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="F4" s="13" t="s">
-        <v>51</v>
+      <c r="C4" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="30" t="s">
+        <v>28</v>
+      </c>
+      <c r="E4" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" s="12" t="s">
+        <v>50</v>
       </c>
       <c r="G4" s="3"/>
       <c r="H4" s="3"/>
     </row>
-    <row r="5" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="13" t="s">
-        <v>51</v>
-      </c>
-      <c r="C5" s="29" t="s">
+      <c r="B5" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="C5" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="13" t="s">
-        <v>51</v>
-      </c>
-      <c r="E5" s="29" t="s">
+      <c r="D5" s="31"/>
+      <c r="E5" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="F5" s="12" t="s">
+      <c r="F5" s="11" t="s">
         <v>11</v>
       </c>
       <c r="G5" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="H5" s="4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="H5" s="30" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" s="31"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="31"/>
-      <c r="F6" s="29" t="s">
+      <c r="B6" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="26"/>
+      <c r="D6" s="59" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6" s="26"/>
+      <c r="F6" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="G6" s="13" t="s">
-        <v>51</v>
-      </c>
-      <c r="H6" s="13" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="G6" s="3"/>
+      <c r="H6" s="31"/>
+    </row>
+    <row r="7" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="27" t="s">
+      <c r="B7" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="51" t="s">
+      <c r="C7" s="43" t="s">
         <v>44</v>
       </c>
-      <c r="D7" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="E7" s="3"/>
-      <c r="F7" s="30"/>
-      <c r="G7" s="42" t="s">
+      <c r="D7" s="61"/>
+      <c r="E7" s="63" t="s">
+        <v>71</v>
+      </c>
+      <c r="F7" s="27"/>
+      <c r="G7" s="40" t="s">
         <v>18</v>
       </c>
-      <c r="H7" s="34" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="H7" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="28"/>
-      <c r="C8" s="52"/>
-      <c r="D8" s="12" t="s">
+      <c r="B8" s="29"/>
+      <c r="C8" s="44"/>
+      <c r="D8" s="11" t="s">
         <v>11</v>
       </c>
       <c r="E8" s="3"/>
-      <c r="F8" s="31"/>
-      <c r="G8" s="43"/>
-      <c r="H8" s="35"/>
-    </row>
-    <row r="9" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="F8" s="26"/>
+      <c r="G8" s="41"/>
+      <c r="H8" s="3"/>
+    </row>
+    <row r="9" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B9" s="36" t="s">
+      <c r="B9" s="62" t="s">
         <v>28</v>
       </c>
-      <c r="C9" s="27" t="s">
+      <c r="C9" s="28" t="s">
         <v>22</v>
       </c>
-      <c r="D9" s="27" t="s">
+      <c r="D9" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="E9" s="27" t="s">
+      <c r="E9" s="28" t="s">
         <v>22</v>
       </c>
-      <c r="F9" s="3"/>
-      <c r="G9" s="44"/>
-      <c r="H9" s="36" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="F9" s="64" t="s">
+        <v>73</v>
+      </c>
+      <c r="G9" s="42"/>
+      <c r="H9" s="70" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B10" s="37"/>
-      <c r="C10" s="28"/>
-      <c r="D10" s="28"/>
-      <c r="E10" s="28"/>
-      <c r="F10" s="3"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="29"/>
+      <c r="D10" s="29"/>
+      <c r="E10" s="29"/>
+      <c r="F10" s="72" t="s">
+        <v>78</v>
+      </c>
       <c r="G10" s="3"/>
-      <c r="H10" s="37"/>
-    </row>
-    <row r="11" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="H10" s="71"/>
+    </row>
+    <row r="11" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B11" s="29" t="s">
-        <v>25</v>
-      </c>
-      <c r="C11" s="27" t="s">
+      <c r="B11" s="25" t="s">
+        <v>75</v>
+      </c>
+      <c r="C11" s="28" t="s">
         <v>26</v>
       </c>
-      <c r="D11" s="27" t="s">
+      <c r="D11" s="28" t="s">
         <v>27</v>
       </c>
-      <c r="E11" s="27" t="s">
+      <c r="E11" s="28" t="s">
         <v>26</v>
       </c>
-      <c r="F11" s="27" t="s">
+      <c r="F11" s="28" t="s">
         <v>27</v>
       </c>
-      <c r="G11" s="36" t="s">
-        <v>28</v>
-      </c>
+      <c r="G11" s="3"/>
       <c r="H11" s="3"/>
     </row>
-    <row r="12" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="B12" s="30"/>
-      <c r="C12" s="28"/>
-      <c r="D12" s="28"/>
-      <c r="E12" s="28"/>
-      <c r="F12" s="28"/>
-      <c r="G12" s="37"/>
-      <c r="H12" s="3"/>
-    </row>
-    <row r="13" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="B12" s="27"/>
+      <c r="C12" s="29"/>
+      <c r="D12" s="29"/>
+      <c r="E12" s="29"/>
+      <c r="F12" s="29"/>
+      <c r="G12" s="3"/>
+      <c r="H12" s="40" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B13" s="31"/>
-      <c r="C13" s="61" t="s">
-        <v>50</v>
+      <c r="B13" s="26"/>
+      <c r="C13" s="63" t="s">
+        <v>71</v>
       </c>
       <c r="D13" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="E13" s="61" t="s">
-        <v>50</v>
+      <c r="E13" s="30" t="s">
+        <v>28</v>
       </c>
       <c r="F13" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="G13" s="3"/>
-      <c r="H13" s="3"/>
-    </row>
-    <row r="14" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G13" s="72" t="s">
+        <v>78</v>
+      </c>
+      <c r="H13" s="41"/>
+    </row>
+    <row r="14" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
         <v>32</v>
       </c>
       <c r="B14" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="C14" s="62"/>
-      <c r="D14" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="E14" s="62"/>
-      <c r="F14" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="G14" s="25" t="s">
-        <v>18</v>
+      <c r="C14" s="62" t="s">
+        <v>28</v>
+      </c>
+      <c r="D14" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="E14" s="31"/>
+      <c r="F14" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="G14" s="59" t="s">
+        <v>19</v>
       </c>
       <c r="H14" s="3"/>
     </row>
-    <row r="15" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="B15" s="12" t="s">
+      <c r="B15" s="11" t="s">
         <v>11</v>
       </c>
       <c r="C15" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="D15" s="25" t="s">
-        <v>18</v>
-      </c>
+      <c r="D15" s="3"/>
       <c r="E15" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="F15" s="34" t="s">
-        <v>19</v>
-      </c>
-      <c r="G15" s="26"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="61"/>
       <c r="H15" s="3"/>
     </row>
-    <row r="16" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="B16" s="3"/>
-      <c r="C16" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="D16" s="26"/>
-      <c r="E16" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="F16" s="35"/>
+      <c r="B16" s="64" t="s">
+        <v>73</v>
+      </c>
+      <c r="C16" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="D16" s="40" t="s">
+        <v>18</v>
+      </c>
+      <c r="E16" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="F16" s="40" t="s">
+        <v>18</v>
+      </c>
       <c r="G16" s="3"/>
-      <c r="H16" s="3"/>
-    </row>
-    <row r="17" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="H16" s="10" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="B17" s="3"/>
-      <c r="C17" s="13" t="s">
-        <v>51</v>
-      </c>
-      <c r="D17" s="34" t="s">
-        <v>19</v>
-      </c>
-      <c r="E17" s="13" t="s">
-        <v>51</v>
-      </c>
-      <c r="F17" s="3"/>
+      <c r="B17" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="C17" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="D17" s="41"/>
+      <c r="E17" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="F17" s="41"/>
       <c r="G17" s="3"/>
-      <c r="H17" s="25" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="H17" s="43" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="B18" s="3"/>
-      <c r="C18" s="3"/>
-      <c r="D18" s="35"/>
-      <c r="E18" s="3"/>
+      <c r="B18" s="65" t="s">
+        <v>72</v>
+      </c>
+      <c r="C18" s="40" t="s">
+        <v>18</v>
+      </c>
+      <c r="D18" s="64" t="s">
+        <v>73</v>
+      </c>
+      <c r="E18" s="59" t="s">
+        <v>19</v>
+      </c>
       <c r="F18" s="3"/>
       <c r="G18" s="3"/>
-      <c r="H18" s="26"/>
-    </row>
-    <row r="19" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="H18" s="44"/>
+    </row>
+    <row r="19" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
         <v>38</v>
       </c>
       <c r="B19" s="3"/>
-      <c r="C19" s="3"/>
+      <c r="C19" s="42"/>
       <c r="D19" s="3"/>
-      <c r="E19" s="3"/>
+      <c r="E19" s="61"/>
       <c r="F19" s="3"/>
       <c r="G19" s="3"/>
       <c r="H19" s="3"/>
     </row>
+    <row r="20" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <mergeCells count="25">
-    <mergeCell ref="H7:H8"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="D9:D10"/>
-    <mergeCell ref="E9:E10"/>
-    <mergeCell ref="G11:G12"/>
-    <mergeCell ref="H9:H10"/>
+  <mergeCells count="26">
+    <mergeCell ref="E18:E19"/>
+    <mergeCell ref="H5:H6"/>
+    <mergeCell ref="H12:H13"/>
+    <mergeCell ref="H17:H18"/>
+    <mergeCell ref="D16:D17"/>
+    <mergeCell ref="F16:F17"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="B11:B13"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="E11:E12"/>
+    <mergeCell ref="F11:F12"/>
+    <mergeCell ref="G14:G15"/>
+    <mergeCell ref="E13:E14"/>
+    <mergeCell ref="C18:C19"/>
     <mergeCell ref="C5:C6"/>
     <mergeCell ref="E5:E6"/>
     <mergeCell ref="F6:F8"/>
     <mergeCell ref="B7:B8"/>
     <mergeCell ref="G7:G9"/>
-    <mergeCell ref="B9:B10"/>
     <mergeCell ref="C7:C8"/>
-    <mergeCell ref="H17:H18"/>
-    <mergeCell ref="B11:B13"/>
-    <mergeCell ref="C11:C12"/>
-    <mergeCell ref="D11:D12"/>
-    <mergeCell ref="E11:E12"/>
-    <mergeCell ref="F11:F12"/>
-    <mergeCell ref="D17:D18"/>
-    <mergeCell ref="G14:G15"/>
-    <mergeCell ref="D15:D16"/>
-    <mergeCell ref="F15:F16"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="E13:E14"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="E9:E10"/>
+    <mergeCell ref="H9:H10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>

</xml_diff>

<commit_message>
Modificacion fds semana 2. Actualizacion eventos lunes y martes
</commit_message>
<xml_diff>
--- a/Programar_dias.xlsx
+++ b/Programar_dias.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Estudio\OneDrive - Universidad de Antioquia\Estudio\Materias\Informatica II\Calendario_semanal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1438537A-D84A-4FA5-8008-6D52DC7AA0E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECEA7DC2-E3BC-44C6-9B15-7EF2C89BC86C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{CC961CB2-F623-4B13-8239-4B70F16E4462}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="2" xr2:uid="{CC961CB2-F623-4B13-8239-4B70F16E4462}"/>
   </bookViews>
   <sheets>
     <sheet name="Semana 1" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="341" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="78">
   <si>
     <t>LUNES</t>
   </si>
@@ -267,12 +267,6 @@
     <t>CIRCUITOS II</t>
   </si>
   <si>
-    <t>Mercado</t>
-  </si>
-  <si>
-    <t>Estudiar Especiales (1:30)</t>
-  </si>
-  <si>
     <t>Kaggle</t>
   </si>
   <si>
@@ -300,9 +294,6 @@
     <t>Leer</t>
   </si>
   <si>
-    <t>Asesoría Esp.</t>
-  </si>
-  <si>
     <t>Informe Lab.</t>
   </si>
   <si>
@@ -318,20 +309,26 @@
     <t>LAB INFORMÁTICA</t>
   </si>
   <si>
-    <t>Est. Especiales</t>
-  </si>
-  <si>
     <t>Repaso Metodos</t>
   </si>
   <si>
     <t>Est. Física.</t>
+  </si>
+  <si>
+    <t>Est. Fisca</t>
+  </si>
+  <si>
+    <t>Estu. Especiales</t>
+  </si>
+  <si>
+    <t>Act. Semillero</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -403,8 +400,15 @@
       <name val="Yu Gothic UI"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Yu Gothic UI"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="21">
+  <fills count="22">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -521,12 +525,18 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.59999389629810485"/>
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -586,11 +596,24 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="73">
+  <cellXfs count="77">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -654,64 +677,85 @@
     <xf numFmtId="0" fontId="2" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="17" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -720,12 +764,6 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -738,6 +776,18 @@
     <xf numFmtId="0" fontId="4" fillId="14" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -756,53 +806,38 @@
     <xf numFmtId="0" fontId="2" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="17" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="19" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="20" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="18" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="18" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="20" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="21" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1217,13 +1252,13 @@
       <c r="B5" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="25" t="s">
+      <c r="C5" s="32" t="s">
         <v>13</v>
       </c>
       <c r="D5" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="E5" s="25" t="s">
+      <c r="E5" s="32" t="s">
         <v>13</v>
       </c>
       <c r="F5" s="11" t="s">
@@ -1239,12 +1274,12 @@
       <c r="B6" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="26"/>
+      <c r="C6" s="34"/>
       <c r="D6" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="E6" s="26"/>
-      <c r="F6" s="25" t="s">
+      <c r="E6" s="34"/>
+      <c r="F6" s="32" t="s">
         <v>15</v>
       </c>
       <c r="G6" s="3"/>
@@ -1254,17 +1289,17 @@
       <c r="A7" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="28" t="s">
+      <c r="B7" s="30" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="30" t="s">
+      <c r="C7" s="39" t="s">
         <v>28</v>
       </c>
       <c r="D7" s="3"/>
-      <c r="E7" s="23" t="s">
+      <c r="E7" s="46" t="s">
         <v>47</v>
       </c>
-      <c r="F7" s="27"/>
+      <c r="F7" s="33"/>
       <c r="G7" s="3"/>
       <c r="H7" s="4" t="s">
         <v>10</v>
@@ -1274,15 +1309,15 @@
       <c r="A8" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="29"/>
-      <c r="C8" s="31"/>
+      <c r="B8" s="31"/>
+      <c r="C8" s="40"/>
       <c r="D8" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="E8" s="24"/>
-      <c r="F8" s="26"/>
+      <c r="E8" s="47"/>
+      <c r="F8" s="34"/>
       <c r="G8" s="3"/>
-      <c r="H8" s="32" t="s">
+      <c r="H8" s="28" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1293,30 +1328,30 @@
       <c r="B9" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="C9" s="28" t="s">
+      <c r="C9" s="30" t="s">
         <v>22</v>
       </c>
-      <c r="D9" s="28" t="s">
+      <c r="D9" s="30" t="s">
         <v>17</v>
       </c>
-      <c r="E9" s="28" t="s">
+      <c r="E9" s="30" t="s">
         <v>22</v>
       </c>
-      <c r="F9" s="30" t="s">
+      <c r="F9" s="39" t="s">
         <v>28</v>
       </c>
       <c r="G9" s="3"/>
-      <c r="H9" s="33"/>
+      <c r="H9" s="29"/>
     </row>
     <row r="10" spans="1:10" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>23</v>
       </c>
       <c r="B10" s="13"/>
-      <c r="C10" s="29"/>
-      <c r="D10" s="29"/>
-      <c r="E10" s="29"/>
-      <c r="F10" s="31"/>
+      <c r="C10" s="31"/>
+      <c r="D10" s="31"/>
+      <c r="E10" s="31"/>
+      <c r="F10" s="40"/>
       <c r="G10" s="3"/>
       <c r="H10" s="3"/>
     </row>
@@ -1324,23 +1359,23 @@
       <c r="A11" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B11" s="25" t="s">
+      <c r="B11" s="32" t="s">
         <v>25</v>
       </c>
-      <c r="C11" s="28" t="s">
+      <c r="C11" s="30" t="s">
         <v>26</v>
       </c>
-      <c r="D11" s="28" t="s">
+      <c r="D11" s="30" t="s">
         <v>27</v>
       </c>
       <c r="E11" s="3"/>
-      <c r="F11" s="28" t="s">
+      <c r="F11" s="30" t="s">
         <v>56</v>
       </c>
-      <c r="G11" s="23" t="s">
+      <c r="G11" s="46" t="s">
         <v>47</v>
       </c>
-      <c r="H11" s="32" t="s">
+      <c r="H11" s="28" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1348,22 +1383,22 @@
       <c r="A12" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="B12" s="27"/>
-      <c r="C12" s="29"/>
-      <c r="D12" s="29"/>
-      <c r="F12" s="29"/>
-      <c r="G12" s="24"/>
-      <c r="H12" s="33"/>
+      <c r="B12" s="33"/>
+      <c r="C12" s="31"/>
+      <c r="D12" s="31"/>
+      <c r="F12" s="31"/>
+      <c r="G12" s="47"/>
+      <c r="H12" s="29"/>
     </row>
     <row r="13" spans="1:10" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B13" s="26"/>
+      <c r="B13" s="34"/>
       <c r="C13" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="D13" s="38" t="s">
+      <c r="D13" s="41" t="s">
         <v>31</v>
       </c>
       <c r="E13" s="11" t="s">
@@ -1384,10 +1419,10 @@
         <v>11</v>
       </c>
       <c r="C14" s="3"/>
-      <c r="D14" s="39"/>
+      <c r="D14" s="42"/>
       <c r="E14" s="3"/>
       <c r="F14" s="3"/>
-      <c r="G14" s="34" t="s">
+      <c r="G14" s="35" t="s">
         <v>44</v>
       </c>
       <c r="H14" s="3" t="s">
@@ -1400,7 +1435,7 @@
         <v>34</v>
       </c>
       <c r="B15" s="3"/>
-      <c r="C15" s="34" t="s">
+      <c r="C15" s="35" t="s">
         <v>44</v>
       </c>
       <c r="D15" s="14" t="s">
@@ -1408,7 +1443,7 @@
       </c>
       <c r="E15" s="3"/>
       <c r="F15" s="3"/>
-      <c r="G15" s="35"/>
+      <c r="G15" s="36"/>
       <c r="H15" s="11" t="s">
         <v>11</v>
       </c>
@@ -1418,18 +1453,18 @@
         <v>35</v>
       </c>
       <c r="B16" s="3"/>
-      <c r="C16" s="35"/>
+      <c r="C16" s="36"/>
       <c r="D16" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="E16" s="30" t="s">
+      <c r="E16" s="39" t="s">
         <v>28</v>
       </c>
       <c r="F16" s="3"/>
-      <c r="G16" s="40" t="s">
+      <c r="G16" s="43" t="s">
         <v>18</v>
       </c>
-      <c r="H16" s="30" t="s">
+      <c r="H16" s="39" t="s">
         <v>28</v>
       </c>
     </row>
@@ -1442,32 +1477,32 @@
       </c>
       <c r="C17" s="3"/>
       <c r="D17" s="3"/>
-      <c r="E17" s="31"/>
+      <c r="E17" s="40"/>
       <c r="F17" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="G17" s="41"/>
-      <c r="H17" s="31"/>
+      <c r="G17" s="44"/>
+      <c r="H17" s="40"/>
     </row>
     <row r="18" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="B18" s="32" t="s">
+      <c r="B18" s="28" t="s">
         <v>18</v>
       </c>
-      <c r="C18" s="34" t="s">
+      <c r="C18" s="35" t="s">
         <v>44</v>
       </c>
-      <c r="D18" s="36" t="s">
+      <c r="D18" s="37" t="s">
         <v>19</v>
       </c>
-      <c r="E18" s="32" t="s">
+      <c r="E18" s="28" t="s">
         <v>18</v>
       </c>
       <c r="F18" s="3"/>
-      <c r="G18" s="42"/>
-      <c r="H18" s="32" t="s">
+      <c r="G18" s="45"/>
+      <c r="H18" s="28" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1475,16 +1510,28 @@
       <c r="A19" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="B19" s="33"/>
-      <c r="C19" s="35"/>
-      <c r="D19" s="37"/>
-      <c r="E19" s="33"/>
+      <c r="B19" s="29"/>
+      <c r="C19" s="36"/>
+      <c r="D19" s="38"/>
+      <c r="E19" s="29"/>
       <c r="F19" s="3"/>
       <c r="G19" s="3"/>
-      <c r="H19" s="33"/>
+      <c r="H19" s="29"/>
     </row>
   </sheetData>
   <mergeCells count="28">
+    <mergeCell ref="G11:G12"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="F6:F8"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="E9:E10"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="F9:F10"/>
+    <mergeCell ref="E7:E8"/>
     <mergeCell ref="H8:H9"/>
     <mergeCell ref="H11:H12"/>
     <mergeCell ref="B18:B19"/>
@@ -1501,18 +1548,6 @@
     <mergeCell ref="H16:H17"/>
     <mergeCell ref="G14:G15"/>
     <mergeCell ref="G16:G18"/>
-    <mergeCell ref="G11:G12"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="E5:E6"/>
-    <mergeCell ref="F6:F8"/>
-    <mergeCell ref="C11:C12"/>
-    <mergeCell ref="D11:D12"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="D9:D10"/>
-    <mergeCell ref="E9:E10"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="F9:F10"/>
-    <mergeCell ref="E7:E8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1523,8 +1558,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF8929EB-A174-48F2-BDBD-469036EC404B}">
   <dimension ref="A1:J19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7:G9"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11:D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1567,11 +1602,11 @@
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
+      <c r="F2" s="68"/>
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
       <c r="J2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -1583,14 +1618,10 @@
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
-      <c r="G3" s="14" t="s">
-        <v>55</v>
-      </c>
-      <c r="H3" s="32" t="s">
-        <v>18</v>
-      </c>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
       <c r="J3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -1603,7 +1634,7 @@
       <c r="C4" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="47" t="s">
+      <c r="D4" s="52" t="s">
         <v>44</v>
       </c>
       <c r="E4" s="11" t="s">
@@ -1613,214 +1644,200 @@
         <v>50</v>
       </c>
       <c r="G4" s="3"/>
-      <c r="H4" s="33"/>
+      <c r="H4" s="3"/>
       <c r="J4" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="32" t="s">
+      <c r="B5" s="28" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="25" t="s">
+      <c r="C5" s="32" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="48"/>
-      <c r="E5" s="25" t="s">
+      <c r="D5" s="53"/>
+      <c r="E5" s="32" t="s">
         <v>13</v>
       </c>
       <c r="F5" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="G5" s="4" t="s">
-        <v>10</v>
+      <c r="G5" s="43" t="s">
+        <v>18</v>
       </c>
       <c r="H5" s="4" t="s">
         <v>10</v>
       </c>
       <c r="J5" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="33"/>
-      <c r="C6" s="26"/>
-      <c r="D6" s="45" t="s">
+      <c r="B6" s="29"/>
+      <c r="C6" s="34"/>
+      <c r="D6" s="48" t="s">
         <v>33</v>
       </c>
-      <c r="E6" s="26"/>
-      <c r="F6" s="25" t="s">
+      <c r="E6" s="34"/>
+      <c r="F6" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="G6" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="H6" s="12" t="s">
-        <v>50</v>
-      </c>
+      <c r="G6" s="44"/>
+      <c r="H6" s="3"/>
       <c r="J6" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="28" t="s">
+      <c r="B7" s="30" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="45" t="s">
+      <c r="C7" s="48" t="s">
         <v>33</v>
       </c>
-      <c r="D7" s="46"/>
+      <c r="D7" s="49"/>
       <c r="E7" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="F7" s="27"/>
-      <c r="G7" s="40" t="s">
-        <v>18</v>
-      </c>
-      <c r="H7" s="36" t="s">
-        <v>19</v>
-      </c>
+      <c r="F7" s="33"/>
+      <c r="G7" s="44"/>
+      <c r="H7" s="3"/>
       <c r="J7" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="29"/>
-      <c r="C8" s="46"/>
-      <c r="D8" s="30" t="s">
+      <c r="B8" s="31"/>
+      <c r="C8" s="49"/>
+      <c r="D8" s="39" t="s">
         <v>28</v>
       </c>
       <c r="E8" s="22" t="s">
         <v>54</v>
       </c>
-      <c r="F8" s="26"/>
-      <c r="G8" s="41"/>
-      <c r="H8" s="37"/>
+      <c r="F8" s="34"/>
+      <c r="G8" s="44"/>
+      <c r="H8" s="48" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="9" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B9" s="23" t="s">
+      <c r="B9" s="46" t="s">
         <v>47</v>
       </c>
-      <c r="C9" s="25" t="s">
+      <c r="C9" s="32" t="s">
         <v>51</v>
       </c>
-      <c r="D9" s="31"/>
-      <c r="E9" s="25" t="s">
+      <c r="D9" s="40"/>
+      <c r="E9" s="32" t="s">
         <v>51</v>
       </c>
       <c r="F9" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="G9" s="42"/>
-      <c r="H9" s="43" t="s">
-        <v>44</v>
-      </c>
+      <c r="G9" s="44"/>
+      <c r="H9" s="71"/>
     </row>
     <row r="10" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B10" s="24"/>
-      <c r="C10" s="26"/>
+      <c r="B10" s="47"/>
+      <c r="C10" s="34"/>
       <c r="D10" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="E10" s="26"/>
+      <c r="E10" s="34"/>
       <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
-      <c r="H10" s="44"/>
+      <c r="G10" s="45"/>
+      <c r="H10" s="49"/>
     </row>
     <row r="11" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B11" s="25" t="s">
+      <c r="B11" s="32" t="s">
         <v>25</v>
       </c>
-      <c r="C11" s="25" t="s">
+      <c r="C11" s="32" t="s">
         <v>58</v>
       </c>
-      <c r="D11" s="25" t="s">
+      <c r="D11" s="32" t="s">
         <v>56</v>
       </c>
-      <c r="E11" s="25" t="s">
+      <c r="E11" s="32" t="s">
         <v>58</v>
       </c>
-      <c r="F11" s="49" t="s">
+      <c r="F11" s="54" t="s">
         <v>43</v>
       </c>
-      <c r="G11" s="30" t="s">
-        <v>28</v>
-      </c>
+      <c r="G11" s="3"/>
       <c r="H11" s="3"/>
     </row>
     <row r="12" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="B12" s="27"/>
-      <c r="C12" s="26"/>
-      <c r="D12" s="26"/>
-      <c r="E12" s="26"/>
-      <c r="F12" s="50"/>
-      <c r="G12" s="31"/>
-      <c r="H12" s="3"/>
+      <c r="B12" s="33"/>
+      <c r="C12" s="34"/>
+      <c r="D12" s="34"/>
+      <c r="E12" s="34"/>
+      <c r="F12" s="55"/>
+      <c r="G12" s="3"/>
+      <c r="H12" s="48" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="13" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B13" s="26"/>
+      <c r="B13" s="34"/>
       <c r="C13" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="D13" s="38" t="s">
+      <c r="D13" s="41" t="s">
         <v>31</v>
       </c>
-      <c r="E13" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="F13" s="8" t="s">
+      <c r="E13" s="69" t="s">
+        <v>11</v>
+      </c>
+      <c r="F13" s="70" t="s">
         <v>42</v>
       </c>
-      <c r="G13" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="H13" s="40" t="s">
-        <v>18</v>
-      </c>
+      <c r="G13" s="3"/>
+      <c r="H13" s="49"/>
     </row>
     <row r="14" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
         <v>32</v>
       </c>
       <c r="B14" s="3"/>
-      <c r="C14" s="30" t="s">
+      <c r="C14" s="39" t="s">
         <v>28</v>
       </c>
-      <c r="D14" s="39"/>
-      <c r="F14" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="G14" s="63" t="s">
-        <v>71</v>
-      </c>
-      <c r="H14" s="41"/>
+      <c r="D14" s="42"/>
+      <c r="F14" s="70"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="43" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="15" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
@@ -1829,54 +1846,52 @@
       <c r="B15" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="C15" s="31"/>
+      <c r="C15" s="40"/>
       <c r="D15" s="3"/>
-      <c r="E15" s="30" t="s">
+      <c r="E15" s="39" t="s">
         <v>28</v>
       </c>
-      <c r="F15" s="45" t="s">
-        <v>60</v>
-      </c>
-      <c r="G15" s="45" t="s">
-        <v>33</v>
-      </c>
-      <c r="H15" s="42"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3"/>
+      <c r="H15" s="45"/>
     </row>
     <row r="16" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="B16" s="47" t="s">
+      <c r="B16" s="52" t="s">
         <v>44</v>
       </c>
-      <c r="C16" s="47" t="s">
+      <c r="C16" s="52" t="s">
         <v>44</v>
       </c>
       <c r="D16" s="3"/>
-      <c r="E16" s="31"/>
-      <c r="F16" s="46"/>
-      <c r="G16" s="46"/>
-      <c r="H16" s="67" t="s">
-        <v>28</v>
-      </c>
+      <c r="E16" s="40"/>
+      <c r="F16" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="G16" s="3"/>
+      <c r="H16" s="3"/>
     </row>
     <row r="17" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="B17" s="48"/>
-      <c r="C17" s="48"/>
+      <c r="B17" s="53"/>
+      <c r="C17" s="53"/>
       <c r="D17" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="E17" s="30" t="s">
+      <c r="E17" s="39" t="s">
         <v>28</v>
       </c>
       <c r="F17" s="17" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="G17" s="3"/>
-      <c r="H17" s="68"/>
+      <c r="H17" s="43" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="18" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
@@ -1885,64 +1900,44 @@
       <c r="B18" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="C18" s="45" t="s">
+      <c r="C18" s="48" t="s">
         <v>33</v>
       </c>
-      <c r="D18" s="45" t="s">
+      <c r="D18" s="48" t="s">
         <v>33</v>
       </c>
-      <c r="E18" s="31"/>
-      <c r="F18" s="40" t="s">
+      <c r="E18" s="40"/>
+      <c r="F18" s="43" t="s">
         <v>18</v>
       </c>
-      <c r="G18" s="17" t="s">
-        <v>61</v>
-      </c>
-      <c r="H18" s="69"/>
+      <c r="G18" s="3"/>
+      <c r="H18" s="44"/>
     </row>
     <row r="19" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
         <v>38</v>
       </c>
       <c r="B19" s="3"/>
-      <c r="C19" s="46"/>
-      <c r="D19" s="46"/>
+      <c r="C19" s="49"/>
+      <c r="D19" s="49"/>
       <c r="E19" s="14" t="s">
         <v>55</v>
       </c>
-      <c r="F19" s="42"/>
-      <c r="G19" s="14" t="s">
-        <v>55</v>
-      </c>
-      <c r="H19" s="66" t="s">
-        <v>76</v>
-      </c>
+      <c r="F19" s="45"/>
+      <c r="G19" s="3"/>
+      <c r="H19" s="45"/>
     </row>
   </sheetData>
-  <mergeCells count="35">
-    <mergeCell ref="H7:H8"/>
-    <mergeCell ref="E15:E16"/>
-    <mergeCell ref="E17:E18"/>
-    <mergeCell ref="H16:H18"/>
-    <mergeCell ref="F18:F19"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="C16:C17"/>
-    <mergeCell ref="G15:G16"/>
-    <mergeCell ref="F15:F16"/>
-    <mergeCell ref="C18:C19"/>
-    <mergeCell ref="D13:D14"/>
-    <mergeCell ref="D18:D19"/>
-    <mergeCell ref="H13:H15"/>
-    <mergeCell ref="B16:B17"/>
-    <mergeCell ref="B11:B13"/>
-    <mergeCell ref="E11:E12"/>
-    <mergeCell ref="D11:D12"/>
-    <mergeCell ref="F11:F12"/>
-    <mergeCell ref="C11:C12"/>
-    <mergeCell ref="G11:G12"/>
-    <mergeCell ref="H9:H10"/>
+  <mergeCells count="32">
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="F6:F8"/>
+    <mergeCell ref="F13:F14"/>
+    <mergeCell ref="G5:G10"/>
+    <mergeCell ref="H8:H10"/>
+    <mergeCell ref="H12:H13"/>
+    <mergeCell ref="H14:H15"/>
     <mergeCell ref="B7:B8"/>
-    <mergeCell ref="G7:G9"/>
     <mergeCell ref="C7:C8"/>
     <mergeCell ref="D6:D7"/>
     <mergeCell ref="B5:B6"/>
@@ -1951,10 +1946,21 @@
     <mergeCell ref="D8:D9"/>
     <mergeCell ref="C9:C10"/>
     <mergeCell ref="E9:E10"/>
-    <mergeCell ref="H3:H4"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="E5:E6"/>
-    <mergeCell ref="F6:F8"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="B11:B13"/>
+    <mergeCell ref="E11:E12"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="F11:F12"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="C16:C17"/>
+    <mergeCell ref="C18:C19"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="D18:D19"/>
+    <mergeCell ref="E15:E16"/>
+    <mergeCell ref="E17:E18"/>
+    <mergeCell ref="F18:F19"/>
+    <mergeCell ref="H17:H19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1965,8 +1971,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B17F021-0D0A-4F72-92FE-4A0D3181A797}">
   <dimension ref="A1:H19"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11:G12"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2028,14 +2034,12 @@
       <c r="A4" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="4" t="s">
-        <v>10</v>
-      </c>
+      <c r="B4" s="3"/>
       <c r="C4" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="4" t="s">
-        <v>10</v>
+      <c r="D4" s="19" t="s">
+        <v>76</v>
       </c>
       <c r="E4" s="11" t="s">
         <v>11</v>
@@ -2051,15 +2055,15 @@
         <v>12</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>63</v>
-      </c>
-      <c r="C5" s="25" t="s">
+        <v>61</v>
+      </c>
+      <c r="C5" s="32" t="s">
         <v>13</v>
       </c>
       <c r="D5" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="E5" s="25" t="s">
+      <c r="E5" s="32" t="s">
         <v>13</v>
       </c>
       <c r="F5" s="11" t="s">
@@ -2079,12 +2083,12 @@
       <c r="B6" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="26"/>
+      <c r="C6" s="34"/>
       <c r="D6" s="19" t="s">
-        <v>61</v>
-      </c>
-      <c r="E6" s="26"/>
-      <c r="F6" s="25" t="s">
+        <v>59</v>
+      </c>
+      <c r="E6" s="34"/>
+      <c r="F6" s="32" t="s">
         <v>15</v>
       </c>
       <c r="H6" s="12" t="s">
@@ -2095,23 +2099,21 @@
       <c r="A7" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="49" t="s">
-        <v>62</v>
-      </c>
-      <c r="C7" s="43" t="s">
-        <v>44</v>
-      </c>
-      <c r="D7" s="63" t="s">
-        <v>71</v>
-      </c>
-      <c r="E7" s="54" t="s">
+      <c r="B7" s="54" t="s">
+        <v>60</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="D7" s="3"/>
+      <c r="E7" s="63" t="s">
         <v>49</v>
       </c>
-      <c r="F7" s="27"/>
-      <c r="G7" s="51" t="s">
+      <c r="F7" s="33"/>
+      <c r="G7" s="60" t="s">
         <v>18</v>
       </c>
-      <c r="H7" s="59" t="s">
+      <c r="H7" s="56" t="s">
         <v>19</v>
       </c>
     </row>
@@ -2119,37 +2121,35 @@
       <c r="A8" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="50"/>
-      <c r="C8" s="44"/>
+      <c r="B8" s="55"/>
+      <c r="C8" s="3"/>
       <c r="D8" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="E8" s="55"/>
-      <c r="F8" s="26"/>
-      <c r="G8" s="52"/>
-      <c r="H8" s="61"/>
+      <c r="E8" s="64"/>
+      <c r="F8" s="34"/>
+      <c r="G8" s="61"/>
+      <c r="H8" s="57"/>
     </row>
     <row r="9" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B9" s="20" t="s">
-        <v>28</v>
-      </c>
-      <c r="C9" s="25" t="s">
+      <c r="B9" s="3"/>
+      <c r="C9" s="32" t="s">
         <v>51</v>
       </c>
-      <c r="D9" s="28" t="s">
+      <c r="D9" s="30" t="s">
         <v>17</v>
       </c>
-      <c r="E9" s="57" t="s">
+      <c r="E9" s="58" t="s">
         <v>46</v>
       </c>
-      <c r="F9" s="56" t="s">
+      <c r="F9" s="65" t="s">
         <v>52</v>
       </c>
-      <c r="G9" s="53"/>
-      <c r="H9" s="43" t="s">
+      <c r="G9" s="62"/>
+      <c r="H9" s="50" t="s">
         <v>44</v>
       </c>
     </row>
@@ -2157,36 +2157,36 @@
       <c r="A10" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B10" s="18" t="s">
-        <v>70</v>
-      </c>
-      <c r="C10" s="26"/>
-      <c r="D10" s="29"/>
-      <c r="E10" s="58"/>
-      <c r="F10" s="24"/>
+      <c r="B10" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10" s="34"/>
+      <c r="D10" s="31"/>
+      <c r="E10" s="59"/>
+      <c r="F10" s="47"/>
       <c r="G10" s="3"/>
-      <c r="H10" s="44"/>
+      <c r="H10" s="51"/>
     </row>
     <row r="11" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B11" s="25" t="s">
+      <c r="B11" s="32" t="s">
         <v>25</v>
       </c>
-      <c r="C11" s="25" t="s">
+      <c r="C11" s="32" t="s">
         <v>58</v>
       </c>
-      <c r="D11" s="57" t="s">
+      <c r="D11" s="32" t="s">
+        <v>56</v>
+      </c>
+      <c r="E11" s="58" t="s">
+        <v>45</v>
+      </c>
+      <c r="F11" s="58" t="s">
         <v>57</v>
       </c>
-      <c r="E11" s="57" t="s">
-        <v>45</v>
-      </c>
-      <c r="F11" s="28" t="s">
-        <v>27</v>
-      </c>
-      <c r="G11" s="30" t="s">
+      <c r="G11" s="39" t="s">
         <v>28</v>
       </c>
       <c r="H11" s="3"/>
@@ -2195,13 +2195,13 @@
       <c r="A12" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="B12" s="27"/>
-      <c r="C12" s="26"/>
-      <c r="D12" s="58"/>
-      <c r="E12" s="58"/>
-      <c r="F12" s="29"/>
-      <c r="G12" s="31"/>
-      <c r="H12" s="45" t="s">
+      <c r="B12" s="33"/>
+      <c r="C12" s="34"/>
+      <c r="D12" s="34"/>
+      <c r="E12" s="59"/>
+      <c r="F12" s="59"/>
+      <c r="G12" s="40"/>
+      <c r="H12" s="48" t="s">
         <v>33</v>
       </c>
     </row>
@@ -2209,36 +2209,36 @@
       <c r="A13" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B13" s="26"/>
-      <c r="C13" s="30" t="s">
+      <c r="B13" s="34"/>
+      <c r="C13" s="39" t="s">
         <v>28</v>
       </c>
-      <c r="D13" s="38" t="s">
+      <c r="D13" s="41" t="s">
         <v>31</v>
       </c>
-      <c r="E13" s="30" t="s">
+      <c r="E13" s="39" t="s">
         <v>28</v>
       </c>
       <c r="F13" s="8" t="s">
         <v>42</v>
       </c>
       <c r="G13" s="3"/>
-      <c r="H13" s="46"/>
+      <c r="H13" s="49"/>
     </row>
     <row r="14" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B14" s="8" t="s">
+      <c r="B14" s="72" t="s">
         <v>42</v>
       </c>
-      <c r="C14" s="31"/>
-      <c r="D14" s="39"/>
-      <c r="E14" s="31"/>
+      <c r="C14" s="40"/>
+      <c r="D14" s="42"/>
+      <c r="E14" s="40"/>
       <c r="F14" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="G14" s="59" t="s">
+      <c r="G14" s="56" t="s">
         <v>19</v>
       </c>
       <c r="H14" s="3"/>
@@ -2247,9 +2247,7 @@
       <c r="A15" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="B15" s="11" t="s">
-        <v>11</v>
-      </c>
+      <c r="B15" s="73"/>
       <c r="C15" s="9" t="s">
         <v>48</v>
       </c>
@@ -2259,29 +2257,27 @@
       <c r="E15" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="G15" s="61"/>
+      <c r="G15" s="57"/>
       <c r="H15" s="3"/>
     </row>
     <row r="16" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="B16" s="45" t="s">
-        <v>33</v>
+      <c r="B16" s="11" t="s">
+        <v>11</v>
       </c>
       <c r="C16" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="D16" s="63" t="s">
-        <v>71</v>
-      </c>
+      <c r="D16" s="3"/>
       <c r="E16" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="F16" s="32" t="s">
+      <c r="F16" s="28" t="s">
         <v>18</v>
       </c>
-      <c r="G16" s="43" t="s">
+      <c r="G16" s="50" t="s">
         <v>44</v>
       </c>
       <c r="H16" s="3"/>
@@ -2290,19 +2286,21 @@
       <c r="A17" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="B17" s="46"/>
-      <c r="C17" s="59" t="s">
+      <c r="B17" s="75" t="s">
         <v>19</v>
       </c>
-      <c r="D17" s="32" t="s">
+      <c r="C17" s="76" t="s">
+        <v>19</v>
+      </c>
+      <c r="D17" s="28" t="s">
         <v>18</v>
       </c>
       <c r="E17" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="F17" s="33"/>
-      <c r="G17" s="44"/>
-      <c r="H17" s="30" t="s">
+      <c r="F17" s="29"/>
+      <c r="G17" s="51"/>
+      <c r="H17" s="39" t="s">
         <v>28</v>
       </c>
     </row>
@@ -2311,22 +2309,28 @@
         <v>37</v>
       </c>
       <c r="B18" s="19" t="s">
-        <v>61</v>
-      </c>
-      <c r="C18" s="60"/>
-      <c r="D18" s="33"/>
+        <v>76</v>
+      </c>
+      <c r="C18" s="19" t="s">
+        <v>76</v>
+      </c>
+      <c r="D18" s="29"/>
       <c r="E18" s="3"/>
       <c r="G18" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="H18" s="31"/>
+      <c r="H18" s="40"/>
     </row>
     <row r="19" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="B19" s="3"/>
-      <c r="C19" s="61"/>
+      <c r="B19" s="74" t="s">
+        <v>75</v>
+      </c>
+      <c r="C19" s="18" t="s">
+        <v>77</v>
+      </c>
       <c r="D19" s="3"/>
       <c r="E19" s="3"/>
       <c r="F19" s="3"/>
@@ -2334,14 +2338,26 @@
       <c r="H19" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="30">
+  <mergeCells count="28">
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="G7:G9"/>
+    <mergeCell ref="E7:E8"/>
+    <mergeCell ref="F9:F10"/>
+    <mergeCell ref="H7:H8"/>
+    <mergeCell ref="E9:E10"/>
+    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="H9:H10"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="F6:F8"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="C11:C12"/>
     <mergeCell ref="G11:G12"/>
     <mergeCell ref="C9:C10"/>
-    <mergeCell ref="B16:B17"/>
     <mergeCell ref="H12:H13"/>
     <mergeCell ref="H17:H18"/>
     <mergeCell ref="F16:F17"/>
-    <mergeCell ref="C17:C19"/>
     <mergeCell ref="D13:D14"/>
     <mergeCell ref="D17:D18"/>
     <mergeCell ref="C13:C14"/>
@@ -2350,21 +2366,7 @@
     <mergeCell ref="G14:G15"/>
     <mergeCell ref="B11:B13"/>
     <mergeCell ref="E11:E12"/>
-    <mergeCell ref="D11:D12"/>
     <mergeCell ref="F11:F12"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="E5:E6"/>
-    <mergeCell ref="F6:F8"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="C11:C12"/>
-    <mergeCell ref="G7:G9"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="E7:E8"/>
-    <mergeCell ref="F9:F10"/>
-    <mergeCell ref="H7:H8"/>
-    <mergeCell ref="E9:E10"/>
-    <mergeCell ref="D9:D10"/>
-    <mergeCell ref="H9:H10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2443,7 +2445,7 @@
       <c r="C4" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="30" t="s">
+      <c r="D4" s="39" t="s">
         <v>28</v>
       </c>
       <c r="E4" s="11" t="s">
@@ -2462,11 +2464,11 @@
       <c r="B5" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="C5" s="25" t="s">
+      <c r="C5" s="32" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="31"/>
-      <c r="E5" s="25" t="s">
+      <c r="D5" s="40"/>
+      <c r="E5" s="32" t="s">
         <v>13</v>
       </c>
       <c r="F5" s="11" t="s">
@@ -2475,7 +2477,7 @@
       <c r="G5" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="H5" s="30" t="s">
+      <c r="H5" s="39" t="s">
         <v>28</v>
       </c>
     </row>
@@ -2486,33 +2488,33 @@
       <c r="B6" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="26"/>
-      <c r="D6" s="59" t="s">
+      <c r="C6" s="34"/>
+      <c r="D6" s="56" t="s">
         <v>19</v>
       </c>
-      <c r="E6" s="26"/>
-      <c r="F6" s="25" t="s">
+      <c r="E6" s="34"/>
+      <c r="F6" s="32" t="s">
         <v>15</v>
       </c>
       <c r="G6" s="3"/>
-      <c r="H6" s="31"/>
+      <c r="H6" s="40"/>
     </row>
     <row r="7" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="28" t="s">
+      <c r="B7" s="30" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="43" t="s">
+      <c r="C7" s="50" t="s">
         <v>44</v>
       </c>
-      <c r="D7" s="61"/>
-      <c r="E7" s="63" t="s">
-        <v>71</v>
-      </c>
-      <c r="F7" s="27"/>
-      <c r="G7" s="40" t="s">
+      <c r="D7" s="57"/>
+      <c r="E7" s="24" t="s">
+        <v>68</v>
+      </c>
+      <c r="F7" s="33"/>
+      <c r="G7" s="43" t="s">
         <v>18</v>
       </c>
       <c r="H7" s="4" t="s">
@@ -2523,38 +2525,38 @@
       <c r="A8" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="29"/>
-      <c r="C8" s="44"/>
+      <c r="B8" s="31"/>
+      <c r="C8" s="51"/>
       <c r="D8" s="11" t="s">
         <v>11</v>
       </c>
       <c r="E8" s="3"/>
-      <c r="F8" s="26"/>
-      <c r="G8" s="41"/>
+      <c r="F8" s="34"/>
+      <c r="G8" s="44"/>
       <c r="H8" s="3"/>
     </row>
     <row r="9" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B9" s="62" t="s">
+      <c r="B9" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="C9" s="28" t="s">
+      <c r="C9" s="30" t="s">
         <v>22</v>
       </c>
-      <c r="D9" s="28" t="s">
+      <c r="D9" s="30" t="s">
         <v>17</v>
       </c>
-      <c r="E9" s="28" t="s">
+      <c r="E9" s="30" t="s">
         <v>22</v>
       </c>
-      <c r="F9" s="64" t="s">
-        <v>73</v>
-      </c>
-      <c r="G9" s="42"/>
-      <c r="H9" s="70" t="s">
-        <v>73</v>
+      <c r="F9" s="25" t="s">
+        <v>70</v>
+      </c>
+      <c r="G9" s="45"/>
+      <c r="H9" s="66" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -2562,32 +2564,32 @@
         <v>23</v>
       </c>
       <c r="B10" s="3"/>
-      <c r="C10" s="29"/>
-      <c r="D10" s="29"/>
-      <c r="E10" s="29"/>
-      <c r="F10" s="72" t="s">
-        <v>78</v>
+      <c r="C10" s="31"/>
+      <c r="D10" s="31"/>
+      <c r="E10" s="31"/>
+      <c r="F10" s="27" t="s">
+        <v>74</v>
       </c>
       <c r="G10" s="3"/>
-      <c r="H10" s="71"/>
+      <c r="H10" s="67"/>
     </row>
     <row r="11" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B11" s="25" t="s">
-        <v>75</v>
-      </c>
-      <c r="C11" s="28" t="s">
+      <c r="B11" s="32" t="s">
+        <v>72</v>
+      </c>
+      <c r="C11" s="30" t="s">
         <v>26</v>
       </c>
-      <c r="D11" s="28" t="s">
+      <c r="D11" s="30" t="s">
         <v>27</v>
       </c>
-      <c r="E11" s="28" t="s">
+      <c r="E11" s="30" t="s">
         <v>26</v>
       </c>
-      <c r="F11" s="28" t="s">
+      <c r="F11" s="30" t="s">
         <v>27</v>
       </c>
       <c r="G11" s="3"/>
@@ -2597,13 +2599,13 @@
       <c r="A12" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="B12" s="27"/>
-      <c r="C12" s="29"/>
-      <c r="D12" s="29"/>
-      <c r="E12" s="29"/>
-      <c r="F12" s="29"/>
+      <c r="B12" s="33"/>
+      <c r="C12" s="31"/>
+      <c r="D12" s="31"/>
+      <c r="E12" s="31"/>
+      <c r="F12" s="31"/>
       <c r="G12" s="3"/>
-      <c r="H12" s="40" t="s">
+      <c r="H12" s="43" t="s">
         <v>18</v>
       </c>
     </row>
@@ -2611,23 +2613,23 @@
       <c r="A13" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B13" s="26"/>
-      <c r="C13" s="63" t="s">
-        <v>71</v>
+      <c r="B13" s="34"/>
+      <c r="C13" s="24" t="s">
+        <v>68</v>
       </c>
       <c r="D13" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="E13" s="30" t="s">
+      <c r="E13" s="39" t="s">
         <v>28</v>
       </c>
       <c r="F13" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="G13" s="72" t="s">
-        <v>78</v>
-      </c>
-      <c r="H13" s="41"/>
+      <c r="G13" s="27" t="s">
+        <v>74</v>
+      </c>
+      <c r="H13" s="44"/>
     </row>
     <row r="14" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
@@ -2636,17 +2638,17 @@
       <c r="B14" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="C14" s="62" t="s">
+      <c r="C14" s="23" t="s">
         <v>28</v>
       </c>
       <c r="D14" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="E14" s="31"/>
+      <c r="E14" s="40"/>
       <c r="F14" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="G14" s="59" t="s">
+      <c r="G14" s="56" t="s">
         <v>19</v>
       </c>
       <c r="H14" s="3"/>
@@ -2666,31 +2668,31 @@
         <v>48</v>
       </c>
       <c r="F15" s="3"/>
-      <c r="G15" s="61"/>
+      <c r="G15" s="57"/>
       <c r="H15" s="3"/>
     </row>
     <row r="16" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="B16" s="64" t="s">
-        <v>73</v>
+      <c r="B16" s="25" t="s">
+        <v>70</v>
       </c>
       <c r="C16" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="D16" s="40" t="s">
+      <c r="D16" s="43" t="s">
         <v>18</v>
       </c>
       <c r="E16" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="F16" s="40" t="s">
+      <c r="F16" s="43" t="s">
         <v>18</v>
       </c>
       <c r="G16" s="3"/>
       <c r="H16" s="10" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -2698,18 +2700,18 @@
         <v>36</v>
       </c>
       <c r="B17" s="15" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C17" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="D17" s="41"/>
+      <c r="D17" s="44"/>
       <c r="E17" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="F17" s="41"/>
+      <c r="F17" s="44"/>
       <c r="G17" s="3"/>
-      <c r="H17" s="43" t="s">
+      <c r="H17" s="50" t="s">
         <v>44</v>
       </c>
     </row>
@@ -2717,30 +2719,30 @@
       <c r="A18" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="B18" s="65" t="s">
-        <v>72</v>
-      </c>
-      <c r="C18" s="40" t="s">
+      <c r="B18" s="26" t="s">
+        <v>69</v>
+      </c>
+      <c r="C18" s="43" t="s">
         <v>18</v>
       </c>
-      <c r="D18" s="64" t="s">
-        <v>73</v>
-      </c>
-      <c r="E18" s="59" t="s">
+      <c r="D18" s="25" t="s">
+        <v>70</v>
+      </c>
+      <c r="E18" s="56" t="s">
         <v>19</v>
       </c>
       <c r="F18" s="3"/>
       <c r="G18" s="3"/>
-      <c r="H18" s="44"/>
+      <c r="H18" s="51"/>
     </row>
     <row r="19" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
         <v>38</v>
       </c>
       <c r="B19" s="3"/>
-      <c r="C19" s="42"/>
+      <c r="C19" s="45"/>
       <c r="D19" s="3"/>
-      <c r="E19" s="61"/>
+      <c r="E19" s="57"/>
       <c r="F19" s="3"/>
       <c r="G19" s="3"/>
       <c r="H19" s="3"/>
@@ -2748,6 +2750,21 @@
     <row r="20" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="26">
+    <mergeCell ref="C18:C19"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="F6:F8"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="E9:E10"/>
+    <mergeCell ref="B11:B13"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="E11:E12"/>
+    <mergeCell ref="F11:F12"/>
+    <mergeCell ref="E13:E14"/>
     <mergeCell ref="E18:E19"/>
     <mergeCell ref="H5:H6"/>
     <mergeCell ref="H12:H13"/>
@@ -2756,23 +2773,8 @@
     <mergeCell ref="F16:F17"/>
     <mergeCell ref="D6:D7"/>
     <mergeCell ref="D4:D5"/>
-    <mergeCell ref="B11:B13"/>
-    <mergeCell ref="C11:C12"/>
-    <mergeCell ref="D11:D12"/>
-    <mergeCell ref="E11:E12"/>
-    <mergeCell ref="F11:F12"/>
     <mergeCell ref="G14:G15"/>
-    <mergeCell ref="E13:E14"/>
-    <mergeCell ref="C18:C19"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="E5:E6"/>
-    <mergeCell ref="F6:F8"/>
-    <mergeCell ref="B7:B8"/>
     <mergeCell ref="G7:G9"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="D9:D10"/>
-    <mergeCell ref="E9:E10"/>
     <mergeCell ref="H9:H10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Modificacion actividades miercoles y resto de semana 3
</commit_message>
<xml_diff>
--- a/Programar_dias.xlsx
+++ b/Programar_dias.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Estudio\OneDrive - Universidad de Antioquia\Estudio\Materias\Informatica II\Calendario_semanal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECEA7DC2-E3BC-44C6-9B15-7EF2C89BC86C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{529469FC-46FB-43CD-97C4-F7712F39BF8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="2" xr2:uid="{CC961CB2-F623-4B13-8239-4B70F16E4462}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="75">
   <si>
     <t>LUNES</t>
   </si>
@@ -224,16 +224,10 @@
     <t>Yoga</t>
   </si>
   <si>
-    <t>Programar Kaggle</t>
-  </si>
-  <si>
     <t>Estudiar Inglés</t>
   </si>
   <si>
     <t xml:space="preserve">MATH. ESPECIALES </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Estudiar Métodos. </t>
   </si>
   <si>
     <t>Feb 27- Marzo 5</t>
@@ -319,9 +313,6 @@
   </si>
   <si>
     <t>Estu. Especiales</t>
-  </si>
-  <si>
-    <t>Act. Semillero</t>
   </si>
 </sst>
 </file>
@@ -613,7 +604,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="77">
+  <cellXfs count="74">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -663,9 +654,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -692,27 +680,51 @@
     <xf numFmtId="0" fontId="1" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="20" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="21" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -725,12 +737,6 @@
     <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -746,97 +752,73 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="18" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="18" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="20" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="21" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -846,6 +828,72 @@
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
     <mruColors>
       <color rgb="FFCC66FF"/>
       <color rgb="FFFFFF66"/>
@@ -1252,13 +1300,13 @@
       <c r="B5" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="32" t="s">
+      <c r="C5" s="33" t="s">
         <v>13</v>
       </c>
       <c r="D5" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="E5" s="32" t="s">
+        <v>49</v>
+      </c>
+      <c r="E5" s="33" t="s">
         <v>13</v>
       </c>
       <c r="F5" s="11" t="s">
@@ -1279,7 +1327,7 @@
         <v>11</v>
       </c>
       <c r="E6" s="34"/>
-      <c r="F6" s="32" t="s">
+      <c r="F6" s="33" t="s">
         <v>15</v>
       </c>
       <c r="G6" s="3"/>
@@ -1289,17 +1337,17 @@
       <c r="A7" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="30" t="s">
+      <c r="B7" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="39" t="s">
+      <c r="C7" s="38" t="s">
         <v>28</v>
       </c>
       <c r="D7" s="3"/>
-      <c r="E7" s="46" t="s">
+      <c r="E7" s="31" t="s">
         <v>47</v>
       </c>
-      <c r="F7" s="33"/>
+      <c r="F7" s="35"/>
       <c r="G7" s="3"/>
       <c r="H7" s="4" t="s">
         <v>10</v>
@@ -1309,15 +1357,15 @@
       <c r="A8" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="31"/>
-      <c r="C8" s="40"/>
+      <c r="B8" s="37"/>
+      <c r="C8" s="39"/>
       <c r="D8" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="E8" s="47"/>
+        <v>52</v>
+      </c>
+      <c r="E8" s="32"/>
       <c r="F8" s="34"/>
       <c r="G8" s="3"/>
-      <c r="H8" s="28" t="s">
+      <c r="H8" s="40" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1328,30 +1376,30 @@
       <c r="B9" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="C9" s="30" t="s">
+      <c r="C9" s="36" t="s">
         <v>22</v>
       </c>
-      <c r="D9" s="30" t="s">
+      <c r="D9" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="E9" s="30" t="s">
+      <c r="E9" s="36" t="s">
         <v>22</v>
       </c>
-      <c r="F9" s="39" t="s">
+      <c r="F9" s="38" t="s">
         <v>28</v>
       </c>
       <c r="G9" s="3"/>
-      <c r="H9" s="29"/>
+      <c r="H9" s="41"/>
     </row>
     <row r="10" spans="1:10" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>23</v>
       </c>
       <c r="B10" s="13"/>
-      <c r="C10" s="31"/>
-      <c r="D10" s="31"/>
-      <c r="E10" s="31"/>
-      <c r="F10" s="40"/>
+      <c r="C10" s="37"/>
+      <c r="D10" s="37"/>
+      <c r="E10" s="37"/>
+      <c r="F10" s="39"/>
       <c r="G10" s="3"/>
       <c r="H10" s="3"/>
     </row>
@@ -1359,23 +1407,23 @@
       <c r="A11" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B11" s="32" t="s">
+      <c r="B11" s="33" t="s">
         <v>25</v>
       </c>
-      <c r="C11" s="30" t="s">
+      <c r="C11" s="36" t="s">
         <v>26</v>
       </c>
-      <c r="D11" s="30" t="s">
+      <c r="D11" s="36" t="s">
         <v>27</v>
       </c>
       <c r="E11" s="3"/>
-      <c r="F11" s="30" t="s">
-        <v>56</v>
-      </c>
-      <c r="G11" s="46" t="s">
+      <c r="F11" s="36" t="s">
+        <v>54</v>
+      </c>
+      <c r="G11" s="31" t="s">
         <v>47</v>
       </c>
-      <c r="H11" s="28" t="s">
+      <c r="H11" s="40" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1383,12 +1431,12 @@
       <c r="A12" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="B12" s="33"/>
-      <c r="C12" s="31"/>
-      <c r="D12" s="31"/>
-      <c r="F12" s="31"/>
-      <c r="G12" s="47"/>
-      <c r="H12" s="29"/>
+      <c r="B12" s="35"/>
+      <c r="C12" s="37"/>
+      <c r="D12" s="37"/>
+      <c r="F12" s="37"/>
+      <c r="G12" s="32"/>
+      <c r="H12" s="41"/>
     </row>
     <row r="13" spans="1:10" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
@@ -1398,7 +1446,7 @@
       <c r="C13" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="D13" s="41" t="s">
+      <c r="D13" s="46" t="s">
         <v>31</v>
       </c>
       <c r="E13" s="11" t="s">
@@ -1419,10 +1467,10 @@
         <v>11</v>
       </c>
       <c r="C14" s="3"/>
-      <c r="D14" s="42"/>
+      <c r="D14" s="47"/>
       <c r="E14" s="3"/>
       <c r="F14" s="3"/>
-      <c r="G14" s="35" t="s">
+      <c r="G14" s="42" t="s">
         <v>44</v>
       </c>
       <c r="H14" s="3" t="s">
@@ -1435,15 +1483,15 @@
         <v>34</v>
       </c>
       <c r="B15" s="3"/>
-      <c r="C15" s="35" t="s">
+      <c r="C15" s="42" t="s">
         <v>44</v>
       </c>
       <c r="D15" s="14" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E15" s="3"/>
       <c r="F15" s="3"/>
-      <c r="G15" s="36"/>
+      <c r="G15" s="43"/>
       <c r="H15" s="11" t="s">
         <v>11</v>
       </c>
@@ -1453,18 +1501,18 @@
         <v>35</v>
       </c>
       <c r="B16" s="3"/>
-      <c r="C16" s="36"/>
+      <c r="C16" s="43"/>
       <c r="D16" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="E16" s="39" t="s">
+      <c r="E16" s="38" t="s">
         <v>28</v>
       </c>
       <c r="F16" s="3"/>
-      <c r="G16" s="43" t="s">
+      <c r="G16" s="48" t="s">
         <v>18</v>
       </c>
-      <c r="H16" s="39" t="s">
+      <c r="H16" s="38" t="s">
         <v>28</v>
       </c>
     </row>
@@ -1473,36 +1521,36 @@
         <v>36</v>
       </c>
       <c r="B17" s="10" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C17" s="3"/>
       <c r="D17" s="3"/>
-      <c r="E17" s="40"/>
+      <c r="E17" s="39"/>
       <c r="F17" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="G17" s="44"/>
-      <c r="H17" s="40"/>
+      <c r="G17" s="49"/>
+      <c r="H17" s="39"/>
     </row>
     <row r="18" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="B18" s="28" t="s">
+      <c r="B18" s="40" t="s">
         <v>18</v>
       </c>
-      <c r="C18" s="35" t="s">
+      <c r="C18" s="42" t="s">
         <v>44</v>
       </c>
-      <c r="D18" s="37" t="s">
+      <c r="D18" s="44" t="s">
         <v>19</v>
       </c>
-      <c r="E18" s="28" t="s">
+      <c r="E18" s="40" t="s">
         <v>18</v>
       </c>
       <c r="F18" s="3"/>
-      <c r="G18" s="45"/>
-      <c r="H18" s="28" t="s">
+      <c r="G18" s="50"/>
+      <c r="H18" s="40" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1510,28 +1558,16 @@
       <c r="A19" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="B19" s="29"/>
-      <c r="C19" s="36"/>
-      <c r="D19" s="38"/>
-      <c r="E19" s="29"/>
+      <c r="B19" s="41"/>
+      <c r="C19" s="43"/>
+      <c r="D19" s="45"/>
+      <c r="E19" s="41"/>
       <c r="F19" s="3"/>
       <c r="G19" s="3"/>
-      <c r="H19" s="29"/>
+      <c r="H19" s="41"/>
     </row>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="G11:G12"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="E5:E6"/>
-    <mergeCell ref="F6:F8"/>
-    <mergeCell ref="C11:C12"/>
-    <mergeCell ref="D11:D12"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="D9:D10"/>
-    <mergeCell ref="E9:E10"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="F9:F10"/>
-    <mergeCell ref="E7:E8"/>
     <mergeCell ref="H8:H9"/>
     <mergeCell ref="H11:H12"/>
     <mergeCell ref="B18:B19"/>
@@ -1548,6 +1584,18 @@
     <mergeCell ref="H16:H17"/>
     <mergeCell ref="G14:G15"/>
     <mergeCell ref="G16:G18"/>
+    <mergeCell ref="G11:G12"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="F6:F8"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="E9:E10"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="F9:F10"/>
+    <mergeCell ref="E7:E8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1602,11 +1650,11 @@
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
-      <c r="F2" s="68"/>
+      <c r="F2" s="27"/>
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
       <c r="J2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -1621,7 +1669,7 @@
       <c r="G3" s="3"/>
       <c r="H3" s="3"/>
       <c r="J3" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -1634,103 +1682,103 @@
       <c r="C4" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="52" t="s">
+      <c r="D4" s="55" t="s">
         <v>44</v>
       </c>
       <c r="E4" s="11" t="s">
         <v>11</v>
       </c>
       <c r="F4" s="12" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G4" s="3"/>
       <c r="H4" s="3"/>
       <c r="J4" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="28" t="s">
+      <c r="B5" s="40" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="32" t="s">
+      <c r="C5" s="33" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="53"/>
-      <c r="E5" s="32" t="s">
+      <c r="D5" s="56"/>
+      <c r="E5" s="33" t="s">
         <v>13</v>
       </c>
       <c r="F5" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="G5" s="43" t="s">
+      <c r="G5" s="48" t="s">
         <v>18</v>
       </c>
       <c r="H5" s="4" t="s">
         <v>10</v>
       </c>
       <c r="J5" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="29"/>
+      <c r="B6" s="41"/>
       <c r="C6" s="34"/>
-      <c r="D6" s="48" t="s">
+      <c r="D6" s="52" t="s">
         <v>33</v>
       </c>
       <c r="E6" s="34"/>
-      <c r="F6" s="32" t="s">
+      <c r="F6" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="G6" s="44"/>
+      <c r="G6" s="49"/>
       <c r="H6" s="3"/>
       <c r="J6" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="30" t="s">
+      <c r="B7" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="48" t="s">
+      <c r="C7" s="52" t="s">
         <v>33</v>
       </c>
-      <c r="D7" s="49"/>
-      <c r="E7" s="21" t="s">
+      <c r="D7" s="54"/>
+      <c r="E7" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="F7" s="33"/>
-      <c r="G7" s="44"/>
+      <c r="F7" s="35"/>
+      <c r="G7" s="49"/>
       <c r="H7" s="3"/>
       <c r="J7" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="31"/>
-      <c r="C8" s="49"/>
-      <c r="D8" s="39" t="s">
+      <c r="B8" s="37"/>
+      <c r="C8" s="54"/>
+      <c r="D8" s="38" t="s">
         <v>28</v>
       </c>
-      <c r="E8" s="22" t="s">
-        <v>54</v>
+      <c r="E8" s="21" t="s">
+        <v>52</v>
       </c>
       <c r="F8" s="34"/>
-      <c r="G8" s="44"/>
-      <c r="H8" s="48" t="s">
+      <c r="G8" s="49"/>
+      <c r="H8" s="52" t="s">
         <v>33</v>
       </c>
     </row>
@@ -1738,53 +1786,53 @@
       <c r="A9" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B9" s="46" t="s">
+      <c r="B9" s="31" t="s">
         <v>47</v>
       </c>
-      <c r="C9" s="32" t="s">
-        <v>51</v>
-      </c>
-      <c r="D9" s="40"/>
-      <c r="E9" s="32" t="s">
-        <v>51</v>
+      <c r="C9" s="33" t="s">
+        <v>50</v>
+      </c>
+      <c r="D9" s="39"/>
+      <c r="E9" s="33" t="s">
+        <v>50</v>
       </c>
       <c r="F9" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="G9" s="44"/>
-      <c r="H9" s="71"/>
+      <c r="G9" s="49"/>
+      <c r="H9" s="53"/>
     </row>
     <row r="10" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B10" s="47"/>
+      <c r="B10" s="32"/>
       <c r="C10" s="34"/>
       <c r="D10" s="11" t="s">
         <v>11</v>
       </c>
       <c r="E10" s="34"/>
       <c r="F10" s="3"/>
-      <c r="G10" s="45"/>
-      <c r="H10" s="49"/>
+      <c r="G10" s="50"/>
+      <c r="H10" s="54"/>
     </row>
     <row r="11" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B11" s="32" t="s">
+      <c r="B11" s="33" t="s">
         <v>25</v>
       </c>
-      <c r="C11" s="32" t="s">
-        <v>58</v>
-      </c>
-      <c r="D11" s="32" t="s">
+      <c r="C11" s="33" t="s">
         <v>56</v>
       </c>
-      <c r="E11" s="32" t="s">
-        <v>58</v>
-      </c>
-      <c r="F11" s="54" t="s">
+      <c r="D11" s="33" t="s">
+        <v>54</v>
+      </c>
+      <c r="E11" s="33" t="s">
+        <v>56</v>
+      </c>
+      <c r="F11" s="57" t="s">
         <v>43</v>
       </c>
       <c r="G11" s="3"/>
@@ -1794,13 +1842,13 @@
       <c r="A12" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="B12" s="33"/>
+      <c r="B12" s="35"/>
       <c r="C12" s="34"/>
       <c r="D12" s="34"/>
       <c r="E12" s="34"/>
-      <c r="F12" s="55"/>
+      <c r="F12" s="58"/>
       <c r="G12" s="3"/>
-      <c r="H12" s="48" t="s">
+      <c r="H12" s="52" t="s">
         <v>33</v>
       </c>
     </row>
@@ -1812,30 +1860,30 @@
       <c r="C13" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="D13" s="41" t="s">
+      <c r="D13" s="46" t="s">
         <v>31</v>
       </c>
-      <c r="E13" s="69" t="s">
-        <v>11</v>
-      </c>
-      <c r="F13" s="70" t="s">
+      <c r="E13" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="F13" s="51" t="s">
         <v>42</v>
       </c>
       <c r="G13" s="3"/>
-      <c r="H13" s="49"/>
+      <c r="H13" s="54"/>
     </row>
     <row r="14" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
         <v>32</v>
       </c>
       <c r="B14" s="3"/>
-      <c r="C14" s="39" t="s">
+      <c r="C14" s="38" t="s">
         <v>28</v>
       </c>
-      <c r="D14" s="42"/>
-      <c r="F14" s="70"/>
+      <c r="D14" s="47"/>
+      <c r="F14" s="51"/>
       <c r="G14" s="3"/>
-      <c r="H14" s="43" t="s">
+      <c r="H14" s="48" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1846,27 +1894,27 @@
       <c r="B15" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="C15" s="40"/>
+      <c r="C15" s="39"/>
       <c r="D15" s="3"/>
-      <c r="E15" s="39" t="s">
+      <c r="E15" s="38" t="s">
         <v>28</v>
       </c>
       <c r="F15" s="3"/>
       <c r="G15" s="3"/>
-      <c r="H15" s="45"/>
+      <c r="H15" s="50"/>
     </row>
     <row r="16" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="B16" s="52" t="s">
+      <c r="B16" s="55" t="s">
         <v>44</v>
       </c>
-      <c r="C16" s="52" t="s">
+      <c r="C16" s="55" t="s">
         <v>44</v>
       </c>
       <c r="D16" s="3"/>
-      <c r="E16" s="40"/>
+      <c r="E16" s="39"/>
       <c r="F16" s="11" t="s">
         <v>11</v>
       </c>
@@ -1877,19 +1925,19 @@
       <c r="A17" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="B17" s="53"/>
-      <c r="C17" s="53"/>
+      <c r="B17" s="56"/>
+      <c r="C17" s="56"/>
       <c r="D17" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="E17" s="39" t="s">
+      <c r="E17" s="38" t="s">
         <v>28</v>
       </c>
       <c r="F17" s="17" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="G17" s="3"/>
-      <c r="H17" s="43" t="s">
+      <c r="H17" s="48" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1900,40 +1948,50 @@
       <c r="B18" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="C18" s="48" t="s">
+      <c r="C18" s="52" t="s">
         <v>33</v>
       </c>
-      <c r="D18" s="48" t="s">
+      <c r="D18" s="52" t="s">
         <v>33</v>
       </c>
-      <c r="E18" s="40"/>
-      <c r="F18" s="43" t="s">
+      <c r="E18" s="39"/>
+      <c r="F18" s="48" t="s">
         <v>18</v>
       </c>
       <c r="G18" s="3"/>
-      <c r="H18" s="44"/>
+      <c r="H18" s="49"/>
     </row>
     <row r="19" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
         <v>38</v>
       </c>
       <c r="B19" s="3"/>
-      <c r="C19" s="49"/>
-      <c r="D19" s="49"/>
+      <c r="C19" s="54"/>
+      <c r="D19" s="54"/>
       <c r="E19" s="14" t="s">
-        <v>55</v>
-      </c>
-      <c r="F19" s="45"/>
+        <v>53</v>
+      </c>
+      <c r="F19" s="50"/>
       <c r="G19" s="3"/>
-      <c r="H19" s="45"/>
+      <c r="H19" s="50"/>
     </row>
   </sheetData>
   <mergeCells count="32">
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="E5:E6"/>
-    <mergeCell ref="F6:F8"/>
-    <mergeCell ref="F13:F14"/>
-    <mergeCell ref="G5:G10"/>
+    <mergeCell ref="F18:F19"/>
+    <mergeCell ref="H17:H19"/>
+    <mergeCell ref="C18:C19"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="D18:D19"/>
+    <mergeCell ref="E15:E16"/>
+    <mergeCell ref="E17:E18"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="B11:B13"/>
+    <mergeCell ref="E11:E12"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="F11:F12"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="C16:C17"/>
     <mergeCell ref="H8:H10"/>
     <mergeCell ref="H12:H13"/>
     <mergeCell ref="H14:H15"/>
@@ -1946,21 +2004,11 @@
     <mergeCell ref="D8:D9"/>
     <mergeCell ref="C9:C10"/>
     <mergeCell ref="E9:E10"/>
-    <mergeCell ref="B16:B17"/>
-    <mergeCell ref="B11:B13"/>
-    <mergeCell ref="E11:E12"/>
-    <mergeCell ref="D11:D12"/>
-    <mergeCell ref="F11:F12"/>
-    <mergeCell ref="C11:C12"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="C16:C17"/>
-    <mergeCell ref="C18:C19"/>
-    <mergeCell ref="D13:D14"/>
-    <mergeCell ref="D18:D19"/>
-    <mergeCell ref="E15:E16"/>
-    <mergeCell ref="E17:E18"/>
-    <mergeCell ref="F18:F19"/>
-    <mergeCell ref="H17:H19"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="F6:F8"/>
+    <mergeCell ref="F13:F14"/>
+    <mergeCell ref="G5:G10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1972,17 +2020,19 @@
   <dimension ref="A1:H19"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="G11" sqref="G11:G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="8" width="18.7109375" customWidth="1"/>
+    <col min="1" max="3" width="18.7109375" customWidth="1"/>
+    <col min="4" max="4" width="21" customWidth="1"/>
+    <col min="5" max="8" width="18.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -2038,14 +2088,12 @@
       <c r="C4" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="19" t="s">
-        <v>76</v>
-      </c>
+      <c r="D4" s="3"/>
       <c r="E4" s="11" t="s">
         <v>11</v>
       </c>
       <c r="F4" s="12" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G4" s="3"/>
       <c r="H4" s="3"/>
@@ -2055,15 +2103,15 @@
         <v>12</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>61</v>
-      </c>
-      <c r="C5" s="32" t="s">
+        <v>59</v>
+      </c>
+      <c r="C5" s="33" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="E5" s="32" t="s">
+      <c r="D5" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="33" t="s">
         <v>13</v>
       </c>
       <c r="F5" s="11" t="s">
@@ -2084,36 +2132,38 @@
         <v>11</v>
       </c>
       <c r="C6" s="34"/>
-      <c r="D6" s="19" t="s">
-        <v>59</v>
+      <c r="D6" s="18" t="s">
+        <v>74</v>
       </c>
       <c r="E6" s="34"/>
-      <c r="F6" s="32" t="s">
+      <c r="F6" s="33" t="s">
         <v>15</v>
       </c>
       <c r="H6" s="12" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="54" t="s">
-        <v>60</v>
+      <c r="B7" s="57" t="s">
+        <v>58</v>
       </c>
       <c r="C7" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="D7" s="3"/>
-      <c r="E7" s="63" t="s">
-        <v>49</v>
-      </c>
-      <c r="F7" s="33"/>
-      <c r="G7" s="60" t="s">
+      <c r="D7" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="E7" s="30" t="s">
+        <v>19</v>
+      </c>
+      <c r="F7" s="35"/>
+      <c r="G7" s="61" t="s">
         <v>18</v>
       </c>
-      <c r="H7" s="56" t="s">
+      <c r="H7" s="64" t="s">
         <v>19</v>
       </c>
     </row>
@@ -2121,35 +2171,35 @@
       <c r="A8" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="55"/>
+      <c r="B8" s="58"/>
       <c r="C8" s="3"/>
-      <c r="D8" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="E8" s="64"/>
+      <c r="D8" s="72" t="s">
+        <v>44</v>
+      </c>
+      <c r="E8" s="73"/>
       <c r="F8" s="34"/>
-      <c r="G8" s="61"/>
-      <c r="H8" s="57"/>
+      <c r="G8" s="62"/>
+      <c r="H8" s="65"/>
     </row>
     <row r="9" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>21</v>
       </c>
       <c r="B9" s="3"/>
-      <c r="C9" s="32" t="s">
-        <v>51</v>
-      </c>
-      <c r="D9" s="30" t="s">
+      <c r="C9" s="33" t="s">
+        <v>50</v>
+      </c>
+      <c r="D9" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="E9" s="58" t="s">
+      <c r="E9" s="66" t="s">
         <v>46</v>
       </c>
-      <c r="F9" s="65" t="s">
-        <v>52</v>
-      </c>
-      <c r="G9" s="62"/>
-      <c r="H9" s="50" t="s">
+      <c r="F9" s="40" t="s">
+        <v>18</v>
+      </c>
+      <c r="G9" s="63"/>
+      <c r="H9" s="68" t="s">
         <v>44</v>
       </c>
     </row>
@@ -2157,37 +2207,37 @@
       <c r="A10" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B10" s="20" t="s">
+      <c r="B10" s="19" t="s">
         <v>28</v>
       </c>
       <c r="C10" s="34"/>
-      <c r="D10" s="31"/>
-      <c r="E10" s="59"/>
-      <c r="F10" s="47"/>
+      <c r="D10" s="37"/>
+      <c r="E10" s="67"/>
+      <c r="F10" s="41"/>
       <c r="G10" s="3"/>
-      <c r="H10" s="51"/>
+      <c r="H10" s="69"/>
     </row>
     <row r="11" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B11" s="32" t="s">
+      <c r="B11" s="33" t="s">
         <v>25</v>
       </c>
-      <c r="C11" s="32" t="s">
-        <v>58</v>
-      </c>
-      <c r="D11" s="32" t="s">
+      <c r="C11" s="33" t="s">
         <v>56</v>
       </c>
-      <c r="E11" s="58" t="s">
+      <c r="D11" s="33" t="s">
+        <v>54</v>
+      </c>
+      <c r="E11" s="66" t="s">
         <v>45</v>
       </c>
-      <c r="F11" s="58" t="s">
-        <v>57</v>
-      </c>
-      <c r="G11" s="39" t="s">
-        <v>28</v>
+      <c r="F11" s="66" t="s">
+        <v>55</v>
+      </c>
+      <c r="G11" s="40" t="s">
+        <v>18</v>
       </c>
       <c r="H11" s="3"/>
     </row>
@@ -2195,13 +2245,13 @@
       <c r="A12" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="B12" s="33"/>
+      <c r="B12" s="35"/>
       <c r="C12" s="34"/>
       <c r="D12" s="34"/>
-      <c r="E12" s="59"/>
-      <c r="F12" s="59"/>
-      <c r="G12" s="40"/>
-      <c r="H12" s="48" t="s">
+      <c r="E12" s="67"/>
+      <c r="F12" s="67"/>
+      <c r="G12" s="41"/>
+      <c r="H12" s="52" t="s">
         <v>33</v>
       </c>
     </row>
@@ -2210,35 +2260,35 @@
         <v>30</v>
       </c>
       <c r="B13" s="34"/>
-      <c r="C13" s="39" t="s">
+      <c r="C13" s="38" t="s">
         <v>28</v>
       </c>
-      <c r="D13" s="41" t="s">
+      <c r="D13" s="46" t="s">
         <v>31</v>
       </c>
-      <c r="E13" s="39" t="s">
+      <c r="E13" s="38" t="s">
         <v>28</v>
       </c>
       <c r="F13" s="8" t="s">
         <v>42</v>
       </c>
       <c r="G13" s="3"/>
-      <c r="H13" s="49"/>
+      <c r="H13" s="54"/>
     </row>
     <row r="14" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B14" s="72" t="s">
+      <c r="B14" s="59" t="s">
         <v>42</v>
       </c>
-      <c r="C14" s="40"/>
-      <c r="D14" s="42"/>
-      <c r="E14" s="40"/>
+      <c r="C14" s="39"/>
+      <c r="D14" s="47"/>
+      <c r="E14" s="39"/>
       <c r="F14" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="G14" s="56" t="s">
+      <c r="G14" s="64" t="s">
         <v>19</v>
       </c>
       <c r="H14" s="3"/>
@@ -2247,7 +2297,7 @@
       <c r="A15" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="B15" s="73"/>
+      <c r="B15" s="60"/>
       <c r="C15" s="9" t="s">
         <v>48</v>
       </c>
@@ -2257,7 +2307,7 @@
       <c r="E15" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="G15" s="57"/>
+      <c r="G15" s="65"/>
       <c r="H15" s="3"/>
     </row>
     <row r="16" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -2267,17 +2317,16 @@
       <c r="B16" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="C16" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="D16" s="3"/>
+      <c r="D16" s="3" t="s">
+        <v>52</v>
+      </c>
       <c r="E16" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="F16" s="28" t="s">
+      <c r="F16" s="40" t="s">
         <v>18</v>
       </c>
-      <c r="G16" s="50" t="s">
+      <c r="G16" s="68" t="s">
         <v>44</v>
       </c>
       <c r="H16" s="3"/>
@@ -2286,21 +2335,21 @@
       <c r="A17" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="B17" s="75" t="s">
+      <c r="B17" s="30" t="s">
         <v>19</v>
       </c>
-      <c r="C17" s="76" t="s">
+      <c r="C17" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="D17" s="30" t="s">
         <v>19</v>
       </c>
-      <c r="D17" s="28" t="s">
-        <v>18</v>
-      </c>
       <c r="E17" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="F17" s="29"/>
-      <c r="G17" s="51"/>
-      <c r="H17" s="39" t="s">
+        <v>49</v>
+      </c>
+      <c r="F17" s="41"/>
+      <c r="G17" s="69"/>
+      <c r="H17" s="38" t="s">
         <v>28</v>
       </c>
     </row>
@@ -2308,42 +2357,54 @@
       <c r="A18" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="B18" s="19" t="s">
-        <v>76</v>
-      </c>
-      <c r="C18" s="19" t="s">
-        <v>76</v>
-      </c>
-      <c r="D18" s="29"/>
-      <c r="E18" s="3"/>
+      <c r="B18" s="18" t="s">
+        <v>74</v>
+      </c>
+      <c r="C18" s="18" t="s">
+        <v>74</v>
+      </c>
+      <c r="D18" s="18" t="s">
+        <v>74</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="F18" s="40" t="s">
+        <v>18</v>
+      </c>
       <c r="G18" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="H18" s="40"/>
+        <v>49</v>
+      </c>
+      <c r="H18" s="39"/>
     </row>
     <row r="19" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="B19" s="74" t="s">
-        <v>75</v>
-      </c>
-      <c r="C19" s="18" t="s">
-        <v>77</v>
+      <c r="B19" s="29" t="s">
+        <v>73</v>
+      </c>
+      <c r="C19" s="30" t="s">
+        <v>19</v>
       </c>
       <c r="D19" s="3"/>
       <c r="E19" s="3"/>
-      <c r="F19" s="3"/>
+      <c r="F19" s="41"/>
       <c r="G19" s="3"/>
       <c r="H19" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="28">
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="D11:D12"/>
-    <mergeCell ref="G7:G9"/>
-    <mergeCell ref="E7:E8"/>
-    <mergeCell ref="F9:F10"/>
+  <mergeCells count="27">
+    <mergeCell ref="H12:H13"/>
+    <mergeCell ref="H17:H18"/>
+    <mergeCell ref="F16:F17"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="E13:E14"/>
+    <mergeCell ref="G16:G17"/>
+    <mergeCell ref="G14:G15"/>
+    <mergeCell ref="E11:E12"/>
+    <mergeCell ref="F11:F12"/>
+    <mergeCell ref="F18:F19"/>
     <mergeCell ref="H7:H8"/>
     <mergeCell ref="E9:E10"/>
     <mergeCell ref="D9:D10"/>
@@ -2351,22 +2412,16 @@
     <mergeCell ref="C5:C6"/>
     <mergeCell ref="E5:E6"/>
     <mergeCell ref="F6:F8"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="G7:G9"/>
+    <mergeCell ref="F9:F10"/>
     <mergeCell ref="B7:B8"/>
     <mergeCell ref="C11:C12"/>
     <mergeCell ref="G11:G12"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="H12:H13"/>
-    <mergeCell ref="H17:H18"/>
-    <mergeCell ref="F16:F17"/>
-    <mergeCell ref="D13:D14"/>
-    <mergeCell ref="D17:D18"/>
     <mergeCell ref="C13:C14"/>
-    <mergeCell ref="E13:E14"/>
-    <mergeCell ref="G16:G17"/>
-    <mergeCell ref="G14:G15"/>
     <mergeCell ref="B11:B13"/>
-    <mergeCell ref="E11:E12"/>
-    <mergeCell ref="F11:F12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2445,14 +2500,14 @@
       <c r="C4" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="39" t="s">
+      <c r="D4" s="38" t="s">
         <v>28</v>
       </c>
       <c r="E4" s="11" t="s">
         <v>11</v>
       </c>
       <c r="F4" s="12" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G4" s="3"/>
       <c r="H4" s="3"/>
@@ -2462,13 +2517,13 @@
         <v>12</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="C5" s="32" t="s">
+        <v>49</v>
+      </c>
+      <c r="C5" s="33" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="40"/>
-      <c r="E5" s="32" t="s">
+      <c r="D5" s="39"/>
+      <c r="E5" s="33" t="s">
         <v>13</v>
       </c>
       <c r="F5" s="11" t="s">
@@ -2477,7 +2532,7 @@
       <c r="G5" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="H5" s="39" t="s">
+      <c r="H5" s="38" t="s">
         <v>28</v>
       </c>
     </row>
@@ -2489,32 +2544,32 @@
         <v>11</v>
       </c>
       <c r="C6" s="34"/>
-      <c r="D6" s="56" t="s">
+      <c r="D6" s="64" t="s">
         <v>19</v>
       </c>
       <c r="E6" s="34"/>
-      <c r="F6" s="32" t="s">
+      <c r="F6" s="33" t="s">
         <v>15</v>
       </c>
       <c r="G6" s="3"/>
-      <c r="H6" s="40"/>
+      <c r="H6" s="39"/>
     </row>
     <row r="7" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="30" t="s">
+      <c r="B7" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="50" t="s">
+      <c r="C7" s="68" t="s">
         <v>44</v>
       </c>
-      <c r="D7" s="57"/>
-      <c r="E7" s="24" t="s">
-        <v>68</v>
-      </c>
-      <c r="F7" s="33"/>
-      <c r="G7" s="43" t="s">
+      <c r="D7" s="65"/>
+      <c r="E7" s="23" t="s">
+        <v>66</v>
+      </c>
+      <c r="F7" s="35"/>
+      <c r="G7" s="48" t="s">
         <v>18</v>
       </c>
       <c r="H7" s="4" t="s">
@@ -2525,38 +2580,38 @@
       <c r="A8" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="31"/>
-      <c r="C8" s="51"/>
+      <c r="B8" s="37"/>
+      <c r="C8" s="69"/>
       <c r="D8" s="11" t="s">
         <v>11</v>
       </c>
       <c r="E8" s="3"/>
       <c r="F8" s="34"/>
-      <c r="G8" s="44"/>
+      <c r="G8" s="49"/>
       <c r="H8" s="3"/>
     </row>
     <row r="9" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B9" s="23" t="s">
+      <c r="B9" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="C9" s="30" t="s">
+      <c r="C9" s="36" t="s">
         <v>22</v>
       </c>
-      <c r="D9" s="30" t="s">
+      <c r="D9" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="E9" s="30" t="s">
+      <c r="E9" s="36" t="s">
         <v>22</v>
       </c>
-      <c r="F9" s="25" t="s">
-        <v>70</v>
-      </c>
-      <c r="G9" s="45"/>
-      <c r="H9" s="66" t="s">
-        <v>70</v>
+      <c r="F9" s="24" t="s">
+        <v>68</v>
+      </c>
+      <c r="G9" s="50"/>
+      <c r="H9" s="70" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -2564,32 +2619,32 @@
         <v>23</v>
       </c>
       <c r="B10" s="3"/>
-      <c r="C10" s="31"/>
-      <c r="D10" s="31"/>
-      <c r="E10" s="31"/>
-      <c r="F10" s="27" t="s">
-        <v>74</v>
+      <c r="C10" s="37"/>
+      <c r="D10" s="37"/>
+      <c r="E10" s="37"/>
+      <c r="F10" s="26" t="s">
+        <v>72</v>
       </c>
       <c r="G10" s="3"/>
-      <c r="H10" s="67"/>
+      <c r="H10" s="71"/>
     </row>
     <row r="11" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B11" s="32" t="s">
-        <v>72</v>
-      </c>
-      <c r="C11" s="30" t="s">
+      <c r="B11" s="33" t="s">
+        <v>70</v>
+      </c>
+      <c r="C11" s="36" t="s">
         <v>26</v>
       </c>
-      <c r="D11" s="30" t="s">
+      <c r="D11" s="36" t="s">
         <v>27</v>
       </c>
-      <c r="E11" s="30" t="s">
+      <c r="E11" s="36" t="s">
         <v>26</v>
       </c>
-      <c r="F11" s="30" t="s">
+      <c r="F11" s="36" t="s">
         <v>27</v>
       </c>
       <c r="G11" s="3"/>
@@ -2599,13 +2654,13 @@
       <c r="A12" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="B12" s="33"/>
-      <c r="C12" s="31"/>
-      <c r="D12" s="31"/>
-      <c r="E12" s="31"/>
-      <c r="F12" s="31"/>
+      <c r="B12" s="35"/>
+      <c r="C12" s="37"/>
+      <c r="D12" s="37"/>
+      <c r="E12" s="37"/>
+      <c r="F12" s="37"/>
       <c r="G12" s="3"/>
-      <c r="H12" s="43" t="s">
+      <c r="H12" s="48" t="s">
         <v>18</v>
       </c>
     </row>
@@ -2614,22 +2669,22 @@
         <v>30</v>
       </c>
       <c r="B13" s="34"/>
-      <c r="C13" s="24" t="s">
-        <v>68</v>
+      <c r="C13" s="23" t="s">
+        <v>66</v>
       </c>
       <c r="D13" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="E13" s="39" t="s">
+      <c r="E13" s="38" t="s">
         <v>28</v>
       </c>
       <c r="F13" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="G13" s="27" t="s">
-        <v>74</v>
-      </c>
-      <c r="H13" s="44"/>
+      <c r="G13" s="26" t="s">
+        <v>72</v>
+      </c>
+      <c r="H13" s="49"/>
     </row>
     <row r="14" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
@@ -2638,17 +2693,17 @@
       <c r="B14" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="C14" s="23" t="s">
+      <c r="C14" s="22" t="s">
         <v>28</v>
       </c>
       <c r="D14" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="E14" s="40"/>
+      <c r="E14" s="39"/>
       <c r="F14" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="G14" s="56" t="s">
+      <c r="G14" s="64" t="s">
         <v>19</v>
       </c>
       <c r="H14" s="3"/>
@@ -2668,31 +2723,31 @@
         <v>48</v>
       </c>
       <c r="F15" s="3"/>
-      <c r="G15" s="57"/>
+      <c r="G15" s="65"/>
       <c r="H15" s="3"/>
     </row>
     <row r="16" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="B16" s="25" t="s">
-        <v>70</v>
+      <c r="B16" s="24" t="s">
+        <v>68</v>
       </c>
       <c r="C16" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="D16" s="43" t="s">
+      <c r="D16" s="48" t="s">
         <v>18</v>
       </c>
       <c r="E16" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="F16" s="43" t="s">
+      <c r="F16" s="48" t="s">
         <v>18</v>
       </c>
       <c r="G16" s="3"/>
       <c r="H16" s="10" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -2700,18 +2755,18 @@
         <v>36</v>
       </c>
       <c r="B17" s="15" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C17" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="D17" s="44"/>
+        <v>49</v>
+      </c>
+      <c r="D17" s="49"/>
       <c r="E17" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="F17" s="44"/>
+        <v>49</v>
+      </c>
+      <c r="F17" s="49"/>
       <c r="G17" s="3"/>
-      <c r="H17" s="50" t="s">
+      <c r="H17" s="68" t="s">
         <v>44</v>
       </c>
     </row>
@@ -2719,30 +2774,30 @@
       <c r="A18" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="B18" s="26" t="s">
-        <v>69</v>
-      </c>
-      <c r="C18" s="43" t="s">
+      <c r="B18" s="25" t="s">
+        <v>67</v>
+      </c>
+      <c r="C18" s="48" t="s">
         <v>18</v>
       </c>
-      <c r="D18" s="25" t="s">
-        <v>70</v>
-      </c>
-      <c r="E18" s="56" t="s">
+      <c r="D18" s="24" t="s">
+        <v>68</v>
+      </c>
+      <c r="E18" s="64" t="s">
         <v>19</v>
       </c>
       <c r="F18" s="3"/>
       <c r="G18" s="3"/>
-      <c r="H18" s="51"/>
+      <c r="H18" s="69"/>
     </row>
     <row r="19" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
         <v>38</v>
       </c>
       <c r="B19" s="3"/>
-      <c r="C19" s="45"/>
+      <c r="C19" s="50"/>
       <c r="D19" s="3"/>
-      <c r="E19" s="57"/>
+      <c r="E19" s="65"/>
       <c r="F19" s="3"/>
       <c r="G19" s="3"/>
       <c r="H19" s="3"/>
@@ -2750,6 +2805,16 @@
     <row r="20" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="26">
+    <mergeCell ref="H5:H6"/>
+    <mergeCell ref="H12:H13"/>
+    <mergeCell ref="H17:H18"/>
+    <mergeCell ref="D16:D17"/>
+    <mergeCell ref="F16:F17"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="G14:G15"/>
+    <mergeCell ref="G7:G9"/>
+    <mergeCell ref="H9:H10"/>
     <mergeCell ref="C18:C19"/>
     <mergeCell ref="C5:C6"/>
     <mergeCell ref="E5:E6"/>
@@ -2766,16 +2831,6 @@
     <mergeCell ref="F11:F12"/>
     <mergeCell ref="E13:E14"/>
     <mergeCell ref="E18:E19"/>
-    <mergeCell ref="H5:H6"/>
-    <mergeCell ref="H12:H13"/>
-    <mergeCell ref="H17:H18"/>
-    <mergeCell ref="D16:D17"/>
-    <mergeCell ref="F16:F17"/>
-    <mergeCell ref="D6:D7"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="G14:G15"/>
-    <mergeCell ref="G7:G9"/>
-    <mergeCell ref="H9:H10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>

</xml_diff>

<commit_message>
Modificación horas estudio fds 3. Modificación del día jueves s.3
</commit_message>
<xml_diff>
--- a/Programar_dias.xlsx
+++ b/Programar_dias.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Estudio\OneDrive - Universidad de Antioquia\Estudio\Materias\Informatica II\Calendario_semanal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{529469FC-46FB-43CD-97C4-F7712F39BF8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F164586-5EB2-4C6F-98F4-8BD2C9D2F3F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="2" xr2:uid="{CC961CB2-F623-4B13-8239-4B70F16E4462}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="76">
   <si>
     <t>LUNES</t>
   </si>
@@ -313,6 +313,9 @@
   </si>
   <si>
     <t>Estu. Especiales</t>
+  </si>
+  <si>
+    <t>Est Informatica</t>
   </si>
 </sst>
 </file>
@@ -399,7 +402,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="22">
+  <fills count="21">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -463,12 +466,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="3" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -634,10 +631,10 @@
     <xf numFmtId="0" fontId="2" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -653,7 +650,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -662,35 +659,89 @@
     <xf numFmtId="0" fontId="2" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="17" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="19" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="20" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="21" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -698,82 +749,46 @@
     <xf numFmtId="0" fontId="6" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -791,35 +806,17 @@
     <xf numFmtId="0" fontId="9" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="18" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="17" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="18" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="17" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="20" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="20" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -828,72 +825,6 @@
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
     <mruColors>
       <color rgb="FFCC66FF"/>
       <color rgb="FFFFFF66"/>
@@ -1300,13 +1231,13 @@
       <c r="B5" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="33" t="s">
+      <c r="C5" s="35" t="s">
         <v>13</v>
       </c>
       <c r="D5" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="E5" s="33" t="s">
+      <c r="E5" s="35" t="s">
         <v>13</v>
       </c>
       <c r="F5" s="11" t="s">
@@ -1322,12 +1253,12 @@
       <c r="B6" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="34"/>
+      <c r="C6" s="37"/>
       <c r="D6" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="E6" s="34"/>
-      <c r="F6" s="33" t="s">
+      <c r="E6" s="37"/>
+      <c r="F6" s="35" t="s">
         <v>15</v>
       </c>
       <c r="G6" s="3"/>
@@ -1337,17 +1268,17 @@
       <c r="A7" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="36" t="s">
+      <c r="B7" s="33" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="38" t="s">
+      <c r="C7" s="42" t="s">
         <v>28</v>
       </c>
       <c r="D7" s="3"/>
-      <c r="E7" s="31" t="s">
+      <c r="E7" s="49" t="s">
         <v>47</v>
       </c>
-      <c r="F7" s="35"/>
+      <c r="F7" s="36"/>
       <c r="G7" s="3"/>
       <c r="H7" s="4" t="s">
         <v>10</v>
@@ -1357,15 +1288,15 @@
       <c r="A8" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="37"/>
-      <c r="C8" s="39"/>
+      <c r="B8" s="34"/>
+      <c r="C8" s="43"/>
       <c r="D8" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="E8" s="32"/>
-      <c r="F8" s="34"/>
+      <c r="E8" s="50"/>
+      <c r="F8" s="37"/>
       <c r="G8" s="3"/>
-      <c r="H8" s="40" t="s">
+      <c r="H8" s="31" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1376,30 +1307,30 @@
       <c r="B9" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="C9" s="36" t="s">
+      <c r="C9" s="33" t="s">
         <v>22</v>
       </c>
-      <c r="D9" s="36" t="s">
+      <c r="D9" s="33" t="s">
         <v>17</v>
       </c>
-      <c r="E9" s="36" t="s">
+      <c r="E9" s="33" t="s">
         <v>22</v>
       </c>
-      <c r="F9" s="38" t="s">
+      <c r="F9" s="42" t="s">
         <v>28</v>
       </c>
       <c r="G9" s="3"/>
-      <c r="H9" s="41"/>
+      <c r="H9" s="32"/>
     </row>
     <row r="10" spans="1:10" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>23</v>
       </c>
       <c r="B10" s="13"/>
-      <c r="C10" s="37"/>
-      <c r="D10" s="37"/>
-      <c r="E10" s="37"/>
-      <c r="F10" s="39"/>
+      <c r="C10" s="34"/>
+      <c r="D10" s="34"/>
+      <c r="E10" s="34"/>
+      <c r="F10" s="43"/>
       <c r="G10" s="3"/>
       <c r="H10" s="3"/>
     </row>
@@ -1407,23 +1338,23 @@
       <c r="A11" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B11" s="33" t="s">
+      <c r="B11" s="35" t="s">
         <v>25</v>
       </c>
-      <c r="C11" s="36" t="s">
+      <c r="C11" s="33" t="s">
         <v>26</v>
       </c>
-      <c r="D11" s="36" t="s">
+      <c r="D11" s="33" t="s">
         <v>27</v>
       </c>
       <c r="E11" s="3"/>
-      <c r="F11" s="36" t="s">
+      <c r="F11" s="33" t="s">
         <v>54</v>
       </c>
-      <c r="G11" s="31" t="s">
+      <c r="G11" s="49" t="s">
         <v>47</v>
       </c>
-      <c r="H11" s="40" t="s">
+      <c r="H11" s="31" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1431,22 +1362,22 @@
       <c r="A12" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="B12" s="35"/>
-      <c r="C12" s="37"/>
-      <c r="D12" s="37"/>
-      <c r="F12" s="37"/>
-      <c r="G12" s="32"/>
-      <c r="H12" s="41"/>
+      <c r="B12" s="36"/>
+      <c r="C12" s="34"/>
+      <c r="D12" s="34"/>
+      <c r="F12" s="34"/>
+      <c r="G12" s="50"/>
+      <c r="H12" s="32"/>
     </row>
     <row r="13" spans="1:10" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B13" s="34"/>
+      <c r="B13" s="37"/>
       <c r="C13" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="D13" s="46" t="s">
+      <c r="D13" s="44" t="s">
         <v>31</v>
       </c>
       <c r="E13" s="11" t="s">
@@ -1467,10 +1398,10 @@
         <v>11</v>
       </c>
       <c r="C14" s="3"/>
-      <c r="D14" s="47"/>
+      <c r="D14" s="45"/>
       <c r="E14" s="3"/>
       <c r="F14" s="3"/>
-      <c r="G14" s="42" t="s">
+      <c r="G14" s="38" t="s">
         <v>44</v>
       </c>
       <c r="H14" s="3" t="s">
@@ -1483,7 +1414,7 @@
         <v>34</v>
       </c>
       <c r="B15" s="3"/>
-      <c r="C15" s="42" t="s">
+      <c r="C15" s="38" t="s">
         <v>44</v>
       </c>
       <c r="D15" s="14" t="s">
@@ -1491,7 +1422,7 @@
       </c>
       <c r="E15" s="3"/>
       <c r="F15" s="3"/>
-      <c r="G15" s="43"/>
+      <c r="G15" s="39"/>
       <c r="H15" s="11" t="s">
         <v>11</v>
       </c>
@@ -1501,18 +1432,18 @@
         <v>35</v>
       </c>
       <c r="B16" s="3"/>
-      <c r="C16" s="43"/>
+      <c r="C16" s="39"/>
       <c r="D16" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="E16" s="38" t="s">
+      <c r="E16" s="42" t="s">
         <v>28</v>
       </c>
       <c r="F16" s="3"/>
-      <c r="G16" s="48" t="s">
+      <c r="G16" s="46" t="s">
         <v>18</v>
       </c>
-      <c r="H16" s="38" t="s">
+      <c r="H16" s="42" t="s">
         <v>28</v>
       </c>
     </row>
@@ -1525,32 +1456,32 @@
       </c>
       <c r="C17" s="3"/>
       <c r="D17" s="3"/>
-      <c r="E17" s="39"/>
+      <c r="E17" s="43"/>
       <c r="F17" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="G17" s="49"/>
-      <c r="H17" s="39"/>
+      <c r="G17" s="47"/>
+      <c r="H17" s="43"/>
     </row>
     <row r="18" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="B18" s="40" t="s">
+      <c r="B18" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="C18" s="42" t="s">
+      <c r="C18" s="38" t="s">
         <v>44</v>
       </c>
-      <c r="D18" s="44" t="s">
+      <c r="D18" s="40" t="s">
         <v>19</v>
       </c>
-      <c r="E18" s="40" t="s">
+      <c r="E18" s="31" t="s">
         <v>18</v>
       </c>
       <c r="F18" s="3"/>
-      <c r="G18" s="50"/>
-      <c r="H18" s="40" t="s">
+      <c r="G18" s="48"/>
+      <c r="H18" s="31" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1558,16 +1489,28 @@
       <c r="A19" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="B19" s="41"/>
-      <c r="C19" s="43"/>
-      <c r="D19" s="45"/>
-      <c r="E19" s="41"/>
+      <c r="B19" s="32"/>
+      <c r="C19" s="39"/>
+      <c r="D19" s="41"/>
+      <c r="E19" s="32"/>
       <c r="F19" s="3"/>
       <c r="G19" s="3"/>
-      <c r="H19" s="41"/>
+      <c r="H19" s="32"/>
     </row>
   </sheetData>
   <mergeCells count="28">
+    <mergeCell ref="G11:G12"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="F6:F8"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="E9:E10"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="F9:F10"/>
+    <mergeCell ref="E7:E8"/>
     <mergeCell ref="H8:H9"/>
     <mergeCell ref="H11:H12"/>
     <mergeCell ref="B18:B19"/>
@@ -1584,18 +1527,6 @@
     <mergeCell ref="H16:H17"/>
     <mergeCell ref="G14:G15"/>
     <mergeCell ref="G16:G18"/>
-    <mergeCell ref="G11:G12"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="E5:E6"/>
-    <mergeCell ref="F6:F8"/>
-    <mergeCell ref="C11:C12"/>
-    <mergeCell ref="D11:D12"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="D9:D10"/>
-    <mergeCell ref="E9:E10"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="F9:F10"/>
-    <mergeCell ref="E7:E8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1682,7 +1613,7 @@
       <c r="C4" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="55" t="s">
+      <c r="D4" s="53" t="s">
         <v>44</v>
       </c>
       <c r="E4" s="11" t="s">
@@ -1701,20 +1632,20 @@
       <c r="A5" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="40" t="s">
+      <c r="B5" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="33" t="s">
+      <c r="C5" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="56"/>
-      <c r="E5" s="33" t="s">
+      <c r="D5" s="54"/>
+      <c r="E5" s="35" t="s">
         <v>13</v>
       </c>
       <c r="F5" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="G5" s="48" t="s">
+      <c r="G5" s="46" t="s">
         <v>18</v>
       </c>
       <c r="H5" s="4" t="s">
@@ -1728,16 +1659,16 @@
       <c r="A6" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="41"/>
-      <c r="C6" s="34"/>
-      <c r="D6" s="52" t="s">
+      <c r="B6" s="32"/>
+      <c r="C6" s="37"/>
+      <c r="D6" s="51" t="s">
         <v>33</v>
       </c>
-      <c r="E6" s="34"/>
-      <c r="F6" s="33" t="s">
+      <c r="E6" s="37"/>
+      <c r="F6" s="35" t="s">
         <v>15</v>
       </c>
-      <c r="G6" s="49"/>
+      <c r="G6" s="47"/>
       <c r="H6" s="3"/>
       <c r="J6" t="s">
         <v>64</v>
@@ -1747,18 +1678,18 @@
       <c r="A7" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="36" t="s">
+      <c r="B7" s="33" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="52" t="s">
+      <c r="C7" s="51" t="s">
         <v>33</v>
       </c>
-      <c r="D7" s="54"/>
+      <c r="D7" s="52"/>
       <c r="E7" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="F7" s="35"/>
-      <c r="G7" s="49"/>
+      <c r="F7" s="36"/>
+      <c r="G7" s="47"/>
       <c r="H7" s="3"/>
       <c r="J7" t="s">
         <v>65</v>
@@ -1768,17 +1699,17 @@
       <c r="A8" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="37"/>
-      <c r="C8" s="54"/>
-      <c r="D8" s="38" t="s">
+      <c r="B8" s="34"/>
+      <c r="C8" s="52"/>
+      <c r="D8" s="42" t="s">
         <v>28</v>
       </c>
       <c r="E8" s="21" t="s">
         <v>52</v>
       </c>
-      <c r="F8" s="34"/>
-      <c r="G8" s="49"/>
-      <c r="H8" s="52" t="s">
+      <c r="F8" s="37"/>
+      <c r="G8" s="47"/>
+      <c r="H8" s="51" t="s">
         <v>33</v>
       </c>
     </row>
@@ -1786,53 +1717,53 @@
       <c r="A9" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B9" s="31" t="s">
+      <c r="B9" s="49" t="s">
         <v>47</v>
       </c>
-      <c r="C9" s="33" t="s">
+      <c r="C9" s="35" t="s">
         <v>50</v>
       </c>
-      <c r="D9" s="39"/>
-      <c r="E9" s="33" t="s">
+      <c r="D9" s="43"/>
+      <c r="E9" s="35" t="s">
         <v>50</v>
       </c>
       <c r="F9" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="G9" s="49"/>
-      <c r="H9" s="53"/>
+      <c r="G9" s="47"/>
+      <c r="H9" s="57"/>
     </row>
     <row r="10" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B10" s="32"/>
-      <c r="C10" s="34"/>
+      <c r="B10" s="50"/>
+      <c r="C10" s="37"/>
       <c r="D10" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="E10" s="34"/>
+      <c r="E10" s="37"/>
       <c r="F10" s="3"/>
-      <c r="G10" s="50"/>
-      <c r="H10" s="54"/>
+      <c r="G10" s="48"/>
+      <c r="H10" s="52"/>
     </row>
     <row r="11" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B11" s="33" t="s">
+      <c r="B11" s="35" t="s">
         <v>25</v>
       </c>
-      <c r="C11" s="33" t="s">
+      <c r="C11" s="35" t="s">
         <v>56</v>
       </c>
-      <c r="D11" s="33" t="s">
+      <c r="D11" s="35" t="s">
         <v>54</v>
       </c>
-      <c r="E11" s="33" t="s">
+      <c r="E11" s="35" t="s">
         <v>56</v>
       </c>
-      <c r="F11" s="57" t="s">
+      <c r="F11" s="55" t="s">
         <v>43</v>
       </c>
       <c r="G11" s="3"/>
@@ -1842,13 +1773,13 @@
       <c r="A12" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="B12" s="35"/>
-      <c r="C12" s="34"/>
-      <c r="D12" s="34"/>
-      <c r="E12" s="34"/>
-      <c r="F12" s="58"/>
+      <c r="B12" s="36"/>
+      <c r="C12" s="37"/>
+      <c r="D12" s="37"/>
+      <c r="E12" s="37"/>
+      <c r="F12" s="56"/>
       <c r="G12" s="3"/>
-      <c r="H12" s="52" t="s">
+      <c r="H12" s="51" t="s">
         <v>33</v>
       </c>
     </row>
@@ -1856,34 +1787,34 @@
       <c r="A13" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B13" s="34"/>
+      <c r="B13" s="37"/>
       <c r="C13" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="D13" s="46" t="s">
+      <c r="D13" s="44" t="s">
         <v>31</v>
       </c>
       <c r="E13" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="F13" s="51" t="s">
+      <c r="F13" s="58" t="s">
         <v>42</v>
       </c>
       <c r="G13" s="3"/>
-      <c r="H13" s="54"/>
+      <c r="H13" s="52"/>
     </row>
     <row r="14" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
         <v>32</v>
       </c>
       <c r="B14" s="3"/>
-      <c r="C14" s="38" t="s">
+      <c r="C14" s="42" t="s">
         <v>28</v>
       </c>
-      <c r="D14" s="47"/>
-      <c r="F14" s="51"/>
+      <c r="D14" s="45"/>
+      <c r="F14" s="58"/>
       <c r="G14" s="3"/>
-      <c r="H14" s="48" t="s">
+      <c r="H14" s="46" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1894,27 +1825,27 @@
       <c r="B15" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="C15" s="39"/>
+      <c r="C15" s="43"/>
       <c r="D15" s="3"/>
-      <c r="E15" s="38" t="s">
+      <c r="E15" s="42" t="s">
         <v>28</v>
       </c>
       <c r="F15" s="3"/>
       <c r="G15" s="3"/>
-      <c r="H15" s="50"/>
+      <c r="H15" s="48"/>
     </row>
     <row r="16" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="B16" s="55" t="s">
+      <c r="B16" s="53" t="s">
         <v>44</v>
       </c>
-      <c r="C16" s="55" t="s">
+      <c r="C16" s="53" t="s">
         <v>44</v>
       </c>
       <c r="D16" s="3"/>
-      <c r="E16" s="39"/>
+      <c r="E16" s="43"/>
       <c r="F16" s="11" t="s">
         <v>11</v>
       </c>
@@ -1925,19 +1856,19 @@
       <c r="A17" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="B17" s="56"/>
-      <c r="C17" s="56"/>
+      <c r="B17" s="54"/>
+      <c r="C17" s="54"/>
       <c r="D17" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="E17" s="38" t="s">
+      <c r="E17" s="42" t="s">
         <v>28</v>
       </c>
       <c r="F17" s="17" t="s">
         <v>57</v>
       </c>
       <c r="G17" s="3"/>
-      <c r="H17" s="48" t="s">
+      <c r="H17" s="46" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1948,50 +1879,36 @@
       <c r="B18" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="C18" s="52" t="s">
+      <c r="C18" s="51" t="s">
         <v>33</v>
       </c>
-      <c r="D18" s="52" t="s">
+      <c r="D18" s="51" t="s">
         <v>33</v>
       </c>
-      <c r="E18" s="39"/>
-      <c r="F18" s="48" t="s">
+      <c r="E18" s="43"/>
+      <c r="F18" s="46" t="s">
         <v>18</v>
       </c>
       <c r="G18" s="3"/>
-      <c r="H18" s="49"/>
+      <c r="H18" s="47"/>
     </row>
     <row r="19" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
         <v>38</v>
       </c>
       <c r="B19" s="3"/>
-      <c r="C19" s="54"/>
-      <c r="D19" s="54"/>
+      <c r="C19" s="52"/>
+      <c r="D19" s="52"/>
       <c r="E19" s="14" t="s">
         <v>53</v>
       </c>
-      <c r="F19" s="50"/>
+      <c r="F19" s="48"/>
       <c r="G19" s="3"/>
-      <c r="H19" s="50"/>
+      <c r="H19" s="48"/>
     </row>
   </sheetData>
   <mergeCells count="32">
-    <mergeCell ref="F18:F19"/>
-    <mergeCell ref="H17:H19"/>
-    <mergeCell ref="C18:C19"/>
-    <mergeCell ref="D13:D14"/>
-    <mergeCell ref="D18:D19"/>
-    <mergeCell ref="E15:E16"/>
-    <mergeCell ref="E17:E18"/>
-    <mergeCell ref="B16:B17"/>
-    <mergeCell ref="B11:B13"/>
-    <mergeCell ref="E11:E12"/>
-    <mergeCell ref="D11:D12"/>
-    <mergeCell ref="F11:F12"/>
-    <mergeCell ref="C11:C12"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="C16:C17"/>
+    <mergeCell ref="G5:G10"/>
     <mergeCell ref="H8:H10"/>
     <mergeCell ref="H12:H13"/>
     <mergeCell ref="H14:H15"/>
@@ -2008,7 +1925,21 @@
     <mergeCell ref="E5:E6"/>
     <mergeCell ref="F6:F8"/>
     <mergeCell ref="F13:F14"/>
-    <mergeCell ref="G5:G10"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="B11:B13"/>
+    <mergeCell ref="E11:E12"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="F11:F12"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="C16:C17"/>
+    <mergeCell ref="F18:F19"/>
+    <mergeCell ref="H17:H19"/>
+    <mergeCell ref="C18:C19"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="D18:D19"/>
+    <mergeCell ref="E15:E16"/>
+    <mergeCell ref="E17:E18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2019,8 +1950,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B17F021-0D0A-4F72-92FE-4A0D3181A797}">
   <dimension ref="A1:H19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11:G12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7:H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2063,7 +1994,9 @@
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
+      <c r="E2" s="72" t="s">
+        <v>19</v>
+      </c>
       <c r="F2" s="3"/>
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
@@ -2075,9 +2008,11 @@
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
+      <c r="E3" s="73"/>
       <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
+      <c r="G3" s="51" t="s">
+        <v>33</v>
+      </c>
       <c r="H3" s="3"/>
     </row>
     <row r="4" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -2089,13 +2024,13 @@
         <v>11</v>
       </c>
       <c r="D4" s="3"/>
-      <c r="E4" s="11" t="s">
-        <v>11</v>
+      <c r="E4" s="25" t="s">
+        <v>75</v>
       </c>
       <c r="F4" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="G4" s="3"/>
+      <c r="G4" s="52"/>
       <c r="H4" s="3"/>
     </row>
     <row r="5" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -2105,14 +2040,14 @@
       <c r="B5" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="C5" s="33" t="s">
+      <c r="C5" s="35" t="s">
         <v>13</v>
       </c>
       <c r="D5" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="33" t="s">
-        <v>13</v>
+      <c r="E5" s="18" t="s">
+        <v>74</v>
       </c>
       <c r="F5" s="11" t="s">
         <v>11</v>
@@ -2131,12 +2066,14 @@
       <c r="B6" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="34"/>
+      <c r="C6" s="37"/>
       <c r="D6" s="18" t="s">
         <v>74</v>
       </c>
-      <c r="E6" s="34"/>
-      <c r="F6" s="33" t="s">
+      <c r="E6" s="25" t="s">
+        <v>75</v>
+      </c>
+      <c r="F6" s="35" t="s">
         <v>15</v>
       </c>
       <c r="H6" s="12" t="s">
@@ -2147,7 +2084,7 @@
       <c r="A7" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="57" t="s">
+      <c r="B7" s="55" t="s">
         <v>58</v>
       </c>
       <c r="C7" s="8" t="s">
@@ -2156,14 +2093,11 @@
       <c r="D7" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="E7" s="30" t="s">
-        <v>19</v>
-      </c>
-      <c r="F7" s="35"/>
-      <c r="G7" s="61" t="s">
+      <c r="F7" s="36"/>
+      <c r="G7" s="67" t="s">
         <v>18</v>
       </c>
-      <c r="H7" s="64" t="s">
+      <c r="H7" s="61" t="s">
         <v>19</v>
       </c>
     </row>
@@ -2171,36 +2105,38 @@
       <c r="A8" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="58"/>
+      <c r="B8" s="56"/>
       <c r="C8" s="3"/>
-      <c r="D8" s="72" t="s">
+      <c r="D8" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="E8" s="73"/>
-      <c r="F8" s="34"/>
-      <c r="G8" s="62"/>
-      <c r="H8" s="65"/>
+      <c r="E8" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="F8" s="37"/>
+      <c r="G8" s="68"/>
+      <c r="H8" s="62"/>
     </row>
     <row r="9" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>21</v>
       </c>
       <c r="B9" s="3"/>
-      <c r="C9" s="33" t="s">
+      <c r="C9" s="35" t="s">
         <v>50</v>
       </c>
-      <c r="D9" s="36" t="s">
+      <c r="D9" s="33" t="s">
         <v>17</v>
       </c>
-      <c r="E9" s="66" t="s">
+      <c r="E9" s="63" t="s">
         <v>46</v>
       </c>
-      <c r="F9" s="40" t="s">
+      <c r="F9" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="G9" s="63"/>
-      <c r="H9" s="68" t="s">
-        <v>44</v>
+      <c r="G9" s="69"/>
+      <c r="H9" s="31" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -2210,33 +2146,33 @@
       <c r="B10" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="C10" s="34"/>
-      <c r="D10" s="37"/>
-      <c r="E10" s="67"/>
-      <c r="F10" s="41"/>
+      <c r="C10" s="37"/>
+      <c r="D10" s="34"/>
+      <c r="E10" s="64"/>
+      <c r="F10" s="32"/>
       <c r="G10" s="3"/>
-      <c r="H10" s="69"/>
+      <c r="H10" s="32"/>
     </row>
     <row r="11" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B11" s="33" t="s">
+      <c r="B11" s="35" t="s">
         <v>25</v>
       </c>
-      <c r="C11" s="33" t="s">
+      <c r="C11" s="35" t="s">
         <v>56</v>
       </c>
-      <c r="D11" s="33" t="s">
+      <c r="D11" s="35" t="s">
         <v>54</v>
       </c>
-      <c r="E11" s="66" t="s">
+      <c r="E11" s="63" t="s">
         <v>45</v>
       </c>
-      <c r="F11" s="66" t="s">
+      <c r="F11" s="63" t="s">
         <v>55</v>
       </c>
-      <c r="G11" s="40" t="s">
+      <c r="G11" s="31" t="s">
         <v>18</v>
       </c>
       <c r="H11" s="3"/>
@@ -2245,13 +2181,13 @@
       <c r="A12" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="B12" s="35"/>
-      <c r="C12" s="34"/>
-      <c r="D12" s="34"/>
-      <c r="E12" s="67"/>
-      <c r="F12" s="67"/>
-      <c r="G12" s="41"/>
-      <c r="H12" s="52" t="s">
+      <c r="B12" s="36"/>
+      <c r="C12" s="37"/>
+      <c r="D12" s="37"/>
+      <c r="E12" s="64"/>
+      <c r="F12" s="64"/>
+      <c r="G12" s="32"/>
+      <c r="H12" s="51" t="s">
         <v>33</v>
       </c>
     </row>
@@ -2259,45 +2195,44 @@
       <c r="A13" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B13" s="34"/>
-      <c r="C13" s="38" t="s">
+      <c r="B13" s="37"/>
+      <c r="C13" s="42" t="s">
         <v>28</v>
       </c>
-      <c r="D13" s="46" t="s">
+      <c r="D13" s="44" t="s">
         <v>31</v>
-      </c>
-      <c r="E13" s="38" t="s">
-        <v>28</v>
       </c>
       <c r="F13" s="8" t="s">
         <v>42</v>
       </c>
       <c r="G13" s="3"/>
-      <c r="H13" s="54"/>
+      <c r="H13" s="52"/>
     </row>
     <row r="14" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B14" s="59" t="s">
+      <c r="B14" s="65" t="s">
         <v>42</v>
       </c>
-      <c r="C14" s="39"/>
-      <c r="D14" s="47"/>
-      <c r="E14" s="39"/>
+      <c r="C14" s="43"/>
+      <c r="D14" s="45"/>
+      <c r="E14" s="22" t="s">
+        <v>28</v>
+      </c>
       <c r="F14" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="G14" s="64" t="s">
+      <c r="G14" s="3"/>
+      <c r="H14" s="61" t="s">
         <v>19</v>
       </c>
-      <c r="H14" s="3"/>
     </row>
     <row r="15" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="B15" s="60"/>
+      <c r="B15" s="66"/>
       <c r="C15" s="9" t="s">
         <v>48</v>
       </c>
@@ -2307,8 +2242,7 @@
       <c r="E15" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="G15" s="65"/>
-      <c r="H15" s="3"/>
+      <c r="H15" s="62"/>
     </row>
     <row r="16" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
@@ -2323,10 +2257,10 @@
       <c r="E16" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="F16" s="40" t="s">
+      <c r="F16" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="G16" s="68" t="s">
+      <c r="G16" s="59" t="s">
         <v>44</v>
       </c>
       <c r="H16" s="3"/>
@@ -2344,13 +2278,11 @@
       <c r="D17" s="30" t="s">
         <v>19</v>
       </c>
-      <c r="E17" s="12" t="s">
-        <v>49</v>
-      </c>
-      <c r="F17" s="41"/>
-      <c r="G17" s="69"/>
-      <c r="H17" s="38" t="s">
-        <v>28</v>
+      <c r="E17" s="3"/>
+      <c r="F17" s="32"/>
+      <c r="G17" s="60"/>
+      <c r="H17" s="61" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -2369,13 +2301,13 @@
       <c r="E18" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="F18" s="40" t="s">
+      <c r="F18" s="31" t="s">
         <v>18</v>
       </c>
       <c r="G18" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="H18" s="39"/>
+      <c r="H18" s="62"/>
     </row>
     <row r="19" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
@@ -2389,30 +2321,12 @@
       </c>
       <c r="D19" s="3"/>
       <c r="E19" s="3"/>
-      <c r="F19" s="41"/>
+      <c r="F19" s="32"/>
       <c r="G19" s="3"/>
       <c r="H19" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="H12:H13"/>
-    <mergeCell ref="H17:H18"/>
-    <mergeCell ref="F16:F17"/>
-    <mergeCell ref="D13:D14"/>
-    <mergeCell ref="E13:E14"/>
-    <mergeCell ref="G16:G17"/>
-    <mergeCell ref="G14:G15"/>
-    <mergeCell ref="E11:E12"/>
-    <mergeCell ref="F11:F12"/>
-    <mergeCell ref="F18:F19"/>
-    <mergeCell ref="H7:H8"/>
-    <mergeCell ref="E9:E10"/>
-    <mergeCell ref="D9:D10"/>
-    <mergeCell ref="H9:H10"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="E5:E6"/>
-    <mergeCell ref="F6:F8"/>
-    <mergeCell ref="C9:C10"/>
     <mergeCell ref="B14:B15"/>
     <mergeCell ref="D11:D12"/>
     <mergeCell ref="G7:G9"/>
@@ -2422,6 +2336,24 @@
     <mergeCell ref="G11:G12"/>
     <mergeCell ref="C13:C14"/>
     <mergeCell ref="B11:B13"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="G3:G4"/>
+    <mergeCell ref="H7:H8"/>
+    <mergeCell ref="E9:E10"/>
+    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="H9:H10"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="F6:F8"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="H12:H13"/>
+    <mergeCell ref="H17:H18"/>
+    <mergeCell ref="F16:F17"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="G16:G17"/>
+    <mergeCell ref="H14:H15"/>
+    <mergeCell ref="E11:E12"/>
+    <mergeCell ref="F11:F12"/>
+    <mergeCell ref="F18:F19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2500,7 +2432,7 @@
       <c r="C4" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="38" t="s">
+      <c r="D4" s="42" t="s">
         <v>28</v>
       </c>
       <c r="E4" s="11" t="s">
@@ -2519,11 +2451,11 @@
       <c r="B5" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="C5" s="33" t="s">
+      <c r="C5" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="39"/>
-      <c r="E5" s="33" t="s">
+      <c r="D5" s="43"/>
+      <c r="E5" s="35" t="s">
         <v>13</v>
       </c>
       <c r="F5" s="11" t="s">
@@ -2532,7 +2464,7 @@
       <c r="G5" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="H5" s="38" t="s">
+      <c r="H5" s="42" t="s">
         <v>28</v>
       </c>
     </row>
@@ -2543,33 +2475,33 @@
       <c r="B6" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="34"/>
-      <c r="D6" s="64" t="s">
+      <c r="C6" s="37"/>
+      <c r="D6" s="61" t="s">
         <v>19</v>
       </c>
-      <c r="E6" s="34"/>
-      <c r="F6" s="33" t="s">
+      <c r="E6" s="37"/>
+      <c r="F6" s="35" t="s">
         <v>15</v>
       </c>
       <c r="G6" s="3"/>
-      <c r="H6" s="39"/>
+      <c r="H6" s="43"/>
     </row>
     <row r="7" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="36" t="s">
+      <c r="B7" s="33" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="68" t="s">
+      <c r="C7" s="59" t="s">
         <v>44</v>
       </c>
-      <c r="D7" s="65"/>
+      <c r="D7" s="62"/>
       <c r="E7" s="23" t="s">
         <v>66</v>
       </c>
-      <c r="F7" s="35"/>
-      <c r="G7" s="48" t="s">
+      <c r="F7" s="36"/>
+      <c r="G7" s="46" t="s">
         <v>18</v>
       </c>
       <c r="H7" s="4" t="s">
@@ -2580,14 +2512,14 @@
       <c r="A8" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="37"/>
-      <c r="C8" s="69"/>
+      <c r="B8" s="34"/>
+      <c r="C8" s="60"/>
       <c r="D8" s="11" t="s">
         <v>11</v>
       </c>
       <c r="E8" s="3"/>
-      <c r="F8" s="34"/>
-      <c r="G8" s="49"/>
+      <c r="F8" s="37"/>
+      <c r="G8" s="47"/>
       <c r="H8" s="3"/>
     </row>
     <row r="9" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -2597,19 +2529,19 @@
       <c r="B9" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="C9" s="36" t="s">
+      <c r="C9" s="33" t="s">
         <v>22</v>
       </c>
-      <c r="D9" s="36" t="s">
+      <c r="D9" s="33" t="s">
         <v>17</v>
       </c>
-      <c r="E9" s="36" t="s">
+      <c r="E9" s="33" t="s">
         <v>22</v>
       </c>
       <c r="F9" s="24" t="s">
         <v>68</v>
       </c>
-      <c r="G9" s="50"/>
+      <c r="G9" s="48"/>
       <c r="H9" s="70" t="s">
         <v>68</v>
       </c>
@@ -2619,9 +2551,9 @@
         <v>23</v>
       </c>
       <c r="B10" s="3"/>
-      <c r="C10" s="37"/>
-      <c r="D10" s="37"/>
-      <c r="E10" s="37"/>
+      <c r="C10" s="34"/>
+      <c r="D10" s="34"/>
+      <c r="E10" s="34"/>
       <c r="F10" s="26" t="s">
         <v>72</v>
       </c>
@@ -2632,19 +2564,19 @@
       <c r="A11" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B11" s="33" t="s">
+      <c r="B11" s="35" t="s">
         <v>70</v>
       </c>
-      <c r="C11" s="36" t="s">
+      <c r="C11" s="33" t="s">
         <v>26</v>
       </c>
-      <c r="D11" s="36" t="s">
+      <c r="D11" s="33" t="s">
         <v>27</v>
       </c>
-      <c r="E11" s="36" t="s">
+      <c r="E11" s="33" t="s">
         <v>26</v>
       </c>
-      <c r="F11" s="36" t="s">
+      <c r="F11" s="33" t="s">
         <v>27</v>
       </c>
       <c r="G11" s="3"/>
@@ -2654,13 +2586,13 @@
       <c r="A12" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="B12" s="35"/>
-      <c r="C12" s="37"/>
-      <c r="D12" s="37"/>
-      <c r="E12" s="37"/>
-      <c r="F12" s="37"/>
+      <c r="B12" s="36"/>
+      <c r="C12" s="34"/>
+      <c r="D12" s="34"/>
+      <c r="E12" s="34"/>
+      <c r="F12" s="34"/>
       <c r="G12" s="3"/>
-      <c r="H12" s="48" t="s">
+      <c r="H12" s="46" t="s">
         <v>18</v>
       </c>
     </row>
@@ -2668,14 +2600,14 @@
       <c r="A13" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B13" s="34"/>
+      <c r="B13" s="37"/>
       <c r="C13" s="23" t="s">
         <v>66</v>
       </c>
       <c r="D13" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="E13" s="38" t="s">
+      <c r="E13" s="42" t="s">
         <v>28</v>
       </c>
       <c r="F13" s="8" t="s">
@@ -2684,7 +2616,7 @@
       <c r="G13" s="26" t="s">
         <v>72</v>
       </c>
-      <c r="H13" s="49"/>
+      <c r="H13" s="47"/>
     </row>
     <row r="14" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
@@ -2699,11 +2631,11 @@
       <c r="D14" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="E14" s="39"/>
+      <c r="E14" s="43"/>
       <c r="F14" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="G14" s="64" t="s">
+      <c r="G14" s="61" t="s">
         <v>19</v>
       </c>
       <c r="H14" s="3"/>
@@ -2723,7 +2655,7 @@
         <v>48</v>
       </c>
       <c r="F15" s="3"/>
-      <c r="G15" s="65"/>
+      <c r="G15" s="62"/>
       <c r="H15" s="3"/>
     </row>
     <row r="16" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -2736,13 +2668,13 @@
       <c r="C16" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="D16" s="48" t="s">
+      <c r="D16" s="46" t="s">
         <v>18</v>
       </c>
       <c r="E16" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="F16" s="48" t="s">
+      <c r="F16" s="46" t="s">
         <v>18</v>
       </c>
       <c r="G16" s="3"/>
@@ -2760,13 +2692,13 @@
       <c r="C17" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="D17" s="49"/>
+      <c r="D17" s="47"/>
       <c r="E17" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="F17" s="49"/>
+      <c r="F17" s="47"/>
       <c r="G17" s="3"/>
-      <c r="H17" s="68" t="s">
+      <c r="H17" s="59" t="s">
         <v>44</v>
       </c>
     </row>
@@ -2777,27 +2709,27 @@
       <c r="B18" s="25" t="s">
         <v>67</v>
       </c>
-      <c r="C18" s="48" t="s">
+      <c r="C18" s="46" t="s">
         <v>18</v>
       </c>
       <c r="D18" s="24" t="s">
         <v>68</v>
       </c>
-      <c r="E18" s="64" t="s">
+      <c r="E18" s="61" t="s">
         <v>19</v>
       </c>
       <c r="F18" s="3"/>
       <c r="G18" s="3"/>
-      <c r="H18" s="69"/>
+      <c r="H18" s="60"/>
     </row>
     <row r="19" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
         <v>38</v>
       </c>
       <c r="B19" s="3"/>
-      <c r="C19" s="50"/>
+      <c r="C19" s="48"/>
       <c r="D19" s="3"/>
-      <c r="E19" s="65"/>
+      <c r="E19" s="62"/>
       <c r="F19" s="3"/>
       <c r="G19" s="3"/>
       <c r="H19" s="3"/>
@@ -2805,16 +2737,6 @@
     <row r="20" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="H5:H6"/>
-    <mergeCell ref="H12:H13"/>
-    <mergeCell ref="H17:H18"/>
-    <mergeCell ref="D16:D17"/>
-    <mergeCell ref="F16:F17"/>
-    <mergeCell ref="D6:D7"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="G14:G15"/>
-    <mergeCell ref="G7:G9"/>
-    <mergeCell ref="H9:H10"/>
     <mergeCell ref="C18:C19"/>
     <mergeCell ref="C5:C6"/>
     <mergeCell ref="E5:E6"/>
@@ -2831,6 +2753,16 @@
     <mergeCell ref="F11:F12"/>
     <mergeCell ref="E13:E14"/>
     <mergeCell ref="E18:E19"/>
+    <mergeCell ref="H5:H6"/>
+    <mergeCell ref="H12:H13"/>
+    <mergeCell ref="H17:H18"/>
+    <mergeCell ref="D16:D17"/>
+    <mergeCell ref="F16:F17"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="G14:G15"/>
+    <mergeCell ref="G7:G9"/>
+    <mergeCell ref="H9:H10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>

</xml_diff>

<commit_message>
Ajuste horas estudio Info II semana 4
</commit_message>
<xml_diff>
--- a/Programar_dias.xlsx
+++ b/Programar_dias.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Estudio\OneDrive - Universidad de Antioquia\Estudio\Materias\Informatica II\Calendario_semanal\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://udeaeduco-my.sharepoint.com/personal/santiago_vargas5_udea_edu_co/Documents/Estudio/Materias/Informatica II/Calendario_semanal/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F164586-5EB2-4C6F-98F4-8BD2C9D2F3F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="8" documentId="13_ncr:1_{227E79E7-125C-48EA-A75C-9FF21A2F4D4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C2DC93DA-B6C6-42D1-8E7D-63F522AAAA32}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="2" xr2:uid="{CC961CB2-F623-4B13-8239-4B70F16E4462}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="3" xr2:uid="{CC961CB2-F623-4B13-8239-4B70F16E4462}"/>
   </bookViews>
   <sheets>
     <sheet name="Semana 1" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="76">
   <si>
     <t>LUNES</t>
   </si>
@@ -322,7 +322,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -382,14 +382,6 @@
     </font>
     <font>
       <sz val="9"/>
-      <color theme="1"/>
-      <name val="Yu Gothic UI"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <i/>
-      <sz val="11"/>
       <color theme="1"/>
       <name val="Yu Gothic UI"/>
       <family val="2"/>
@@ -601,7 +593,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="74">
+  <cellXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -677,7 +669,7 @@
     <xf numFmtId="0" fontId="1" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -689,27 +681,39 @@
     <xf numFmtId="0" fontId="1" fillId="20" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -722,12 +726,6 @@
     <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -743,15 +741,12 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -767,55 +762,43 @@
     <xf numFmtId="0" fontId="4" fillId="13" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="20" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="20" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="17" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="17" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="20" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="20" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1231,13 +1214,13 @@
       <c r="B5" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="35" t="s">
+      <c r="C5" s="33" t="s">
         <v>13</v>
       </c>
       <c r="D5" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="E5" s="35" t="s">
+      <c r="E5" s="33" t="s">
         <v>13</v>
       </c>
       <c r="F5" s="11" t="s">
@@ -1253,12 +1236,12 @@
       <c r="B6" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="37"/>
+      <c r="C6" s="34"/>
       <c r="D6" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="E6" s="37"/>
-      <c r="F6" s="35" t="s">
+      <c r="E6" s="34"/>
+      <c r="F6" s="33" t="s">
         <v>15</v>
       </c>
       <c r="G6" s="3"/>
@@ -1268,17 +1251,17 @@
       <c r="A7" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="33" t="s">
+      <c r="B7" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="42" t="s">
+      <c r="C7" s="38" t="s">
         <v>28</v>
       </c>
       <c r="D7" s="3"/>
-      <c r="E7" s="49" t="s">
+      <c r="E7" s="31" t="s">
         <v>47</v>
       </c>
-      <c r="F7" s="36"/>
+      <c r="F7" s="35"/>
       <c r="G7" s="3"/>
       <c r="H7" s="4" t="s">
         <v>10</v>
@@ -1288,15 +1271,15 @@
       <c r="A8" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="34"/>
-      <c r="C8" s="43"/>
+      <c r="B8" s="37"/>
+      <c r="C8" s="39"/>
       <c r="D8" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="E8" s="50"/>
-      <c r="F8" s="37"/>
+      <c r="E8" s="32"/>
+      <c r="F8" s="34"/>
       <c r="G8" s="3"/>
-      <c r="H8" s="31" t="s">
+      <c r="H8" s="40" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1307,30 +1290,30 @@
       <c r="B9" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="C9" s="33" t="s">
+      <c r="C9" s="36" t="s">
         <v>22</v>
       </c>
-      <c r="D9" s="33" t="s">
+      <c r="D9" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="E9" s="33" t="s">
+      <c r="E9" s="36" t="s">
         <v>22</v>
       </c>
-      <c r="F9" s="42" t="s">
+      <c r="F9" s="38" t="s">
         <v>28</v>
       </c>
       <c r="G9" s="3"/>
-      <c r="H9" s="32"/>
+      <c r="H9" s="41"/>
     </row>
     <row r="10" spans="1:10" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>23</v>
       </c>
       <c r="B10" s="13"/>
-      <c r="C10" s="34"/>
-      <c r="D10" s="34"/>
-      <c r="E10" s="34"/>
-      <c r="F10" s="43"/>
+      <c r="C10" s="37"/>
+      <c r="D10" s="37"/>
+      <c r="E10" s="37"/>
+      <c r="F10" s="39"/>
       <c r="G10" s="3"/>
       <c r="H10" s="3"/>
     </row>
@@ -1338,23 +1321,23 @@
       <c r="A11" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B11" s="35" t="s">
+      <c r="B11" s="33" t="s">
         <v>25</v>
       </c>
-      <c r="C11" s="33" t="s">
+      <c r="C11" s="36" t="s">
         <v>26</v>
       </c>
-      <c r="D11" s="33" t="s">
+      <c r="D11" s="36" t="s">
         <v>27</v>
       </c>
       <c r="E11" s="3"/>
-      <c r="F11" s="33" t="s">
+      <c r="F11" s="36" t="s">
         <v>54</v>
       </c>
-      <c r="G11" s="49" t="s">
+      <c r="G11" s="31" t="s">
         <v>47</v>
       </c>
-      <c r="H11" s="31" t="s">
+      <c r="H11" s="40" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1362,22 +1345,22 @@
       <c r="A12" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="B12" s="36"/>
-      <c r="C12" s="34"/>
-      <c r="D12" s="34"/>
-      <c r="F12" s="34"/>
-      <c r="G12" s="50"/>
-      <c r="H12" s="32"/>
+      <c r="B12" s="35"/>
+      <c r="C12" s="37"/>
+      <c r="D12" s="37"/>
+      <c r="F12" s="37"/>
+      <c r="G12" s="32"/>
+      <c r="H12" s="41"/>
     </row>
     <row r="13" spans="1:10" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B13" s="37"/>
+      <c r="B13" s="34"/>
       <c r="C13" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="D13" s="44" t="s">
+      <c r="D13" s="46" t="s">
         <v>31</v>
       </c>
       <c r="E13" s="11" t="s">
@@ -1398,10 +1381,10 @@
         <v>11</v>
       </c>
       <c r="C14" s="3"/>
-      <c r="D14" s="45"/>
+      <c r="D14" s="47"/>
       <c r="E14" s="3"/>
       <c r="F14" s="3"/>
-      <c r="G14" s="38" t="s">
+      <c r="G14" s="42" t="s">
         <v>44</v>
       </c>
       <c r="H14" s="3" t="s">
@@ -1414,7 +1397,7 @@
         <v>34</v>
       </c>
       <c r="B15" s="3"/>
-      <c r="C15" s="38" t="s">
+      <c r="C15" s="42" t="s">
         <v>44</v>
       </c>
       <c r="D15" s="14" t="s">
@@ -1422,7 +1405,7 @@
       </c>
       <c r="E15" s="3"/>
       <c r="F15" s="3"/>
-      <c r="G15" s="39"/>
+      <c r="G15" s="43"/>
       <c r="H15" s="11" t="s">
         <v>11</v>
       </c>
@@ -1432,18 +1415,18 @@
         <v>35</v>
       </c>
       <c r="B16" s="3"/>
-      <c r="C16" s="39"/>
+      <c r="C16" s="43"/>
       <c r="D16" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="E16" s="42" t="s">
+      <c r="E16" s="38" t="s">
         <v>28</v>
       </c>
       <c r="F16" s="3"/>
-      <c r="G16" s="46" t="s">
+      <c r="G16" s="48" t="s">
         <v>18</v>
       </c>
-      <c r="H16" s="42" t="s">
+      <c r="H16" s="38" t="s">
         <v>28</v>
       </c>
     </row>
@@ -1456,32 +1439,32 @@
       </c>
       <c r="C17" s="3"/>
       <c r="D17" s="3"/>
-      <c r="E17" s="43"/>
+      <c r="E17" s="39"/>
       <c r="F17" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="G17" s="47"/>
-      <c r="H17" s="43"/>
+      <c r="G17" s="49"/>
+      <c r="H17" s="39"/>
     </row>
     <row r="18" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="B18" s="31" t="s">
+      <c r="B18" s="40" t="s">
         <v>18</v>
       </c>
-      <c r="C18" s="38" t="s">
+      <c r="C18" s="42" t="s">
         <v>44</v>
       </c>
-      <c r="D18" s="40" t="s">
+      <c r="D18" s="44" t="s">
         <v>19</v>
       </c>
-      <c r="E18" s="31" t="s">
+      <c r="E18" s="40" t="s">
         <v>18</v>
       </c>
       <c r="F18" s="3"/>
-      <c r="G18" s="48"/>
-      <c r="H18" s="31" t="s">
+      <c r="G18" s="50"/>
+      <c r="H18" s="40" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1489,28 +1472,16 @@
       <c r="A19" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="B19" s="32"/>
-      <c r="C19" s="39"/>
-      <c r="D19" s="41"/>
-      <c r="E19" s="32"/>
+      <c r="B19" s="41"/>
+      <c r="C19" s="43"/>
+      <c r="D19" s="45"/>
+      <c r="E19" s="41"/>
       <c r="F19" s="3"/>
       <c r="G19" s="3"/>
-      <c r="H19" s="32"/>
+      <c r="H19" s="41"/>
     </row>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="G11:G12"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="E5:E6"/>
-    <mergeCell ref="F6:F8"/>
-    <mergeCell ref="C11:C12"/>
-    <mergeCell ref="D11:D12"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="D9:D10"/>
-    <mergeCell ref="E9:E10"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="F9:F10"/>
-    <mergeCell ref="E7:E8"/>
     <mergeCell ref="H8:H9"/>
     <mergeCell ref="H11:H12"/>
     <mergeCell ref="B18:B19"/>
@@ -1527,6 +1498,18 @@
     <mergeCell ref="H16:H17"/>
     <mergeCell ref="G14:G15"/>
     <mergeCell ref="G16:G18"/>
+    <mergeCell ref="G11:G12"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="F6:F8"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="E9:E10"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="F9:F10"/>
+    <mergeCell ref="E7:E8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1613,7 +1596,7 @@
       <c r="C4" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="53" t="s">
+      <c r="D4" s="54" t="s">
         <v>44</v>
       </c>
       <c r="E4" s="11" t="s">
@@ -1632,20 +1615,20 @@
       <c r="A5" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="31" t="s">
+      <c r="B5" s="40" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="35" t="s">
+      <c r="C5" s="33" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="54"/>
-      <c r="E5" s="35" t="s">
+      <c r="D5" s="55"/>
+      <c r="E5" s="33" t="s">
         <v>13</v>
       </c>
       <c r="F5" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="G5" s="46" t="s">
+      <c r="G5" s="48" t="s">
         <v>18</v>
       </c>
       <c r="H5" s="4" t="s">
@@ -1659,16 +1642,16 @@
       <c r="A6" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="32"/>
-      <c r="C6" s="37"/>
+      <c r="B6" s="41"/>
+      <c r="C6" s="34"/>
       <c r="D6" s="51" t="s">
         <v>33</v>
       </c>
-      <c r="E6" s="37"/>
-      <c r="F6" s="35" t="s">
+      <c r="E6" s="34"/>
+      <c r="F6" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="G6" s="47"/>
+      <c r="G6" s="49"/>
       <c r="H6" s="3"/>
       <c r="J6" t="s">
         <v>64</v>
@@ -1678,18 +1661,18 @@
       <c r="A7" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="33" t="s">
+      <c r="B7" s="36" t="s">
         <v>17</v>
       </c>
       <c r="C7" s="51" t="s">
         <v>33</v>
       </c>
-      <c r="D7" s="52"/>
+      <c r="D7" s="53"/>
       <c r="E7" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="F7" s="36"/>
-      <c r="G7" s="47"/>
+      <c r="F7" s="35"/>
+      <c r="G7" s="49"/>
       <c r="H7" s="3"/>
       <c r="J7" t="s">
         <v>65</v>
@@ -1699,16 +1682,16 @@
       <c r="A8" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="34"/>
-      <c r="C8" s="52"/>
-      <c r="D8" s="42" t="s">
+      <c r="B8" s="37"/>
+      <c r="C8" s="53"/>
+      <c r="D8" s="38" t="s">
         <v>28</v>
       </c>
       <c r="E8" s="21" t="s">
         <v>52</v>
       </c>
-      <c r="F8" s="37"/>
-      <c r="G8" s="47"/>
+      <c r="F8" s="34"/>
+      <c r="G8" s="49"/>
       <c r="H8" s="51" t="s">
         <v>33</v>
       </c>
@@ -1717,53 +1700,53 @@
       <c r="A9" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B9" s="49" t="s">
+      <c r="B9" s="31" t="s">
         <v>47</v>
       </c>
-      <c r="C9" s="35" t="s">
+      <c r="C9" s="33" t="s">
         <v>50</v>
       </c>
-      <c r="D9" s="43"/>
-      <c r="E9" s="35" t="s">
+      <c r="D9" s="39"/>
+      <c r="E9" s="33" t="s">
         <v>50</v>
       </c>
       <c r="F9" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="G9" s="47"/>
-      <c r="H9" s="57"/>
+      <c r="G9" s="49"/>
+      <c r="H9" s="52"/>
     </row>
     <row r="10" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B10" s="50"/>
-      <c r="C10" s="37"/>
+      <c r="B10" s="32"/>
+      <c r="C10" s="34"/>
       <c r="D10" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="E10" s="37"/>
+      <c r="E10" s="34"/>
       <c r="F10" s="3"/>
-      <c r="G10" s="48"/>
-      <c r="H10" s="52"/>
+      <c r="G10" s="50"/>
+      <c r="H10" s="53"/>
     </row>
     <row r="11" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B11" s="35" t="s">
+      <c r="B11" s="33" t="s">
         <v>25</v>
       </c>
-      <c r="C11" s="35" t="s">
+      <c r="C11" s="33" t="s">
         <v>56</v>
       </c>
-      <c r="D11" s="35" t="s">
+      <c r="D11" s="33" t="s">
         <v>54</v>
       </c>
-      <c r="E11" s="35" t="s">
+      <c r="E11" s="33" t="s">
         <v>56</v>
       </c>
-      <c r="F11" s="55" t="s">
+      <c r="F11" s="56" t="s">
         <v>43</v>
       </c>
       <c r="G11" s="3"/>
@@ -1773,11 +1756,11 @@
       <c r="A12" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="B12" s="36"/>
-      <c r="C12" s="37"/>
-      <c r="D12" s="37"/>
-      <c r="E12" s="37"/>
-      <c r="F12" s="56"/>
+      <c r="B12" s="35"/>
+      <c r="C12" s="34"/>
+      <c r="D12" s="34"/>
+      <c r="E12" s="34"/>
+      <c r="F12" s="57"/>
       <c r="G12" s="3"/>
       <c r="H12" s="51" t="s">
         <v>33</v>
@@ -1787,11 +1770,11 @@
       <c r="A13" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B13" s="37"/>
+      <c r="B13" s="34"/>
       <c r="C13" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="D13" s="44" t="s">
+      <c r="D13" s="46" t="s">
         <v>31</v>
       </c>
       <c r="E13" s="28" t="s">
@@ -1801,20 +1784,20 @@
         <v>42</v>
       </c>
       <c r="G13" s="3"/>
-      <c r="H13" s="52"/>
+      <c r="H13" s="53"/>
     </row>
     <row r="14" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
         <v>32</v>
       </c>
       <c r="B14" s="3"/>
-      <c r="C14" s="42" t="s">
+      <c r="C14" s="38" t="s">
         <v>28</v>
       </c>
-      <c r="D14" s="45"/>
+      <c r="D14" s="47"/>
       <c r="F14" s="58"/>
       <c r="G14" s="3"/>
-      <c r="H14" s="46" t="s">
+      <c r="H14" s="48" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1825,27 +1808,27 @@
       <c r="B15" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="C15" s="43"/>
+      <c r="C15" s="39"/>
       <c r="D15" s="3"/>
-      <c r="E15" s="42" t="s">
+      <c r="E15" s="38" t="s">
         <v>28</v>
       </c>
       <c r="F15" s="3"/>
       <c r="G15" s="3"/>
-      <c r="H15" s="48"/>
+      <c r="H15" s="50"/>
     </row>
     <row r="16" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="B16" s="53" t="s">
+      <c r="B16" s="54" t="s">
         <v>44</v>
       </c>
-      <c r="C16" s="53" t="s">
+      <c r="C16" s="54" t="s">
         <v>44</v>
       </c>
       <c r="D16" s="3"/>
-      <c r="E16" s="43"/>
+      <c r="E16" s="39"/>
       <c r="F16" s="11" t="s">
         <v>11</v>
       </c>
@@ -1856,19 +1839,19 @@
       <c r="A17" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="B17" s="54"/>
-      <c r="C17" s="54"/>
+      <c r="B17" s="55"/>
+      <c r="C17" s="55"/>
       <c r="D17" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="E17" s="42" t="s">
+      <c r="E17" s="38" t="s">
         <v>28</v>
       </c>
       <c r="F17" s="17" t="s">
         <v>57</v>
       </c>
       <c r="G17" s="3"/>
-      <c r="H17" s="46" t="s">
+      <c r="H17" s="48" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1885,29 +1868,45 @@
       <c r="D18" s="51" t="s">
         <v>33</v>
       </c>
-      <c r="E18" s="43"/>
-      <c r="F18" s="46" t="s">
+      <c r="E18" s="39"/>
+      <c r="F18" s="48" t="s">
         <v>18</v>
       </c>
       <c r="G18" s="3"/>
-      <c r="H18" s="47"/>
+      <c r="H18" s="49"/>
     </row>
     <row r="19" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
         <v>38</v>
       </c>
       <c r="B19" s="3"/>
-      <c r="C19" s="52"/>
-      <c r="D19" s="52"/>
+      <c r="C19" s="53"/>
+      <c r="D19" s="53"/>
       <c r="E19" s="14" t="s">
         <v>53</v>
       </c>
-      <c r="F19" s="48"/>
+      <c r="F19" s="50"/>
       <c r="G19" s="3"/>
-      <c r="H19" s="48"/>
+      <c r="H19" s="50"/>
     </row>
   </sheetData>
   <mergeCells count="32">
+    <mergeCell ref="F18:F19"/>
+    <mergeCell ref="H17:H19"/>
+    <mergeCell ref="C18:C19"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="D18:D19"/>
+    <mergeCell ref="E15:E16"/>
+    <mergeCell ref="E17:E18"/>
+    <mergeCell ref="F13:F14"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="B11:B13"/>
+    <mergeCell ref="E11:E12"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="F11:F12"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="C16:C17"/>
     <mergeCell ref="G5:G10"/>
     <mergeCell ref="H8:H10"/>
     <mergeCell ref="H12:H13"/>
@@ -1924,22 +1923,6 @@
     <mergeCell ref="C5:C6"/>
     <mergeCell ref="E5:E6"/>
     <mergeCell ref="F6:F8"/>
-    <mergeCell ref="F13:F14"/>
-    <mergeCell ref="B16:B17"/>
-    <mergeCell ref="B11:B13"/>
-    <mergeCell ref="E11:E12"/>
-    <mergeCell ref="D11:D12"/>
-    <mergeCell ref="F11:F12"/>
-    <mergeCell ref="C11:C12"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="C16:C17"/>
-    <mergeCell ref="F18:F19"/>
-    <mergeCell ref="H17:H19"/>
-    <mergeCell ref="C18:C19"/>
-    <mergeCell ref="D13:D14"/>
-    <mergeCell ref="D18:D19"/>
-    <mergeCell ref="E15:E16"/>
-    <mergeCell ref="E17:E18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1950,8 +1933,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B17F021-0D0A-4F72-92FE-4A0D3181A797}">
   <dimension ref="A1:H19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7:H8"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="H17" sqref="H17:H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1994,7 +1977,7 @@
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
-      <c r="E2" s="72" t="s">
+      <c r="E2" s="61" t="s">
         <v>19</v>
       </c>
       <c r="F2" s="3"/>
@@ -2008,11 +1991,9 @@
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
-      <c r="E3" s="73"/>
+      <c r="E3" s="62"/>
       <c r="F3" s="3"/>
-      <c r="G3" s="51" t="s">
-        <v>33</v>
-      </c>
+      <c r="G3" s="3"/>
       <c r="H3" s="3"/>
     </row>
     <row r="4" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -2030,8 +2011,10 @@
       <c r="F4" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="G4" s="52"/>
-      <c r="H4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="12" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="5" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
@@ -2040,7 +2023,7 @@
       <c r="B5" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="C5" s="35" t="s">
+      <c r="C5" s="33" t="s">
         <v>13</v>
       </c>
       <c r="D5" s="11" t="s">
@@ -2052,12 +2035,8 @@
       <c r="F5" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="G5" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="H5" s="4" t="s">
-        <v>10</v>
-      </c>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
     </row>
     <row r="6" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
@@ -2066,25 +2045,24 @@
       <c r="B6" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="37"/>
+      <c r="C6" s="34"/>
       <c r="D6" s="18" t="s">
         <v>74</v>
       </c>
       <c r="E6" s="25" t="s">
         <v>75</v>
       </c>
-      <c r="F6" s="35" t="s">
+      <c r="F6" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="H6" s="12" t="s">
-        <v>49</v>
-      </c>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
     </row>
     <row r="7" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="55" t="s">
+      <c r="B7" s="56" t="s">
         <v>58</v>
       </c>
       <c r="C7" s="8" t="s">
@@ -2093,19 +2071,17 @@
       <c r="D7" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="F7" s="36"/>
-      <c r="G7" s="67" t="s">
+      <c r="F7" s="35"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="40" t="s">
         <v>18</v>
-      </c>
-      <c r="H7" s="61" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="56"/>
+      <c r="B8" s="57"/>
       <c r="C8" s="3"/>
       <c r="D8" s="5" t="s">
         <v>44</v>
@@ -2113,29 +2089,29 @@
       <c r="E8" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="F8" s="37"/>
-      <c r="G8" s="68"/>
-      <c r="H8" s="62"/>
+      <c r="F8" s="34"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="41"/>
     </row>
     <row r="9" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>21</v>
       </c>
       <c r="B9" s="3"/>
-      <c r="C9" s="35" t="s">
+      <c r="C9" s="33" t="s">
         <v>50</v>
       </c>
-      <c r="D9" s="33" t="s">
+      <c r="D9" s="36" t="s">
         <v>17</v>
       </c>
       <c r="E9" s="63" t="s">
         <v>46</v>
       </c>
-      <c r="F9" s="31" t="s">
+      <c r="F9" s="40" t="s">
         <v>18</v>
       </c>
-      <c r="G9" s="69"/>
-      <c r="H9" s="31" t="s">
+      <c r="G9" s="3"/>
+      <c r="H9" s="40" t="s">
         <v>18</v>
       </c>
     </row>
@@ -2146,24 +2122,24 @@
       <c r="B10" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="C10" s="37"/>
-      <c r="D10" s="34"/>
+      <c r="C10" s="34"/>
+      <c r="D10" s="37"/>
       <c r="E10" s="64"/>
-      <c r="F10" s="32"/>
+      <c r="F10" s="41"/>
       <c r="G10" s="3"/>
-      <c r="H10" s="32"/>
+      <c r="H10" s="41"/>
     </row>
     <row r="11" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B11" s="35" t="s">
+      <c r="B11" s="33" t="s">
         <v>25</v>
       </c>
-      <c r="C11" s="35" t="s">
+      <c r="C11" s="33" t="s">
         <v>56</v>
       </c>
-      <c r="D11" s="35" t="s">
+      <c r="D11" s="33" t="s">
         <v>54</v>
       </c>
       <c r="E11" s="63" t="s">
@@ -2172,59 +2148,55 @@
       <c r="F11" s="63" t="s">
         <v>55</v>
       </c>
-      <c r="G11" s="31" t="s">
-        <v>18</v>
-      </c>
+      <c r="G11" s="3"/>
       <c r="H11" s="3"/>
     </row>
     <row r="12" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="B12" s="36"/>
-      <c r="C12" s="37"/>
-      <c r="D12" s="37"/>
+      <c r="B12" s="35"/>
+      <c r="C12" s="34"/>
+      <c r="D12" s="34"/>
       <c r="E12" s="64"/>
       <c r="F12" s="64"/>
-      <c r="G12" s="32"/>
-      <c r="H12" s="51" t="s">
-        <v>33</v>
+      <c r="G12" s="3"/>
+      <c r="H12" s="40" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B13" s="37"/>
-      <c r="C13" s="42" t="s">
+      <c r="B13" s="34"/>
+      <c r="C13" s="38" t="s">
         <v>28</v>
       </c>
-      <c r="D13" s="44" t="s">
+      <c r="D13" s="46" t="s">
         <v>31</v>
       </c>
       <c r="F13" s="8" t="s">
         <v>42</v>
       </c>
       <c r="G13" s="3"/>
-      <c r="H13" s="52"/>
+      <c r="H13" s="41"/>
     </row>
     <row r="14" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B14" s="65" t="s">
+      <c r="B14" s="59" t="s">
         <v>42</v>
       </c>
-      <c r="C14" s="43"/>
-      <c r="D14" s="45"/>
+      <c r="C14" s="39"/>
+      <c r="D14" s="47"/>
       <c r="E14" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="F14" s="11" t="s">
-        <v>11</v>
-      </c>
+      <c r="F14" s="3"/>
       <c r="G14" s="3"/>
-      <c r="H14" s="61" t="s">
+      <c r="H14" s="65" t="s">
         <v>19</v>
       </c>
     </row>
@@ -2232,7 +2204,7 @@
       <c r="A15" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="B15" s="66"/>
+      <c r="B15" s="60"/>
       <c r="C15" s="9" t="s">
         <v>48</v>
       </c>
@@ -2242,7 +2214,9 @@
       <c r="E15" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="H15" s="62"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3"/>
+      <c r="H15" s="66"/>
     </row>
     <row r="16" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
@@ -2257,11 +2231,9 @@
       <c r="E16" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="F16" s="31" t="s">
+      <c r="F16" s="3"/>
+      <c r="G16" s="40" t="s">
         <v>18</v>
-      </c>
-      <c r="G16" s="59" t="s">
-        <v>44</v>
       </c>
       <c r="H16" s="3"/>
     </row>
@@ -2279,10 +2251,10 @@
         <v>19</v>
       </c>
       <c r="E17" s="3"/>
-      <c r="F17" s="32"/>
-      <c r="G17" s="60"/>
-      <c r="H17" s="61" t="s">
-        <v>19</v>
+      <c r="F17" s="3"/>
+      <c r="G17" s="41"/>
+      <c r="H17" s="40" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -2301,13 +2273,11 @@
       <c r="E18" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="F18" s="31" t="s">
-        <v>18</v>
-      </c>
+      <c r="F18" s="3"/>
       <c r="G18" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="H18" s="62"/>
+      <c r="H18" s="41"/>
     </row>
     <row r="19" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
@@ -2321,39 +2291,36 @@
       </c>
       <c r="D19" s="3"/>
       <c r="E19" s="3"/>
-      <c r="F19" s="32"/>
+      <c r="F19" s="11" t="s">
+        <v>11</v>
+      </c>
       <c r="G19" s="3"/>
       <c r="H19" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="27">
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="D11:D12"/>
-    <mergeCell ref="G7:G9"/>
-    <mergeCell ref="F9:F10"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="C11:C12"/>
-    <mergeCell ref="G11:G12"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="B11:B13"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="G3:G4"/>
-    <mergeCell ref="H7:H8"/>
-    <mergeCell ref="E9:E10"/>
-    <mergeCell ref="D9:D10"/>
-    <mergeCell ref="H9:H10"/>
+  <mergeCells count="22">
     <mergeCell ref="C5:C6"/>
     <mergeCell ref="F6:F8"/>
     <mergeCell ref="C9:C10"/>
     <mergeCell ref="H12:H13"/>
     <mergeCell ref="H17:H18"/>
-    <mergeCell ref="F16:F17"/>
     <mergeCell ref="D13:D14"/>
     <mergeCell ref="G16:G17"/>
     <mergeCell ref="H14:H15"/>
     <mergeCell ref="E11:E12"/>
     <mergeCell ref="F11:F12"/>
-    <mergeCell ref="F18:F19"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="H7:H8"/>
+    <mergeCell ref="E9:E10"/>
+    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="H9:H10"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="F9:F10"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="B11:B13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2364,8 +2331,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68112DEB-F6E4-415D-A916-ADDDEC95DDF2}">
   <dimension ref="A1:H20"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14:G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2432,8 +2399,8 @@
       <c r="C4" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="42" t="s">
-        <v>28</v>
+      <c r="D4" s="48" t="s">
+        <v>18</v>
       </c>
       <c r="E4" s="11" t="s">
         <v>11</v>
@@ -2451,11 +2418,11 @@
       <c r="B5" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="C5" s="35" t="s">
+      <c r="C5" s="33" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="43"/>
-      <c r="E5" s="35" t="s">
+      <c r="D5" s="49"/>
+      <c r="E5" s="33" t="s">
         <v>13</v>
       </c>
       <c r="F5" s="11" t="s">
@@ -2464,7 +2431,7 @@
       <c r="G5" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="H5" s="42" t="s">
+      <c r="H5" s="38" t="s">
         <v>28</v>
       </c>
     </row>
@@ -2475,33 +2442,33 @@
       <c r="B6" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="37"/>
-      <c r="D6" s="61" t="s">
+      <c r="C6" s="34"/>
+      <c r="D6" s="65" t="s">
         <v>19</v>
       </c>
-      <c r="E6" s="37"/>
-      <c r="F6" s="35" t="s">
+      <c r="E6" s="34"/>
+      <c r="F6" s="33" t="s">
         <v>15</v>
       </c>
       <c r="G6" s="3"/>
-      <c r="H6" s="43"/>
+      <c r="H6" s="39"/>
     </row>
     <row r="7" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="33" t="s">
+      <c r="B7" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="59" t="s">
+      <c r="C7" s="67" t="s">
         <v>44</v>
       </c>
-      <c r="D7" s="62"/>
+      <c r="D7" s="66"/>
       <c r="E7" s="23" t="s">
         <v>66</v>
       </c>
-      <c r="F7" s="36"/>
-      <c r="G7" s="46" t="s">
+      <c r="F7" s="35"/>
+      <c r="G7" s="48" t="s">
         <v>18</v>
       </c>
       <c r="H7" s="4" t="s">
@@ -2512,37 +2479,37 @@
       <c r="A8" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="34"/>
-      <c r="C8" s="60"/>
+      <c r="B8" s="37"/>
+      <c r="C8" s="68"/>
       <c r="D8" s="11" t="s">
         <v>11</v>
       </c>
       <c r="E8" s="3"/>
-      <c r="F8" s="37"/>
-      <c r="G8" s="47"/>
+      <c r="F8" s="34"/>
+      <c r="G8" s="49"/>
       <c r="H8" s="3"/>
     </row>
     <row r="9" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B9" s="22" t="s">
-        <v>28</v>
-      </c>
-      <c r="C9" s="33" t="s">
+      <c r="B9" s="25" t="s">
+        <v>67</v>
+      </c>
+      <c r="C9" s="36" t="s">
         <v>22</v>
       </c>
-      <c r="D9" s="33" t="s">
+      <c r="D9" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="E9" s="33" t="s">
+      <c r="E9" s="36" t="s">
         <v>22</v>
       </c>
       <c r="F9" s="24" t="s">
         <v>68</v>
       </c>
-      <c r="G9" s="48"/>
-      <c r="H9" s="70" t="s">
+      <c r="G9" s="50"/>
+      <c r="H9" s="69" t="s">
         <v>68</v>
       </c>
     </row>
@@ -2550,33 +2517,35 @@
       <c r="A10" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B10" s="3"/>
-      <c r="C10" s="34"/>
-      <c r="D10" s="34"/>
-      <c r="E10" s="34"/>
+      <c r="B10" s="15" t="s">
+        <v>69</v>
+      </c>
+      <c r="C10" s="37"/>
+      <c r="D10" s="37"/>
+      <c r="E10" s="37"/>
       <c r="F10" s="26" t="s">
         <v>72</v>
       </c>
       <c r="G10" s="3"/>
-      <c r="H10" s="71"/>
+      <c r="H10" s="70"/>
     </row>
     <row r="11" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B11" s="35" t="s">
+      <c r="B11" s="33" t="s">
         <v>70</v>
       </c>
-      <c r="C11" s="33" t="s">
+      <c r="C11" s="36" t="s">
         <v>26</v>
       </c>
-      <c r="D11" s="33" t="s">
+      <c r="D11" s="36" t="s">
         <v>27</v>
       </c>
-      <c r="E11" s="33" t="s">
+      <c r="E11" s="36" t="s">
         <v>26</v>
       </c>
-      <c r="F11" s="33" t="s">
+      <c r="F11" s="36" t="s">
         <v>27</v>
       </c>
       <c r="G11" s="3"/>
@@ -2586,13 +2555,13 @@
       <c r="A12" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="B12" s="36"/>
-      <c r="C12" s="34"/>
-      <c r="D12" s="34"/>
-      <c r="E12" s="34"/>
-      <c r="F12" s="34"/>
+      <c r="B12" s="35"/>
+      <c r="C12" s="37"/>
+      <c r="D12" s="37"/>
+      <c r="E12" s="37"/>
+      <c r="F12" s="37"/>
       <c r="G12" s="3"/>
-      <c r="H12" s="46" t="s">
+      <c r="H12" s="48" t="s">
         <v>18</v>
       </c>
     </row>
@@ -2600,14 +2569,14 @@
       <c r="A13" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B13" s="37"/>
+      <c r="B13" s="34"/>
       <c r="C13" s="23" t="s">
         <v>66</v>
       </c>
       <c r="D13" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="E13" s="42" t="s">
+      <c r="E13" s="38" t="s">
         <v>28</v>
       </c>
       <c r="F13" s="8" t="s">
@@ -2616,7 +2585,7 @@
       <c r="G13" s="26" t="s">
         <v>72</v>
       </c>
-      <c r="H13" s="47"/>
+      <c r="H13" s="49"/>
     </row>
     <row r="14" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
@@ -2628,14 +2597,14 @@
       <c r="C14" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="D14" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="E14" s="43"/>
+      <c r="D14" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="E14" s="39"/>
       <c r="F14" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="G14" s="61" t="s">
+      <c r="G14" s="65" t="s">
         <v>19</v>
       </c>
       <c r="H14" s="3"/>
@@ -2650,12 +2619,14 @@
       <c r="C15" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="D15" s="3"/>
+      <c r="D15" s="11" t="s">
+        <v>11</v>
+      </c>
       <c r="E15" s="9" t="s">
         <v>48</v>
       </c>
       <c r="F15" s="3"/>
-      <c r="G15" s="62"/>
+      <c r="G15" s="66"/>
       <c r="H15" s="3"/>
     </row>
     <row r="16" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -2668,13 +2639,13 @@
       <c r="C16" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="D16" s="46" t="s">
+      <c r="D16" s="48" t="s">
         <v>18</v>
       </c>
       <c r="E16" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="F16" s="46" t="s">
+      <c r="F16" s="48" t="s">
         <v>18</v>
       </c>
       <c r="G16" s="3"/>
@@ -2692,13 +2663,13 @@
       <c r="C17" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="D17" s="47"/>
+      <c r="D17" s="49"/>
       <c r="E17" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="F17" s="47"/>
+      <c r="F17" s="49"/>
       <c r="G17" s="3"/>
-      <c r="H17" s="59" t="s">
+      <c r="H17" s="67" t="s">
         <v>44</v>
       </c>
     </row>
@@ -2709,27 +2680,27 @@
       <c r="B18" s="25" t="s">
         <v>67</v>
       </c>
-      <c r="C18" s="46" t="s">
+      <c r="C18" s="48" t="s">
         <v>18</v>
       </c>
       <c r="D18" s="24" t="s">
         <v>68</v>
       </c>
-      <c r="E18" s="61" t="s">
+      <c r="E18" s="65" t="s">
         <v>19</v>
       </c>
       <c r="F18" s="3"/>
       <c r="G18" s="3"/>
-      <c r="H18" s="60"/>
+      <c r="H18" s="68"/>
     </row>
     <row r="19" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
         <v>38</v>
       </c>
       <c r="B19" s="3"/>
-      <c r="C19" s="48"/>
+      <c r="C19" s="50"/>
       <c r="D19" s="3"/>
-      <c r="E19" s="62"/>
+      <c r="E19" s="66"/>
       <c r="F19" s="3"/>
       <c r="G19" s="3"/>
       <c r="H19" s="3"/>
@@ -2737,6 +2708,16 @@
     <row r="20" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="26">
+    <mergeCell ref="H5:H6"/>
+    <mergeCell ref="H12:H13"/>
+    <mergeCell ref="H17:H18"/>
+    <mergeCell ref="D16:D17"/>
+    <mergeCell ref="F16:F17"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="G14:G15"/>
+    <mergeCell ref="G7:G9"/>
+    <mergeCell ref="H9:H10"/>
     <mergeCell ref="C18:C19"/>
     <mergeCell ref="C5:C6"/>
     <mergeCell ref="E5:E6"/>
@@ -2753,16 +2734,6 @@
     <mergeCell ref="F11:F12"/>
     <mergeCell ref="E13:E14"/>
     <mergeCell ref="E18:E19"/>
-    <mergeCell ref="H5:H6"/>
-    <mergeCell ref="H12:H13"/>
-    <mergeCell ref="H17:H18"/>
-    <mergeCell ref="D16:D17"/>
-    <mergeCell ref="F16:F17"/>
-    <mergeCell ref="D6:D7"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="G14:G15"/>
-    <mergeCell ref="G7:G9"/>
-    <mergeCell ref="H9:H10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>

</xml_diff>

<commit_message>
Cambio algunas actividades y hora transporte miercoles-viernes S4
</commit_message>
<xml_diff>
--- a/Programar_dias.xlsx
+++ b/Programar_dias.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://udeaeduco-my.sharepoint.com/personal/santiago_vargas5_udea_edu_co/Documents/Estudio/Materias/Informatica II/Calendario_semanal/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Estudio\OneDrive - Universidad de Antioquia\Estudio\Materias\Informatica II\Calendario_semanal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="8" documentId="13_ncr:1_{227E79E7-125C-48EA-A75C-9FF21A2F4D4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C2DC93DA-B6C6-42D1-8E7D-63F522AAAA32}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CAB564A-32C2-4F78-87F5-26242805D36B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="3" xr2:uid="{CC961CB2-F623-4B13-8239-4B70F16E4462}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="77">
   <si>
     <t>LUNES</t>
   </si>
@@ -288,9 +288,6 @@
     <t>Leer</t>
   </si>
   <si>
-    <t>Informe Lab.</t>
-  </si>
-  <si>
     <t>Repaso Info II</t>
   </si>
   <si>
@@ -316,6 +313,12 @@
   </si>
   <si>
     <t>Est Informatica</t>
+  </si>
+  <si>
+    <t>Programar</t>
+  </si>
+  <si>
+    <t>Estudiar Info</t>
   </si>
 </sst>
 </file>
@@ -394,7 +397,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="21">
+  <fills count="20">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -482,12 +485,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -593,7 +590,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="71">
+  <cellXfs count="72">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -663,23 +660,23 @@
     <xf numFmtId="0" fontId="1" fillId="17" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="19" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="20" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -771,10 +768,10 @@
     <xf numFmtId="0" fontId="2" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="20" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="20" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -795,11 +792,14 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="17" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="17" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1564,7 +1564,7 @@
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
-      <c r="F2" s="27"/>
+      <c r="F2" s="26"/>
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
       <c r="J2" t="s">
@@ -1777,7 +1777,7 @@
       <c r="D13" s="46" t="s">
         <v>31</v>
       </c>
-      <c r="E13" s="28" t="s">
+      <c r="E13" s="27" t="s">
         <v>11</v>
       </c>
       <c r="F13" s="58" t="s">
@@ -2005,8 +2005,8 @@
         <v>11</v>
       </c>
       <c r="D4" s="3"/>
-      <c r="E4" s="25" t="s">
-        <v>75</v>
+      <c r="E4" s="24" t="s">
+        <v>74</v>
       </c>
       <c r="F4" s="12" t="s">
         <v>49</v>
@@ -2030,7 +2030,7 @@
         <v>11</v>
       </c>
       <c r="E5" s="18" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F5" s="11" t="s">
         <v>11</v>
@@ -2047,10 +2047,10 @@
       </c>
       <c r="C6" s="34"/>
       <c r="D6" s="18" t="s">
+        <v>73</v>
+      </c>
+      <c r="E6" s="24" t="s">
         <v>74</v>
-      </c>
-      <c r="E6" s="25" t="s">
-        <v>75</v>
       </c>
       <c r="F6" s="33" t="s">
         <v>15</v>
@@ -2241,13 +2241,13 @@
       <c r="A17" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="B17" s="30" t="s">
+      <c r="B17" s="29" t="s">
         <v>19</v>
       </c>
       <c r="C17" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="D17" s="30" t="s">
+      <c r="D17" s="29" t="s">
         <v>19</v>
       </c>
       <c r="E17" s="3"/>
@@ -2262,13 +2262,13 @@
         <v>37</v>
       </c>
       <c r="B18" s="18" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C18" s="18" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D18" s="18" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E18" s="3" t="s">
         <v>52</v>
@@ -2283,10 +2283,10 @@
       <c r="A19" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="B19" s="29" t="s">
-        <v>73</v>
-      </c>
-      <c r="C19" s="30" t="s">
+      <c r="B19" s="28" t="s">
+        <v>72</v>
+      </c>
+      <c r="C19" s="29" t="s">
         <v>19</v>
       </c>
       <c r="D19" s="3"/>
@@ -2331,8 +2331,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68112DEB-F6E4-415D-A916-ADDDEC95DDF2}">
   <dimension ref="A1:H20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14:G15"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2396,17 +2396,12 @@
         <v>9</v>
       </c>
       <c r="B4" s="3"/>
-      <c r="C4" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" s="48" t="s">
-        <v>18</v>
-      </c>
+      <c r="D4" s="3"/>
       <c r="E4" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="F4" s="12" t="s">
-        <v>49</v>
+      <c r="F4" s="11" t="s">
+        <v>11</v>
       </c>
       <c r="G4" s="3"/>
       <c r="H4" s="3"/>
@@ -2421,7 +2416,9 @@
       <c r="C5" s="33" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="49"/>
+      <c r="D5" s="11" t="s">
+        <v>11</v>
+      </c>
       <c r="E5" s="33" t="s">
         <v>13</v>
       </c>
@@ -2443,9 +2440,7 @@
         <v>11</v>
       </c>
       <c r="C6" s="34"/>
-      <c r="D6" s="65" t="s">
-        <v>19</v>
-      </c>
+      <c r="D6" s="3"/>
       <c r="E6" s="34"/>
       <c r="F6" s="33" t="s">
         <v>15</v>
@@ -2460,13 +2455,11 @@
       <c r="B7" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="67" t="s">
-        <v>44</v>
-      </c>
-      <c r="D7" s="66"/>
-      <c r="E7" s="23" t="s">
-        <v>66</v>
-      </c>
+      <c r="C7" s="3"/>
+      <c r="D7" s="48" t="s">
+        <v>18</v>
+      </c>
+      <c r="E7" s="3"/>
       <c r="F7" s="35"/>
       <c r="G7" s="48" t="s">
         <v>18</v>
@@ -2480,10 +2473,10 @@
         <v>20</v>
       </c>
       <c r="B8" s="37"/>
-      <c r="C8" s="68"/>
-      <c r="D8" s="11" t="s">
-        <v>11</v>
-      </c>
+      <c r="C8" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" s="49"/>
       <c r="E8" s="3"/>
       <c r="F8" s="34"/>
       <c r="G8" s="49"/>
@@ -2493,8 +2486,8 @@
       <c r="A9" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B9" s="25" t="s">
-        <v>67</v>
+      <c r="B9" s="24" t="s">
+        <v>66</v>
       </c>
       <c r="C9" s="36" t="s">
         <v>22</v>
@@ -2505,12 +2498,12 @@
       <c r="E9" s="36" t="s">
         <v>22</v>
       </c>
-      <c r="F9" s="24" t="s">
-        <v>68</v>
+      <c r="F9" s="23" t="s">
+        <v>18</v>
       </c>
       <c r="G9" s="50"/>
       <c r="H9" s="69" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -2518,13 +2511,13 @@
         <v>23</v>
       </c>
       <c r="B10" s="15" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C10" s="37"/>
       <c r="D10" s="37"/>
       <c r="E10" s="37"/>
-      <c r="F10" s="26" t="s">
-        <v>72</v>
+      <c r="F10" s="25" t="s">
+        <v>71</v>
       </c>
       <c r="G10" s="3"/>
       <c r="H10" s="70"/>
@@ -2534,7 +2527,7 @@
         <v>24</v>
       </c>
       <c r="B11" s="33" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C11" s="36" t="s">
         <v>26</v>
@@ -2570,20 +2563,20 @@
         <v>30</v>
       </c>
       <c r="B13" s="34"/>
-      <c r="C13" s="23" t="s">
-        <v>66</v>
+      <c r="C13" s="65" t="s">
+        <v>19</v>
       </c>
       <c r="D13" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="E13" s="38" t="s">
-        <v>28</v>
+      <c r="E13" s="65" t="s">
+        <v>19</v>
       </c>
       <c r="F13" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="G13" s="26" t="s">
-        <v>72</v>
+      <c r="G13" s="25" t="s">
+        <v>71</v>
       </c>
       <c r="H13" s="49"/>
     </row>
@@ -2594,15 +2587,13 @@
       <c r="B14" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="C14" s="22" t="s">
-        <v>28</v>
-      </c>
-      <c r="D14" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="E14" s="39"/>
-      <c r="F14" s="11" t="s">
-        <v>11</v>
+      <c r="C14" s="66"/>
+      <c r="D14" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="E14" s="66"/>
+      <c r="F14" s="8" t="s">
+        <v>42</v>
       </c>
       <c r="G14" s="65" t="s">
         <v>19</v>
@@ -2619,8 +2610,8 @@
       <c r="C15" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="D15" s="11" t="s">
-        <v>11</v>
+      <c r="D15" s="48" t="s">
+        <v>18</v>
       </c>
       <c r="E15" s="9" t="s">
         <v>48</v>
@@ -2633,24 +2624,20 @@
       <c r="A16" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="B16" s="24" t="s">
-        <v>68</v>
-      </c>
-      <c r="C16" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="D16" s="48" t="s">
-        <v>18</v>
-      </c>
+      <c r="B16" s="23" t="s">
+        <v>67</v>
+      </c>
+      <c r="C16" s="3"/>
+      <c r="D16" s="49"/>
       <c r="E16" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="F16" s="48" t="s">
-        <v>18</v>
+      <c r="F16" s="11" t="s">
+        <v>11</v>
       </c>
       <c r="G16" s="3"/>
       <c r="H16" s="10" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -2658,16 +2645,14 @@
         <v>36</v>
       </c>
       <c r="B17" s="15" t="s">
-        <v>69</v>
-      </c>
-      <c r="C17" s="12" t="s">
-        <v>49</v>
-      </c>
-      <c r="D17" s="49"/>
-      <c r="E17" s="12" t="s">
-        <v>49</v>
-      </c>
-      <c r="F17" s="49"/>
+        <v>68</v>
+      </c>
+      <c r="C17" s="3"/>
+      <c r="D17" s="65" t="s">
+        <v>19</v>
+      </c>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
       <c r="G17" s="3"/>
       <c r="H17" s="67" t="s">
         <v>44</v>
@@ -2677,19 +2662,19 @@
       <c r="A18" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="B18" s="25" t="s">
-        <v>67</v>
-      </c>
-      <c r="C18" s="48" t="s">
+      <c r="B18" s="24" t="s">
+        <v>66</v>
+      </c>
+      <c r="C18" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="D18" s="66"/>
+      <c r="E18" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="F18" s="48" t="s">
         <v>18</v>
       </c>
-      <c r="D18" s="24" t="s">
-        <v>68</v>
-      </c>
-      <c r="E18" s="65" t="s">
-        <v>19</v>
-      </c>
-      <c r="F18" s="3"/>
       <c r="G18" s="3"/>
       <c r="H18" s="68"/>
     </row>
@@ -2698,32 +2683,30 @@
         <v>38</v>
       </c>
       <c r="B19" s="3"/>
-      <c r="C19" s="50"/>
+      <c r="C19" s="71" t="s">
+        <v>75</v>
+      </c>
       <c r="D19" s="3"/>
-      <c r="E19" s="66"/>
-      <c r="F19" s="3"/>
+      <c r="E19" s="30" t="s">
+        <v>76</v>
+      </c>
+      <c r="F19" s="50"/>
       <c r="G19" s="3"/>
       <c r="H19" s="3"/>
     </row>
     <row r="20" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <mergeCells count="26">
+  <mergeCells count="24">
     <mergeCell ref="H5:H6"/>
     <mergeCell ref="H12:H13"/>
     <mergeCell ref="H17:H18"/>
-    <mergeCell ref="D16:D17"/>
-    <mergeCell ref="F16:F17"/>
-    <mergeCell ref="D6:D7"/>
-    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="F18:F19"/>
     <mergeCell ref="G14:G15"/>
     <mergeCell ref="G7:G9"/>
     <mergeCell ref="H9:H10"/>
-    <mergeCell ref="C18:C19"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="E5:E6"/>
-    <mergeCell ref="F6:F8"/>
+    <mergeCell ref="D15:D16"/>
+    <mergeCell ref="D17:D18"/>
     <mergeCell ref="B7:B8"/>
-    <mergeCell ref="C7:C8"/>
     <mergeCell ref="C9:C10"/>
     <mergeCell ref="D9:D10"/>
     <mergeCell ref="E9:E10"/>
@@ -2731,9 +2714,13 @@
     <mergeCell ref="C11:C12"/>
     <mergeCell ref="D11:D12"/>
     <mergeCell ref="E11:E12"/>
+    <mergeCell ref="E13:E14"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="D7:D8"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="F6:F8"/>
     <mergeCell ref="F11:F12"/>
-    <mergeCell ref="E13:E14"/>
-    <mergeCell ref="E18:E19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>

</xml_diff>

<commit_message>
Actividades realizadas fin de semana 4
</commit_message>
<xml_diff>
--- a/Programar_dias.xlsx
+++ b/Programar_dias.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Estudio\OneDrive - Universidad de Antioquia\Estudio\Materias\Informatica II\Calendario_semanal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CAB564A-32C2-4F78-87F5-26242805D36B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5776509D-3F50-4293-9ED0-EC17D0F4588C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="3" xr2:uid="{CC961CB2-F623-4B13-8239-4B70F16E4462}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="76">
   <si>
     <t>LUNES</t>
   </si>
@@ -298,9 +298,6 @@
   </si>
   <si>
     <t>LAB INFORMÁTICA</t>
-  </si>
-  <si>
-    <t>Repaso Metodos</t>
   </si>
   <si>
     <t>Est. Física.</t>
@@ -590,7 +587,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="72">
+  <cellXfs count="68">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -675,8 +672,62 @@
     <xf numFmtId="0" fontId="1" fillId="19" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -684,82 +735,46 @@
     <xf numFmtId="0" fontId="6" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -768,37 +783,7 @@
     <xf numFmtId="0" fontId="2" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="19" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="19" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1214,13 +1199,13 @@
       <c r="B5" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="33" t="s">
+      <c r="C5" s="35" t="s">
         <v>13</v>
       </c>
       <c r="D5" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="E5" s="33" t="s">
+      <c r="E5" s="35" t="s">
         <v>13</v>
       </c>
       <c r="F5" s="11" t="s">
@@ -1236,12 +1221,12 @@
       <c r="B6" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="34"/>
+      <c r="C6" s="37"/>
       <c r="D6" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="E6" s="34"/>
-      <c r="F6" s="33" t="s">
+      <c r="E6" s="37"/>
+      <c r="F6" s="35" t="s">
         <v>15</v>
       </c>
       <c r="G6" s="3"/>
@@ -1251,17 +1236,17 @@
       <c r="A7" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="36" t="s">
+      <c r="B7" s="33" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="38" t="s">
+      <c r="C7" s="42" t="s">
         <v>28</v>
       </c>
       <c r="D7" s="3"/>
-      <c r="E7" s="31" t="s">
+      <c r="E7" s="49" t="s">
         <v>47</v>
       </c>
-      <c r="F7" s="35"/>
+      <c r="F7" s="36"/>
       <c r="G7" s="3"/>
       <c r="H7" s="4" t="s">
         <v>10</v>
@@ -1271,15 +1256,15 @@
       <c r="A8" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="37"/>
-      <c r="C8" s="39"/>
+      <c r="B8" s="34"/>
+      <c r="C8" s="43"/>
       <c r="D8" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="E8" s="32"/>
-      <c r="F8" s="34"/>
+      <c r="E8" s="50"/>
+      <c r="F8" s="37"/>
       <c r="G8" s="3"/>
-      <c r="H8" s="40" t="s">
+      <c r="H8" s="31" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1290,30 +1275,30 @@
       <c r="B9" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="C9" s="36" t="s">
+      <c r="C9" s="33" t="s">
         <v>22</v>
       </c>
-      <c r="D9" s="36" t="s">
+      <c r="D9" s="33" t="s">
         <v>17</v>
       </c>
-      <c r="E9" s="36" t="s">
+      <c r="E9" s="33" t="s">
         <v>22</v>
       </c>
-      <c r="F9" s="38" t="s">
+      <c r="F9" s="42" t="s">
         <v>28</v>
       </c>
       <c r="G9" s="3"/>
-      <c r="H9" s="41"/>
+      <c r="H9" s="32"/>
     </row>
     <row r="10" spans="1:10" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>23</v>
       </c>
       <c r="B10" s="13"/>
-      <c r="C10" s="37"/>
-      <c r="D10" s="37"/>
-      <c r="E10" s="37"/>
-      <c r="F10" s="39"/>
+      <c r="C10" s="34"/>
+      <c r="D10" s="34"/>
+      <c r="E10" s="34"/>
+      <c r="F10" s="43"/>
       <c r="G10" s="3"/>
       <c r="H10" s="3"/>
     </row>
@@ -1321,23 +1306,23 @@
       <c r="A11" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B11" s="33" t="s">
+      <c r="B11" s="35" t="s">
         <v>25</v>
       </c>
-      <c r="C11" s="36" t="s">
+      <c r="C11" s="33" t="s">
         <v>26</v>
       </c>
-      <c r="D11" s="36" t="s">
+      <c r="D11" s="33" t="s">
         <v>27</v>
       </c>
       <c r="E11" s="3"/>
-      <c r="F11" s="36" t="s">
+      <c r="F11" s="33" t="s">
         <v>54</v>
       </c>
-      <c r="G11" s="31" t="s">
+      <c r="G11" s="49" t="s">
         <v>47</v>
       </c>
-      <c r="H11" s="40" t="s">
+      <c r="H11" s="31" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1345,22 +1330,22 @@
       <c r="A12" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="B12" s="35"/>
-      <c r="C12" s="37"/>
-      <c r="D12" s="37"/>
-      <c r="F12" s="37"/>
-      <c r="G12" s="32"/>
-      <c r="H12" s="41"/>
+      <c r="B12" s="36"/>
+      <c r="C12" s="34"/>
+      <c r="D12" s="34"/>
+      <c r="F12" s="34"/>
+      <c r="G12" s="50"/>
+      <c r="H12" s="32"/>
     </row>
     <row r="13" spans="1:10" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B13" s="34"/>
+      <c r="B13" s="37"/>
       <c r="C13" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="D13" s="46" t="s">
+      <c r="D13" s="44" t="s">
         <v>31</v>
       </c>
       <c r="E13" s="11" t="s">
@@ -1381,10 +1366,10 @@
         <v>11</v>
       </c>
       <c r="C14" s="3"/>
-      <c r="D14" s="47"/>
+      <c r="D14" s="45"/>
       <c r="E14" s="3"/>
       <c r="F14" s="3"/>
-      <c r="G14" s="42" t="s">
+      <c r="G14" s="38" t="s">
         <v>44</v>
       </c>
       <c r="H14" s="3" t="s">
@@ -1397,7 +1382,7 @@
         <v>34</v>
       </c>
       <c r="B15" s="3"/>
-      <c r="C15" s="42" t="s">
+      <c r="C15" s="38" t="s">
         <v>44</v>
       </c>
       <c r="D15" s="14" t="s">
@@ -1405,7 +1390,7 @@
       </c>
       <c r="E15" s="3"/>
       <c r="F15" s="3"/>
-      <c r="G15" s="43"/>
+      <c r="G15" s="39"/>
       <c r="H15" s="11" t="s">
         <v>11</v>
       </c>
@@ -1415,18 +1400,18 @@
         <v>35</v>
       </c>
       <c r="B16" s="3"/>
-      <c r="C16" s="43"/>
+      <c r="C16" s="39"/>
       <c r="D16" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="E16" s="38" t="s">
+      <c r="E16" s="42" t="s">
         <v>28</v>
       </c>
       <c r="F16" s="3"/>
-      <c r="G16" s="48" t="s">
+      <c r="G16" s="46" t="s">
         <v>18</v>
       </c>
-      <c r="H16" s="38" t="s">
+      <c r="H16" s="42" t="s">
         <v>28</v>
       </c>
     </row>
@@ -1439,32 +1424,32 @@
       </c>
       <c r="C17" s="3"/>
       <c r="D17" s="3"/>
-      <c r="E17" s="39"/>
+      <c r="E17" s="43"/>
       <c r="F17" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="G17" s="49"/>
-      <c r="H17" s="39"/>
+      <c r="G17" s="47"/>
+      <c r="H17" s="43"/>
     </row>
     <row r="18" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="B18" s="40" t="s">
+      <c r="B18" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="C18" s="42" t="s">
+      <c r="C18" s="38" t="s">
         <v>44</v>
       </c>
-      <c r="D18" s="44" t="s">
+      <c r="D18" s="40" t="s">
         <v>19</v>
       </c>
-      <c r="E18" s="40" t="s">
+      <c r="E18" s="31" t="s">
         <v>18</v>
       </c>
       <c r="F18" s="3"/>
-      <c r="G18" s="50"/>
-      <c r="H18" s="40" t="s">
+      <c r="G18" s="48"/>
+      <c r="H18" s="31" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1472,16 +1457,28 @@
       <c r="A19" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="B19" s="41"/>
-      <c r="C19" s="43"/>
-      <c r="D19" s="45"/>
-      <c r="E19" s="41"/>
+      <c r="B19" s="32"/>
+      <c r="C19" s="39"/>
+      <c r="D19" s="41"/>
+      <c r="E19" s="32"/>
       <c r="F19" s="3"/>
       <c r="G19" s="3"/>
-      <c r="H19" s="41"/>
+      <c r="H19" s="32"/>
     </row>
   </sheetData>
   <mergeCells count="28">
+    <mergeCell ref="G11:G12"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="F6:F8"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="E9:E10"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="F9:F10"/>
+    <mergeCell ref="E7:E8"/>
     <mergeCell ref="H8:H9"/>
     <mergeCell ref="H11:H12"/>
     <mergeCell ref="B18:B19"/>
@@ -1498,18 +1495,6 @@
     <mergeCell ref="H16:H17"/>
     <mergeCell ref="G14:G15"/>
     <mergeCell ref="G16:G18"/>
-    <mergeCell ref="G11:G12"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="E5:E6"/>
-    <mergeCell ref="F6:F8"/>
-    <mergeCell ref="C11:C12"/>
-    <mergeCell ref="D11:D12"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="D9:D10"/>
-    <mergeCell ref="E9:E10"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="F9:F10"/>
-    <mergeCell ref="E7:E8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1615,20 +1600,20 @@
       <c r="A5" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="40" t="s">
+      <c r="B5" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="33" t="s">
+      <c r="C5" s="35" t="s">
         <v>13</v>
       </c>
       <c r="D5" s="55"/>
-      <c r="E5" s="33" t="s">
+      <c r="E5" s="35" t="s">
         <v>13</v>
       </c>
       <c r="F5" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="G5" s="48" t="s">
+      <c r="G5" s="46" t="s">
         <v>18</v>
       </c>
       <c r="H5" s="4" t="s">
@@ -1642,16 +1627,16 @@
       <c r="A6" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="41"/>
-      <c r="C6" s="34"/>
+      <c r="B6" s="32"/>
+      <c r="C6" s="37"/>
       <c r="D6" s="51" t="s">
         <v>33</v>
       </c>
-      <c r="E6" s="34"/>
-      <c r="F6" s="33" t="s">
+      <c r="E6" s="37"/>
+      <c r="F6" s="35" t="s">
         <v>15</v>
       </c>
-      <c r="G6" s="49"/>
+      <c r="G6" s="47"/>
       <c r="H6" s="3"/>
       <c r="J6" t="s">
         <v>64</v>
@@ -1661,18 +1646,18 @@
       <c r="A7" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="36" t="s">
+      <c r="B7" s="33" t="s">
         <v>17</v>
       </c>
       <c r="C7" s="51" t="s">
         <v>33</v>
       </c>
-      <c r="D7" s="53"/>
+      <c r="D7" s="52"/>
       <c r="E7" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="F7" s="35"/>
-      <c r="G7" s="49"/>
+      <c r="F7" s="36"/>
+      <c r="G7" s="47"/>
       <c r="H7" s="3"/>
       <c r="J7" t="s">
         <v>65</v>
@@ -1682,16 +1667,16 @@
       <c r="A8" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="37"/>
-      <c r="C8" s="53"/>
-      <c r="D8" s="38" t="s">
+      <c r="B8" s="34"/>
+      <c r="C8" s="52"/>
+      <c r="D8" s="42" t="s">
         <v>28</v>
       </c>
       <c r="E8" s="21" t="s">
         <v>52</v>
       </c>
-      <c r="F8" s="34"/>
-      <c r="G8" s="49"/>
+      <c r="F8" s="37"/>
+      <c r="G8" s="47"/>
       <c r="H8" s="51" t="s">
         <v>33</v>
       </c>
@@ -1700,50 +1685,50 @@
       <c r="A9" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B9" s="31" t="s">
+      <c r="B9" s="49" t="s">
         <v>47</v>
       </c>
-      <c r="C9" s="33" t="s">
+      <c r="C9" s="35" t="s">
         <v>50</v>
       </c>
-      <c r="D9" s="39"/>
-      <c r="E9" s="33" t="s">
+      <c r="D9" s="43"/>
+      <c r="E9" s="35" t="s">
         <v>50</v>
       </c>
       <c r="F9" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="G9" s="49"/>
-      <c r="H9" s="52"/>
+      <c r="G9" s="47"/>
+      <c r="H9" s="58"/>
     </row>
     <row r="10" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B10" s="32"/>
-      <c r="C10" s="34"/>
+      <c r="B10" s="50"/>
+      <c r="C10" s="37"/>
       <c r="D10" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="E10" s="34"/>
+      <c r="E10" s="37"/>
       <c r="F10" s="3"/>
-      <c r="G10" s="50"/>
-      <c r="H10" s="53"/>
+      <c r="G10" s="48"/>
+      <c r="H10" s="52"/>
     </row>
     <row r="11" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B11" s="33" t="s">
+      <c r="B11" s="35" t="s">
         <v>25</v>
       </c>
-      <c r="C11" s="33" t="s">
+      <c r="C11" s="35" t="s">
         <v>56</v>
       </c>
-      <c r="D11" s="33" t="s">
+      <c r="D11" s="35" t="s">
         <v>54</v>
       </c>
-      <c r="E11" s="33" t="s">
+      <c r="E11" s="35" t="s">
         <v>56</v>
       </c>
       <c r="F11" s="56" t="s">
@@ -1756,10 +1741,10 @@
       <c r="A12" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="B12" s="35"/>
-      <c r="C12" s="34"/>
-      <c r="D12" s="34"/>
-      <c r="E12" s="34"/>
+      <c r="B12" s="36"/>
+      <c r="C12" s="37"/>
+      <c r="D12" s="37"/>
+      <c r="E12" s="37"/>
       <c r="F12" s="57"/>
       <c r="G12" s="3"/>
       <c r="H12" s="51" t="s">
@@ -1770,34 +1755,34 @@
       <c r="A13" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B13" s="34"/>
+      <c r="B13" s="37"/>
       <c r="C13" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="D13" s="46" t="s">
+      <c r="D13" s="44" t="s">
         <v>31</v>
       </c>
       <c r="E13" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="F13" s="58" t="s">
+      <c r="F13" s="53" t="s">
         <v>42</v>
       </c>
       <c r="G13" s="3"/>
-      <c r="H13" s="53"/>
+      <c r="H13" s="52"/>
     </row>
     <row r="14" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
         <v>32</v>
       </c>
       <c r="B14" s="3"/>
-      <c r="C14" s="38" t="s">
+      <c r="C14" s="42" t="s">
         <v>28</v>
       </c>
-      <c r="D14" s="47"/>
-      <c r="F14" s="58"/>
+      <c r="D14" s="45"/>
+      <c r="F14" s="53"/>
       <c r="G14" s="3"/>
-      <c r="H14" s="48" t="s">
+      <c r="H14" s="46" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1808,14 +1793,14 @@
       <c r="B15" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="C15" s="39"/>
+      <c r="C15" s="43"/>
       <c r="D15" s="3"/>
-      <c r="E15" s="38" t="s">
+      <c r="E15" s="42" t="s">
         <v>28</v>
       </c>
       <c r="F15" s="3"/>
       <c r="G15" s="3"/>
-      <c r="H15" s="50"/>
+      <c r="H15" s="48"/>
     </row>
     <row r="16" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
@@ -1828,7 +1813,7 @@
         <v>44</v>
       </c>
       <c r="D16" s="3"/>
-      <c r="E16" s="39"/>
+      <c r="E16" s="43"/>
       <c r="F16" s="11" t="s">
         <v>11</v>
       </c>
@@ -1844,14 +1829,14 @@
       <c r="D17" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="E17" s="38" t="s">
+      <c r="E17" s="42" t="s">
         <v>28</v>
       </c>
       <c r="F17" s="17" t="s">
         <v>57</v>
       </c>
       <c r="G17" s="3"/>
-      <c r="H17" s="48" t="s">
+      <c r="H17" s="46" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1868,45 +1853,29 @@
       <c r="D18" s="51" t="s">
         <v>33</v>
       </c>
-      <c r="E18" s="39"/>
-      <c r="F18" s="48" t="s">
+      <c r="E18" s="43"/>
+      <c r="F18" s="46" t="s">
         <v>18</v>
       </c>
       <c r="G18" s="3"/>
-      <c r="H18" s="49"/>
+      <c r="H18" s="47"/>
     </row>
     <row r="19" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
         <v>38</v>
       </c>
       <c r="B19" s="3"/>
-      <c r="C19" s="53"/>
-      <c r="D19" s="53"/>
+      <c r="C19" s="52"/>
+      <c r="D19" s="52"/>
       <c r="E19" s="14" t="s">
         <v>53</v>
       </c>
-      <c r="F19" s="50"/>
+      <c r="F19" s="48"/>
       <c r="G19" s="3"/>
-      <c r="H19" s="50"/>
+      <c r="H19" s="48"/>
     </row>
   </sheetData>
   <mergeCells count="32">
-    <mergeCell ref="F18:F19"/>
-    <mergeCell ref="H17:H19"/>
-    <mergeCell ref="C18:C19"/>
-    <mergeCell ref="D13:D14"/>
-    <mergeCell ref="D18:D19"/>
-    <mergeCell ref="E15:E16"/>
-    <mergeCell ref="E17:E18"/>
-    <mergeCell ref="F13:F14"/>
-    <mergeCell ref="B16:B17"/>
-    <mergeCell ref="B11:B13"/>
-    <mergeCell ref="E11:E12"/>
-    <mergeCell ref="D11:D12"/>
-    <mergeCell ref="F11:F12"/>
-    <mergeCell ref="C11:C12"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="C16:C17"/>
     <mergeCell ref="G5:G10"/>
     <mergeCell ref="H8:H10"/>
     <mergeCell ref="H12:H13"/>
@@ -1923,6 +1892,22 @@
     <mergeCell ref="C5:C6"/>
     <mergeCell ref="E5:E6"/>
     <mergeCell ref="F6:F8"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="B11:B13"/>
+    <mergeCell ref="E11:E12"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="F11:F12"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="C16:C17"/>
+    <mergeCell ref="F18:F19"/>
+    <mergeCell ref="H17:H19"/>
+    <mergeCell ref="C18:C19"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="D18:D19"/>
+    <mergeCell ref="E15:E16"/>
+    <mergeCell ref="E17:E18"/>
+    <mergeCell ref="F13:F14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1977,7 +1962,7 @@
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
-      <c r="E2" s="61" t="s">
+      <c r="E2" s="63" t="s">
         <v>19</v>
       </c>
       <c r="F2" s="3"/>
@@ -1991,7 +1976,7 @@
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
-      <c r="E3" s="62"/>
+      <c r="E3" s="64"/>
       <c r="F3" s="3"/>
       <c r="G3" s="3"/>
       <c r="H3" s="3"/>
@@ -2006,7 +1991,7 @@
       </c>
       <c r="D4" s="3"/>
       <c r="E4" s="24" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F4" s="12" t="s">
         <v>49</v>
@@ -2023,14 +2008,14 @@
       <c r="B5" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="C5" s="33" t="s">
+      <c r="C5" s="35" t="s">
         <v>13</v>
       </c>
       <c r="D5" s="11" t="s">
         <v>11</v>
       </c>
       <c r="E5" s="18" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F5" s="11" t="s">
         <v>11</v>
@@ -2045,14 +2030,14 @@
       <c r="B6" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="34"/>
+      <c r="C6" s="37"/>
       <c r="D6" s="18" t="s">
+        <v>72</v>
+      </c>
+      <c r="E6" s="24" t="s">
         <v>73</v>
       </c>
-      <c r="E6" s="24" t="s">
-        <v>74</v>
-      </c>
-      <c r="F6" s="33" t="s">
+      <c r="F6" s="35" t="s">
         <v>15</v>
       </c>
       <c r="G6" s="3"/>
@@ -2071,9 +2056,9 @@
       <c r="D7" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="F7" s="35"/>
+      <c r="F7" s="36"/>
       <c r="G7" s="3"/>
-      <c r="H7" s="40" t="s">
+      <c r="H7" s="31" t="s">
         <v>18</v>
       </c>
     </row>
@@ -2089,29 +2074,29 @@
       <c r="E8" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="F8" s="34"/>
+      <c r="F8" s="37"/>
       <c r="G8" s="3"/>
-      <c r="H8" s="41"/>
+      <c r="H8" s="32"/>
     </row>
     <row r="9" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>21</v>
       </c>
       <c r="B9" s="3"/>
-      <c r="C9" s="33" t="s">
+      <c r="C9" s="35" t="s">
         <v>50</v>
       </c>
-      <c r="D9" s="36" t="s">
+      <c r="D9" s="33" t="s">
         <v>17</v>
       </c>
-      <c r="E9" s="63" t="s">
+      <c r="E9" s="61" t="s">
         <v>46</v>
       </c>
-      <c r="F9" s="40" t="s">
+      <c r="F9" s="31" t="s">
         <v>18</v>
       </c>
       <c r="G9" s="3"/>
-      <c r="H9" s="40" t="s">
+      <c r="H9" s="31" t="s">
         <v>18</v>
       </c>
     </row>
@@ -2122,30 +2107,30 @@
       <c r="B10" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="C10" s="34"/>
-      <c r="D10" s="37"/>
-      <c r="E10" s="64"/>
-      <c r="F10" s="41"/>
+      <c r="C10" s="37"/>
+      <c r="D10" s="34"/>
+      <c r="E10" s="62"/>
+      <c r="F10" s="32"/>
       <c r="G10" s="3"/>
-      <c r="H10" s="41"/>
+      <c r="H10" s="32"/>
     </row>
     <row r="11" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B11" s="33" t="s">
+      <c r="B11" s="35" t="s">
         <v>25</v>
       </c>
-      <c r="C11" s="33" t="s">
+      <c r="C11" s="35" t="s">
         <v>56</v>
       </c>
-      <c r="D11" s="33" t="s">
+      <c r="D11" s="35" t="s">
         <v>54</v>
       </c>
-      <c r="E11" s="63" t="s">
+      <c r="E11" s="61" t="s">
         <v>45</v>
       </c>
-      <c r="F11" s="63" t="s">
+      <c r="F11" s="61" t="s">
         <v>55</v>
       </c>
       <c r="G11" s="3"/>
@@ -2155,13 +2140,13 @@
       <c r="A12" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="B12" s="35"/>
-      <c r="C12" s="34"/>
-      <c r="D12" s="34"/>
-      <c r="E12" s="64"/>
-      <c r="F12" s="64"/>
+      <c r="B12" s="36"/>
+      <c r="C12" s="37"/>
+      <c r="D12" s="37"/>
+      <c r="E12" s="62"/>
+      <c r="F12" s="62"/>
       <c r="G12" s="3"/>
-      <c r="H12" s="40" t="s">
+      <c r="H12" s="31" t="s">
         <v>18</v>
       </c>
     </row>
@@ -2169,34 +2154,34 @@
       <c r="A13" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B13" s="34"/>
-      <c r="C13" s="38" t="s">
+      <c r="B13" s="37"/>
+      <c r="C13" s="42" t="s">
         <v>28</v>
       </c>
-      <c r="D13" s="46" t="s">
+      <c r="D13" s="44" t="s">
         <v>31</v>
       </c>
       <c r="F13" s="8" t="s">
         <v>42</v>
       </c>
       <c r="G13" s="3"/>
-      <c r="H13" s="41"/>
+      <c r="H13" s="32"/>
     </row>
     <row r="14" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B14" s="59" t="s">
+      <c r="B14" s="65" t="s">
         <v>42</v>
       </c>
-      <c r="C14" s="39"/>
-      <c r="D14" s="47"/>
+      <c r="C14" s="43"/>
+      <c r="D14" s="45"/>
       <c r="E14" s="22" t="s">
         <v>28</v>
       </c>
       <c r="F14" s="3"/>
       <c r="G14" s="3"/>
-      <c r="H14" s="65" t="s">
+      <c r="H14" s="59" t="s">
         <v>19</v>
       </c>
     </row>
@@ -2204,7 +2189,7 @@
       <c r="A15" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="B15" s="60"/>
+      <c r="B15" s="66"/>
       <c r="C15" s="9" t="s">
         <v>48</v>
       </c>
@@ -2216,7 +2201,7 @@
       </c>
       <c r="F15" s="3"/>
       <c r="G15" s="3"/>
-      <c r="H15" s="66"/>
+      <c r="H15" s="60"/>
     </row>
     <row r="16" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
@@ -2232,7 +2217,7 @@
         <v>11</v>
       </c>
       <c r="F16" s="3"/>
-      <c r="G16" s="40" t="s">
+      <c r="G16" s="31" t="s">
         <v>18</v>
       </c>
       <c r="H16" s="3"/>
@@ -2252,8 +2237,8 @@
       </c>
       <c r="E17" s="3"/>
       <c r="F17" s="3"/>
-      <c r="G17" s="41"/>
-      <c r="H17" s="40" t="s">
+      <c r="G17" s="32"/>
+      <c r="H17" s="31" t="s">
         <v>18</v>
       </c>
     </row>
@@ -2262,13 +2247,13 @@
         <v>37</v>
       </c>
       <c r="B18" s="18" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C18" s="18" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D18" s="18" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E18" s="3" t="s">
         <v>52</v>
@@ -2277,14 +2262,14 @@
       <c r="G18" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="H18" s="41"/>
+      <c r="H18" s="32"/>
     </row>
     <row r="19" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
         <v>38</v>
       </c>
       <c r="B19" s="28" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C19" s="29" t="s">
         <v>19</v>
@@ -2299,6 +2284,18 @@
     </row>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="F9:F10"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="B11:B13"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="H7:H8"/>
+    <mergeCell ref="E9:E10"/>
+    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="H9:H10"/>
     <mergeCell ref="C5:C6"/>
     <mergeCell ref="F6:F8"/>
     <mergeCell ref="C9:C10"/>
@@ -2309,18 +2306,6 @@
     <mergeCell ref="H14:H15"/>
     <mergeCell ref="E11:E12"/>
     <mergeCell ref="F11:F12"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="H7:H8"/>
-    <mergeCell ref="E9:E10"/>
-    <mergeCell ref="D9:D10"/>
-    <mergeCell ref="H9:H10"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="D11:D12"/>
-    <mergeCell ref="F9:F10"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="C11:C12"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="B11:B13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2331,8 +2316,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68112DEB-F6E4-415D-A916-ADDDEC95DDF2}">
   <dimension ref="A1:H20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2413,13 +2398,13 @@
       <c r="B5" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="C5" s="33" t="s">
+      <c r="C5" s="35" t="s">
         <v>13</v>
       </c>
       <c r="D5" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="33" t="s">
+      <c r="E5" s="35" t="s">
         <v>13</v>
       </c>
       <c r="F5" s="11" t="s">
@@ -2428,8 +2413,8 @@
       <c r="G5" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="H5" s="38" t="s">
-        <v>28</v>
+      <c r="H5" s="46" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -2439,48 +2424,48 @@
       <c r="B6" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="34"/>
+      <c r="C6" s="37"/>
       <c r="D6" s="3"/>
-      <c r="E6" s="34"/>
-      <c r="F6" s="33" t="s">
+      <c r="E6" s="37"/>
+      <c r="F6" s="35" t="s">
         <v>15</v>
       </c>
       <c r="G6" s="3"/>
-      <c r="H6" s="39"/>
+      <c r="H6" s="47"/>
     </row>
     <row r="7" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="36" t="s">
+      <c r="B7" s="33" t="s">
         <v>17</v>
       </c>
       <c r="C7" s="3"/>
-      <c r="D7" s="48" t="s">
+      <c r="D7" s="46" t="s">
         <v>18</v>
       </c>
       <c r="E7" s="3"/>
-      <c r="F7" s="35"/>
-      <c r="G7" s="48" t="s">
+      <c r="F7" s="36"/>
+      <c r="G7" s="46" t="s">
         <v>18</v>
       </c>
-      <c r="H7" s="4" t="s">
-        <v>10</v>
-      </c>
+      <c r="H7" s="3"/>
     </row>
     <row r="8" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="37"/>
+      <c r="B8" s="34"/>
       <c r="C8" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="D8" s="49"/>
+      <c r="D8" s="47"/>
       <c r="E8" s="3"/>
-      <c r="F8" s="34"/>
-      <c r="G8" s="49"/>
-      <c r="H8" s="3"/>
+      <c r="F8" s="37"/>
+      <c r="G8" s="47"/>
+      <c r="H8" s="4" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="9" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
@@ -2489,21 +2474,21 @@
       <c r="B9" s="24" t="s">
         <v>66</v>
       </c>
-      <c r="C9" s="36" t="s">
+      <c r="C9" s="33" t="s">
         <v>22</v>
       </c>
-      <c r="D9" s="36" t="s">
+      <c r="D9" s="33" t="s">
         <v>17</v>
       </c>
-      <c r="E9" s="36" t="s">
+      <c r="E9" s="33" t="s">
         <v>22</v>
       </c>
       <c r="F9" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="G9" s="50"/>
-      <c r="H9" s="69" t="s">
-        <v>67</v>
+      <c r="G9" s="48"/>
+      <c r="H9" s="46" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -2513,72 +2498,72 @@
       <c r="B10" s="15" t="s">
         <v>68</v>
       </c>
-      <c r="C10" s="37"/>
-      <c r="D10" s="37"/>
-      <c r="E10" s="37"/>
+      <c r="C10" s="34"/>
+      <c r="D10" s="34"/>
+      <c r="E10" s="34"/>
       <c r="F10" s="25" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G10" s="3"/>
-      <c r="H10" s="70"/>
+      <c r="H10" s="47"/>
     </row>
     <row r="11" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B11" s="33" t="s">
+      <c r="B11" s="35" t="s">
         <v>69</v>
       </c>
-      <c r="C11" s="36" t="s">
+      <c r="C11" s="33" t="s">
         <v>26</v>
       </c>
-      <c r="D11" s="36" t="s">
+      <c r="D11" s="33" t="s">
         <v>27</v>
       </c>
-      <c r="E11" s="36" t="s">
+      <c r="E11" s="33" t="s">
         <v>26</v>
       </c>
-      <c r="F11" s="36" t="s">
+      <c r="F11" s="33" t="s">
         <v>27</v>
       </c>
-      <c r="G11" s="3"/>
+      <c r="G11" s="46" t="s">
+        <v>18</v>
+      </c>
       <c r="H11" s="3"/>
     </row>
     <row r="12" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="B12" s="35"/>
-      <c r="C12" s="37"/>
-      <c r="D12" s="37"/>
-      <c r="E12" s="37"/>
-      <c r="F12" s="37"/>
-      <c r="G12" s="3"/>
-      <c r="H12" s="48" t="s">
-        <v>18</v>
-      </c>
+      <c r="B12" s="36"/>
+      <c r="C12" s="34"/>
+      <c r="D12" s="34"/>
+      <c r="E12" s="34"/>
+      <c r="F12" s="34"/>
+      <c r="G12" s="47"/>
+      <c r="H12" s="3"/>
     </row>
     <row r="13" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B13" s="34"/>
-      <c r="C13" s="65" t="s">
+      <c r="B13" s="37"/>
+      <c r="C13" s="59" t="s">
         <v>19</v>
       </c>
       <c r="D13" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="E13" s="65" t="s">
+      <c r="E13" s="59" t="s">
         <v>19</v>
       </c>
       <c r="F13" s="8" t="s">
         <v>42</v>
       </c>
       <c r="G13" s="25" t="s">
-        <v>71</v>
-      </c>
-      <c r="H13" s="49"/>
+        <v>70</v>
+      </c>
+      <c r="H13" s="3"/>
     </row>
     <row r="14" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
@@ -2587,15 +2572,15 @@
       <c r="B14" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="C14" s="66"/>
+      <c r="C14" s="60"/>
       <c r="D14" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="E14" s="66"/>
+      <c r="E14" s="60"/>
       <c r="F14" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="G14" s="65" t="s">
+      <c r="G14" s="67" t="s">
         <v>19</v>
       </c>
       <c r="H14" s="3"/>
@@ -2610,14 +2595,16 @@
       <c r="C15" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="D15" s="48" t="s">
+      <c r="D15" s="46" t="s">
         <v>18</v>
       </c>
       <c r="E15" s="9" t="s">
         <v>48</v>
       </c>
       <c r="F15" s="3"/>
-      <c r="G15" s="66"/>
+      <c r="G15" s="46" t="s">
+        <v>18</v>
+      </c>
       <c r="H15" s="3"/>
     </row>
     <row r="16" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -2628,17 +2615,15 @@
         <v>67</v>
       </c>
       <c r="C16" s="3"/>
-      <c r="D16" s="49"/>
+      <c r="D16" s="47"/>
       <c r="E16" s="11" t="s">
         <v>11</v>
       </c>
       <c r="F16" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="G16" s="3"/>
-      <c r="H16" s="10" t="s">
-        <v>70</v>
-      </c>
+      <c r="G16" s="47"/>
+      <c r="H16" s="3"/>
     </row>
     <row r="17" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
@@ -2648,15 +2633,13 @@
         <v>68</v>
       </c>
       <c r="C17" s="3"/>
-      <c r="D17" s="65" t="s">
+      <c r="D17" s="59" t="s">
         <v>19</v>
       </c>
       <c r="E17" s="3"/>
       <c r="F17" s="3"/>
       <c r="G17" s="3"/>
-      <c r="H17" s="67" t="s">
-        <v>44</v>
-      </c>
+      <c r="H17" s="3"/>
     </row>
     <row r="18" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
@@ -2668,47 +2651,40 @@
       <c r="C18" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="D18" s="66"/>
+      <c r="D18" s="60"/>
       <c r="E18" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="F18" s="48" t="s">
+      <c r="F18" s="46" t="s">
         <v>18</v>
       </c>
       <c r="G18" s="3"/>
-      <c r="H18" s="68"/>
+      <c r="H18" s="3"/>
     </row>
     <row r="19" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
         <v>38</v>
       </c>
       <c r="B19" s="3"/>
-      <c r="C19" s="71" t="s">
-        <v>75</v>
+      <c r="C19" s="30" t="s">
+        <v>74</v>
       </c>
       <c r="D19" s="3"/>
       <c r="E19" s="30" t="s">
-        <v>76</v>
-      </c>
-      <c r="F19" s="50"/>
+        <v>75</v>
+      </c>
+      <c r="F19" s="48"/>
       <c r="G19" s="3"/>
       <c r="H19" s="3"/>
     </row>
     <row r="20" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <mergeCells count="24">
-    <mergeCell ref="H5:H6"/>
-    <mergeCell ref="H12:H13"/>
-    <mergeCell ref="H17:H18"/>
-    <mergeCell ref="F18:F19"/>
-    <mergeCell ref="G14:G15"/>
-    <mergeCell ref="G7:G9"/>
-    <mergeCell ref="H9:H10"/>
-    <mergeCell ref="D15:D16"/>
-    <mergeCell ref="D17:D18"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="D9:D10"/>
+  <mergeCells count="23">
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="F6:F8"/>
+    <mergeCell ref="F11:F12"/>
+    <mergeCell ref="G15:G16"/>
     <mergeCell ref="E9:E10"/>
     <mergeCell ref="B11:B13"/>
     <mergeCell ref="C11:C12"/>
@@ -2716,11 +2692,17 @@
     <mergeCell ref="E11:E12"/>
     <mergeCell ref="E13:E14"/>
     <mergeCell ref="C13:C14"/>
+    <mergeCell ref="D15:D16"/>
+    <mergeCell ref="D17:D18"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="D9:D10"/>
     <mergeCell ref="D7:D8"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="E5:E6"/>
-    <mergeCell ref="F6:F8"/>
-    <mergeCell ref="F11:F12"/>
+    <mergeCell ref="H5:H6"/>
+    <mergeCell ref="H9:H10"/>
+    <mergeCell ref="F18:F19"/>
+    <mergeCell ref="G7:G9"/>
+    <mergeCell ref="G11:G12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>

</xml_diff>